<commit_message>
Update Excel files from OneDrive - Tue May  6 19:52:10 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Solar_Lab_Tests.xlsx
+++ b/data/Solar_Lab_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E4810376-5079-480C-AD5D-EDB4AC25BA17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A86C8BB-C392-4523-BE15-10DAC8F43D23}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="1" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
   </bookViews>
@@ -961,8 +961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9401EE47-EA52-49C7-BBC0-21F5B88254FB}">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -975,7 +975,7 @@
     <col min="6" max="6" width="27.42578125" customWidth="1"/>
     <col min="7" max="7" width="16.140625" customWidth="1"/>
     <col min="8" max="8" width="14.140625" customWidth="1"/>
-    <col min="11" max="11" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.140625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Tue May  6 20:11:53 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Solar_Lab_Tests.xlsx
+++ b/data/Solar_Lab_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A86C8BB-C392-4523-BE15-10DAC8F43D23}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{30D2FC72-894E-4CDB-A39E-82F54409F0E7}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="1" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
   </bookViews>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="51">
   <si>
     <t>BOM</t>
   </si>
@@ -962,7 +962,7 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K1048576"/>
+      <selection activeCell="A25" sqref="A25:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -1627,30 +1627,10 @@
       </c>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B25" t="s">
-        <v>4</v>
-      </c>
-      <c r="C25" t="s">
-        <v>38</v>
-      </c>
-      <c r="D25" s="5">
-        <v>45759</v>
-      </c>
-      <c r="E25" s="4">
-        <v>45760</v>
-      </c>
-      <c r="F25" s="4">
-        <v>45761</v>
-      </c>
-      <c r="G25" t="s">
-        <v>32</v>
-      </c>
-      <c r="H25" t="s">
-        <v>33</v>
-      </c>
+      <c r="A25" s="1"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
     </row>
   </sheetData>
   <dataValidations count="1">

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Wed May  7 02:01:50 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Solar_Lab_Tests.xlsx
+++ b/data/Solar_Lab_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5B482A4F-3899-4504-A526-7475FF5C9440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{30D2FC72-894E-4CDB-A39E-82F54409F0E7}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="1" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
   </bookViews>
@@ -962,7 +962,7 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="A25" sqref="A25:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Wed May  7 12:54:00 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Solar_Lab_Tests.xlsx
+++ b/data/Solar_Lab_Tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4207DB06-6DF1-4386-AF13-B1449D37FC42}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{64B65780-BA01-49CD-955B-374C9A8E6489}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="2" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="3" activeTab="1" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Tests Map" sheetId="4" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="51">
   <si>
     <t>BOM</t>
   </si>
@@ -280,7 +280,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -289,7 +289,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -957,6 +956,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="6mAsTuNaFVeCD5g+zbw63AhnzTXD72yi1ghX1shFf5OE2p770Axyvf9L1MPcgHvGMKh+VHB60tcSvrXxFx403w==" saltValue="zXriFu7oaSJJokxkPEralw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -968,8 +968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9401EE47-EA52-49C7-BBC0-21F5B88254FB}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -1640,18 +1640,7 @@
       <c r="F25" s="4"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D26" s="7"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
+      <c r="D26" s="6"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -1706,8 +1695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17D43621-542F-4136-850B-43C25D2B7AAC}">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -2013,6 +2002,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="4JQc9cXYgqGOBT7i/JzzwM1CBuwHcEJ6svmyBfMIe1WAFxRFVcs53eHYdDEVQr4rzqRCBTaSvFyrCctY+I4fSg==" saltValue="C/yLHIjqvs+VWwjVoYsMbA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Wed May  7 16:26:05 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Solar_Lab_Tests.xlsx
+++ b/data/Solar_Lab_Tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{64B65780-BA01-49CD-955B-374C9A8E6489}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F14A1647-B4C9-4373-B76F-01045A2FE648}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="3" activeTab="1" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="1" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Tests Map" sheetId="4" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="51">
   <si>
     <t>BOM</t>
   </si>
@@ -969,7 +969,7 @@
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:XFD26"/>
+      <selection activeCell="A24" sqref="A24:H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -1608,30 +1608,10 @@
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B24" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24" t="s">
-        <v>37</v>
-      </c>
-      <c r="D24" s="5">
-        <v>45770</v>
-      </c>
-      <c r="E24" s="4">
-        <v>45771</v>
-      </c>
-      <c r="F24" s="4">
-        <v>45772</v>
-      </c>
-      <c r="G24" t="s">
-        <v>35</v>
-      </c>
-      <c r="H24" t="s">
-        <v>36</v>
-      </c>
+      <c r="A24" s="1"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="1"/>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Thu May  8 07:45:52 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Solar_Lab_Tests.xlsx
+++ b/data/Solar_Lab_Tests.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28906"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F14A1647-B4C9-4373-B76F-01045A2FE648}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F0FED20F-30E0-442C-B2C0-663B5D7742D1}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="1" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
   </bookViews>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="51">
   <si>
     <t>BOM</t>
   </si>
@@ -968,8 +968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9401EE47-EA52-49C7-BBC0-21F5B88254FB}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:H24"/>
+    <sheetView tabSelected="1" topLeftCell="G13" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:Z23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -1582,30 +1582,10 @@
       </c>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B23" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" t="s">
-        <v>41</v>
-      </c>
-      <c r="D23" s="5">
-        <v>45767</v>
-      </c>
-      <c r="E23" s="4">
-        <v>45768</v>
-      </c>
-      <c r="F23" s="4">
-        <v>45769</v>
-      </c>
-      <c r="G23" t="s">
-        <v>32</v>
-      </c>
-      <c r="H23" t="s">
-        <v>33</v>
-      </c>
+      <c r="A23" s="1"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="1"/>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Mon May 26 09:57:27 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Solar_Lab_Tests.xlsx
+++ b/data/Solar_Lab_Tests.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28906"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28922"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F0FED20F-30E0-442C-B2C0-663B5D7742D1}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CBE38A9B-BED4-445C-87BA-31604447B4FF}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="1" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
   </bookViews>
@@ -220,9 +220,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
-  </numFmts>
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -280,16 +277,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -313,7 +307,7 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -968,8 +962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9401EE47-EA52-49C7-BBC0-21F5B88254FB}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G13" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:Z23"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -1600,7 +1594,7 @@
       <c r="F25" s="4"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="D26" s="6"/>
+      <c r="D26" s="5"/>
     </row>
   </sheetData>
   <dataValidations count="1">

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Mon May 26 13:43:58 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Solar_Lab_Tests.xlsx
+++ b/data/Solar_Lab_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CBE38A9B-BED4-445C-87BA-31604447B4FF}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{79B6E4EA-35C4-4835-B51A-C9FD80B5C669}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="1" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
   </bookViews>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="47">
   <si>
     <t>BOM</t>
   </si>
@@ -153,10 +153,34 @@
     <t>STATUS</t>
   </si>
   <si>
-    <t>Vendor A</t>
-  </si>
-  <si>
-    <t>15/04/2025</t>
+    <t>HIUV</t>
+  </si>
+  <si>
+    <t>SUNBEZ</t>
+  </si>
+  <si>
+    <t>GLASS</t>
+  </si>
+  <si>
+    <t>FRAME</t>
+  </si>
+  <si>
+    <t>WHITE SEALANT</t>
+  </si>
+  <si>
+    <t>RM Type</t>
+  </si>
+  <si>
+    <t>Test Type</t>
+  </si>
+  <si>
+    <t>Vendor Names</t>
+  </si>
+  <si>
+    <t>Test Results</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
   <si>
     <t>Pass</t>
@@ -165,52 +189,16 @@
     <t>Completed</t>
   </si>
   <si>
-    <t>Vendor B</t>
-  </si>
-  <si>
     <t>Pending</t>
   </si>
   <si>
     <t>In Progress</t>
   </si>
   <si>
-    <t>Vendor C</t>
-  </si>
-  <si>
-    <t>Vendor D</t>
-  </si>
-  <si>
     <t>Fail</t>
   </si>
   <si>
     <t>Failed</t>
-  </si>
-  <si>
-    <t>Vendor E</t>
-  </si>
-  <si>
-    <t>GLASS</t>
-  </si>
-  <si>
-    <t>FRAME</t>
-  </si>
-  <si>
-    <t>WHITE SEALANT</t>
-  </si>
-  <si>
-    <t>RM Type</t>
-  </si>
-  <si>
-    <t>Test Type</t>
-  </si>
-  <si>
-    <t>Vendor Names</t>
-  </si>
-  <si>
-    <t>Test Results</t>
-  </si>
-  <si>
-    <t>Status</t>
   </si>
   <si>
     <t>STANDARD DURATION (DAYS)</t>
@@ -307,7 +295,7 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -962,8 +950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9401EE47-EA52-49C7-BBC0-21F5B88254FB}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -1010,78 +998,48 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" s="4">
-        <v>45763</v>
-      </c>
-      <c r="F2" s="4">
-        <v>45765</v>
-      </c>
-      <c r="G2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H2" t="s">
-        <v>33</v>
-      </c>
+      <c r="D2" s="5">
+        <v>45773</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D3" s="5">
-        <v>45767</v>
-      </c>
-      <c r="E3" s="4">
-        <v>45768</v>
-      </c>
-      <c r="F3" s="4">
-        <v>45770</v>
-      </c>
-      <c r="G3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H3" t="s">
-        <v>36</v>
-      </c>
+        <v>45773</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D4" s="5">
-        <v>45764</v>
-      </c>
-      <c r="E4" s="4">
-        <v>45765</v>
-      </c>
-      <c r="F4" s="4">
-        <v>45766</v>
-      </c>
-      <c r="G4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H4" t="s">
-        <v>33</v>
-      </c>
+        <v>45777</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="1" t="s">
@@ -1091,516 +1049,167 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D5" s="5">
-        <v>45769</v>
-      </c>
-      <c r="E5" s="4">
-        <v>45770</v>
-      </c>
-      <c r="F5" s="4">
-        <v>45773</v>
-      </c>
-      <c r="G5" t="s">
-        <v>35</v>
-      </c>
-      <c r="H5" t="s">
-        <v>36</v>
-      </c>
+        <v>45777</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="5">
-        <v>45760</v>
-      </c>
-      <c r="E6" s="4">
-        <v>45761</v>
-      </c>
-      <c r="F6" s="4">
-        <v>45762</v>
-      </c>
-      <c r="G6" t="s">
-        <v>32</v>
-      </c>
-      <c r="H6" t="s">
-        <v>33</v>
-      </c>
+      <c r="A6" s="1"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7" s="5">
-        <v>45759</v>
-      </c>
-      <c r="E7" s="4">
-        <v>45761</v>
-      </c>
-      <c r="F7" s="4">
-        <v>45764</v>
-      </c>
-      <c r="G7" t="s">
-        <v>39</v>
-      </c>
-      <c r="H7" t="s">
-        <v>40</v>
-      </c>
+      <c r="A7" s="1"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" s="5">
-        <v>45762</v>
-      </c>
-      <c r="E8" s="4">
-        <v>45763</v>
-      </c>
-      <c r="F8" s="4">
-        <v>45766</v>
-      </c>
-      <c r="G8" t="s">
-        <v>32</v>
-      </c>
-      <c r="H8" t="s">
-        <v>33</v>
-      </c>
+      <c r="A8" s="1"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
       <c r="K8" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="5">
-        <v>45765</v>
-      </c>
-      <c r="E9" s="4">
-        <v>45766</v>
-      </c>
-      <c r="F9" s="4">
-        <v>45767</v>
-      </c>
-      <c r="G9" t="s">
-        <v>32</v>
-      </c>
-      <c r="H9" t="s">
-        <v>33</v>
-      </c>
+      <c r="A9" s="1"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
       <c r="K9" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="5">
-        <v>45772</v>
-      </c>
-      <c r="E10" s="4">
-        <v>45773</v>
-      </c>
-      <c r="F10" s="4">
-        <v>45776</v>
-      </c>
-      <c r="G10" t="s">
-        <v>35</v>
-      </c>
-      <c r="H10" t="s">
-        <v>35</v>
-      </c>
+      <c r="A10" s="1"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
       <c r="K10" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="5">
-        <v>45761</v>
-      </c>
-      <c r="E11" s="4">
-        <v>45762</v>
-      </c>
-      <c r="F11" s="4">
-        <v>45763</v>
-      </c>
-      <c r="G11" t="s">
-        <v>32</v>
-      </c>
-      <c r="H11" t="s">
-        <v>33</v>
-      </c>
+      <c r="A11" s="1"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
       <c r="K11" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="5">
-        <v>45765</v>
-      </c>
-      <c r="E12" s="4">
-        <v>45766</v>
-      </c>
-      <c r="F12" s="4">
-        <v>45769</v>
-      </c>
-      <c r="G12" t="s">
+      <c r="A12" s="1"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="K12" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="1"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="K13" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="H12" t="s">
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="1"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="K14" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="K12" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="A13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="5">
-        <v>45763</v>
-      </c>
-      <c r="E13" s="4">
-        <v>45764</v>
-      </c>
-      <c r="F13" s="4">
-        <v>45767</v>
-      </c>
-      <c r="G13" t="s">
-        <v>32</v>
-      </c>
-      <c r="H13" t="s">
-        <v>33</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="A14" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="5">
-        <v>45757</v>
-      </c>
-      <c r="E14" s="4">
-        <v>45758</v>
-      </c>
-      <c r="F14" s="4">
-        <v>45763</v>
-      </c>
-      <c r="G14" t="s">
-        <v>32</v>
-      </c>
-      <c r="H14" t="s">
-        <v>33</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="A15" s="1"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="K15" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="5">
-        <v>45769</v>
-      </c>
-      <c r="E15" s="4">
-        <v>45770</v>
-      </c>
-      <c r="F15" s="4">
-        <v>45773</v>
-      </c>
-      <c r="G15" t="s">
-        <v>35</v>
-      </c>
-      <c r="H15" t="s">
-        <v>36</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" t="s">
-        <v>37</v>
-      </c>
-      <c r="D16" s="5">
-        <v>45763</v>
-      </c>
-      <c r="E16" s="4">
-        <v>45764</v>
-      </c>
-      <c r="F16" s="4">
-        <v>45765</v>
-      </c>
-      <c r="G16" t="s">
-        <v>32</v>
-      </c>
-      <c r="H16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" s="5">
-        <v>45762</v>
-      </c>
-      <c r="E17" s="4">
-        <v>45763</v>
-      </c>
-      <c r="F17" s="4">
-        <v>45764</v>
-      </c>
-      <c r="G17" t="s">
-        <v>32</v>
-      </c>
-      <c r="H17" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="5">
-        <v>45766</v>
-      </c>
-      <c r="E18" s="4">
-        <v>45767</v>
-      </c>
-      <c r="F18" s="4">
-        <v>45769</v>
-      </c>
-      <c r="G18" t="s">
-        <v>39</v>
-      </c>
-      <c r="H18" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B19" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" t="s">
-        <v>41</v>
-      </c>
-      <c r="D19" s="5">
-        <v>45771</v>
-      </c>
-      <c r="E19" s="4">
-        <v>45772</v>
-      </c>
-      <c r="F19" s="4">
-        <v>45776</v>
-      </c>
-      <c r="G19" t="s">
-        <v>35</v>
-      </c>
-      <c r="H19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B20" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20" s="5">
-        <v>45768</v>
-      </c>
-      <c r="E20" s="4">
-        <v>45769</v>
-      </c>
-      <c r="F20" s="4">
-        <v>45771</v>
-      </c>
-      <c r="G20" t="s">
-        <v>35</v>
-      </c>
-      <c r="H20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B21" t="s">
-        <v>9</v>
-      </c>
-      <c r="C21" t="s">
-        <v>30</v>
-      </c>
-      <c r="D21" s="5">
-        <v>45760</v>
-      </c>
-      <c r="E21" s="4">
-        <v>45761</v>
-      </c>
-      <c r="F21" s="4">
-        <v>45763</v>
-      </c>
-      <c r="G21" t="s">
-        <v>32</v>
-      </c>
-      <c r="H21" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B22" t="s">
-        <v>16</v>
-      </c>
-      <c r="C22" t="s">
-        <v>34</v>
-      </c>
-      <c r="D22" s="5">
-        <v>45764</v>
-      </c>
-      <c r="E22" s="4">
-        <v>45765</v>
-      </c>
-      <c r="F22" s="4">
-        <v>45767</v>
-      </c>
-      <c r="G22" t="s">
-        <v>39</v>
-      </c>
-      <c r="H22" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
+      <c r="A16" s="1"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="1"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="1"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="1"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="1"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="1"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="1"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" s="1"/>
       <c r="D23" s="5"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:6">
       <c r="A24" s="1"/>
       <c r="D24" s="5"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:6">
       <c r="A25" s="1"/>
       <c r="D25" s="5"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:6">
       <c r="D26" s="5"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K8:K15" xr:uid="{C3958E6F-28D2-429E-9DF5-7DAD65BBE2ED}">
       <formula1>$K:$K</formula1>
     </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576" xr:uid="{8C537B12-83B7-48DB-9398-33493EB60A9D}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -1608,7 +1217,7 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{363D4652-FA42-4545-94CD-50D28C1428B4}">
           <x14:formula1>
             <xm:f>Ref!$A$2:$A$1048576</xm:f>
@@ -1620,12 +1229,6 @@
             <xm:f>Ref!$C$2:$C$1048576</xm:f>
           </x14:formula1>
           <xm:sqref>B2:B1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F69C2AEF-2CB5-47D7-BDA7-51B0C1ADE034}">
-          <x14:formula1>
-            <xm:f>Ref!$E$2:$E$1048576</xm:f>
-          </x14:formula1>
-          <xm:sqref>C2:C1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{54B9EF97-0E92-4D14-A170-39C732012C46}">
           <x14:formula1>
@@ -1664,19 +1267,19 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C1" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="E1" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="G1" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="I1" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -1686,14 +1289,11 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
-        <v>30</v>
-      </c>
       <c r="G2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="I2" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1703,14 +1303,11 @@
       <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" t="s">
-        <v>34</v>
-      </c>
       <c r="G3" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="I3" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -1720,14 +1317,11 @@
       <c r="C4" t="s">
         <v>5</v>
       </c>
-      <c r="E4" t="s">
-        <v>37</v>
-      </c>
       <c r="G4" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="I4" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -1737,11 +1331,8 @@
       <c r="C5" t="s">
         <v>6</v>
       </c>
-      <c r="E5" t="s">
-        <v>38</v>
-      </c>
       <c r="I5" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -1751,13 +1342,10 @@
       <c r="C6" t="s">
         <v>7</v>
       </c>
-      <c r="E6" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
@@ -1765,7 +1353,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
@@ -1773,7 +1361,7 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
         <v>12</v>
@@ -1840,7 +1428,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:2">

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Tue May 27 05:55:35 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Solar_Lab_Tests.xlsx
+++ b/data/Solar_Lab_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{79B6E4EA-35C4-4835-B51A-C9FD80B5C669}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E4E5004-2024-4332-A5FC-30FBDD7F9F48}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="1" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
   </bookViews>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="47">
   <si>
     <t>BOM</t>
   </si>
@@ -156,6 +156,15 @@
     <t>HIUV</t>
   </si>
   <si>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
     <t>SUNBEZ</t>
   </si>
   <si>
@@ -181,15 +190,6 @@
   </si>
   <si>
     <t>Status</t>
-  </si>
-  <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>Completed</t>
-  </si>
-  <si>
-    <t>Pending</t>
   </si>
   <si>
     <t>In Progress</t>
@@ -295,7 +295,7 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -950,8 +950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9401EE47-EA52-49C7-BBC0-21F5B88254FB}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -1006,8 +1006,18 @@
       <c r="D2" s="5">
         <v>45773</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
+      <c r="E2" s="4">
+        <v>45804</v>
+      </c>
+      <c r="F2" s="4">
+        <v>45804</v>
+      </c>
+      <c r="G2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="1" t="s">
@@ -1022,8 +1032,18 @@
       <c r="D3" s="5">
         <v>45773</v>
       </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
+      <c r="E3" s="4">
+        <v>45802</v>
+      </c>
+      <c r="F3" s="4">
+        <v>45802</v>
+      </c>
+      <c r="G3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="1" t="s">
@@ -1033,13 +1053,23 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D4" s="5">
         <v>45777</v>
       </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
+      <c r="E4" s="4">
+        <v>45804</v>
+      </c>
+      <c r="F4" s="4">
+        <v>45804</v>
+      </c>
+      <c r="G4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="1" t="s">
@@ -1049,13 +1079,23 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D5" s="5">
         <v>45777</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
+      <c r="E5" s="4">
+        <v>45802</v>
+      </c>
+      <c r="F5" s="4">
+        <v>45802</v>
+      </c>
+      <c r="G5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="1"/>
@@ -1120,7 +1160,7 @@
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="K13" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1129,7 +1169,7 @@
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="K14" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1138,7 +1178,7 @@
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="K15" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1253,7 +1293,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -1267,19 +1307,19 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="I1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -1290,10 +1330,10 @@
         <v>3</v>
       </c>
       <c r="G2" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="I2" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1304,7 +1344,7 @@
         <v>4</v>
       </c>
       <c r="G3" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="I3" t="s">
         <v>43</v>
@@ -1332,7 +1372,7 @@
         <v>6</v>
       </c>
       <c r="I5" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -1345,7 +1385,7 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
@@ -1353,7 +1393,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
@@ -1361,7 +1401,7 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C9" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Tue May 27 11:34:14 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Solar_Lab_Tests.xlsx
+++ b/data/Solar_Lab_Tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="61" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E4E5004-2024-4332-A5FC-30FBDD7F9F48}"/>
+  <xr:revisionPtr revIDLastSave="63" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6983862D-6D05-4904-BA99-3DF2024A9C49}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="1" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="2" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Tests Map" sheetId="4" r:id="rId1"/>
@@ -411,7 +411,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{5748FE72-0B2B-4923-BB7E-7F7C064431FD}" name="Table7" displayName="Table7" ref="E1:E6" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{5748FE72-0B2B-4923-BB7E-7F7C064431FD}" name="Table7" displayName="Table7" ref="E1:E7" totalsRowShown="0">
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{6F677042-42AB-4417-A85B-2C01CA87EEAE}" name="Vendor Names"/>
   </tableColumns>
@@ -950,8 +950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9401EE47-EA52-49C7-BBC0-21F5B88254FB}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -1292,8 +1292,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17D43621-542F-4136-850B-43C25D2B7AAC}">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Tue Jun  3 09:40:03 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Solar_Lab_Tests.xlsx
+++ b/data/Solar_Lab_Tests.xlsx
@@ -1,26 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28922"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28926"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="63" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6983862D-6D05-4904-BA99-3DF2024A9C49}"/>
+  <xr:revisionPtr revIDLastSave="146" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{01536FF7-59F6-4F11-94AF-CAC9B72560AA}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="2" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="3" activeTab="3" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Tests Map" sheetId="4" r:id="rId1"/>
     <sheet name="Test Data" sheetId="5" r:id="rId2"/>
     <sheet name="Ref" sheetId="8" r:id="rId3"/>
-    <sheet name="Standard test times" sheetId="6" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="9" r:id="rId4"/>
+    <sheet name="Standard test times" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
+    <definedName name="ENCAPTYPE">Ref!$K$2:$K$1048576</definedName>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">'Material Tests Map'!$A$1:$B$20</definedName>
-    <definedName name="ExternalData_1" localSheetId="3" hidden="1">'Standard test times'!$A$1:$B$15</definedName>
+    <definedName name="ExternalData_1" localSheetId="4" hidden="1">'Standard test times'!$A$1:$B$15</definedName>
     <definedName name="ExternalData_1" localSheetId="1" hidden="1">'Test Data'!$A$1:$H$26</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
@@ -61,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="66">
   <si>
     <t>BOM</t>
   </si>
@@ -192,13 +194,70 @@
     <t>Status</t>
   </si>
   <si>
+    <t>ENCAPSULANT TYPE</t>
+  </si>
+  <si>
+    <t>FRONT EPE</t>
+  </si>
+  <si>
     <t>In Progress</t>
   </si>
   <si>
+    <t>BACK EVA</t>
+  </si>
+  <si>
     <t>Fail</t>
   </si>
   <si>
     <t>Failed</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Column2</t>
+  </si>
+  <si>
+    <t>Column3</t>
+  </si>
+  <si>
+    <t>Column4</t>
+  </si>
+  <si>
+    <t>Column5</t>
+  </si>
+  <si>
+    <t>Column6</t>
+  </si>
+  <si>
+    <t>Column7</t>
+  </si>
+  <si>
+    <t>Column8</t>
+  </si>
+  <si>
+    <t>Column9</t>
+  </si>
+  <si>
+    <t>Column10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                                                              WITHOUT HIT </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                                                     WITH HIT  </t>
+  </si>
+  <si>
+    <t>TD1</t>
+  </si>
+  <si>
+    <t>TD2</t>
+  </si>
+  <si>
+    <t>MD1</t>
+  </si>
+  <si>
+    <t>MD2</t>
   </si>
   <si>
     <t>STANDARD DURATION (DAYS)</t>
@@ -208,7 +267,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -216,8 +275,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -230,8 +303,26 @@
         <bgColor theme="9" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -261,11 +352,60 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -274,13 +414,43 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="12">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="medium">
+          <color rgb="FF000000"/>
+        </top>
+      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -295,7 +465,7 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -369,8 +539,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2651D75B-871E-4C48-A5BC-EA62B7E4365B}" name="materialmap" displayName="materialmap" ref="A1:B20" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:B20" xr:uid="{2651D75B-871E-4C48-A5BC-EA62B7E4365B}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{FB02FE47-E9DA-4BCF-85A4-754E419FEDE3}" uniqueName="1" name="BOM" queryTableFieldId="1" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{887E7320-FACA-4349-93A6-9DD0A9102ACA}" uniqueName="2" name="TEST NAME" queryTableFieldId="2" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{FB02FE47-E9DA-4BCF-85A4-754E419FEDE3}" uniqueName="1" name="BOM" queryTableFieldId="1" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{887E7320-FACA-4349-93A6-9DD0A9102ACA}" uniqueName="2" name="TEST NAME" queryTableFieldId="2" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -379,14 +549,14 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{06A3AD80-C098-4015-85FF-3495CE4443EA}" name="Test_Data" displayName="Test_Data" ref="A1:H26" tableType="queryTable" totalsRowShown="0">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{87F75B08-44C4-4718-834D-87FEE9F87970}" uniqueName="1" name="BOM" queryTableFieldId="1" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{1E5F4521-5E5C-4948-AEB2-FC5F712DB353}" uniqueName="2" name="TEST NAME" queryTableFieldId="2" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{22629B97-1F38-4A88-B08E-7589CFF4C28D}" uniqueName="3" name="VENDOR NAME" queryTableFieldId="3" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{D6678E87-972B-4807-86C4-4086EF552262}" uniqueName="4" name="GRN GENERATION TIME" queryTableFieldId="4" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{62C80EA2-76AB-4742-87FF-05248307AF93}" uniqueName="5" name="TEST START DATE AND TIME" queryTableFieldId="5" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{DDA3B4DC-3A06-4223-8D24-00B8C4C20678}" uniqueName="6" name="TEST END DATE AND TIME" queryTableFieldId="6" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{F2102600-A33C-449C-8C79-361FEA6C4BCE}" uniqueName="7" name="TEST RESULT" queryTableFieldId="7" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{E5E91A8D-E194-48B6-8D9A-FFD1939E8ACF}" uniqueName="8" name="STATUS" queryTableFieldId="8" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{87F75B08-44C4-4718-834D-87FEE9F87970}" uniqueName="1" name="BOM" queryTableFieldId="1" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{1E5F4521-5E5C-4948-AEB2-FC5F712DB353}" uniqueName="2" name="TEST NAME" queryTableFieldId="2" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{22629B97-1F38-4A88-B08E-7589CFF4C28D}" uniqueName="3" name="VENDOR NAME" queryTableFieldId="3" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{D6678E87-972B-4807-86C4-4086EF552262}" uniqueName="4" name="GRN GENERATION TIME" queryTableFieldId="4" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{62C80EA2-76AB-4742-87FF-05248307AF93}" uniqueName="5" name="TEST START DATE AND TIME" queryTableFieldId="5" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{DDA3B4DC-3A06-4223-8D24-00B8C4C20678}" uniqueName="6" name="TEST END DATE AND TIME" queryTableFieldId="6" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{F2102600-A33C-449C-8C79-361FEA6C4BCE}" uniqueName="7" name="TEST RESULT" queryTableFieldId="7" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{E5E91A8D-E194-48B6-8D9A-FFD1939E8ACF}" uniqueName="8" name="STATUS" queryTableFieldId="8" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -438,6 +608,25 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{B3363982-6183-49D5-AF98-D55C850396A0}" name="Table11" displayName="Table11" ref="A1:J1048574" totalsRowShown="0" tableBorderDxfId="1">
+  <autoFilter ref="A1:J1048574" xr:uid="{B3363982-6183-49D5-AF98-D55C850396A0}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{1F9180D7-CB71-431A-98B3-47E5AF984C00}" name="Column1"/>
+    <tableColumn id="2" xr3:uid="{8114EEEE-8721-4936-82EB-71B034CA9B84}" name="Column2"/>
+    <tableColumn id="3" xr3:uid="{455C1559-D23A-4C56-AE5A-D1160DFF53B1}" name="Column3"/>
+    <tableColumn id="4" xr3:uid="{82022E84-BA89-437A-8C60-BC564A01E80A}" name="Column4"/>
+    <tableColumn id="5" xr3:uid="{6AD890DD-B84E-4CFA-BB9B-37D3F1258C7E}" name="Column5"/>
+    <tableColumn id="6" xr3:uid="{5D97D99D-6390-4A75-9ADE-12630D000900}" name="Column6"/>
+    <tableColumn id="7" xr3:uid="{F7AB8D2F-BCB6-4D77-BEC3-56D58047407B}" name="Column7"/>
+    <tableColumn id="8" xr3:uid="{DBC8B8B9-9DD3-4D10-8699-3EDCCC2EA3F5}" name="Column8"/>
+    <tableColumn id="9" xr3:uid="{39FD58ED-4D12-4A3D-876E-6B9F57A95388}" name="Column9"/>
+    <tableColumn id="10" xr3:uid="{81BAF384-43CF-4C8A-96C5-5EEDD0CEFF38}" name="Column10"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{68171DB0-643B-43C2-B0C7-B755548E6CA4}" name="standard_test_time" displayName="standard_test_time" ref="A1:B15" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:B15" xr:uid="{68171DB0-643B-43C2-B0C7-B755548E6CA4}"/>
   <tableColumns count="2">
@@ -951,7 +1140,7 @@
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -1290,10 +1479,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17D43621-542F-4136-850B-43C25D2B7AAC}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -1305,7 +1494,7 @@
     <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -1321,8 +1510,11 @@
       <c r="I1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="K1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1335,8 +1527,11 @@
       <c r="I2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="K2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1347,10 +1542,13 @@
         <v>31</v>
       </c>
       <c r="I3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>45</v>
+      </c>
+      <c r="K3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1358,13 +1556,13 @@
         <v>5</v>
       </c>
       <c r="G4" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="I4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -1375,7 +1573,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1383,7 +1581,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -1391,7 +1589,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -1399,7 +1597,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>37</v>
       </c>
@@ -1407,32 +1605,32 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:11">
       <c r="C10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:11">
       <c r="C11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:11">
       <c r="C12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15">
+    <row r="13" spans="1:11" ht="15">
       <c r="C13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15">
+    <row r="14" spans="1:11" ht="15">
       <c r="C14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15">
+    <row r="15" spans="1:11" ht="15">
       <c r="C15" t="s">
         <v>22</v>
       </c>
@@ -1450,6 +1648,128 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3918A122-26E2-4D34-B5FF-7C2ED2C764FA}">
+  <dimension ref="A1:J3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A454" workbookViewId="0">
+      <selection activeCell="J463" sqref="J463"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1"/>
+    <col min="8" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="16"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A3" xr:uid="{9F12B590-F114-48F7-8BAD-0EB523C04B3F}"/>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E6175966-B22B-4DAC-8FC2-A47DA6041621}">
+          <x14:formula1>
+            <xm:f>Ref!$K$2:$K$1048576</xm:f>
+          </x14:formula1>
+          <xm:sqref>A2:A1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBA2255C-9286-47F7-8F7E-14EDD259611E}">
   <dimension ref="A1:B15"/>
   <sheetViews>
@@ -1468,7 +1788,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:2">

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Wed Jun 11 17:39:28 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Solar_Lab_Tests.xlsx
+++ b/data/Solar_Lab_Tests.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="415" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC86944F-CD9E-4DF9-AACD-F0A036B62125}"/>
+  <xr:revisionPtr revIDLastSave="416" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5B698DCB-D879-4324-92E3-9FEDC8ED6F15}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="7" activeTab="6" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="6" activeTab="3" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Tests Map" sheetId="4" state="hidden" r:id="rId1"/>
     <sheet name="Test Data" sheetId="5" r:id="rId2"/>
     <sheet name="Ref" sheetId="8" state="hidden" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="9" r:id="rId4"/>
+    <sheet name="Shrinkage" sheetId="9" r:id="rId4"/>
     <sheet name="Adhesion" sheetId="10" r:id="rId5"/>
     <sheet name="Tensile Strength" sheetId="11" r:id="rId6"/>
     <sheet name="GSM" sheetId="12" r:id="rId7"/>
@@ -2450,7 +2450,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3918A122-26E2-4D34-B5FF-7C2ED2C764FA}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -2785,9 +2785,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C0F3BDD-3989-4880-8737-F370069E1383}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1048560" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Mon Jun 16 08:07:39 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Solar_Lab_Tests.xlsx
+++ b/data/Solar_Lab_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="466" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B97FEBB-4826-4077-9E77-725177D261B1}"/>
+  <xr:revisionPtr revIDLastSave="467" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{26532CBC-0839-4FEB-84B1-3F4121EED342}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="7" activeTab="5" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
   </bookViews>
@@ -573,7 +573,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -646,7 +646,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1929,8 +1928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9401EE47-EA52-49C7-BBC0-21F5B88254FB}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -2730,10 +2729,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C8152F1-3340-4C7F-9B6C-3F6BB96763BA}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="A3" sqref="A3:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2787,28 +2786,25 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="F3" s="44"/>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B3" t="s">
         <v>35</v>
       </c>
-      <c r="C4">
+      <c r="C3">
         <v>10.74</v>
       </c>
-      <c r="F4">
+      <c r="F3">
         <v>1150.03</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A1048576" xr:uid="{04F856B6-1846-4FF1-B3BB-4FE58494E678}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3 F3 F5:F1048576" xr:uid="{FCBF55FC-869D-43C4-B484-27D4BFDDD5A4}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A1048576 A3" xr:uid="{04F856B6-1846-4FF1-B3BB-4FE58494E678}">
       <formula1>"ENCAPSULANT, RIBBON"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 F3:F1048576" xr:uid="{FCBF55FC-869D-43C4-B484-27D4BFDDD5A4}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Mon Jun 16 14:33:48 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Solar_Lab_Tests.xlsx
+++ b/data/Solar_Lab_Tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="469" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3AD9B3F6-8054-4912-B912-058BB7FA7EF4}"/>
+  <xr:revisionPtr revIDLastSave="474" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B458D5EB-A705-49EF-ACDB-817B269F04F7}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="5" activeTab="1" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="5" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Tests Map" sheetId="4" state="hidden" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="94">
   <si>
     <t>BOM</t>
   </si>
@@ -300,19 +300,7 @@
     <t>min</t>
   </si>
   <si>
-    <t>Column33</t>
-  </si>
-  <si>
-    <t>Column32</t>
-  </si>
-  <si>
     <t>BREAK</t>
-  </si>
-  <si>
-    <t>INITIAL LENGTH</t>
-  </si>
-  <si>
-    <t>FINAL LENGTH</t>
   </si>
   <si>
     <t>CHANGE IN ELONGATION %</t>
@@ -980,14 +968,12 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{9AF05D4E-990A-4C94-8850-9D7BC3D120A4}" name="Table14" displayName="Table14" ref="A1:F4" totalsRowShown="0">
-  <autoFilter ref="A1:F4" xr:uid="{9AF05D4E-990A-4C94-8850-9D7BC3D120A4}"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{9AF05D4E-990A-4C94-8850-9D7BC3D120A4}" name="Table14" displayName="Table14" ref="A1:D4" totalsRowShown="0">
+  <autoFilter ref="A1:D4" xr:uid="{9AF05D4E-990A-4C94-8850-9D7BC3D120A4}"/>
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{695E2580-F157-4DF3-A6A1-0C66057F77F2}" name="Column1"/>
     <tableColumn id="2" xr3:uid="{93E753E6-35FE-4C78-817F-5319A79D1951}" name="Column2"/>
     <tableColumn id="3" xr3:uid="{02BC0EB7-058E-4C0F-863A-525E0890CB40}" name="Column3"/>
-    <tableColumn id="6" xr3:uid="{091C1F14-CF5C-481F-B83B-09B6BE97229E}" name="Column33"/>
-    <tableColumn id="5" xr3:uid="{D18C8D34-D4E4-431A-AEE1-549520ECA814}" name="Column32"/>
     <tableColumn id="4" xr3:uid="{FB9ACFDB-0FEB-47ED-8942-8907B8871FAA}" name="Column4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1708,10 +1694,10 @@
         <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1765,7 +1751,7 @@
         <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1800,7 +1786,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1928,8 +1914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9401EE47-EA52-49C7-BBC0-21F5B88254FB}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -2729,10 +2715,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C8152F1-3340-4C7F-9B6C-3F6BB96763BA}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2740,12 +2726,10 @@
     <col min="1" max="1" width="14.42578125" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>53</v>
       </c>
@@ -2756,16 +2740,10 @@
         <v>55</v>
       </c>
       <c r="D1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="19" customFormat="1">
+    <row r="2" spans="1:4" s="19" customFormat="1">
       <c r="A2" s="19" t="s">
         <v>0</v>
       </c>
@@ -2773,19 +2751,13 @@
         <v>24</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="E2" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="F2" s="19" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2795,13 +2767,13 @@
       <c r="C3">
         <v>10.74</v>
       </c>
-      <c r="F3">
+      <c r="D3">
         <v>1150.03</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3 F3 F5:F1048576" xr:uid="{FCBF55FC-869D-43C4-B484-27D4BFDDD5A4}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3 D3 D5:D1048576" xr:uid="{FCBF55FC-869D-43C4-B484-27D4BFDDD5A4}"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A1048576 A3" xr:uid="{04F856B6-1846-4FF1-B3BB-4FE58494E678}">
       <formula1>"ENCAPSULANT, RIBBON"</formula1>
     </dataValidation>
@@ -2835,7 +2807,7 @@
         <v>53</v>
       </c>
       <c r="B1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C1" t="s">
         <v>54</v>
@@ -2867,25 +2839,25 @@
         <v>24</v>
       </c>
       <c r="C2" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="G2" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="H2" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="I2" s="26" t="s">
         <v>85</v>
-      </c>
-      <c r="F2" s="27" t="s">
-        <v>86</v>
-      </c>
-      <c r="G2" s="27" t="s">
-        <v>87</v>
-      </c>
-      <c r="H2" s="27" t="s">
-        <v>88</v>
-      </c>
-      <c r="I2" s="26" t="s">
-        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -2946,7 +2918,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B2" t="s">
         <v>45</v>
@@ -2955,7 +2927,7 @@
         <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -3012,10 +2984,10 @@
         <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:4">

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Mon Jun 16 14:43:23 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Solar_Lab_Tests.xlsx
+++ b/data/Solar_Lab_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="474" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B458D5EB-A705-49EF-ACDB-817B269F04F7}"/>
+  <xr:revisionPtr revIDLastSave="484" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F4092202-43DD-4EAF-A07D-8A3A71645F42}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="5" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
   </bookViews>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="94">
   <si>
     <t>BOM</t>
   </si>
@@ -971,10 +971,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{9AF05D4E-990A-4C94-8850-9D7BC3D120A4}" name="Table14" displayName="Table14" ref="A1:D4" totalsRowShown="0">
   <autoFilter ref="A1:D4" xr:uid="{9AF05D4E-990A-4C94-8850-9D7BC3D120A4}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{695E2580-F157-4DF3-A6A1-0C66057F77F2}" name="Column1"/>
-    <tableColumn id="2" xr3:uid="{93E753E6-35FE-4C78-817F-5319A79D1951}" name="Column2"/>
-    <tableColumn id="3" xr3:uid="{02BC0EB7-058E-4C0F-863A-525E0890CB40}" name="Column3"/>
-    <tableColumn id="4" xr3:uid="{FB9ACFDB-0FEB-47ED-8942-8907B8871FAA}" name="Column4"/>
+    <tableColumn id="1" xr3:uid="{695E2580-F157-4DF3-A6A1-0C66057F77F2}" name="BOM"/>
+    <tableColumn id="2" xr3:uid="{93E753E6-35FE-4C78-817F-5319A79D1951}" name="VENDOR NAME"/>
+    <tableColumn id="3" xr3:uid="{02BC0EB7-058E-4C0F-863A-525E0890CB40}" name="BREAK"/>
+    <tableColumn id="4" xr3:uid="{FB9ACFDB-0FEB-47ED-8942-8907B8871FAA}" name="CHANGE IN ELONGATION %"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1914,9 +1914,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9401EE47-EA52-49C7-BBC0-21F5B88254FB}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:H6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
@@ -2715,10 +2713,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C8152F1-3340-4C7F-9B6C-3F6BB96763BA}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2726,55 +2724,43 @@
     <col min="1" max="1" width="14.42578125" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" s="19" customFormat="1">
-      <c r="A2" s="19" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B1" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C1" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D1" s="19" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
+    <row r="2" spans="1:6" s="19" customFormat="1">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B2" t="s">
         <v>35</v>
       </c>
-      <c r="C3">
+      <c r="C2">
         <v>10.74</v>
       </c>
-      <c r="D3">
+      <c r="D2">
         <v>1150.03</v>
       </c>
+      <c r="E2"/>
+      <c r="F2"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3 D3 D5:D1048576" xr:uid="{FCBF55FC-869D-43C4-B484-27D4BFDDD5A4}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A1048576 A3" xr:uid="{04F856B6-1846-4FF1-B3BB-4FE58494E678}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B3 D2:D3 D5:D1048576" xr:uid="{FCBF55FC-869D-43C4-B484-27D4BFDDD5A4}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A1048576 A2:A3" xr:uid="{04F856B6-1846-4FF1-B3BB-4FE58494E678}">
       <formula1>"ENCAPSULANT, RIBBON"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Mon Jun 16 15:40:40 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Solar_Lab_Tests.xlsx
+++ b/data/Solar_Lab_Tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="484" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F4092202-43DD-4EAF-A07D-8A3A71645F42}"/>
+  <xr:revisionPtr revIDLastSave="500" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD2C88A1-D5FA-441B-AFBA-12D0B3ACBA19}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="5" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="4" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Tests Map" sheetId="4" state="hidden" r:id="rId1"/>
@@ -2452,7 +2452,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2573,7 +2573,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2030CC0-E8AF-4949-8297-EBC385BFEF95}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
@@ -2715,8 +2715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C8152F1-3340-4C7F-9B6C-3F6BB96763BA}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Tue Jun 17 17:01:34 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Solar_Lab_Tests.xlsx
+++ b/data/Solar_Lab_Tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="500" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD2C88A1-D5FA-441B-AFBA-12D0B3ACBA19}"/>
+  <xr:revisionPtr revIDLastSave="517" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AEE4036C-5BC0-4C63-B7A5-C1CEF5C514EB}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="4" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="4" activeTab="6" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Tests Map" sheetId="4" state="hidden" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="95">
   <si>
     <t>BOM</t>
   </si>
@@ -178,6 +178,9 @@
   </si>
   <si>
     <t>Hangzhou First</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
   <si>
     <t>GLASS</t>
@@ -561,7 +564,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -634,6 +637,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -981,8 +985,8 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{97A8C2A7-46C0-4446-B562-6550EA520638}" name="Table10" displayName="Table10" ref="A1:I2" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:I2" xr:uid="{97A8C2A7-46C0-4446-B562-6550EA520638}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{97A8C2A7-46C0-4446-B562-6550EA520638}" name="Table10" displayName="Table10" ref="A1:I3" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:I3" xr:uid="{97A8C2A7-46C0-4446-B562-6550EA520638}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{FE721515-FBBB-4487-ABCE-AAB6A5B1513A}" name="Column1" dataDxfId="9"/>
     <tableColumn id="9" xr3:uid="{304FA6D2-898E-427A-8AC1-958C15295938}" name="Column12" dataDxfId="8"/>
@@ -1674,16 +1678,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1694,10 +1698,10 @@
         <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1721,7 +1725,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{333C0630-51CF-46CA-8CAD-98FEF9AC181F}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1734,13 +1738,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1751,7 +1755,7 @@
         <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1786,7 +1790,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1914,7 +1918,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9401EE47-EA52-49C7-BBC0-21F5B88254FB}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
@@ -2083,10 +2089,27 @@
       </c>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="1"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
+      <c r="A7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="5">
+        <v>45825</v>
+      </c>
+      <c r="E7" s="4">
+        <v>45825</v>
+      </c>
+      <c r="F7" s="4">
+        <v>45825</v>
+      </c>
+      <c r="H7" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="1"/>
@@ -2139,7 +2162,7 @@
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="K13" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -2148,7 +2171,7 @@
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="K14" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -2157,7 +2180,7 @@
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="K15" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -2286,25 +2309,25 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="N1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -2321,10 +2344,10 @@
         <v>33</v>
       </c>
       <c r="K2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="N2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -2338,13 +2361,13 @@
         <v>31</v>
       </c>
       <c r="I3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -2355,10 +2378,10 @@
         <v>5</v>
       </c>
       <c r="G4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -2382,7 +2405,7 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
@@ -2390,7 +2413,7 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
@@ -2398,7 +2421,7 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
         <v>12</v>
@@ -2468,51 +2491,51 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="I1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="J1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>24</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D2" s="14"/>
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
       <c r="G2" s="18" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H2" s="15"/>
       <c r="I2" s="15"/>
@@ -2522,28 +2545,28 @@
       <c r="A3" s="10"/>
       <c r="B3" s="10"/>
       <c r="C3" s="11" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D3" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="G3" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="H3" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="I3" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="G3" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>67</v>
-      </c>
       <c r="J3" s="13" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -2573,8 +2596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2030CC0-E8AF-4949-8297-EBC385BFEF95}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="4" topLeftCell="B5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -2595,47 +2618,47 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="35" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D1" s="40" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E1" s="24" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F1" s="24" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G1" s="24" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H1" s="40" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I1" s="24" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="J1" s="40" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="29" customFormat="1">
       <c r="A2" s="36"/>
       <c r="B2" s="36"/>
       <c r="C2" s="30" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D2" s="31"/>
       <c r="E2" s="30"/>
       <c r="F2" s="31"/>
       <c r="H2" s="36" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J2" s="36"/>
     </row>
@@ -2647,19 +2670,19 @@
         <v>24</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D3" s="42"/>
       <c r="E3" s="21" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F3" s="32"/>
       <c r="G3" s="20" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H3" s="42"/>
       <c r="I3" s="21" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="J3" s="32"/>
     </row>
@@ -2667,28 +2690,28 @@
       <c r="A4" s="38"/>
       <c r="B4" s="39"/>
       <c r="C4" s="22" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D4" s="43" t="s">
+        <v>76</v>
+      </c>
+      <c r="E4" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="E4" s="23" t="s">
-        <v>74</v>
-      </c>
       <c r="F4" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="G4" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="G4" s="22" t="s">
-        <v>74</v>
-      </c>
       <c r="H4" s="43" t="s">
+        <v>76</v>
+      </c>
+      <c r="I4" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="I4" s="23" t="s">
-        <v>74</v>
-      </c>
       <c r="J4" s="33" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -2735,10 +2758,10 @@
         <v>24</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="19" customFormat="1">
@@ -2773,9 +2796,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C0F3BDD-3989-4880-8737-F370069E1383}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -2790,31 +2815,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F1" s="25" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G1" s="25" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H1" s="25" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -2825,26 +2850,53 @@
         <v>24</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D2" s="26" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E2" s="26" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F2" s="27" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G2" s="27" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H2" s="27" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="I2" s="26" t="s">
-        <v>85</v>
-      </c>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="44">
+        <v>400</v>
+      </c>
+      <c r="E3" s="44">
+        <v>400</v>
+      </c>
+      <c r="F3" s="25">
+        <v>410</v>
+      </c>
+      <c r="G3" s="25">
+        <v>480</v>
+      </c>
+      <c r="H3" s="25">
+        <v>470</v>
+      </c>
+      <c r="I3" s="44"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -2890,30 +2942,30 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
         <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -2950,16 +3002,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -2970,10 +3022,10 @@
         <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:4">

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Tue Jun 17 17:08:07 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Solar_Lab_Tests.xlsx
+++ b/data/Solar_Lab_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="517" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AEE4036C-5BC0-4C63-B7A5-C1CEF5C514EB}"/>
+  <xr:revisionPtr revIDLastSave="521" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8F127AB-E3C3-4356-B90F-73137876CF7B}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="4" activeTab="6" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
   </bookViews>
@@ -361,7 +361,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -402,6 +402,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="12">
@@ -564,7 +570,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -638,6 +644,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2738,9 +2745,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C8152F1-3340-4C7F-9B6C-3F6BB96763BA}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -2798,13 +2803,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C0F3BDD-3989-4880-8737-F370069E1383}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A1048560" workbookViewId="0">
+      <selection activeCell="I1048567" sqref="I1048567"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" style="44" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" customWidth="1"/>
     <col min="5" max="6" width="12.5703125" customWidth="1"/>
@@ -2875,7 +2881,7 @@
       <c r="A3" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="45" t="s">
         <v>36</v>
       </c>
       <c r="C3" s="44" t="s">

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Tue Jun 17 17:19:18 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Solar_Lab_Tests.xlsx
+++ b/data/Solar_Lab_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="521" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8F127AB-E3C3-4356-B90F-73137876CF7B}"/>
+  <xr:revisionPtr revIDLastSave="524" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{60AFCC08-E835-4DC8-80D4-7F4FB77542D8}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="4" activeTab="6" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
   </bookViews>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="94">
   <si>
     <t>BOM</t>
   </si>
@@ -307,9 +307,6 @@
   </si>
   <si>
     <t>CHANGE IN ELONGATION %</t>
-  </si>
-  <si>
-    <t>Column12</t>
   </si>
   <si>
     <t>Type</t>
@@ -769,7 +766,7 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -781,7 +778,6 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <name val="Aptos Narrow"/>
-        <charset val="1"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -992,18 +988,18 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{97A8C2A7-46C0-4446-B562-6550EA520638}" name="Table10" displayName="Table10" ref="A1:I3" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:I3" xr:uid="{97A8C2A7-46C0-4446-B562-6550EA520638}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{97A8C2A7-46C0-4446-B562-6550EA520638}" name="Table10" displayName="Table10" ref="A1:I2" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:I2" xr:uid="{97A8C2A7-46C0-4446-B562-6550EA520638}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{FE721515-FBBB-4487-ABCE-AAB6A5B1513A}" name="Column1" dataDxfId="9"/>
-    <tableColumn id="9" xr3:uid="{304FA6D2-898E-427A-8AC1-958C15295938}" name="Column12" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{CB22B1B1-F2DB-4A16-825A-FE463620DEF9}" name="Column2" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{37372ACB-68A6-4423-8A58-7EF31F49D3C5}" name="Column3" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{87A17A4F-6A43-4AB0-9B0F-B213AAD6E601}" name="Column4" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{BB8F60AF-F7B1-4306-8198-B69EE3E6D97A}" name="Column5" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{03425EE3-EC03-4913-B402-224F846A29D7}" name="Column6" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{E68E3244-13A5-47AA-8AB7-F602EE938E20}" name="Column7" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{D5BE9073-1EC1-4D18-A75C-7F63CCD62CB2}" name="Column8" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{FE721515-FBBB-4487-ABCE-AAB6A5B1513A}" name="BOM" dataDxfId="9"/>
+    <tableColumn id="9" xr3:uid="{304FA6D2-898E-427A-8AC1-958C15295938}" name="VENDOR NAME" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{CB22B1B1-F2DB-4A16-825A-FE463620DEF9}" name="Type" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{37372ACB-68A6-4423-8A58-7EF31F49D3C5}" name="min value 1 " dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{87A17A4F-6A43-4AB0-9B0F-B213AAD6E601}" name="min value 2" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{BB8F60AF-F7B1-4306-8198-B69EE3E6D97A}" name="min value 3" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{03425EE3-EC03-4913-B402-224F846A29D7}" name="min value 4" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{E68E3244-13A5-47AA-8AB7-F602EE938E20}" name="min value 5" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{D5BE9073-1EC1-4D18-A75C-7F63CCD62CB2}" name="Mean" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1705,10 +1701,10 @@
         <v>24</v>
       </c>
       <c r="C2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" t="s">
         <v>91</v>
-      </c>
-      <c r="D2" t="s">
-        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1762,7 +1758,7 @@
         <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1797,7 +1793,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2801,10 +2797,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C0F3BDD-3989-4880-8737-F370069E1383}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1048560" workbookViewId="0">
-      <selection activeCell="I1048567" sqref="I1048567"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2820,96 +2816,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B1" t="s">
+      <c r="A1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="C1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F1" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="G1" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="H1" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="I1" t="s">
-        <v>61</v>
+      <c r="D1" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="G1" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="H1" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="26" t="s">
-        <v>80</v>
-      </c>
-      <c r="D2" s="26" t="s">
-        <v>81</v>
-      </c>
-      <c r="E2" s="26" t="s">
-        <v>82</v>
-      </c>
-      <c r="F2" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="G2" s="27" t="s">
-        <v>84</v>
-      </c>
-      <c r="H2" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="I2" s="26" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="44" t="s">
+      <c r="A2" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="45" t="s">
+      <c r="B2" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="44" t="s">
+      <c r="C2" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="D3" s="44">
+      <c r="D2" s="44">
         <v>400</v>
       </c>
-      <c r="E3" s="44">
+      <c r="E2" s="44">
         <v>400</v>
       </c>
-      <c r="F3" s="25">
+      <c r="F2" s="25">
         <v>410</v>
       </c>
-      <c r="G3" s="25">
+      <c r="G2" s="25">
         <v>480</v>
       </c>
-      <c r="H3" s="25">
+      <c r="H2" s="25">
         <v>470</v>
       </c>
-      <c r="I3" s="44"/>
+      <c r="I2" s="44"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A1048576" xr:uid="{7F2D1C41-A6FD-4C19-BC7D-7ACE4978C2ED}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576" xr:uid="{7F2D1C41-A6FD-4C19-BC7D-7ACE4978C2ED}">
       <formula1>"ENCAPSULANT"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B1048576" xr:uid="{EE16E65D-6A5C-4676-8547-95F671B6CD63}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{EE16E65D-6A5C-4676-8547-95F671B6CD63}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -2922,7 +2889,7 @@
           <x14:formula1>
             <xm:f>Ref!$N$2:$N$1048576</xm:f>
           </x14:formula1>
-          <xm:sqref>C3:C1048576</xm:sqref>
+          <xm:sqref>C2:C1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2962,7 +2929,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B2" t="s">
         <v>46</v>
@@ -2971,7 +2938,7 @@
         <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -3028,10 +2995,10 @@
         <v>24</v>
       </c>
       <c r="C2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" t="s">
         <v>89</v>
-      </c>
-      <c r="D2" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:4">

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Tue Jun 17 17:39:53 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Solar_Lab_Tests.xlsx
+++ b/data/Solar_Lab_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="524" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{60AFCC08-E835-4DC8-80D4-7F4FB77542D8}"/>
+  <xr:revisionPtr revIDLastSave="526" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CAD347D0-0707-4136-8D4E-489DAF809FEF}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="4" activeTab="6" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
   </bookViews>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="94">
   <si>
     <t>BOM</t>
   </si>
@@ -2800,13 +2800,13 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.85546875" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" style="44" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" style="44" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" customWidth="1"/>
     <col min="5" max="6" width="12.5703125" customWidth="1"/>
@@ -2845,30 +2845,14 @@
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="45" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="44" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" s="44">
-        <v>400</v>
-      </c>
-      <c r="E2" s="44">
-        <v>400</v>
-      </c>
-      <c r="F2" s="25">
-        <v>410</v>
-      </c>
-      <c r="G2" s="25">
-        <v>480</v>
-      </c>
-      <c r="H2" s="25">
-        <v>470</v>
-      </c>
+      <c r="A2" s="44"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
       <c r="I2" s="44"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Thu Jun 19 06:46:28 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Solar_Lab_Tests.xlsx
+++ b/data/Solar_Lab_Tests.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="542" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C8A0E22-3D08-44A9-A4EB-15F4628D105A}"/>
+  <xr:revisionPtr revIDLastSave="592" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{953DCB16-BCED-4740-9931-962806D22CDC}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="6" activeTab="3" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="10" activeTab="10" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Tests Map" sheetId="4" state="hidden" r:id="rId1"/>
     <sheet name="Test Data" sheetId="5" r:id="rId2"/>
     <sheet name="Ref" sheetId="8" state="hidden" r:id="rId3"/>
     <sheet name="Shrinkage" sheetId="17" r:id="rId4"/>
-    <sheet name="Adhesion" sheetId="10" r:id="rId5"/>
+    <sheet name="Adhesion" sheetId="18" r:id="rId5"/>
     <sheet name="Tensile Strength" sheetId="11" r:id="rId6"/>
     <sheet name="GSM" sheetId="12" r:id="rId7"/>
     <sheet name="Resistance" sheetId="13" r:id="rId8"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="92">
   <si>
     <t>BOM</t>
   </si>
@@ -180,7 +180,7 @@
     <t>Hangzhou First</t>
   </si>
   <si>
-    <t>test</t>
+    <t>In Progress</t>
   </si>
   <si>
     <t>GLASS</t>
@@ -219,9 +219,6 @@
     <t>OLD : 420 to 480</t>
   </si>
   <si>
-    <t>In Progress</t>
-  </si>
-  <si>
     <t>BACK EVA</t>
   </si>
   <si>
@@ -280,9 +277,6 @@
   </si>
   <si>
     <t>Column10</t>
-  </si>
-  <si>
-    <t>Column11</t>
   </si>
   <si>
     <t xml:space="preserve">                                                                                                                           PRE PCT</t>
@@ -473,12 +467,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="-0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="3" tint="0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -495,8 +483,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -597,11 +591,44 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="6"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -611,77 +638,74 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="46">
+  <dxfs count="45">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -817,96 +841,92 @@
       </font>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-      </font>
-      <border>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <border>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <border>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <border>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <border>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="7" tint="-0.499984740745262"/>
+          <bgColor theme="2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -1091,8 +1111,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2651D75B-871E-4C48-A5BC-EA62B7E4365B}" name="materialmap" displayName="materialmap" ref="A1:B20" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:B20" xr:uid="{2651D75B-871E-4C48-A5BC-EA62B7E4365B}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{FB02FE47-E9DA-4BCF-85A4-754E419FEDE3}" uniqueName="1" name="BOM" queryTableFieldId="1" dataDxfId="45"/>
-    <tableColumn id="2" xr3:uid="{887E7320-FACA-4349-93A6-9DD0A9102ACA}" uniqueName="2" name="TEST NAME" queryTableFieldId="2" dataDxfId="44"/>
+    <tableColumn id="1" xr3:uid="{FB02FE47-E9DA-4BCF-85A4-754E419FEDE3}" uniqueName="1" name="BOM" queryTableFieldId="1" dataDxfId="44"/>
+    <tableColumn id="2" xr3:uid="{887E7320-FACA-4349-93A6-9DD0A9102ACA}" uniqueName="2" name="TEST NAME" queryTableFieldId="2" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1133,10 +1153,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{20A38E0C-9EF6-4C45-A435-A35C875E6079}" name="Table4" displayName="Table4" ref="A1:D3" totalsRowShown="0">
   <autoFilter ref="A1:D3" xr:uid="{20A38E0C-9EF6-4C45-A435-A35C875E6079}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{81484900-FCE7-4687-AE80-25067EEBF4DF}" name="Column1"/>
-    <tableColumn id="2" xr3:uid="{98C35052-5143-4722-B228-CDF4595728A7}" name="Column2"/>
-    <tableColumn id="3" xr3:uid="{DC0A72BF-A20E-4169-808D-31BFAFA45357}" name="Column3"/>
-    <tableColumn id="4" xr3:uid="{C58F8BC5-05CB-47D9-818A-1926632D9181}" name="Column4"/>
+    <tableColumn id="1" xr3:uid="{81484900-FCE7-4687-AE80-25067EEBF4DF}" name="BOM "/>
+    <tableColumn id="2" xr3:uid="{98C35052-5143-4722-B228-CDF4595728A7}" name="TYPE"/>
+    <tableColumn id="3" xr3:uid="{DC0A72BF-A20E-4169-808D-31BFAFA45357}" name="VENDOR NAME"/>
+    <tableColumn id="4" xr3:uid="{C58F8BC5-05CB-47D9-818A-1926632D9181}" name="MEASURED VALUE"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1146,10 +1166,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{8C209182-09AA-48EA-902C-6AAC66F47A76}" name="Table12" displayName="Table12" ref="A1:D3" totalsRowShown="0">
   <autoFilter ref="A1:D3" xr:uid="{8C209182-09AA-48EA-902C-6AAC66F47A76}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{27C63457-5CD9-4E66-9147-3F02C3CC7E21}" name="Column1"/>
-    <tableColumn id="2" xr3:uid="{F36AEF9E-FAC6-46B7-9647-9D784C7A5C69}" name="Column2"/>
-    <tableColumn id="3" xr3:uid="{3BDF9825-11C5-4BDD-91BF-0B8E1468C930}" name="Column3"/>
-    <tableColumn id="4" xr3:uid="{04616244-E194-439B-9881-6F94D8816660}" name="Column4"/>
+    <tableColumn id="1" xr3:uid="{27C63457-5CD9-4E66-9147-3F02C3CC7E21}" name="BOM"/>
+    <tableColumn id="2" xr3:uid="{F36AEF9E-FAC6-46B7-9647-9D784C7A5C69}" name="VENDOR NAME"/>
+    <tableColumn id="3" xr3:uid="{3BDF9825-11C5-4BDD-91BF-0B8E1468C930}" name="START TIME"/>
+    <tableColumn id="4" xr3:uid="{04616244-E194-439B-9881-6F94D8816660}" name="END TIME"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1159,10 +1179,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{06A1C849-8D31-4C6A-A42D-12719D04B2C4}" name="Table15" displayName="Table15" ref="A1:D2" totalsRowShown="0">
   <autoFilter ref="A1:D2" xr:uid="{06A1C849-8D31-4C6A-A42D-12719D04B2C4}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{19E12D93-C82B-462F-BADB-49B4EB6429DD}" name="Column1"/>
-    <tableColumn id="2" xr3:uid="{35A8E361-756F-45B5-81A0-98D285B9959F}" name="Column2"/>
-    <tableColumn id="3" xr3:uid="{ACA7298A-F8BB-468F-817D-4DB3100368D7}" name="Column3"/>
-    <tableColumn id="4" xr3:uid="{94740E0E-8A3D-46A2-8380-4AD1738F7C06}" name="Column4"/>
+    <tableColumn id="1" xr3:uid="{19E12D93-C82B-462F-BADB-49B4EB6429DD}" name="BOM"/>
+    <tableColumn id="2" xr3:uid="{35A8E361-756F-45B5-81A0-98D285B9959F}" name="VENDOR NAME"/>
+    <tableColumn id="3" xr3:uid="{ACA7298A-F8BB-468F-817D-4DB3100368D7}" name="TIME"/>
+    <tableColumn id="4" xr3:uid="{94740E0E-8A3D-46A2-8380-4AD1738F7C06}" name="DEPTH"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1172,9 +1192,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{5C370BE7-C0F8-462F-9F89-5FC458087319}" name="Table16" displayName="Table16" ref="A1:C3" totalsRowShown="0">
   <autoFilter ref="A1:C3" xr:uid="{5C370BE7-C0F8-462F-9F89-5FC458087319}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{59EA2429-768A-457D-88E6-B34A083DE755}" name="Column1"/>
-    <tableColumn id="2" xr3:uid="{C09F236B-325A-4EF9-B484-B1D592C83B7F}" name="Column2"/>
-    <tableColumn id="3" xr3:uid="{038FF345-6349-48D1-AECF-86999B680B6F}" name="Column3"/>
+    <tableColumn id="1" xr3:uid="{59EA2429-768A-457D-88E6-B34A083DE755}" name="BOM"/>
+    <tableColumn id="2" xr3:uid="{C09F236B-325A-4EF9-B484-B1D592C83B7F}" name="VENDOR NAME"/>
+    <tableColumn id="3" xr3:uid="{038FF345-6349-48D1-AECF-86999B680B6F}" name="MAX TEMPERATURE OF DIODE(Tj)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1194,14 +1214,14 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{06A3AD80-C098-4015-85FF-3495CE4443EA}" name="Test_Data" displayName="Test_Data" ref="A1:H26" tableType="queryTable" totalsRowShown="0">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{87F75B08-44C4-4718-834D-87FEE9F87970}" uniqueName="1" name="BOM" queryTableFieldId="1" dataDxfId="43"/>
-    <tableColumn id="2" xr3:uid="{1E5F4521-5E5C-4948-AEB2-FC5F712DB353}" uniqueName="2" name="TEST NAME" queryTableFieldId="2" dataDxfId="42"/>
-    <tableColumn id="3" xr3:uid="{22629B97-1F38-4A88-B08E-7589CFF4C28D}" uniqueName="3" name="VENDOR NAME" queryTableFieldId="3" dataDxfId="41"/>
-    <tableColumn id="4" xr3:uid="{D6678E87-972B-4807-86C4-4086EF552262}" uniqueName="4" name="GRN GENERATION TIME" queryTableFieldId="4" dataDxfId="40"/>
-    <tableColumn id="5" xr3:uid="{62C80EA2-76AB-4742-87FF-05248307AF93}" uniqueName="5" name="TEST START DATE AND TIME" queryTableFieldId="5" dataDxfId="39"/>
-    <tableColumn id="6" xr3:uid="{DDA3B4DC-3A06-4223-8D24-00B8C4C20678}" uniqueName="6" name="TEST END DATE AND TIME" queryTableFieldId="6" dataDxfId="38"/>
-    <tableColumn id="7" xr3:uid="{F2102600-A33C-449C-8C79-361FEA6C4BCE}" uniqueName="7" name="TEST RESULT" queryTableFieldId="7" dataDxfId="37"/>
-    <tableColumn id="8" xr3:uid="{E5E91A8D-E194-48B6-8D9A-FFD1939E8ACF}" uniqueName="8" name="STATUS" queryTableFieldId="8" dataDxfId="36"/>
+    <tableColumn id="1" xr3:uid="{87F75B08-44C4-4718-834D-87FEE9F87970}" uniqueName="1" name="BOM" queryTableFieldId="1" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{1E5F4521-5E5C-4948-AEB2-FC5F712DB353}" uniqueName="2" name="TEST NAME" queryTableFieldId="2" dataDxfId="41"/>
+    <tableColumn id="3" xr3:uid="{22629B97-1F38-4A88-B08E-7589CFF4C28D}" uniqueName="3" name="VENDOR NAME" queryTableFieldId="3" dataDxfId="40"/>
+    <tableColumn id="4" xr3:uid="{D6678E87-972B-4807-86C4-4086EF552262}" uniqueName="4" name="GRN GENERATION TIME" queryTableFieldId="4" dataDxfId="39"/>
+    <tableColumn id="5" xr3:uid="{62C80EA2-76AB-4742-87FF-05248307AF93}" uniqueName="5" name="TEST START DATE AND TIME" queryTableFieldId="5" dataDxfId="38"/>
+    <tableColumn id="6" xr3:uid="{DDA3B4DC-3A06-4223-8D24-00B8C4C20678}" uniqueName="6" name="TEST END DATE AND TIME" queryTableFieldId="6" dataDxfId="37"/>
+    <tableColumn id="7" xr3:uid="{F2102600-A33C-449C-8C79-361FEA6C4BCE}" uniqueName="7" name="TEST RESULT" queryTableFieldId="7" dataDxfId="36"/>
+    <tableColumn id="8" xr3:uid="{E5E91A8D-E194-48B6-8D9A-FFD1939E8ACF}" uniqueName="8" name="STATUS" queryTableFieldId="8" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1253,40 +1273,40 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{7FFEF855-2CB7-4EF4-BE50-FB81C544017B}" name="Table18" displayName="Table18" ref="A3:J1048576" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{7FFEF855-2CB7-4EF4-BE50-FB81C544017B}" name="Table18" displayName="Table18" ref="A3:J1048576" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
   <autoFilter ref="A3:J1048576" xr:uid="{7FFEF855-2CB7-4EF4-BE50-FB81C544017B}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{96E09178-FF72-435C-90A9-F2F7FEC7E80C}" name="Column1" dataDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{B7D3E49F-4F89-454D-B9FA-E1364CBF3239}" name="Column2" dataDxfId="32"/>
-    <tableColumn id="3" xr3:uid="{CCA06B22-44E5-4255-8F26-0C1B1279B22C}" name="Column3" dataDxfId="31"/>
-    <tableColumn id="4" xr3:uid="{6F565555-BB1C-4294-A1BA-3B6ADB9C2D2F}" name="Column4" dataDxfId="30"/>
-    <tableColumn id="5" xr3:uid="{33CA8E10-7021-4A52-853E-A6227866156B}" name="Column5" dataDxfId="29"/>
-    <tableColumn id="6" xr3:uid="{870E308E-FC7E-4A0A-A66A-ED0B8741D8AF}" name="Column6" dataDxfId="28"/>
-    <tableColumn id="7" xr3:uid="{FEEFF96D-1CCA-48C1-982D-EAFDB6BC3200}" name="Column7" dataDxfId="27"/>
-    <tableColumn id="8" xr3:uid="{4FEE2433-7AE2-4CF7-A1FC-541524E1FAAF}" name="Column8" dataDxfId="26"/>
-    <tableColumn id="9" xr3:uid="{A6BC8484-A791-4583-A77F-7F6A667CE8C5}" name="Column9" dataDxfId="25"/>
-    <tableColumn id="10" xr3:uid="{192E7774-55A7-4BD2-9715-330A7F12089B}" name="Column10" dataDxfId="24"/>
+    <tableColumn id="1" xr3:uid="{96E09178-FF72-435C-90A9-F2F7FEC7E80C}" name="Column1" dataDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{B7D3E49F-4F89-454D-B9FA-E1364CBF3239}" name="Column2" dataDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{CCA06B22-44E5-4255-8F26-0C1B1279B22C}" name="Column3" dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{6F565555-BB1C-4294-A1BA-3B6ADB9C2D2F}" name="Column4" dataDxfId="29"/>
+    <tableColumn id="5" xr3:uid="{33CA8E10-7021-4A52-853E-A6227866156B}" name="Column5" dataDxfId="28"/>
+    <tableColumn id="6" xr3:uid="{870E308E-FC7E-4A0A-A66A-ED0B8741D8AF}" name="Column6" dataDxfId="27"/>
+    <tableColumn id="7" xr3:uid="{FEEFF96D-1CCA-48C1-982D-EAFDB6BC3200}" name="Column7" dataDxfId="26"/>
+    <tableColumn id="8" xr3:uid="{4FEE2433-7AE2-4CF7-A1FC-541524E1FAAF}" name="Column8" dataDxfId="25"/>
+    <tableColumn id="9" xr3:uid="{A6BC8484-A791-4583-A77F-7F6A667CE8C5}" name="Column9" dataDxfId="24"/>
+    <tableColumn id="10" xr3:uid="{192E7774-55A7-4BD2-9715-330A7F12089B}" name="Column10" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{BA074AAD-8C0D-41FF-8BC8-4F9AB9EFB637}" name="Table13" displayName="Table13" ref="A1:J5" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
-  <autoFilter ref="A1:J5" xr:uid="{BA074AAD-8C0D-41FF-8BC8-4F9AB9EFB637}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{67926097-CCFB-425B-9820-DDDFB77C87C9}" name="Table11" displayName="Table11" ref="A4:J1048576" totalsRowShown="0" dataDxfId="22">
+  <autoFilter ref="A4:J1048576" xr:uid="{67926097-CCFB-425B-9820-DDDFB77C87C9}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{34FD6EFD-96D0-42B3-9884-F0352610FB99}" name="Column1" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{7EC4F1F8-9AB2-42F0-B109-EC2B0D29E400}" name="Column2" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{3C56F111-F279-4173-9940-4CD4758EE3E8}" name="Column3" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{2C1D8A02-D703-4010-B9B1-82F89C7D0B5B}" name="Column4" dataDxfId="18"/>
-    <tableColumn id="6" xr3:uid="{DE9D1FA0-BFE0-44F4-8DCB-3EAB04367C74}" name="Column6" dataDxfId="17"/>
-    <tableColumn id="7" xr3:uid="{6F076E04-D3A7-4DBF-9F5C-6725251E70DF}" name="Column7" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{F5BE61A6-E912-439E-8DBB-EBCF02A592DC}" name="Column8" dataDxfId="15"/>
-    <tableColumn id="8" xr3:uid="{FA958DB1-F4D6-474D-92AC-CF54B9F57097}" name="Column9" dataDxfId="14"/>
-    <tableColumn id="9" xr3:uid="{E15D1EED-85DA-45E5-BBDD-0C8A1AC33FE5}" name="Column10" dataDxfId="13"/>
-    <tableColumn id="10" xr3:uid="{9587C54B-6823-4A9C-8C6B-D8995A5CD8EF}" name="Column11" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{EA92BD46-85A5-4BF3-9843-966A2E5861D9}" name="Column1" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{C24A9AB3-E538-4185-9C80-E9DDC6A05A90}" name="Column2" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{0CA46B2C-315A-49B7-A313-787EA669AF33}" name="Column3" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{AA05AB49-E5DC-4F39-BF84-5C21AE004473}" name="Column4" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{8D9CD07A-CD8E-459F-AD52-C1C64282E998}" name="Column5" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{953BA2E8-443D-4DD4-ACF1-1ECEDB5DE6DD}" name="Column6" dataDxfId="16"/>
+    <tableColumn id="7" xr3:uid="{8ED40F5F-1EB7-4C33-83D6-002E5FC5C1EC}" name="Column7" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{3EC62242-31F0-4282-815A-7D5C6B4310FD}" name="Column8" dataDxfId="14"/>
+    <tableColumn id="9" xr3:uid="{514AC0BC-C14D-43E8-9076-A902208889C3}" name="Column9" dataDxfId="13"/>
+    <tableColumn id="10" xr3:uid="{94E39AAC-5F2B-4668-8EAE-7D440F802CF1}" name="Column10" dataDxfId="12"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1790,10 +1810,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F56F2208-8607-4AD8-86AA-FA94B344C453}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1805,30 +1825,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>61</v>
+        <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>62</v>
+        <v>88</v>
       </c>
       <c r="D1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1850,10 +1856,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{333C0630-51CF-46CA-8CAD-98FEF9AC181F}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1865,24 +1871,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>61</v>
+        <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1917,7 +1912,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2046,13 +2041,13 @@
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" customWidth="1"/>
     <col min="3" max="3" width="19.140625" customWidth="1"/>
     <col min="4" max="4" width="25.42578125" customWidth="1"/>
     <col min="5" max="5" width="30.28515625" customWidth="1"/>
@@ -2223,7 +2218,7 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D7" s="5">
         <v>45825</v>
@@ -2239,19 +2234,47 @@
       </c>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="1"/>
-      <c r="D8" s="5"/>
+      <c r="A8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="5">
+        <v>45825</v>
+      </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
+      <c r="H8" t="s">
+        <v>36</v>
+      </c>
       <c r="K8" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="1"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="4"/>
+      <c r="A9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="5">
+        <v>45825</v>
+      </c>
+      <c r="E9" s="4">
+        <v>45825</v>
+      </c>
       <c r="F9" s="4"/>
+      <c r="H9" t="s">
+        <v>33</v>
+      </c>
       <c r="K9" s="2" t="s">
         <v>15</v>
       </c>
@@ -2488,13 +2511,13 @@
         <v>31</v>
       </c>
       <c r="I3" t="s">
+        <v>36</v>
+      </c>
+      <c r="K3" t="s">
         <v>49</v>
       </c>
-      <c r="K3" t="s">
+      <c r="N3" t="s">
         <v>50</v>
-      </c>
-      <c r="N3" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -2505,10 +2528,10 @@
         <v>5</v>
       </c>
       <c r="G4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I4" t="s">
         <v>52</v>
-      </c>
-      <c r="I4" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -2601,96 +2624,96 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61A5C69B-8639-4E8F-9A05-E59E5511083E}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1048565" sqref="K1048565"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" style="46" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" style="46" customWidth="1"/>
-    <col min="3" max="9" width="11.5703125" style="46" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" style="46" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" style="27" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" style="27" customWidth="1"/>
+    <col min="3" max="9" width="11.5703125" style="27" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" style="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="36" t="s">
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="19"/>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="38"/>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="39"/>
-      <c r="B2" s="39"/>
-      <c r="C2" s="40" t="s">
+      <c r="D2" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="D2" s="41" t="s">
+      <c r="E2" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="41" t="s">
+      <c r="F2" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="F2" s="41" t="s">
+      <c r="G2" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="I2" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="J2" s="25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" hidden="1">
+      <c r="A3" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="G2" s="42" t="s">
-        <v>56</v>
-      </c>
-      <c r="H2" s="43" t="s">
-        <v>57</v>
-      </c>
-      <c r="I2" s="43" t="s">
-        <v>58</v>
-      </c>
-      <c r="J2" s="44" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" hidden="1">
-      <c r="A3" s="45" t="s">
+      <c r="B3" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="45" t="s">
+      <c r="C3" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="C3" s="45" t="s">
+      <c r="D3" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="D3" s="45" t="s">
+      <c r="E3" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="E3" s="45" t="s">
+      <c r="F3" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="F3" s="45" t="s">
+      <c r="G3" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="G3" s="45" t="s">
+      <c r="H3" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="H3" s="45" t="s">
+      <c r="I3" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="I3" s="45" t="s">
+      <c r="J3" s="26" t="s">
         <v>68</v>
-      </c>
-      <c r="J3" s="45" t="s">
-        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -2717,125 +2740,126 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2030CC0-E8AF-4949-8297-EBC385BFEF95}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E993B7F-E878-4ABA-95AD-A4138848D6EF}">
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="4" topLeftCell="B5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" style="21" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" style="21" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" style="21" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" customWidth="1"/>
-    <col min="6" max="6" width="21.28515625" style="21" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" style="6" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" style="28" customWidth="1"/>
-    <col min="9" max="9" width="15" style="6" customWidth="1"/>
-    <col min="10" max="10" width="18.28515625" style="28" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="11.5703125" style="45" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" style="45" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" style="45" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" style="45" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" style="45" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" style="45" customWidth="1"/>
+    <col min="7" max="7" width="16" style="45" customWidth="1"/>
+    <col min="8" max="8" width="20.5703125" style="45" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" style="45" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" style="45" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="45"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:10" customFormat="1">
+      <c r="A1" s="28"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="31"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="I1" s="32"/>
+      <c r="J1" s="29"/>
+    </row>
+    <row r="2" spans="1:10" customFormat="1">
+      <c r="A2" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="36"/>
+      <c r="E2" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" s="38"/>
+      <c r="G2" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="H2" s="11"/>
+      <c r="I2" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="J2" s="38"/>
+    </row>
+    <row r="3" spans="1:10" customFormat="1">
+      <c r="A3" s="39"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="40" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" s="41" t="s">
+        <v>74</v>
+      </c>
+      <c r="E3" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" s="43" t="s">
+        <v>74</v>
+      </c>
+      <c r="G3" s="40" t="s">
+        <v>73</v>
+      </c>
+      <c r="H3" s="41" t="s">
+        <v>74</v>
+      </c>
+      <c r="I3" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="J3" s="43" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" customFormat="1" hidden="1">
+      <c r="A4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="C4" t="s">
         <v>61</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="D4" t="s">
         <v>62</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="E4" t="s">
         <v>63</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="F4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G4" t="s">
         <v>65</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="H4" t="s">
         <v>66</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="I4" t="s">
         <v>67</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="J4" t="s">
         <v>68</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="J1" s="27" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" s="16" customFormat="1">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="D2" s="18"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="18"/>
-      <c r="H2" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="J2" s="23"/>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="D3" s="29"/>
-      <c r="E3" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="F3" s="19"/>
-      <c r="G3" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="H3" s="29"/>
-      <c r="I3" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="J3" s="19"/>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="25"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="D4" s="30" t="s">
-        <v>76</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="F4" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="H4" s="30" t="s">
-        <v>76</v>
-      </c>
-      <c r="I4" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="J4" s="20" t="s">
-        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -2846,11 +2870,11 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EFF1C991-F270-48D6-AD04-45EFEA2D8175}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4CCE333A-172E-45E9-B21C-74FD80B735CA}">
           <x14:formula1>
             <xm:f>Ref!$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>A4:A1048576</xm:sqref>
+          <xm:sqref>A3:A4</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2862,7 +2886,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C8152F1-3340-4C7F-9B6C-3F6BB96763BA}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -2880,10 +2906,10 @@
         <v>24</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="6" customFormat="1">
@@ -2937,39 +2963,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="F1" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="G1" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="H1" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="I1" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="H1" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>85</v>
-      </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="B2" s="31"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -2999,54 +3025,40 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD5452B6-66C2-4964-BBFB-466116F6D217}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.5703125" customWidth="1"/>
     <col min="2" max="2" width="22.85546875" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
     <col min="4" max="4" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="B1" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="C1" t="s">
-        <v>62</v>
+        <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A1048576" xr:uid="{DD727E78-A3B4-474B-9E0A-F14D5EC59A5D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576" xr:uid="{DD727E78-A3B4-474B-9E0A-F14D5EC59A5D}">
       <formula1>"RIBBON"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B1048576" xr:uid="{C53B7015-151D-4397-972A-C85F743B358A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{C53B7015-151D-4397-972A-C85F743B358A}">
       <formula1>"BUS RIBBON, INTERCONNECT RIBBON"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3062,7 +3074,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3075,44 +3087,30 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>61</v>
+        <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="D1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="C3" s="15"/>
+      <c r="C3" s="10"/>
     </row>
     <row r="30" spans="3:3">
-      <c r="C30" s="15"/>
+      <c r="C30" s="10"/>
     </row>
   </sheetData>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A1048576" xr:uid="{37B02B1D-BCBE-4193-818D-7F3B703602BB}">
       <formula1>"SEALANT (POTTING), SEALANT (WHITE)"</formula1>
     </dataValidation>
-    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C1048576 D3:D1048576" xr:uid="{5D231771-3882-478D-A1CA-52A980C397D7}">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:D1048576" xr:uid="{5D231771-3882-478D-A1CA-52A980C397D7}">
       <formula1>0</formula1>
       <formula2>0.999305555555556</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Mon Jun 23 13:49:31 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Solar_Lab_Tests.xlsx
+++ b/data/Solar_Lab_Tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="621" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5AB75CEB-56AE-4F10-AA3A-CE4592D7CAC3}"/>
+  <xr:revisionPtr revIDLastSave="625" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2881928C-CE12-4CFA-90B6-FDE40E8A56CD}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="8" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="8" activeTab="8" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Tests Map" sheetId="4" state="hidden" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="95">
   <si>
     <t>BOM</t>
   </si>
@@ -190,9 +190,6 @@
   </si>
   <si>
     <t>Hutian</t>
-  </si>
-  <si>
-    <t>Fato</t>
   </si>
   <si>
     <t>GLASS</t>
@@ -1843,10 +1840,10 @@
         <v>24</v>
       </c>
       <c r="C1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" t="s">
         <v>92</v>
-      </c>
-      <c r="D1" t="s">
-        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1889,7 +1886,7 @@
         <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1929,7 +1926,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2359,7 +2356,7 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="4">
@@ -2370,7 +2367,7 @@
         <v>36</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -2379,7 +2376,7 @@
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="K14" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -2388,7 +2385,7 @@
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="K15" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -2517,25 +2514,25 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" t="s">
         <v>44</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>45</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>46</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>47</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>48</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>49</v>
-      </c>
-      <c r="N1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -2552,10 +2549,10 @@
         <v>33</v>
       </c>
       <c r="K2" t="s">
+        <v>50</v>
+      </c>
+      <c r="N2" t="s">
         <v>51</v>
-      </c>
-      <c r="N2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -2572,10 +2569,10 @@
         <v>36</v>
       </c>
       <c r="K3" t="s">
+        <v>52</v>
+      </c>
+      <c r="N3" t="s">
         <v>53</v>
-      </c>
-      <c r="N3" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -2586,10 +2583,10 @@
         <v>5</v>
       </c>
       <c r="G4" t="s">
+        <v>54</v>
+      </c>
+      <c r="I4" t="s">
         <v>55</v>
-      </c>
-      <c r="I4" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -2613,7 +2610,7 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
@@ -2621,7 +2618,7 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
@@ -2629,7 +2626,7 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C9" t="s">
         <v>12</v>
@@ -2696,19 +2693,19 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>24</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D1" s="16"/>
       <c r="E1" s="16"/>
       <c r="F1" s="16"/>
       <c r="G1" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H1" s="18"/>
       <c r="I1" s="18"/>
@@ -2718,60 +2715,60 @@
       <c r="A2" s="20"/>
       <c r="B2" s="20"/>
       <c r="C2" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="E2" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="F2" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="F2" s="22" t="s">
-        <v>62</v>
-      </c>
       <c r="G2" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="H2" s="24" t="s">
+      <c r="I2" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="I2" s="24" t="s">
+      <c r="J2" s="25" t="s">
         <v>61</v>
-      </c>
-      <c r="J2" s="25" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:10" hidden="1">
       <c r="A3" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="C3" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="D3" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="E3" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="F3" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="F3" s="26" t="s">
+      <c r="G3" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="G3" s="26" t="s">
+      <c r="H3" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="H3" s="26" t="s">
+      <c r="I3" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="I3" s="26" t="s">
+      <c r="J3" s="26" t="s">
         <v>71</v>
-      </c>
-      <c r="J3" s="26" t="s">
-        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -2824,14 +2821,14 @@
       <c r="A1" s="28"/>
       <c r="B1" s="29"/>
       <c r="C1" s="30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D1" s="31"/>
       <c r="E1" s="30"/>
       <c r="F1" s="31"/>
       <c r="G1" s="32"/>
       <c r="H1" s="44" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I1" s="32"/>
       <c r="J1" s="29"/>
@@ -2844,19 +2841,19 @@
         <v>24</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D2" s="36"/>
       <c r="E2" s="37" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F2" s="38"/>
       <c r="G2" s="35" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="37" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J2" s="38"/>
     </row>
@@ -2864,60 +2861,60 @@
       <c r="A3" s="39"/>
       <c r="B3" s="34"/>
       <c r="C3" s="40" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" s="41" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="41" t="s">
-        <v>78</v>
-      </c>
       <c r="E3" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="F3" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="F3" s="43" t="s">
-        <v>78</v>
-      </c>
       <c r="G3" s="40" t="s">
+        <v>76</v>
+      </c>
+      <c r="H3" s="41" t="s">
         <v>77</v>
       </c>
-      <c r="H3" s="41" t="s">
-        <v>78</v>
-      </c>
       <c r="I3" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="J3" s="43" t="s">
         <v>77</v>
-      </c>
-      <c r="J3" s="43" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:10" customFormat="1" hidden="1">
       <c r="A4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" t="s">
         <v>63</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>64</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>65</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>66</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>67</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>68</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>69</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>70</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>71</v>
-      </c>
-      <c r="J4" t="s">
-        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -2964,10 +2961,10 @@
         <v>24</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>79</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="6" customFormat="1">
@@ -3028,25 +3025,25 @@
         <v>24</v>
       </c>
       <c r="C1" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="H1" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="I1" s="8" t="s">
         <v>86</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -3099,16 +3096,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C1" t="s">
         <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -3132,7 +3129,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3151,10 +3148,10 @@
         <v>24</v>
       </c>
       <c r="C1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" t="s">
         <v>90</v>
-      </c>
-      <c r="D1" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -3165,7 +3162,10 @@
         <v>37</v>
       </c>
       <c r="C3" s="10">
-        <v>0.59791666666666665</v>
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="D3" s="10">
+        <v>0.65</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -3177,6 +3177,9 @@
       </c>
       <c r="C4" s="10">
         <v>0.59791666666666665</v>
+      </c>
+      <c r="D4" s="10">
+        <v>0.60763888888888884</v>
       </c>
     </row>
     <row r="30" spans="3:3">

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Tue Jun 24 11:53:44 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Solar_Lab_Tests.xlsx
+++ b/data/Solar_Lab_Tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="631" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8A04623-E952-447E-BD45-6A162CDE66B7}"/>
+  <xr:revisionPtr revIDLastSave="661" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{130EE011-928E-4AEE-B6D1-9BE4D8C4C34C}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="8" activeTab="10" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="10" activeTab="1" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Tests Map" sheetId="4" state="hidden" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="96">
   <si>
     <t>BOM</t>
   </si>
@@ -1870,7 +1870,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{333C0630-51CF-46CA-8CAD-98FEF9AC181F}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -2060,8 +2060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9401EE47-EA52-49C7-BBC0-21F5B88254FB}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -2072,7 +2072,7 @@
     <col min="4" max="4" width="25.42578125" customWidth="1"/>
     <col min="5" max="5" width="30.28515625" customWidth="1"/>
     <col min="6" max="6" width="27.42578125" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="14.140625" customWidth="1"/>
     <col min="11" max="11" width="17.140625" hidden="1" customWidth="1"/>
   </cols>
@@ -2399,10 +2399,27 @@
       </c>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="1"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
+      <c r="A15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="5">
+        <v>45825</v>
+      </c>
+      <c r="E15" s="5">
+        <v>45807</v>
+      </c>
+      <c r="F15" s="4">
+        <v>45825</v>
+      </c>
+      <c r="H15" t="s">
+        <v>33</v>
+      </c>
       <c r="K15" s="3" t="s">
         <v>43</v>
       </c>
@@ -2475,7 +2492,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K8:K15" xr:uid="{C3958E6F-28D2-429E-9DF5-7DAD65BBE2ED}">
       <formula1>$K:$K</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576 A11" xr:uid="{8C537B12-83B7-48DB-9398-33493EB60A9D}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A11 C1:C1048576" xr:uid="{8C537B12-83B7-48DB-9398-33493EB60A9D}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -2696,10 +2713,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61A5C69B-8639-4E8F-9A05-E59E5511083E}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2790,9 +2807,76 @@
         <v>72</v>
       </c>
     </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="27">
+        <v>200.3</v>
+      </c>
+      <c r="D4" s="27">
+        <v>199.82</v>
+      </c>
+      <c r="E4" s="27">
+        <v>199.62</v>
+      </c>
+      <c r="F4" s="27">
+        <v>200.75</v>
+      </c>
+      <c r="G4" s="27">
+        <v>201.12</v>
+      </c>
+      <c r="H4" s="27">
+        <v>200.16</v>
+      </c>
+      <c r="I4" s="27">
+        <v>199.93</v>
+      </c>
+      <c r="J4" s="27">
+        <v>201.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="27">
+        <v>199.98</v>
+      </c>
+      <c r="D5" s="27">
+        <v>200.79</v>
+      </c>
+      <c r="E5" s="27">
+        <v>199.58</v>
+      </c>
+      <c r="F5" s="27">
+        <v>199.98</v>
+      </c>
+      <c r="G5" s="27">
+        <v>201.21</v>
+      </c>
+      <c r="H5" s="27">
+        <v>202.13</v>
+      </c>
+      <c r="I5" s="27">
+        <v>199.34</v>
+      </c>
+      <c r="J5" s="27">
+        <v>199.9</v>
+      </c>
+    </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2" xr:uid="{5C73BBC5-C68D-4586-BDB5-A3BE48854FB6}"/>
+  <dataValidations count="2">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2 B4:B5" xr:uid="{5C73BBC5-C68D-4586-BDB5-A3BE48854FB6}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4:A1048576" xr:uid="{18FD80CD-FFDC-48A1-BA45-91576461B09B}">
+      <formula1>"FRONT EPE, BACK EVA"</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Wed Jun 25 13:49:48 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Solar_Lab_Tests.xlsx
+++ b/data/Solar_Lab_Tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="661" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{130EE011-928E-4AEE-B6D1-9BE4D8C4C34C}"/>
+  <xr:revisionPtr revIDLastSave="675" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3FADE34F-1E4D-49C5-8031-8738EB6AA421}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="10" activeTab="1" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="3" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Tests Map" sheetId="4" state="hidden" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="96">
   <si>
     <t>BOM</t>
   </si>
@@ -502,7 +502,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -636,11 +636,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -713,6 +726,7 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1285,8 +1299,8 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{7FFEF855-2CB7-4EF4-BE50-FB81C544017B}" name="Table18" displayName="Table18" ref="A3:J1048576" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
-  <autoFilter ref="A3:J1048576" xr:uid="{7FFEF855-2CB7-4EF4-BE50-FB81C544017B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{7FFEF855-2CB7-4EF4-BE50-FB81C544017B}" name="Table18" displayName="Table18" ref="B3:K1048576" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
+  <autoFilter ref="B3:K1048576" xr:uid="{7FFEF855-2CB7-4EF4-BE50-FB81C544017B}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{96E09178-FF72-435C-90A9-F2F7FEC7E80C}" name="Column1" dataDxfId="32"/>
     <tableColumn id="2" xr3:uid="{B7D3E49F-4F89-454D-B9FA-E1364CBF3239}" name="Column2" dataDxfId="31"/>
@@ -2060,8 +2074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9401EE47-EA52-49C7-BBC0-21F5B88254FB}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -2713,169 +2727,1726 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61A5C69B-8639-4E8F-9A05-E59E5511083E}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:K519"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" style="27" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" style="27" customWidth="1"/>
-    <col min="3" max="9" width="11.5703125" style="27" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" style="27" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" style="27" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" style="27" customWidth="1"/>
+    <col min="4" max="10" width="11.5703125" style="27" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" style="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="C1" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="D1" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="16"/>
       <c r="E1" s="16"/>
       <c r="F1" s="16"/>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="16"/>
+      <c r="H1" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="H1" s="18"/>
       <c r="I1" s="18"/>
-      <c r="J1" s="19"/>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="J1" s="18"/>
+      <c r="K1" s="19"/>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="20"/>
       <c r="B2" s="20"/>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="20"/>
+      <c r="D2" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="E2" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="F2" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="G2" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="G2" s="23" t="s">
+      <c r="H2" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="H2" s="24" t="s">
+      <c r="I2" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="I2" s="24" t="s">
+      <c r="J2" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="J2" s="25" t="s">
+      <c r="K2" s="25" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:10" hidden="1">
-      <c r="A3" s="26" t="s">
+    <row r="3" spans="1:11" hidden="1">
+      <c r="A3" s="46"/>
+      <c r="B3" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="C3" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="D3" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="E3" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="F3" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="F3" s="26" t="s">
+      <c r="G3" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="G3" s="26" t="s">
+      <c r="H3" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="H3" s="26" t="s">
+      <c r="I3" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="I3" s="26" t="s">
+      <c r="J3" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="J3" s="26" t="s">
+      <c r="K3" s="26" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="27" t="s">
+    <row r="4" spans="1:11">
+      <c r="A4" s="46" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="27">
+      <c r="D4" s="27">
         <v>200.3</v>
       </c>
-      <c r="D4" s="27">
+      <c r="E4" s="27">
         <v>199.82</v>
       </c>
-      <c r="E4" s="27">
+      <c r="F4" s="27">
         <v>199.62</v>
       </c>
-      <c r="F4" s="27">
+      <c r="G4" s="27">
         <v>200.75</v>
       </c>
-      <c r="G4" s="27">
+      <c r="H4" s="27">
         <v>201.12</v>
       </c>
-      <c r="H4" s="27">
+      <c r="I4" s="27">
         <v>200.16</v>
       </c>
-      <c r="I4" s="27">
+      <c r="J4" s="27">
         <v>199.93</v>
       </c>
-      <c r="J4" s="27">
+      <c r="K4" s="27">
         <v>201.9</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="27" t="s">
+    <row r="5" spans="1:11">
+      <c r="A5" s="46" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="27">
+      <c r="D5" s="27">
         <v>199.98</v>
       </c>
-      <c r="D5" s="27">
+      <c r="E5" s="27">
         <v>200.79</v>
       </c>
-      <c r="E5" s="27">
+      <c r="F5" s="27">
         <v>199.58</v>
       </c>
-      <c r="F5" s="27">
+      <c r="G5" s="27">
         <v>199.98</v>
       </c>
-      <c r="G5" s="27">
+      <c r="H5" s="27">
         <v>201.21</v>
       </c>
-      <c r="H5" s="27">
+      <c r="I5" s="27">
         <v>202.13</v>
       </c>
-      <c r="I5" s="27">
+      <c r="J5" s="27">
         <v>199.34</v>
       </c>
-      <c r="J5" s="27">
+      <c r="K5" s="27">
         <v>199.9</v>
       </c>
     </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="46"/>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="46"/>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="46"/>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="46"/>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="46"/>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="46"/>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="46"/>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="46"/>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="46"/>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="46"/>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="46"/>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="46"/>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="46"/>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="46"/>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="46"/>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="46"/>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="46"/>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="46"/>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="46"/>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="46"/>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="46"/>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" s="46"/>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" s="46"/>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" s="46"/>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" s="46"/>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" s="46"/>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" s="46"/>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="46"/>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="46"/>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="46"/>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="46"/>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" s="46"/>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" s="46"/>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" s="46"/>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" s="46"/>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" s="46"/>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" s="46"/>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" s="46"/>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" s="46"/>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" s="46"/>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" s="46"/>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" s="46"/>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" s="46"/>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" s="46"/>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" s="46"/>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" s="46"/>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" s="46"/>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" s="46"/>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" s="46"/>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" s="46"/>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" s="46"/>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" s="46"/>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" s="46"/>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" s="46"/>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" s="46"/>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" s="46"/>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" s="46"/>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" s="46"/>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" s="46"/>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" s="46"/>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" s="46"/>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" s="46"/>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" s="46"/>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" s="46"/>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" s="46"/>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" s="46"/>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" s="46"/>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" s="46"/>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" s="46"/>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" s="46"/>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" s="46"/>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" s="46"/>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" s="46"/>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" s="46"/>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" s="46"/>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" s="46"/>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" s="46"/>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" s="46"/>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" s="46"/>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" s="46"/>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" s="46"/>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" s="46"/>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" s="46"/>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" s="46"/>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90" s="46"/>
+    </row>
+    <row r="91" spans="1:1">
+      <c r="A91" s="46"/>
+    </row>
+    <row r="92" spans="1:1">
+      <c r="A92" s="46"/>
+    </row>
+    <row r="93" spans="1:1">
+      <c r="A93" s="46"/>
+    </row>
+    <row r="94" spans="1:1">
+      <c r="A94" s="46"/>
+    </row>
+    <row r="95" spans="1:1">
+      <c r="A95" s="46"/>
+    </row>
+    <row r="96" spans="1:1">
+      <c r="A96" s="46"/>
+    </row>
+    <row r="97" spans="1:1">
+      <c r="A97" s="46"/>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98" s="46"/>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99" s="46"/>
+    </row>
+    <row r="100" spans="1:1">
+      <c r="A100" s="46"/>
+    </row>
+    <row r="101" spans="1:1">
+      <c r="A101" s="46"/>
+    </row>
+    <row r="102" spans="1:1">
+      <c r="A102" s="46"/>
+    </row>
+    <row r="103" spans="1:1">
+      <c r="A103" s="46"/>
+    </row>
+    <row r="104" spans="1:1">
+      <c r="A104" s="46"/>
+    </row>
+    <row r="105" spans="1:1">
+      <c r="A105" s="46"/>
+    </row>
+    <row r="106" spans="1:1">
+      <c r="A106" s="46"/>
+    </row>
+    <row r="107" spans="1:1">
+      <c r="A107" s="46"/>
+    </row>
+    <row r="108" spans="1:1">
+      <c r="A108" s="46"/>
+    </row>
+    <row r="109" spans="1:1">
+      <c r="A109" s="46"/>
+    </row>
+    <row r="110" spans="1:1">
+      <c r="A110" s="46"/>
+    </row>
+    <row r="111" spans="1:1">
+      <c r="A111" s="46"/>
+    </row>
+    <row r="112" spans="1:1">
+      <c r="A112" s="46"/>
+    </row>
+    <row r="113" spans="1:1">
+      <c r="A113" s="46"/>
+    </row>
+    <row r="114" spans="1:1">
+      <c r="A114" s="46"/>
+    </row>
+    <row r="115" spans="1:1">
+      <c r="A115" s="46"/>
+    </row>
+    <row r="116" spans="1:1">
+      <c r="A116" s="46"/>
+    </row>
+    <row r="117" spans="1:1">
+      <c r="A117" s="46"/>
+    </row>
+    <row r="118" spans="1:1">
+      <c r="A118" s="46"/>
+    </row>
+    <row r="119" spans="1:1">
+      <c r="A119" s="46"/>
+    </row>
+    <row r="120" spans="1:1">
+      <c r="A120" s="46"/>
+    </row>
+    <row r="121" spans="1:1">
+      <c r="A121" s="46"/>
+    </row>
+    <row r="122" spans="1:1">
+      <c r="A122" s="46"/>
+    </row>
+    <row r="123" spans="1:1">
+      <c r="A123" s="46"/>
+    </row>
+    <row r="124" spans="1:1">
+      <c r="A124" s="46"/>
+    </row>
+    <row r="125" spans="1:1">
+      <c r="A125" s="46"/>
+    </row>
+    <row r="126" spans="1:1">
+      <c r="A126" s="46"/>
+    </row>
+    <row r="127" spans="1:1">
+      <c r="A127" s="46"/>
+    </row>
+    <row r="128" spans="1:1">
+      <c r="A128" s="46"/>
+    </row>
+    <row r="129" spans="1:1">
+      <c r="A129" s="46"/>
+    </row>
+    <row r="130" spans="1:1">
+      <c r="A130" s="46"/>
+    </row>
+    <row r="131" spans="1:1">
+      <c r="A131" s="46"/>
+    </row>
+    <row r="132" spans="1:1">
+      <c r="A132" s="46"/>
+    </row>
+    <row r="133" spans="1:1">
+      <c r="A133" s="46"/>
+    </row>
+    <row r="134" spans="1:1">
+      <c r="A134" s="46"/>
+    </row>
+    <row r="135" spans="1:1">
+      <c r="A135" s="46"/>
+    </row>
+    <row r="136" spans="1:1">
+      <c r="A136" s="46"/>
+    </row>
+    <row r="137" spans="1:1">
+      <c r="A137" s="46"/>
+    </row>
+    <row r="138" spans="1:1">
+      <c r="A138" s="46"/>
+    </row>
+    <row r="139" spans="1:1">
+      <c r="A139" s="46"/>
+    </row>
+    <row r="140" spans="1:1">
+      <c r="A140" s="46"/>
+    </row>
+    <row r="141" spans="1:1">
+      <c r="A141" s="46"/>
+    </row>
+    <row r="142" spans="1:1">
+      <c r="A142" s="46"/>
+    </row>
+    <row r="143" spans="1:1">
+      <c r="A143" s="46"/>
+    </row>
+    <row r="144" spans="1:1">
+      <c r="A144" s="46"/>
+    </row>
+    <row r="145" spans="1:1">
+      <c r="A145" s="46"/>
+    </row>
+    <row r="146" spans="1:1">
+      <c r="A146" s="46"/>
+    </row>
+    <row r="147" spans="1:1">
+      <c r="A147" s="46"/>
+    </row>
+    <row r="148" spans="1:1">
+      <c r="A148" s="46"/>
+    </row>
+    <row r="149" spans="1:1">
+      <c r="A149" s="46"/>
+    </row>
+    <row r="150" spans="1:1">
+      <c r="A150" s="46"/>
+    </row>
+    <row r="151" spans="1:1">
+      <c r="A151" s="46"/>
+    </row>
+    <row r="152" spans="1:1">
+      <c r="A152" s="46"/>
+    </row>
+    <row r="153" spans="1:1">
+      <c r="A153" s="46"/>
+    </row>
+    <row r="154" spans="1:1">
+      <c r="A154" s="46"/>
+    </row>
+    <row r="155" spans="1:1">
+      <c r="A155" s="46"/>
+    </row>
+    <row r="156" spans="1:1">
+      <c r="A156" s="46"/>
+    </row>
+    <row r="157" spans="1:1">
+      <c r="A157" s="46"/>
+    </row>
+    <row r="158" spans="1:1">
+      <c r="A158" s="46"/>
+    </row>
+    <row r="159" spans="1:1">
+      <c r="A159" s="46"/>
+    </row>
+    <row r="160" spans="1:1">
+      <c r="A160" s="46"/>
+    </row>
+    <row r="161" spans="1:1">
+      <c r="A161" s="46"/>
+    </row>
+    <row r="162" spans="1:1">
+      <c r="A162" s="46"/>
+    </row>
+    <row r="163" spans="1:1">
+      <c r="A163" s="46"/>
+    </row>
+    <row r="164" spans="1:1">
+      <c r="A164" s="46"/>
+    </row>
+    <row r="165" spans="1:1">
+      <c r="A165" s="46"/>
+    </row>
+    <row r="166" spans="1:1">
+      <c r="A166" s="46"/>
+    </row>
+    <row r="167" spans="1:1">
+      <c r="A167" s="46"/>
+    </row>
+    <row r="168" spans="1:1">
+      <c r="A168" s="46"/>
+    </row>
+    <row r="169" spans="1:1">
+      <c r="A169" s="46"/>
+    </row>
+    <row r="170" spans="1:1">
+      <c r="A170" s="46"/>
+    </row>
+    <row r="171" spans="1:1">
+      <c r="A171" s="46"/>
+    </row>
+    <row r="172" spans="1:1">
+      <c r="A172" s="46"/>
+    </row>
+    <row r="173" spans="1:1">
+      <c r="A173" s="46"/>
+    </row>
+    <row r="174" spans="1:1">
+      <c r="A174" s="46"/>
+    </row>
+    <row r="175" spans="1:1">
+      <c r="A175" s="46"/>
+    </row>
+    <row r="176" spans="1:1">
+      <c r="A176" s="46"/>
+    </row>
+    <row r="177" spans="1:1">
+      <c r="A177" s="46"/>
+    </row>
+    <row r="178" spans="1:1">
+      <c r="A178" s="46"/>
+    </row>
+    <row r="179" spans="1:1">
+      <c r="A179" s="46"/>
+    </row>
+    <row r="180" spans="1:1">
+      <c r="A180" s="46"/>
+    </row>
+    <row r="181" spans="1:1">
+      <c r="A181" s="46"/>
+    </row>
+    <row r="182" spans="1:1">
+      <c r="A182" s="46"/>
+    </row>
+    <row r="183" spans="1:1">
+      <c r="A183" s="46"/>
+    </row>
+    <row r="184" spans="1:1">
+      <c r="A184" s="46"/>
+    </row>
+    <row r="185" spans="1:1">
+      <c r="A185" s="46"/>
+    </row>
+    <row r="186" spans="1:1">
+      <c r="A186" s="46"/>
+    </row>
+    <row r="187" spans="1:1">
+      <c r="A187" s="46"/>
+    </row>
+    <row r="188" spans="1:1">
+      <c r="A188" s="46"/>
+    </row>
+    <row r="189" spans="1:1">
+      <c r="A189" s="46"/>
+    </row>
+    <row r="190" spans="1:1">
+      <c r="A190" s="46"/>
+    </row>
+    <row r="191" spans="1:1">
+      <c r="A191" s="46"/>
+    </row>
+    <row r="192" spans="1:1">
+      <c r="A192" s="46"/>
+    </row>
+    <row r="193" spans="1:1">
+      <c r="A193" s="46"/>
+    </row>
+    <row r="194" spans="1:1">
+      <c r="A194" s="46"/>
+    </row>
+    <row r="195" spans="1:1">
+      <c r="A195" s="46"/>
+    </row>
+    <row r="196" spans="1:1">
+      <c r="A196" s="46"/>
+    </row>
+    <row r="197" spans="1:1">
+      <c r="A197" s="46"/>
+    </row>
+    <row r="198" spans="1:1">
+      <c r="A198" s="46"/>
+    </row>
+    <row r="199" spans="1:1">
+      <c r="A199" s="46"/>
+    </row>
+    <row r="200" spans="1:1">
+      <c r="A200" s="46"/>
+    </row>
+    <row r="201" spans="1:1">
+      <c r="A201" s="46"/>
+    </row>
+    <row r="202" spans="1:1">
+      <c r="A202" s="46"/>
+    </row>
+    <row r="203" spans="1:1">
+      <c r="A203" s="46"/>
+    </row>
+    <row r="204" spans="1:1">
+      <c r="A204" s="46"/>
+    </row>
+    <row r="205" spans="1:1">
+      <c r="A205" s="46"/>
+    </row>
+    <row r="206" spans="1:1">
+      <c r="A206" s="46"/>
+    </row>
+    <row r="207" spans="1:1">
+      <c r="A207" s="46"/>
+    </row>
+    <row r="208" spans="1:1">
+      <c r="A208" s="46"/>
+    </row>
+    <row r="209" spans="1:1">
+      <c r="A209" s="46"/>
+    </row>
+    <row r="210" spans="1:1">
+      <c r="A210" s="46"/>
+    </row>
+    <row r="211" spans="1:1">
+      <c r="A211" s="46"/>
+    </row>
+    <row r="212" spans="1:1">
+      <c r="A212" s="46"/>
+    </row>
+    <row r="213" spans="1:1">
+      <c r="A213" s="46"/>
+    </row>
+    <row r="214" spans="1:1">
+      <c r="A214" s="46"/>
+    </row>
+    <row r="215" spans="1:1">
+      <c r="A215" s="46"/>
+    </row>
+    <row r="216" spans="1:1">
+      <c r="A216" s="46"/>
+    </row>
+    <row r="217" spans="1:1">
+      <c r="A217" s="46"/>
+    </row>
+    <row r="218" spans="1:1">
+      <c r="A218" s="46"/>
+    </row>
+    <row r="219" spans="1:1">
+      <c r="A219" s="46"/>
+    </row>
+    <row r="220" spans="1:1">
+      <c r="A220" s="46"/>
+    </row>
+    <row r="221" spans="1:1">
+      <c r="A221" s="46"/>
+    </row>
+    <row r="222" spans="1:1">
+      <c r="A222" s="46"/>
+    </row>
+    <row r="223" spans="1:1">
+      <c r="A223" s="46"/>
+    </row>
+    <row r="224" spans="1:1">
+      <c r="A224" s="46"/>
+    </row>
+    <row r="225" spans="1:1">
+      <c r="A225" s="46"/>
+    </row>
+    <row r="226" spans="1:1">
+      <c r="A226" s="46"/>
+    </row>
+    <row r="227" spans="1:1">
+      <c r="A227" s="46"/>
+    </row>
+    <row r="228" spans="1:1">
+      <c r="A228" s="46"/>
+    </row>
+    <row r="229" spans="1:1">
+      <c r="A229" s="46"/>
+    </row>
+    <row r="230" spans="1:1">
+      <c r="A230" s="46"/>
+    </row>
+    <row r="231" spans="1:1">
+      <c r="A231" s="46"/>
+    </row>
+    <row r="232" spans="1:1">
+      <c r="A232" s="46"/>
+    </row>
+    <row r="233" spans="1:1">
+      <c r="A233" s="46"/>
+    </row>
+    <row r="234" spans="1:1">
+      <c r="A234" s="46"/>
+    </row>
+    <row r="235" spans="1:1">
+      <c r="A235" s="46"/>
+    </row>
+    <row r="236" spans="1:1">
+      <c r="A236" s="46"/>
+    </row>
+    <row r="237" spans="1:1">
+      <c r="A237" s="46"/>
+    </row>
+    <row r="238" spans="1:1">
+      <c r="A238" s="46"/>
+    </row>
+    <row r="239" spans="1:1">
+      <c r="A239" s="46"/>
+    </row>
+    <row r="240" spans="1:1">
+      <c r="A240" s="46"/>
+    </row>
+    <row r="241" spans="1:1">
+      <c r="A241" s="46"/>
+    </row>
+    <row r="242" spans="1:1">
+      <c r="A242" s="46"/>
+    </row>
+    <row r="243" spans="1:1">
+      <c r="A243" s="46"/>
+    </row>
+    <row r="244" spans="1:1">
+      <c r="A244" s="46"/>
+    </row>
+    <row r="245" spans="1:1">
+      <c r="A245" s="46"/>
+    </row>
+    <row r="246" spans="1:1">
+      <c r="A246" s="46"/>
+    </row>
+    <row r="247" spans="1:1">
+      <c r="A247" s="46"/>
+    </row>
+    <row r="248" spans="1:1">
+      <c r="A248" s="46"/>
+    </row>
+    <row r="249" spans="1:1">
+      <c r="A249" s="46"/>
+    </row>
+    <row r="250" spans="1:1">
+      <c r="A250" s="46"/>
+    </row>
+    <row r="251" spans="1:1">
+      <c r="A251" s="46"/>
+    </row>
+    <row r="252" spans="1:1">
+      <c r="A252" s="46"/>
+    </row>
+    <row r="253" spans="1:1">
+      <c r="A253" s="46"/>
+    </row>
+    <row r="254" spans="1:1">
+      <c r="A254" s="46"/>
+    </row>
+    <row r="255" spans="1:1">
+      <c r="A255" s="46"/>
+    </row>
+    <row r="256" spans="1:1">
+      <c r="A256" s="46"/>
+    </row>
+    <row r="257" spans="1:1">
+      <c r="A257" s="46"/>
+    </row>
+    <row r="258" spans="1:1">
+      <c r="A258" s="46"/>
+    </row>
+    <row r="259" spans="1:1">
+      <c r="A259" s="46"/>
+    </row>
+    <row r="260" spans="1:1">
+      <c r="A260" s="46"/>
+    </row>
+    <row r="261" spans="1:1">
+      <c r="A261" s="46"/>
+    </row>
+    <row r="262" spans="1:1">
+      <c r="A262" s="46"/>
+    </row>
+    <row r="263" spans="1:1">
+      <c r="A263" s="46"/>
+    </row>
+    <row r="264" spans="1:1">
+      <c r="A264" s="46"/>
+    </row>
+    <row r="265" spans="1:1">
+      <c r="A265" s="46"/>
+    </row>
+    <row r="266" spans="1:1">
+      <c r="A266" s="46"/>
+    </row>
+    <row r="267" spans="1:1">
+      <c r="A267" s="46"/>
+    </row>
+    <row r="268" spans="1:1">
+      <c r="A268" s="46"/>
+    </row>
+    <row r="269" spans="1:1">
+      <c r="A269" s="46"/>
+    </row>
+    <row r="270" spans="1:1">
+      <c r="A270" s="46"/>
+    </row>
+    <row r="271" spans="1:1">
+      <c r="A271" s="46"/>
+    </row>
+    <row r="272" spans="1:1">
+      <c r="A272" s="46"/>
+    </row>
+    <row r="273" spans="1:1">
+      <c r="A273" s="46"/>
+    </row>
+    <row r="274" spans="1:1">
+      <c r="A274" s="46"/>
+    </row>
+    <row r="275" spans="1:1">
+      <c r="A275" s="46"/>
+    </row>
+    <row r="276" spans="1:1">
+      <c r="A276" s="46"/>
+    </row>
+    <row r="277" spans="1:1">
+      <c r="A277" s="46"/>
+    </row>
+    <row r="278" spans="1:1">
+      <c r="A278" s="46"/>
+    </row>
+    <row r="279" spans="1:1">
+      <c r="A279" s="46"/>
+    </row>
+    <row r="280" spans="1:1">
+      <c r="A280" s="46"/>
+    </row>
+    <row r="281" spans="1:1">
+      <c r="A281" s="46"/>
+    </row>
+    <row r="282" spans="1:1">
+      <c r="A282" s="46"/>
+    </row>
+    <row r="283" spans="1:1">
+      <c r="A283" s="46"/>
+    </row>
+    <row r="284" spans="1:1">
+      <c r="A284" s="46"/>
+    </row>
+    <row r="285" spans="1:1">
+      <c r="A285" s="46"/>
+    </row>
+    <row r="286" spans="1:1">
+      <c r="A286" s="46"/>
+    </row>
+    <row r="287" spans="1:1">
+      <c r="A287" s="46"/>
+    </row>
+    <row r="288" spans="1:1">
+      <c r="A288" s="46"/>
+    </row>
+    <row r="289" spans="1:1">
+      <c r="A289" s="46"/>
+    </row>
+    <row r="290" spans="1:1">
+      <c r="A290" s="46"/>
+    </row>
+    <row r="291" spans="1:1">
+      <c r="A291" s="46"/>
+    </row>
+    <row r="292" spans="1:1">
+      <c r="A292" s="46"/>
+    </row>
+    <row r="293" spans="1:1">
+      <c r="A293" s="46"/>
+    </row>
+    <row r="294" spans="1:1">
+      <c r="A294" s="46"/>
+    </row>
+    <row r="295" spans="1:1">
+      <c r="A295" s="46"/>
+    </row>
+    <row r="296" spans="1:1">
+      <c r="A296" s="46"/>
+    </row>
+    <row r="297" spans="1:1">
+      <c r="A297" s="46"/>
+    </row>
+    <row r="298" spans="1:1">
+      <c r="A298" s="46"/>
+    </row>
+    <row r="299" spans="1:1">
+      <c r="A299" s="46"/>
+    </row>
+    <row r="300" spans="1:1">
+      <c r="A300" s="46"/>
+    </row>
+    <row r="301" spans="1:1">
+      <c r="A301" s="46"/>
+    </row>
+    <row r="302" spans="1:1">
+      <c r="A302" s="46"/>
+    </row>
+    <row r="303" spans="1:1">
+      <c r="A303" s="46"/>
+    </row>
+    <row r="304" spans="1:1">
+      <c r="A304" s="46"/>
+    </row>
+    <row r="305" spans="1:1">
+      <c r="A305" s="46"/>
+    </row>
+    <row r="306" spans="1:1">
+      <c r="A306" s="46"/>
+    </row>
+    <row r="307" spans="1:1">
+      <c r="A307" s="46"/>
+    </row>
+    <row r="308" spans="1:1">
+      <c r="A308" s="46"/>
+    </row>
+    <row r="309" spans="1:1">
+      <c r="A309" s="46"/>
+    </row>
+    <row r="310" spans="1:1">
+      <c r="A310" s="46"/>
+    </row>
+    <row r="311" spans="1:1">
+      <c r="A311" s="46"/>
+    </row>
+    <row r="312" spans="1:1">
+      <c r="A312" s="46"/>
+    </row>
+    <row r="313" spans="1:1">
+      <c r="A313" s="46"/>
+    </row>
+    <row r="314" spans="1:1">
+      <c r="A314" s="46"/>
+    </row>
+    <row r="315" spans="1:1">
+      <c r="A315" s="46"/>
+    </row>
+    <row r="316" spans="1:1">
+      <c r="A316" s="46"/>
+    </row>
+    <row r="317" spans="1:1">
+      <c r="A317" s="46"/>
+    </row>
+    <row r="318" spans="1:1">
+      <c r="A318" s="46"/>
+    </row>
+    <row r="319" spans="1:1">
+      <c r="A319" s="46"/>
+    </row>
+    <row r="320" spans="1:1">
+      <c r="A320" s="46"/>
+    </row>
+    <row r="321" spans="1:1">
+      <c r="A321" s="46"/>
+    </row>
+    <row r="322" spans="1:1">
+      <c r="A322" s="46"/>
+    </row>
+    <row r="323" spans="1:1">
+      <c r="A323" s="46"/>
+    </row>
+    <row r="324" spans="1:1">
+      <c r="A324" s="46"/>
+    </row>
+    <row r="325" spans="1:1">
+      <c r="A325" s="46"/>
+    </row>
+    <row r="326" spans="1:1">
+      <c r="A326" s="46"/>
+    </row>
+    <row r="327" spans="1:1">
+      <c r="A327" s="46"/>
+    </row>
+    <row r="328" spans="1:1">
+      <c r="A328" s="46"/>
+    </row>
+    <row r="329" spans="1:1">
+      <c r="A329" s="46"/>
+    </row>
+    <row r="330" spans="1:1">
+      <c r="A330" s="46"/>
+    </row>
+    <row r="331" spans="1:1">
+      <c r="A331" s="46"/>
+    </row>
+    <row r="332" spans="1:1">
+      <c r="A332" s="46"/>
+    </row>
+    <row r="333" spans="1:1">
+      <c r="A333" s="46"/>
+    </row>
+    <row r="334" spans="1:1">
+      <c r="A334" s="46"/>
+    </row>
+    <row r="335" spans="1:1">
+      <c r="A335" s="46"/>
+    </row>
+    <row r="336" spans="1:1">
+      <c r="A336" s="46"/>
+    </row>
+    <row r="337" spans="1:1">
+      <c r="A337" s="46"/>
+    </row>
+    <row r="338" spans="1:1">
+      <c r="A338" s="46"/>
+    </row>
+    <row r="339" spans="1:1">
+      <c r="A339" s="46"/>
+    </row>
+    <row r="340" spans="1:1">
+      <c r="A340" s="46"/>
+    </row>
+    <row r="341" spans="1:1">
+      <c r="A341" s="46"/>
+    </row>
+    <row r="342" spans="1:1">
+      <c r="A342" s="46"/>
+    </row>
+    <row r="343" spans="1:1">
+      <c r="A343" s="46"/>
+    </row>
+    <row r="344" spans="1:1">
+      <c r="A344" s="46"/>
+    </row>
+    <row r="345" spans="1:1">
+      <c r="A345" s="46"/>
+    </row>
+    <row r="346" spans="1:1">
+      <c r="A346" s="46"/>
+    </row>
+    <row r="347" spans="1:1">
+      <c r="A347" s="46"/>
+    </row>
+    <row r="348" spans="1:1">
+      <c r="A348" s="46"/>
+    </row>
+    <row r="349" spans="1:1">
+      <c r="A349" s="46"/>
+    </row>
+    <row r="350" spans="1:1">
+      <c r="A350" s="46"/>
+    </row>
+    <row r="351" spans="1:1">
+      <c r="A351" s="46"/>
+    </row>
+    <row r="352" spans="1:1">
+      <c r="A352" s="46"/>
+    </row>
+    <row r="353" spans="1:1">
+      <c r="A353" s="46"/>
+    </row>
+    <row r="354" spans="1:1">
+      <c r="A354" s="46"/>
+    </row>
+    <row r="355" spans="1:1">
+      <c r="A355" s="46"/>
+    </row>
+    <row r="356" spans="1:1">
+      <c r="A356" s="46"/>
+    </row>
+    <row r="357" spans="1:1">
+      <c r="A357" s="46"/>
+    </row>
+    <row r="358" spans="1:1">
+      <c r="A358" s="46"/>
+    </row>
+    <row r="359" spans="1:1">
+      <c r="A359" s="46"/>
+    </row>
+    <row r="360" spans="1:1">
+      <c r="A360" s="46"/>
+    </row>
+    <row r="361" spans="1:1">
+      <c r="A361" s="46"/>
+    </row>
+    <row r="362" spans="1:1">
+      <c r="A362" s="46"/>
+    </row>
+    <row r="363" spans="1:1">
+      <c r="A363" s="46"/>
+    </row>
+    <row r="364" spans="1:1">
+      <c r="A364" s="46"/>
+    </row>
+    <row r="365" spans="1:1">
+      <c r="A365" s="46"/>
+    </row>
+    <row r="366" spans="1:1">
+      <c r="A366" s="46"/>
+    </row>
+    <row r="367" spans="1:1">
+      <c r="A367" s="46"/>
+    </row>
+    <row r="368" spans="1:1">
+      <c r="A368" s="46"/>
+    </row>
+    <row r="369" spans="1:1">
+      <c r="A369" s="46"/>
+    </row>
+    <row r="370" spans="1:1">
+      <c r="A370" s="46"/>
+    </row>
+    <row r="371" spans="1:1">
+      <c r="A371" s="46"/>
+    </row>
+    <row r="372" spans="1:1">
+      <c r="A372" s="46"/>
+    </row>
+    <row r="373" spans="1:1">
+      <c r="A373" s="46"/>
+    </row>
+    <row r="374" spans="1:1">
+      <c r="A374" s="46"/>
+    </row>
+    <row r="375" spans="1:1">
+      <c r="A375" s="46"/>
+    </row>
+    <row r="376" spans="1:1">
+      <c r="A376" s="46"/>
+    </row>
+    <row r="377" spans="1:1">
+      <c r="A377" s="46"/>
+    </row>
+    <row r="378" spans="1:1">
+      <c r="A378" s="46"/>
+    </row>
+    <row r="379" spans="1:1">
+      <c r="A379" s="46"/>
+    </row>
+    <row r="380" spans="1:1">
+      <c r="A380" s="46"/>
+    </row>
+    <row r="381" spans="1:1">
+      <c r="A381" s="46"/>
+    </row>
+    <row r="382" spans="1:1">
+      <c r="A382" s="46"/>
+    </row>
+    <row r="383" spans="1:1">
+      <c r="A383" s="46"/>
+    </row>
+    <row r="384" spans="1:1">
+      <c r="A384" s="46"/>
+    </row>
+    <row r="385" spans="1:1">
+      <c r="A385" s="46"/>
+    </row>
+    <row r="386" spans="1:1">
+      <c r="A386" s="46"/>
+    </row>
+    <row r="387" spans="1:1">
+      <c r="A387" s="46"/>
+    </row>
+    <row r="388" spans="1:1">
+      <c r="A388" s="46"/>
+    </row>
+    <row r="389" spans="1:1">
+      <c r="A389" s="46"/>
+    </row>
+    <row r="390" spans="1:1">
+      <c r="A390" s="46"/>
+    </row>
+    <row r="391" spans="1:1">
+      <c r="A391" s="46"/>
+    </row>
+    <row r="392" spans="1:1">
+      <c r="A392" s="46"/>
+    </row>
+    <row r="393" spans="1:1">
+      <c r="A393" s="46"/>
+    </row>
+    <row r="394" spans="1:1">
+      <c r="A394" s="46"/>
+    </row>
+    <row r="395" spans="1:1">
+      <c r="A395" s="46"/>
+    </row>
+    <row r="396" spans="1:1">
+      <c r="A396" s="46"/>
+    </row>
+    <row r="397" spans="1:1">
+      <c r="A397" s="46"/>
+    </row>
+    <row r="398" spans="1:1">
+      <c r="A398" s="46"/>
+    </row>
+    <row r="399" spans="1:1">
+      <c r="A399" s="46"/>
+    </row>
+    <row r="400" spans="1:1">
+      <c r="A400" s="46"/>
+    </row>
+    <row r="401" spans="1:1">
+      <c r="A401" s="46"/>
+    </row>
+    <row r="402" spans="1:1">
+      <c r="A402" s="46"/>
+    </row>
+    <row r="403" spans="1:1">
+      <c r="A403" s="46"/>
+    </row>
+    <row r="404" spans="1:1">
+      <c r="A404" s="46"/>
+    </row>
+    <row r="405" spans="1:1">
+      <c r="A405" s="46"/>
+    </row>
+    <row r="406" spans="1:1">
+      <c r="A406" s="46"/>
+    </row>
+    <row r="407" spans="1:1">
+      <c r="A407" s="46"/>
+    </row>
+    <row r="408" spans="1:1">
+      <c r="A408" s="46"/>
+    </row>
+    <row r="409" spans="1:1">
+      <c r="A409" s="46"/>
+    </row>
+    <row r="410" spans="1:1">
+      <c r="A410" s="46"/>
+    </row>
+    <row r="411" spans="1:1">
+      <c r="A411" s="46"/>
+    </row>
+    <row r="412" spans="1:1">
+      <c r="A412" s="46"/>
+    </row>
+    <row r="413" spans="1:1">
+      <c r="A413" s="46"/>
+    </row>
+    <row r="414" spans="1:1">
+      <c r="A414" s="46"/>
+    </row>
+    <row r="415" spans="1:1">
+      <c r="A415" s="46"/>
+    </row>
+    <row r="416" spans="1:1">
+      <c r="A416" s="46"/>
+    </row>
+    <row r="417" spans="1:1">
+      <c r="A417" s="46"/>
+    </row>
+    <row r="418" spans="1:1">
+      <c r="A418" s="46"/>
+    </row>
+    <row r="419" spans="1:1">
+      <c r="A419" s="46"/>
+    </row>
+    <row r="420" spans="1:1">
+      <c r="A420" s="46"/>
+    </row>
+    <row r="421" spans="1:1">
+      <c r="A421" s="46"/>
+    </row>
+    <row r="422" spans="1:1">
+      <c r="A422" s="46"/>
+    </row>
+    <row r="423" spans="1:1">
+      <c r="A423" s="46"/>
+    </row>
+    <row r="424" spans="1:1">
+      <c r="A424" s="46"/>
+    </row>
+    <row r="425" spans="1:1">
+      <c r="A425" s="46"/>
+    </row>
+    <row r="426" spans="1:1">
+      <c r="A426" s="46"/>
+    </row>
+    <row r="427" spans="1:1">
+      <c r="A427" s="46"/>
+    </row>
+    <row r="428" spans="1:1">
+      <c r="A428" s="46"/>
+    </row>
+    <row r="429" spans="1:1">
+      <c r="A429" s="46"/>
+    </row>
+    <row r="430" spans="1:1">
+      <c r="A430" s="46"/>
+    </row>
+    <row r="431" spans="1:1">
+      <c r="A431" s="46"/>
+    </row>
+    <row r="432" spans="1:1">
+      <c r="A432" s="46"/>
+    </row>
+    <row r="433" spans="1:1">
+      <c r="A433" s="46"/>
+    </row>
+    <row r="434" spans="1:1">
+      <c r="A434" s="46"/>
+    </row>
+    <row r="435" spans="1:1">
+      <c r="A435" s="46"/>
+    </row>
+    <row r="436" spans="1:1">
+      <c r="A436" s="46"/>
+    </row>
+    <row r="437" spans="1:1">
+      <c r="A437" s="46"/>
+    </row>
+    <row r="438" spans="1:1">
+      <c r="A438" s="46"/>
+    </row>
+    <row r="439" spans="1:1">
+      <c r="A439" s="46"/>
+    </row>
+    <row r="440" spans="1:1">
+      <c r="A440" s="46"/>
+    </row>
+    <row r="441" spans="1:1">
+      <c r="A441" s="46"/>
+    </row>
+    <row r="442" spans="1:1">
+      <c r="A442" s="46"/>
+    </row>
+    <row r="443" spans="1:1">
+      <c r="A443" s="46"/>
+    </row>
+    <row r="444" spans="1:1">
+      <c r="A444" s="46"/>
+    </row>
+    <row r="445" spans="1:1">
+      <c r="A445" s="46"/>
+    </row>
+    <row r="446" spans="1:1">
+      <c r="A446" s="46"/>
+    </row>
+    <row r="447" spans="1:1">
+      <c r="A447" s="46"/>
+    </row>
+    <row r="448" spans="1:1">
+      <c r="A448" s="46"/>
+    </row>
+    <row r="449" spans="1:1">
+      <c r="A449" s="46"/>
+    </row>
+    <row r="450" spans="1:1">
+      <c r="A450" s="46"/>
+    </row>
+    <row r="451" spans="1:1">
+      <c r="A451" s="46"/>
+    </row>
+    <row r="452" spans="1:1">
+      <c r="A452" s="46"/>
+    </row>
+    <row r="453" spans="1:1">
+      <c r="A453" s="46"/>
+    </row>
+    <row r="454" spans="1:1">
+      <c r="A454" s="46"/>
+    </row>
+    <row r="455" spans="1:1">
+      <c r="A455" s="46"/>
+    </row>
+    <row r="456" spans="1:1">
+      <c r="A456" s="46"/>
+    </row>
+    <row r="457" spans="1:1">
+      <c r="A457" s="46"/>
+    </row>
+    <row r="458" spans="1:1">
+      <c r="A458" s="46"/>
+    </row>
+    <row r="459" spans="1:1">
+      <c r="A459" s="46"/>
+    </row>
+    <row r="460" spans="1:1">
+      <c r="A460" s="46"/>
+    </row>
+    <row r="461" spans="1:1">
+      <c r="A461" s="46"/>
+    </row>
+    <row r="462" spans="1:1">
+      <c r="A462" s="46"/>
+    </row>
+    <row r="463" spans="1:1">
+      <c r="A463" s="46"/>
+    </row>
+    <row r="464" spans="1:1">
+      <c r="A464" s="46"/>
+    </row>
+    <row r="465" spans="1:1">
+      <c r="A465" s="46"/>
+    </row>
+    <row r="466" spans="1:1">
+      <c r="A466" s="46"/>
+    </row>
+    <row r="467" spans="1:1">
+      <c r="A467" s="46"/>
+    </row>
+    <row r="468" spans="1:1">
+      <c r="A468" s="46"/>
+    </row>
+    <row r="469" spans="1:1">
+      <c r="A469" s="46"/>
+    </row>
+    <row r="470" spans="1:1">
+      <c r="A470" s="46"/>
+    </row>
+    <row r="471" spans="1:1">
+      <c r="A471" s="46"/>
+    </row>
+    <row r="472" spans="1:1">
+      <c r="A472" s="46"/>
+    </row>
+    <row r="473" spans="1:1">
+      <c r="A473" s="46"/>
+    </row>
+    <row r="474" spans="1:1">
+      <c r="A474" s="46"/>
+    </row>
+    <row r="475" spans="1:1">
+      <c r="A475" s="46"/>
+    </row>
+    <row r="476" spans="1:1">
+      <c r="A476" s="46"/>
+    </row>
+    <row r="477" spans="1:1">
+      <c r="A477" s="46"/>
+    </row>
+    <row r="478" spans="1:1">
+      <c r="A478" s="46"/>
+    </row>
+    <row r="479" spans="1:1">
+      <c r="A479" s="46"/>
+    </row>
+    <row r="480" spans="1:1">
+      <c r="A480" s="46"/>
+    </row>
+    <row r="481" spans="1:1">
+      <c r="A481" s="46"/>
+    </row>
+    <row r="482" spans="1:1">
+      <c r="A482" s="46"/>
+    </row>
+    <row r="483" spans="1:1">
+      <c r="A483" s="46"/>
+    </row>
+    <row r="484" spans="1:1">
+      <c r="A484" s="46"/>
+    </row>
+    <row r="485" spans="1:1">
+      <c r="A485" s="46"/>
+    </row>
+    <row r="486" spans="1:1">
+      <c r="A486" s="46"/>
+    </row>
+    <row r="487" spans="1:1">
+      <c r="A487" s="46"/>
+    </row>
+    <row r="488" spans="1:1">
+      <c r="A488" s="46"/>
+    </row>
+    <row r="489" spans="1:1">
+      <c r="A489" s="46"/>
+    </row>
+    <row r="490" spans="1:1">
+      <c r="A490" s="46"/>
+    </row>
+    <row r="491" spans="1:1">
+      <c r="A491" s="46"/>
+    </row>
+    <row r="492" spans="1:1">
+      <c r="A492" s="46"/>
+    </row>
+    <row r="493" spans="1:1">
+      <c r="A493" s="46"/>
+    </row>
+    <row r="494" spans="1:1">
+      <c r="A494" s="46"/>
+    </row>
+    <row r="495" spans="1:1">
+      <c r="A495" s="46"/>
+    </row>
+    <row r="496" spans="1:1">
+      <c r="A496" s="46"/>
+    </row>
+    <row r="497" spans="1:1">
+      <c r="A497" s="46"/>
+    </row>
+    <row r="498" spans="1:1">
+      <c r="A498" s="46"/>
+    </row>
+    <row r="499" spans="1:1">
+      <c r="A499" s="46"/>
+    </row>
+    <row r="500" spans="1:1">
+      <c r="A500" s="46"/>
+    </row>
+    <row r="501" spans="1:1">
+      <c r="A501" s="46"/>
+    </row>
+    <row r="502" spans="1:1">
+      <c r="A502" s="46"/>
+    </row>
+    <row r="503" spans="1:1">
+      <c r="A503" s="46"/>
+    </row>
+    <row r="504" spans="1:1">
+      <c r="A504" s="46"/>
+    </row>
+    <row r="505" spans="1:1">
+      <c r="A505" s="46"/>
+    </row>
+    <row r="506" spans="1:1">
+      <c r="A506" s="46"/>
+    </row>
+    <row r="507" spans="1:1">
+      <c r="A507" s="46"/>
+    </row>
+    <row r="508" spans="1:1">
+      <c r="A508" s="46"/>
+    </row>
+    <row r="509" spans="1:1">
+      <c r="A509" s="46"/>
+    </row>
+    <row r="510" spans="1:1">
+      <c r="A510" s="46"/>
+    </row>
+    <row r="511" spans="1:1">
+      <c r="A511" s="46"/>
+    </row>
+    <row r="512" spans="1:1">
+      <c r="A512" s="46"/>
+    </row>
+    <row r="513" spans="1:1">
+      <c r="A513" s="46"/>
+    </row>
+    <row r="514" spans="1:1">
+      <c r="A514" s="46"/>
+    </row>
+    <row r="515" spans="1:1">
+      <c r="A515" s="46"/>
+    </row>
+    <row r="516" spans="1:1">
+      <c r="A516" s="46"/>
+    </row>
+    <row r="517" spans="1:1">
+      <c r="A517" s="46"/>
+    </row>
+    <row r="518" spans="1:1">
+      <c r="A518" s="46"/>
+    </row>
+    <row r="519" spans="1:1">
+      <c r="A519" s="46"/>
+    </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2 B4:B5" xr:uid="{5C73BBC5-C68D-4586-BDB5-A3BE48854FB6}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4:A1048576" xr:uid="{18FD80CD-FFDC-48A1-BA45-91576461B09B}">
+  <dataValidations count="3">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 C4:C5" xr:uid="{5C73BBC5-C68D-4586-BDB5-A3BE48854FB6}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B1048576" xr:uid="{18FD80CD-FFDC-48A1-BA45-91576461B09B}">
       <formula1>"FRONT EPE, BACK EVA"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4:A1048576" xr:uid="{CDEE756C-C284-45D8-BDCE-F4798D4B3C50}">
+      <formula1>"ENCAPSULANT"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2889,7 +4460,7 @@
           <x14:formula1>
             <xm:f>Ref!$K$2:$K$1048576</xm:f>
           </x14:formula1>
-          <xm:sqref>A1:A2</xm:sqref>
+          <xm:sqref>B1:B2</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2902,7 +4473,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P22" sqref="P22"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Fri Jun 27 09:40:18 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Solar_Lab_Tests.xlsx
+++ b/data/Solar_Lab_Tests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29019"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29022"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="675" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3FADE34F-1E4D-49C5-8031-8738EB6AA421}"/>
+  <xr:revisionPtr revIDLastSave="678" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D84C537-CEDD-4213-AA62-7BFB78D5D989}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="3" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="3" activeTab="1" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Tests Map" sheetId="4" state="hidden" r:id="rId1"/>
@@ -180,10 +180,10 @@
     <t>Hangzhou First</t>
   </si>
   <si>
+    <t>Fasto</t>
+  </si>
+  <si>
     <t>In Progress</t>
-  </si>
-  <si>
-    <t>Fasto</t>
   </si>
   <si>
     <t>Tesa 4134</t>
@@ -726,7 +726,7 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2074,8 +2074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9401EE47-EA52-49C7-BBC0-21F5B88254FB}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -2280,10 +2280,14 @@
       <c r="D8" s="5">
         <v>45825</v>
       </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
+      <c r="E8" s="4">
+        <v>45808</v>
+      </c>
+      <c r="F8" s="4">
+        <v>45835</v>
+      </c>
       <c r="H8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>11</v>
@@ -2321,7 +2325,7 @@
         <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="4">
@@ -2329,7 +2333,7 @@
       </c>
       <c r="F10" s="4"/>
       <c r="H10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>20</v>
@@ -2362,7 +2366,7 @@
       </c>
       <c r="F12" s="4"/>
       <c r="H12" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>2</v>
@@ -2376,7 +2380,7 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="4">
@@ -2384,7 +2388,7 @@
       </c>
       <c r="F13" s="4"/>
       <c r="H13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="K13" s="3" t="s">
         <v>40</v>
@@ -2406,7 +2410,7 @@
       </c>
       <c r="F14" s="4"/>
       <c r="H14" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="K14" s="3" t="s">
         <v>42</v>
@@ -2616,7 +2620,7 @@
         <v>31</v>
       </c>
       <c r="I3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="K3" t="s">
         <v>53</v>
@@ -2729,7 +2733,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61A5C69B-8639-4E8F-9A05-E59E5511083E}">
   <dimension ref="A1:K519"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -4473,7 +4477,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4833,7 +4837,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" s="10">
         <v>0.63541666666666663</v>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Fri Jun 27 10:11:06 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Solar_Lab_Tests.xlsx
+++ b/data/Solar_Lab_Tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="678" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D84C537-CEDD-4213-AA62-7BFB78D5D989}"/>
+  <xr:revisionPtr revIDLastSave="689" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A60862E-090F-44B5-8813-0C278FE67C76}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="3" activeTab="1" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="3" activeTab="7" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Tests Map" sheetId="4" state="hidden" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="94">
   <si>
     <t>BOM</t>
   </si>
@@ -301,12 +301,6 @@
   </si>
   <si>
     <t xml:space="preserve">                                                         BACKSHEET to ENCAPSULANT</t>
-  </si>
-  <si>
-    <t>max</t>
-  </si>
-  <si>
-    <t>min</t>
   </si>
   <si>
     <t>BREAK</t>
@@ -502,7 +496,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -649,11 +643,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -727,6 +732,7 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1857,10 +1863,10 @@
         <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1903,7 +1909,7 @@
         <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1946,7 +1952,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2074,8 +2080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9401EE47-EA52-49C7-BBC0-21F5B88254FB}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -4477,7 +4483,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4536,31 +4542,35 @@
       <c r="J2" s="38"/>
     </row>
     <row r="3" spans="1:10" customFormat="1">
-      <c r="A3" s="39"/>
-      <c r="B3" s="34"/>
-      <c r="C3" s="40" t="s">
-        <v>77</v>
-      </c>
-      <c r="D3" s="41" t="s">
-        <v>78</v>
-      </c>
-      <c r="E3" s="42" t="s">
-        <v>77</v>
-      </c>
-      <c r="F3" s="43" t="s">
-        <v>78</v>
-      </c>
-      <c r="G3" s="40" t="s">
-        <v>77</v>
-      </c>
-      <c r="H3" s="41" t="s">
-        <v>78</v>
-      </c>
-      <c r="I3" s="42" t="s">
-        <v>77</v>
-      </c>
-      <c r="J3" s="43" t="s">
-        <v>78</v>
+      <c r="A3" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="40">
+        <v>65</v>
+      </c>
+      <c r="D3" s="41">
+        <v>55</v>
+      </c>
+      <c r="E3" s="42">
+        <v>40</v>
+      </c>
+      <c r="F3" s="43">
+        <v>30</v>
+      </c>
+      <c r="G3" s="40">
+        <v>95</v>
+      </c>
+      <c r="H3" s="41">
+        <v>82</v>
+      </c>
+      <c r="I3" s="42">
+        <v>62</v>
+      </c>
+      <c r="J3" s="43">
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:10" customFormat="1" hidden="1">
@@ -4596,6 +4606,9 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{CC8DB943-48E5-430E-9C46-5758433E9F8F}"/>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -4639,10 +4652,10 @@
         <v>24</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="6" customFormat="1">
@@ -4703,25 +4716,25 @@
         <v>24</v>
       </c>
       <c r="C1" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="F1" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="G1" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="H1" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="I1" s="8" t="s">
         <v>85</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -4760,7 +4773,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD5452B6-66C2-4964-BBFB-466116F6D217}">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -4774,7 +4787,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B1" t="s">
         <v>50</v>
@@ -4783,7 +4796,7 @@
         <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -4826,10 +4839,10 @@
         <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:4">

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Fri Jun 27 10:15:17 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Solar_Lab_Tests.xlsx
+++ b/data/Solar_Lab_Tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="689" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A60862E-090F-44B5-8813-0C278FE67C76}"/>
+  <xr:revisionPtr revIDLastSave="692" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2114832A-BE56-4C04-A1DA-AD2423B913A3}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="3" activeTab="7" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="7" activeTab="1" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Tests Map" sheetId="4" state="hidden" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="94">
   <si>
     <t>BOM</t>
   </si>
@@ -732,7 +732,7 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2080,8 +2080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9401EE47-EA52-49C7-BBC0-21F5B88254FB}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -2449,10 +2449,30 @@
       </c>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="1"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
+      <c r="A16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="5">
+        <v>45825</v>
+      </c>
+      <c r="E16" s="4">
+        <v>45833</v>
+      </c>
+      <c r="F16" s="4">
+        <v>45835</v>
+      </c>
+      <c r="H16" t="s">
+        <v>33</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="1"/>
@@ -2513,7 +2533,7 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K8:K15" xr:uid="{C3958E6F-28D2-429E-9DF5-7DAD65BBE2ED}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K8:K16" xr:uid="{C3958E6F-28D2-429E-9DF5-7DAD65BBE2ED}">
       <formula1>$K:$K</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A11 C1:C1048576" xr:uid="{8C537B12-83B7-48DB-9398-33493EB60A9D}"/>
@@ -2740,7 +2760,7 @@
   <dimension ref="A1:K519"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4488,7 +4508,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" style="45" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" style="45" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" style="45" customWidth="1"/>
     <col min="3" max="3" width="13.140625" style="45" customWidth="1"/>
     <col min="4" max="4" width="18.5703125" style="45" customWidth="1"/>
@@ -4773,7 +4793,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD5452B6-66C2-4964-BBFB-466116F6D217}">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-07-14 11:42:40
</commit_message>
<xml_diff>
--- a/data/Solar_Lab_Tests.xlsx
+++ b/data/Solar_Lab_Tests.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29101"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29108"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="732" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{77DB7ABA-3103-4179-B725-1F6E16689869}"/>
+  <xr:revisionPtr revIDLastSave="763" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C4888019-B618-4AE1-B22A-48C6ACDCC951}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="1" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
   </bookViews>
@@ -30,7 +30,7 @@
     <definedName name="ENCAPTYPE">Ref!$K$2:$K$1048576</definedName>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">'Material Tests Map'!$A$1:$B$20</definedName>
     <definedName name="ExternalData_1" localSheetId="11" hidden="1">'Standard test times'!$A$1:$B$15</definedName>
-    <definedName name="ExternalData_1" localSheetId="1" hidden="1">'Test Data'!$A$1:$H$26</definedName>
+    <definedName name="ExternalData_1" localSheetId="1" hidden="1">'Test Data'!$A$1:$H$27</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="109">
   <si>
     <t>BOM</t>
   </si>
@@ -210,6 +210,33 @@
     <t>FANCY FITTING</t>
   </si>
   <si>
+    <t>UKTR 30A</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>UKTR30U</t>
+  </si>
+  <si>
+    <t>SUNTER</t>
+  </si>
+  <si>
+    <t>UKTR</t>
+  </si>
+  <si>
+    <t>ZJRH</t>
+  </si>
+  <si>
+    <t>VEMOULD30A</t>
+  </si>
+  <si>
+    <t>VEMOULD25A</t>
+  </si>
+  <si>
+    <t>SINOTECH30A</t>
+  </si>
+  <si>
     <t>RM Type</t>
   </si>
   <si>
@@ -237,9 +264,6 @@
     <t>OLD : 420 to 480</t>
   </si>
   <si>
-    <t>In Progress</t>
-  </si>
-  <si>
     <t>BACK EVA</t>
   </si>
   <si>
@@ -367,6 +391,9 @@
   </si>
   <si>
     <t>UKTR 20A MJB</t>
+  </si>
+  <si>
+    <t>UKTR30A</t>
   </si>
   <si>
     <t>STANDARD DURATION (DAYS)</t>
@@ -376,6 +403,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+  </numFmts>
   <fonts count="8">
     <font>
       <sz val="11"/>
@@ -676,7 +706,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -751,6 +781,10 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1239,8 +1273,8 @@
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{5C370BE7-C0F8-462F-9F89-5FC458087319}" name="Table16" displayName="Table16" ref="A1:C6" totalsRowShown="0">
-  <autoFilter ref="A1:C6" xr:uid="{5C370BE7-C0F8-462F-9F89-5FC458087319}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{5C370BE7-C0F8-462F-9F89-5FC458087319}" name="Table16" displayName="Table16" ref="A1:C8" totalsRowShown="0">
+  <autoFilter ref="A1:C8" xr:uid="{5C370BE7-C0F8-462F-9F89-5FC458087319}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{59EA2429-768A-457D-88E6-B34A083DE755}" name="BOM"/>
     <tableColumn id="2" xr3:uid="{C09F236B-325A-4EF9-B484-B1D592C83B7F}" name="VENDOR NAME"/>
@@ -1262,7 +1296,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{06A3AD80-C098-4015-85FF-3495CE4443EA}" name="Test_Data" displayName="Test_Data" ref="A1:H26" tableType="queryTable" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{06A3AD80-C098-4015-85FF-3495CE4443EA}" name="Test_Data" displayName="Test_Data" ref="A1:H27" tableType="queryTable" totalsRowShown="0">
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{87F75B08-44C4-4718-834D-87FEE9F87970}" uniqueName="1" name="BOM" queryTableFieldId="1" dataDxfId="42"/>
     <tableColumn id="2" xr3:uid="{1E5F4521-5E5C-4948-AEB2-FC5F712DB353}" uniqueName="2" name="TEST NAME" queryTableFieldId="2" dataDxfId="41"/>
@@ -1881,10 +1915,10 @@
         <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="D1" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1906,10 +1940,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{333C0630-51CF-46CA-8CAD-98FEF9AC181F}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1927,7 +1961,7 @@
         <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1935,7 +1969,7 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1943,7 +1977,7 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1951,7 +1985,7 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1960,6 +1994,22 @@
       </c>
       <c r="B6" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1994,7 +2044,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2120,10 +2170,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9401EE47-EA52-49C7-BBC0-21F5B88254FB}">
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -2577,42 +2627,125 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="1"/>
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" t="s">
+        <v>46</v>
+      </c>
       <c r="D20" s="5"/>
-      <c r="E20" s="4"/>
+      <c r="E20" s="4">
+        <v>45845</v>
+      </c>
       <c r="F20" s="4"/>
+      <c r="H20" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="1"/>
+      <c r="B21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" t="s">
+        <v>48</v>
+      </c>
       <c r="D21" s="5"/>
-      <c r="E21" s="4"/>
+      <c r="E21" s="4">
+        <v>45845</v>
+      </c>
       <c r="F21" s="4"/>
+      <c r="H21" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="1"/>
+      <c r="B22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" t="s">
+        <v>49</v>
+      </c>
       <c r="D22" s="5"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
+      <c r="H22" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="1"/>
+      <c r="B23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" t="s">
+        <v>50</v>
+      </c>
       <c r="D23" s="5"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
+      <c r="H23" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="1"/>
+      <c r="B24" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" t="s">
+        <v>51</v>
+      </c>
       <c r="D24" s="5"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
+      <c r="H24" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="1"/>
+      <c r="B25" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" t="s">
+        <v>52</v>
+      </c>
       <c r="D25" s="5"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
+      <c r="H25" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="26" spans="1:8">
+      <c r="B26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" t="s">
+        <v>53</v>
+      </c>
       <c r="D26" s="5"/>
+      <c r="H26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="48"/>
+      <c r="B27" s="48" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" s="48" t="s">
+        <v>54</v>
+      </c>
+      <c r="D27" s="49"/>
+      <c r="E27" s="48"/>
+      <c r="F27" s="48"/>
+      <c r="G27" s="48"/>
+      <c r="H27" s="48" t="s">
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -2677,25 +2810,25 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="C1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="E1" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="G1" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="I1" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="K1" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="N1" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -2712,10 +2845,10 @@
         <v>32</v>
       </c>
       <c r="K2" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="N2" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -2729,13 +2862,13 @@
         <v>31</v>
       </c>
       <c r="I3" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="K3" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="N3" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -2746,10 +2879,10 @@
         <v>5</v>
       </c>
       <c r="G4" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="I4" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -2860,19 +2993,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>24</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="E1" s="16"/>
       <c r="F1" s="16"/>
       <c r="G1" s="16"/>
       <c r="H1" s="17" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="I1" s="18"/>
       <c r="J1" s="18"/>
@@ -2883,61 +3016,61 @@
       <c r="B2" s="20"/>
       <c r="C2" s="20"/>
       <c r="D2" s="21" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="F2" s="22" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="G2" s="22" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="H2" s="23" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="I2" s="24" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="J2" s="24" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="K2" s="25" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:11" hidden="1">
       <c r="A3" s="46"/>
       <c r="B3" s="26" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="F3" s="26" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="G3" s="26" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="H3" s="26" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="I3" s="26" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="J3" s="26" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="K3" s="26" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -2945,7 +3078,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="C4" t="s">
         <v>35</v>
@@ -2980,7 +3113,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="C5" t="s">
         <v>35</v>
@@ -4608,14 +4741,14 @@
       <c r="A1" s="28"/>
       <c r="B1" s="29"/>
       <c r="C1" s="30" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="D1" s="31"/>
       <c r="E1" s="30"/>
       <c r="F1" s="31"/>
       <c r="G1" s="32"/>
       <c r="H1" s="44" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="I1" s="32"/>
       <c r="J1" s="29"/>
@@ -4628,19 +4761,19 @@
         <v>24</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="D2" s="36"/>
       <c r="E2" s="37" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="F2" s="38"/>
       <c r="G2" s="35" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="37" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="J2" s="38"/>
     </row>
@@ -4678,34 +4811,34 @@
     </row>
     <row r="4" spans="1:10" customFormat="1" hidden="1">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="C4" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="D4" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="E4" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="F4" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="G4" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="H4" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="I4" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J4" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -4755,10 +4888,10 @@
         <v>24</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="6" customFormat="1">
@@ -4819,25 +4952,25 @@
         <v>24</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -4890,16 +5023,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="B1" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="C1" t="s">
         <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -4942,10 +5075,10 @@
         <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D1" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:4">

</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-07-21 16:54:03
</commit_message>
<xml_diff>
--- a/data/Solar_Lab_Tests.xlsx
+++ b/data/Solar_Lab_Tests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="783" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DFB863CC-6B3E-49B2-A286-32B053DBE989}"/>
+  <xr:revisionPtr revIDLastSave="809" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C69FA02-A7C9-4E16-ACE1-F3B4568B3104}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="10" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="10" activeTab="1" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Tests Map" sheetId="4" state="hidden" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <definedName name="ENCAPTYPE">Ref!$K$2:$K$1048576</definedName>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">'Material Tests Map'!$A$1:$B$20</definedName>
     <definedName name="ExternalData_1" localSheetId="11" hidden="1">'Standard test times'!$A$1:$B$15</definedName>
-    <definedName name="ExternalData_1" localSheetId="1" hidden="1">'Test Data'!$A$1:$H$27</definedName>
+    <definedName name="ExternalData_1" localSheetId="1" hidden="1">'Test Data'!$A$1:$H$29</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="110">
   <si>
     <t>BOM</t>
   </si>
@@ -213,55 +213,58 @@
     <t>UKTR 30A</t>
   </si>
   <si>
+    <t>UKTR30U</t>
+  </si>
+  <si>
+    <t>SUNTER</t>
+  </si>
+  <si>
+    <t>UKTR</t>
+  </si>
+  <si>
+    <t>ZJRH</t>
+  </si>
+  <si>
+    <t>VEMOULD30A</t>
+  </si>
+  <si>
+    <t>VEMOULD25A</t>
+  </si>
+  <si>
+    <t>SINOTECH30A</t>
+  </si>
+  <si>
+    <t>BBETTER</t>
+  </si>
+  <si>
+    <t>RM Type</t>
+  </si>
+  <si>
+    <t>Test Type</t>
+  </si>
+  <si>
+    <t>Vendor Names</t>
+  </si>
+  <si>
+    <t>Test Results</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>ENCAPSULANT TYPE</t>
+  </si>
+  <si>
+    <t>TYPE</t>
+  </si>
+  <si>
+    <t>FRONT EPE</t>
+  </si>
+  <si>
+    <t>OLD : 420 to 480</t>
+  </si>
+  <si>
     <t>In Progress</t>
-  </si>
-  <si>
-    <t>UKTR30U</t>
-  </si>
-  <si>
-    <t>SUNTER</t>
-  </si>
-  <si>
-    <t>UKTR</t>
-  </si>
-  <si>
-    <t>ZJRH</t>
-  </si>
-  <si>
-    <t>VEMOULD30A</t>
-  </si>
-  <si>
-    <t>VEMOULD25A</t>
-  </si>
-  <si>
-    <t>SINOTECH30A</t>
-  </si>
-  <si>
-    <t>RM Type</t>
-  </si>
-  <si>
-    <t>Test Type</t>
-  </si>
-  <si>
-    <t>Vendor Names</t>
-  </si>
-  <si>
-    <t>Test Results</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>ENCAPSULANT TYPE</t>
-  </si>
-  <si>
-    <t>TYPE</t>
-  </si>
-  <si>
-    <t>FRONT EPE</t>
-  </si>
-  <si>
-    <t>OLD : 420 to 480</t>
   </si>
   <si>
     <t>BACK EVA</t>
@@ -706,7 +709,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -784,6 +787,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1295,7 +1299,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{06A3AD80-C098-4015-85FF-3495CE4443EA}" name="Test_Data" displayName="Test_Data" ref="A1:H27" tableType="queryTable" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{06A3AD80-C098-4015-85FF-3495CE4443EA}" name="Test_Data" displayName="Test_Data" ref="A1:H29" tableType="queryTable" totalsRowShown="0">
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{87F75B08-44C4-4718-834D-87FEE9F87970}" uniqueName="1" name="BOM" queryTableFieldId="1" dataDxfId="42"/>
     <tableColumn id="2" xr3:uid="{1E5F4521-5E5C-4948-AEB2-FC5F712DB353}" uniqueName="2" name="TEST NAME" queryTableFieldId="2" dataDxfId="41"/>
@@ -1914,10 +1918,10 @@
         <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1941,7 +1945,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{333C0630-51CF-46CA-8CAD-98FEF9AC181F}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
@@ -1960,7 +1964,7 @@
         <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1968,7 +1972,7 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1976,7 +1980,7 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1984,7 +1988,7 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2000,7 +2004,7 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -2008,7 +2012,7 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -2073,7 +2077,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2199,10 +2203,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9401EE47-EA52-49C7-BBC0-21F5B88254FB}">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView topLeftCell="B16" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="B11" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -2670,7 +2674,7 @@
         <v>45851</v>
       </c>
       <c r="H20" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -2679,7 +2683,7 @@
         <v>16</v>
       </c>
       <c r="C21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="4">
@@ -2689,7 +2693,7 @@
         <v>45851</v>
       </c>
       <c r="H21" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -2698,15 +2702,17 @@
         <v>16</v>
       </c>
       <c r="C22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="4">
         <v>45852</v>
       </c>
-      <c r="F22" s="4"/>
+      <c r="F22" s="4">
+        <v>45857</v>
+      </c>
       <c r="H22" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -2715,15 +2721,17 @@
         <v>16</v>
       </c>
       <c r="C23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="4">
         <v>45852</v>
       </c>
-      <c r="F23" s="4"/>
+      <c r="F23" s="4">
+        <v>45857</v>
+      </c>
       <c r="H23" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -2732,15 +2740,17 @@
         <v>16</v>
       </c>
       <c r="C24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="4">
         <v>45852</v>
       </c>
-      <c r="F24" s="4"/>
+      <c r="F24" s="4">
+        <v>45857</v>
+      </c>
       <c r="H24" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -2749,15 +2759,17 @@
         <v>16</v>
       </c>
       <c r="C25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="4">
         <v>45852</v>
       </c>
-      <c r="F25" s="4"/>
+      <c r="F25" s="4">
+        <v>45857</v>
+      </c>
       <c r="H25" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -2765,14 +2777,17 @@
         <v>16</v>
       </c>
       <c r="C26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="4">
         <v>45852</v>
       </c>
+      <c r="F26" s="4">
+        <v>45857</v>
+      </c>
       <c r="H26" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -2780,15 +2795,46 @@
         <v>16</v>
       </c>
       <c r="C27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D27" s="48"/>
       <c r="E27" s="4">
         <v>45852</v>
       </c>
+      <c r="F27" s="4">
+        <v>45857</v>
+      </c>
       <c r="H27" t="s">
-        <v>47</v>
-      </c>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="49"/>
+      <c r="B28" s="49" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="49" t="s">
+        <v>54</v>
+      </c>
+      <c r="D28" s="48"/>
+      <c r="E28" s="49"/>
+      <c r="F28" s="49"/>
+      <c r="G28" s="49"/>
+      <c r="H28" s="49"/>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="49"/>
+      <c r="B29" s="49" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" s="49" t="s">
+        <v>54</v>
+      </c>
+      <c r="D29" s="48"/>
+      <c r="E29" s="49"/>
+      <c r="F29" s="49"/>
+      <c r="G29" s="49"/>
+      <c r="H29" s="49"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -2905,13 +2951,13 @@
         <v>31</v>
       </c>
       <c r="I3" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="K3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="N3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -2922,10 +2968,10 @@
         <v>5</v>
       </c>
       <c r="G4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="I4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -3042,13 +3088,13 @@
         <v>24</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E1" s="16"/>
       <c r="F1" s="16"/>
       <c r="G1" s="16"/>
       <c r="H1" s="17" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I1" s="18"/>
       <c r="J1" s="18"/>
@@ -3059,61 +3105,61 @@
       <c r="B2" s="20"/>
       <c r="C2" s="20"/>
       <c r="D2" s="21" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E2" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="H2" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="I2" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="J2" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="H2" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="I2" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="J2" s="24" t="s">
-        <v>72</v>
-      </c>
       <c r="K2" s="25" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:11" hidden="1">
       <c r="A3" s="46"/>
       <c r="B3" s="26" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F3" s="26" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G3" s="26" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H3" s="26" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I3" s="26" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J3" s="26" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K3" s="26" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -3156,7 +3202,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C5" t="s">
         <v>35</v>
@@ -4784,14 +4830,14 @@
       <c r="A1" s="28"/>
       <c r="B1" s="29"/>
       <c r="C1" s="30" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D1" s="31"/>
       <c r="E1" s="30"/>
       <c r="F1" s="31"/>
       <c r="G1" s="32"/>
       <c r="H1" s="44" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="I1" s="32"/>
       <c r="J1" s="29"/>
@@ -4804,19 +4850,19 @@
         <v>24</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D2" s="36"/>
       <c r="E2" s="37" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F2" s="38"/>
       <c r="G2" s="35" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="37" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J2" s="38"/>
     </row>
@@ -4854,34 +4900,34 @@
     </row>
     <row r="4" spans="1:10" customFormat="1" hidden="1">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -4931,10 +4977,10 @@
         <v>24</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="6" customFormat="1">
@@ -4995,25 +5041,25 @@
         <v>24</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -5066,7 +5112,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B1" t="s">
         <v>61</v>
@@ -5075,7 +5121,7 @@
         <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -5118,10 +5164,10 @@
         <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:4">

</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-07-25 14:48:29
</commit_message>
<xml_diff>
--- a/data/Solar_Lab_Tests.xlsx
+++ b/data/Solar_Lab_Tests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29122"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="830" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4283FBE9-B052-41A5-BC52-A92E1EA5EFC7}"/>
+  <xr:revisionPtr revIDLastSave="861" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B9B9340C-05B7-4EE4-9642-0FE1DF386EA7}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="10" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="10" activeTab="1" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Tests Map" sheetId="4" state="hidden" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <definedName name="ENCAPTYPE">Ref!$K$2:$K$1048576</definedName>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">'Material Tests Map'!$A$1:$B$20</definedName>
     <definedName name="ExternalData_1" localSheetId="11" hidden="1">'Standard test times'!$A$1:$B$15</definedName>
-    <definedName name="ExternalData_1" localSheetId="1" hidden="1">'Test Data'!$A$1:$H$30</definedName>
+    <definedName name="ExternalData_1" localSheetId="1" hidden="1">'Test Data'!$A$1:$H$35</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="120">
   <si>
     <t>BOM</t>
   </si>
@@ -235,6 +235,21 @@
   </si>
   <si>
     <t>BBETTER</t>
+  </si>
+  <si>
+    <t>SINOTECH</t>
+  </si>
+  <si>
+    <t>QC SOLAR</t>
+  </si>
+  <si>
+    <t>QC SOLAR VITNAM</t>
+  </si>
+  <si>
+    <t>ZERUNE</t>
+  </si>
+  <si>
+    <t>SSEPL</t>
   </si>
   <si>
     <t>RM Type</t>
@@ -724,7 +739,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -802,6 +817,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1317,7 +1333,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{06A3AD80-C098-4015-85FF-3495CE4443EA}" name="Test_Data" displayName="Test_Data" ref="A1:H30" tableType="queryTable" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{06A3AD80-C098-4015-85FF-3495CE4443EA}" name="Test_Data" displayName="Test_Data" ref="A1:H35" tableType="queryTable" totalsRowShown="0">
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{87F75B08-44C4-4718-834D-87FEE9F87970}" uniqueName="1" name="BOM" queryTableFieldId="1" dataDxfId="42"/>
     <tableColumn id="2" xr3:uid="{1E5F4521-5E5C-4948-AEB2-FC5F712DB353}" uniqueName="2" name="TEST NAME" queryTableFieldId="2" dataDxfId="41"/>
@@ -1936,10 +1952,10 @@
         <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="D1" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1963,8 +1979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{333C0630-51CF-46CA-8CAD-98FEF9AC181F}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1986,19 +2002,19 @@
         <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="D1" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="E1" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="F1" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="G1" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -2006,7 +2022,7 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2014,7 +2030,7 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2022,7 +2038,7 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -2038,7 +2054,7 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -2054,27 +2070,39 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>15</v>
       </c>
+      <c r="B9" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>15</v>
       </c>
+      <c r="B10" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>15</v>
       </c>
+      <c r="B11" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -2114,7 +2142,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2240,10 +2268,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9401EE47-EA52-49C7-BBC0-21F5B88254FB}">
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView topLeftCell="B16" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -2867,7 +2895,93 @@
       <c r="B30" t="s">
         <v>16</v>
       </c>
+      <c r="C30" t="s">
+        <v>55</v>
+      </c>
       <c r="D30" s="48"/>
+      <c r="E30" s="4">
+        <v>45861</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="49"/>
+      <c r="B31" s="49" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="D31" s="48"/>
+      <c r="E31" s="4">
+        <v>45861</v>
+      </c>
+      <c r="F31" s="49"/>
+      <c r="G31" s="49"/>
+      <c r="H31" s="49"/>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="49"/>
+      <c r="B32" s="49" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32" s="49" t="s">
+        <v>57</v>
+      </c>
+      <c r="D32" s="48"/>
+      <c r="E32" s="4">
+        <v>45861</v>
+      </c>
+      <c r="F32" s="49"/>
+      <c r="G32" s="49"/>
+      <c r="H32" s="49"/>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="49"/>
+      <c r="B33" s="49" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33" s="49" t="s">
+        <v>58</v>
+      </c>
+      <c r="D33" s="48"/>
+      <c r="E33" s="4">
+        <v>45861</v>
+      </c>
+      <c r="F33" s="49"/>
+      <c r="G33" s="49"/>
+      <c r="H33" s="49"/>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="49"/>
+      <c r="B34" s="49" t="s">
+        <v>16</v>
+      </c>
+      <c r="C34" s="49" t="s">
+        <v>59</v>
+      </c>
+      <c r="D34" s="48"/>
+      <c r="E34" s="4">
+        <v>45861</v>
+      </c>
+      <c r="F34" s="49"/>
+      <c r="G34" s="49"/>
+      <c r="H34" s="49"/>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" s="49"/>
+      <c r="B35" s="49" t="s">
+        <v>16</v>
+      </c>
+      <c r="C35" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="D35" s="48"/>
+      <c r="E35" s="4">
+        <v>45861</v>
+      </c>
+      <c r="F35" s="49"/>
+      <c r="G35" s="49"/>
+      <c r="H35" s="49"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -2932,25 +3046,25 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C1" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="E1" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="G1" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="I1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="K1" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="N1" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -2967,10 +3081,10 @@
         <v>32</v>
       </c>
       <c r="K2" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="N2" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -2984,13 +3098,13 @@
         <v>31</v>
       </c>
       <c r="I3" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="K3" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="N3" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -3001,10 +3115,10 @@
         <v>5</v>
       </c>
       <c r="G4" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="I4" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -3115,19 +3229,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>24</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="E1" s="16"/>
       <c r="F1" s="16"/>
       <c r="G1" s="16"/>
       <c r="H1" s="17" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="I1" s="18"/>
       <c r="J1" s="18"/>
@@ -3138,61 +3252,61 @@
       <c r="B2" s="20"/>
       <c r="C2" s="20"/>
       <c r="D2" s="21" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="F2" s="22" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="G2" s="22" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="H2" s="23" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="I2" s="24" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="J2" s="24" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="K2" s="25" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:11" hidden="1">
       <c r="A3" s="46"/>
       <c r="B3" s="26" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="F3" s="26" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="G3" s="26" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="H3" s="26" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="I3" s="26" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="J3" s="26" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="K3" s="26" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -3200,7 +3314,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="C4" t="s">
         <v>35</v>
@@ -3235,7 +3349,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="C5" t="s">
         <v>35</v>
@@ -4863,14 +4977,14 @@
       <c r="A1" s="28"/>
       <c r="B1" s="29"/>
       <c r="C1" s="30" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D1" s="31"/>
       <c r="E1" s="30"/>
       <c r="F1" s="31"/>
       <c r="G1" s="32"/>
       <c r="H1" s="44" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="I1" s="32"/>
       <c r="J1" s="29"/>
@@ -4883,19 +4997,19 @@
         <v>24</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="D2" s="36"/>
       <c r="E2" s="37" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="F2" s="38"/>
       <c r="G2" s="35" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="37" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="J2" s="38"/>
     </row>
@@ -4933,34 +5047,34 @@
     </row>
     <row r="4" spans="1:10" customFormat="1" hidden="1">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="B4" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="C4" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D4" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="E4" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="F4" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="G4" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="H4" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="I4" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="J4" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -5010,10 +5124,10 @@
         <v>24</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="6" customFormat="1">
@@ -5074,25 +5188,25 @@
         <v>24</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -5145,16 +5259,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="B1" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="C1" t="s">
         <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -5197,10 +5311,10 @@
         <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="D1" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:4">

</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-07-28 13:22:36
</commit_message>
<xml_diff>
--- a/data/Solar_Lab_Tests.xlsx
+++ b/data/Solar_Lab_Tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="861" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B9B9340C-05B7-4EE4-9642-0FE1DF386EA7}"/>
+  <xr:revisionPtr revIDLastSave="866" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{133C314F-C155-4849-B445-5F1E19F61D4B}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="10" activeTab="1" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="5" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Tests Map" sheetId="4" state="hidden" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="120">
   <si>
     <t>BOM</t>
   </si>
@@ -739,7 +739,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -817,7 +817,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2270,8 +2269,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9401EE47-EA52-49C7-BBC0-21F5B88254FB}">
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView topLeftCell="B6" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -2881,6 +2880,9 @@
         <v>54</v>
       </c>
       <c r="D28" s="48"/>
+      <c r="E28" s="4">
+        <v>45866</v>
+      </c>
     </row>
     <row r="29" spans="1:8">
       <c r="B29" t="s">
@@ -2904,84 +2906,64 @@
       </c>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="49"/>
-      <c r="B31" s="49" t="s">
+      <c r="B31" t="s">
         <v>16</v>
       </c>
-      <c r="C31" s="49" t="s">
+      <c r="C31" t="s">
         <v>56</v>
       </c>
       <c r="D31" s="48"/>
       <c r="E31" s="4">
         <v>45861</v>
       </c>
-      <c r="F31" s="49"/>
-      <c r="G31" s="49"/>
-      <c r="H31" s="49"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="49"/>
-      <c r="B32" s="49" t="s">
+      <c r="B32" t="s">
         <v>16</v>
       </c>
-      <c r="C32" s="49" t="s">
+      <c r="C32" t="s">
         <v>57</v>
       </c>
       <c r="D32" s="48"/>
       <c r="E32" s="4">
         <v>45861</v>
       </c>
-      <c r="F32" s="49"/>
-      <c r="G32" s="49"/>
-      <c r="H32" s="49"/>
-    </row>
-    <row r="33" spans="1:8">
-      <c r="A33" s="49"/>
-      <c r="B33" s="49" t="s">
+    </row>
+    <row r="33" spans="2:5">
+      <c r="B33" t="s">
         <v>16</v>
       </c>
-      <c r="C33" s="49" t="s">
+      <c r="C33" t="s">
         <v>58</v>
       </c>
       <c r="D33" s="48"/>
       <c r="E33" s="4">
         <v>45861</v>
       </c>
-      <c r="F33" s="49"/>
-      <c r="G33" s="49"/>
-      <c r="H33" s="49"/>
-    </row>
-    <row r="34" spans="1:8">
-      <c r="A34" s="49"/>
-      <c r="B34" s="49" t="s">
+    </row>
+    <row r="34" spans="2:5">
+      <c r="B34" t="s">
         <v>16</v>
       </c>
-      <c r="C34" s="49" t="s">
+      <c r="C34" t="s">
         <v>59</v>
       </c>
       <c r="D34" s="48"/>
       <c r="E34" s="4">
         <v>45861</v>
       </c>
-      <c r="F34" s="49"/>
-      <c r="G34" s="49"/>
-      <c r="H34" s="49"/>
-    </row>
-    <row r="35" spans="1:8">
-      <c r="A35" s="49"/>
-      <c r="B35" s="49" t="s">
+    </row>
+    <row r="35" spans="2:5">
+      <c r="B35" t="s">
         <v>16</v>
       </c>
-      <c r="C35" s="49" t="s">
+      <c r="C35" t="s">
         <v>45</v>
       </c>
       <c r="D35" s="48"/>
       <c r="E35" s="4">
         <v>45861</v>
       </c>
-      <c r="F35" s="49"/>
-      <c r="G35" s="49"/>
-      <c r="H35" s="49"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -5102,10 +5084,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C8152F1-3340-4C7F-9B6C-3F6BB96763BA}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5145,6 +5127,14 @@
       </c>
       <c r="E2"/>
       <c r="F2"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>54</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="2">

</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-08-01 09:50:07
</commit_message>
<xml_diff>
--- a/data/Solar_Lab_Tests.xlsx
+++ b/data/Solar_Lab_Tests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="866" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{133C314F-C155-4849-B445-5F1E19F61D4B}"/>
+  <xr:revisionPtr revIDLastSave="996" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F442FB0A-140F-4304-8513-5D17AB75BF5A}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="5" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="5" activeTab="1" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Tests Map" sheetId="4" state="hidden" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <definedName name="ENCAPTYPE">Ref!$K$2:$K$1048576</definedName>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">'Material Tests Map'!$A$1:$B$20</definedName>
     <definedName name="ExternalData_1" localSheetId="11" hidden="1">'Standard test times'!$A$1:$B$15</definedName>
-    <definedName name="ExternalData_1" localSheetId="1" hidden="1">'Test Data'!$A$1:$H$35</definedName>
+    <definedName name="ExternalData_1" localSheetId="1" hidden="1">'Test Data'!$A$1:$H$45</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="148">
   <si>
     <t>BOM</t>
   </si>
@@ -186,6 +186,9 @@
     <t>Tesa 4134</t>
   </si>
   <si>
+    <t>In Progress</t>
+  </si>
+  <si>
     <t>Hutian</t>
   </si>
   <si>
@@ -252,6 +255,18 @@
     <t>SSEPL</t>
   </si>
   <si>
+    <t>QC SOLAR SMART JB</t>
+  </si>
+  <si>
+    <t>VISHAKHA</t>
+  </si>
+  <si>
+    <t>RAYBO EPE</t>
+  </si>
+  <si>
+    <t>BARCODE X 50*15</t>
+  </si>
+  <si>
     <t>RM Type</t>
   </si>
   <si>
@@ -279,9 +294,6 @@
     <t>OLD : 420 to 480</t>
   </si>
   <si>
-    <t>In Progress</t>
-  </si>
-  <si>
     <t>BACK EVA</t>
   </si>
   <si>
@@ -342,6 +354,9 @@
     <t>Column10</t>
   </si>
   <si>
+    <t>VISHKHA</t>
+  </si>
+  <si>
     <t xml:space="preserve">                                                                                                                           PRE PCT</t>
   </si>
   <si>
@@ -381,12 +396,36 @@
     <t>Mean</t>
   </si>
   <si>
+    <t>VISHKHA EPE</t>
+  </si>
+  <si>
+    <t>VISHKHA EVA</t>
+  </si>
+  <si>
     <t xml:space="preserve">BOM </t>
   </si>
   <si>
     <t>MEASURED VALUE</t>
   </si>
   <si>
+    <t>INTERCONNECT RIBBON</t>
+  </si>
+  <si>
+    <t>WETOWN 0.24MM</t>
+  </si>
+  <si>
+    <t>.421M</t>
+  </si>
+  <si>
+    <t>BUS RIBBON</t>
+  </si>
+  <si>
+    <t>WETOWN 5MM</t>
+  </si>
+  <si>
+    <t>.009M</t>
+  </si>
+  <si>
     <t>START TIME</t>
   </si>
   <si>
@@ -417,16 +456,61 @@
     <t>CAHORS 30A</t>
   </si>
   <si>
+    <t>262MV</t>
+  </si>
+  <si>
     <t>UKTR BD IEL</t>
   </si>
   <si>
     <t>UKTR 20A MJB</t>
   </si>
   <si>
+    <t>302MV</t>
+  </si>
+  <si>
+    <t>260MV</t>
+  </si>
+  <si>
     <t>UKTR30A</t>
   </si>
   <si>
+    <t>267MV</t>
+  </si>
+  <si>
+    <t>301MV</t>
+  </si>
+  <si>
     <t>QC Vietnam</t>
+  </si>
+  <si>
+    <t>270MV</t>
+  </si>
+  <si>
+    <t>252MV</t>
+  </si>
+  <si>
+    <t>257MV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QC SOLAR SMART </t>
+  </si>
+  <si>
+    <t>243MV</t>
+  </si>
+  <si>
+    <t>VEMOULD20A</t>
+  </si>
+  <si>
+    <t>285MV</t>
+  </si>
+  <si>
+    <t>247MV</t>
+  </si>
+  <si>
+    <t>288MV</t>
+  </si>
+  <si>
+    <t>255MV</t>
   </si>
   <si>
     <t>STANDARD DURATION (DAYS)</t>
@@ -739,7 +823,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -817,6 +901,8 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1248,8 +1334,8 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{97A8C2A7-46C0-4446-B562-6550EA520638}" name="Table10" displayName="Table10" ref="A1:I2" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:I2" xr:uid="{97A8C2A7-46C0-4446-B562-6550EA520638}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{97A8C2A7-46C0-4446-B562-6550EA520638}" name="Table10" displayName="Table10" ref="A1:I3" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:I3" xr:uid="{97A8C2A7-46C0-4446-B562-6550EA520638}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{FE721515-FBBB-4487-ABCE-AAB6A5B1513A}" name="BOM" dataDxfId="9"/>
     <tableColumn id="9" xr3:uid="{304FA6D2-898E-427A-8AC1-958C15295938}" name="VENDOR NAME" dataDxfId="8"/>
@@ -1305,8 +1391,8 @@
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{5C370BE7-C0F8-462F-9F89-5FC458087319}" name="Table16" displayName="Table16" ref="A1:G13" totalsRowShown="0">
-  <autoFilter ref="A1:G13" xr:uid="{5C370BE7-C0F8-462F-9F89-5FC458087319}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{5C370BE7-C0F8-462F-9F89-5FC458087319}" name="Table16" displayName="Table16" ref="A1:G18" totalsRowShown="0">
+  <autoFilter ref="A1:G18" xr:uid="{5C370BE7-C0F8-462F-9F89-5FC458087319}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{59EA2429-768A-457D-88E6-B34A083DE755}" name="BOM"/>
     <tableColumn id="2" xr3:uid="{C09F236B-325A-4EF9-B484-B1D592C83B7F}" name="VENDOR NAME"/>
@@ -1332,7 +1418,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{06A3AD80-C098-4015-85FF-3495CE4443EA}" name="Test_Data" displayName="Test_Data" ref="A1:H35" tableType="queryTable" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{06A3AD80-C098-4015-85FF-3495CE4443EA}" name="Test_Data" displayName="Test_Data" ref="A1:H45" tableType="queryTable" totalsRowShown="0">
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{87F75B08-44C4-4718-834D-87FEE9F87970}" uniqueName="1" name="BOM" queryTableFieldId="1" dataDxfId="42"/>
     <tableColumn id="2" xr3:uid="{1E5F4521-5E5C-4948-AEB2-FC5F712DB353}" uniqueName="2" name="TEST NAME" queryTableFieldId="2" dataDxfId="41"/>
@@ -1951,10 +2037,10 @@
         <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
       <c r="D1" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1976,10 +2062,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{333C0630-51CF-46CA-8CAD-98FEF9AC181F}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2001,19 +2087,19 @@
         <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="D1" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="E1" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="F1" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
       <c r="G1" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -2021,7 +2107,13 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>114</v>
+        <v>127</v>
+      </c>
+      <c r="D2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E2">
+        <v>331</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2029,7 +2121,7 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2037,7 +2129,13 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>116</v>
+        <v>130</v>
+      </c>
+      <c r="D4" t="s">
+        <v>131</v>
+      </c>
+      <c r="E4">
+        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -2045,7 +2143,13 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>46</v>
+      </c>
+      <c r="D5" t="s">
+        <v>132</v>
+      </c>
+      <c r="E5">
+        <v>249</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -2053,7 +2157,13 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>117</v>
+        <v>133</v>
+      </c>
+      <c r="D6" t="s">
+        <v>134</v>
+      </c>
+      <c r="E6">
+        <v>197</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -2061,7 +2171,13 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>48</v>
+      </c>
+      <c r="D7" t="s">
+        <v>135</v>
+      </c>
+      <c r="E7">
+        <v>277</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -2069,7 +2185,13 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>118</v>
+        <v>136</v>
+      </c>
+      <c r="D8" t="s">
+        <v>137</v>
+      </c>
+      <c r="E8">
+        <v>237</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -2077,7 +2199,13 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>59</v>
+        <v>60</v>
+      </c>
+      <c r="D9" t="s">
+        <v>138</v>
+      </c>
+      <c r="E9">
+        <v>325</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -2085,7 +2213,13 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>58</v>
+        <v>59</v>
+      </c>
+      <c r="D10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E10">
+        <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -2093,7 +2227,13 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>57</v>
+      </c>
+      <c r="D11" t="s">
+        <v>131</v>
+      </c>
+      <c r="E11">
+        <v>178</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -2101,12 +2241,91 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>46</v>
+      </c>
+      <c r="D12" t="s">
+        <v>139</v>
+      </c>
+      <c r="E12">
+        <v>227</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" t="s">
+        <v>141</v>
+      </c>
+      <c r="E14">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>142</v>
+      </c>
+      <c r="D15" t="s">
+        <v>143</v>
+      </c>
+      <c r="E15">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" t="s">
+        <v>144</v>
+      </c>
+      <c r="E16">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" t="s">
+        <v>145</v>
+      </c>
+      <c r="E17">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" t="s">
+        <v>146</v>
+      </c>
+      <c r="E18">
+        <v>275</v>
       </c>
     </row>
   </sheetData>
@@ -2141,7 +2360,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>119</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2267,10 +2486,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9401EE47-EA52-49C7-BBC0-21F5B88254FB}">
-  <dimension ref="A1:K35"/>
+  <dimension ref="A1:K45"/>
   <sheetViews>
-    <sheetView topLeftCell="B6" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="B32" workbookViewId="0">
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -2547,7 +2766,7 @@
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="H11" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>23</v>
@@ -2561,7 +2780,7 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="4">
@@ -2598,7 +2817,7 @@
         <v>32</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -2609,7 +2828,7 @@
         <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="4">
@@ -2622,7 +2841,7 @@
         <v>32</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -2648,7 +2867,7 @@
         <v>32</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -2683,13 +2902,15 @@
         <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D17" s="5"/>
-      <c r="E17" s="4"/>
+      <c r="E17" s="4">
+        <v>45869</v>
+      </c>
       <c r="F17" s="4"/>
       <c r="H17" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -2698,13 +2919,15 @@
         <v>18</v>
       </c>
       <c r="C18" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D18" s="5"/>
-      <c r="E18" s="4"/>
+      <c r="E18" s="4">
+        <v>45869</v>
+      </c>
       <c r="F18" s="4"/>
       <c r="H18" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -2713,13 +2936,15 @@
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D19" s="5"/>
-      <c r="E19" s="4"/>
+      <c r="E19" s="4">
+        <v>45869</v>
+      </c>
       <c r="F19" s="4"/>
       <c r="H19" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -2728,7 +2953,7 @@
         <v>16</v>
       </c>
       <c r="C20" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="4">
@@ -2747,7 +2972,7 @@
         <v>16</v>
       </c>
       <c r="C21" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="4">
@@ -2766,7 +2991,7 @@
         <v>16</v>
       </c>
       <c r="C22" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="4">
@@ -2785,7 +3010,7 @@
         <v>16</v>
       </c>
       <c r="C23" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="4">
@@ -2804,7 +3029,7 @@
         <v>16</v>
       </c>
       <c r="C24" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="4">
@@ -2823,7 +3048,7 @@
         <v>16</v>
       </c>
       <c r="C25" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="4">
@@ -2841,7 +3066,7 @@
         <v>16</v>
       </c>
       <c r="C26" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="4">
@@ -2859,7 +3084,7 @@
         <v>16</v>
       </c>
       <c r="C27" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D27" s="48"/>
       <c r="E27" s="4">
@@ -2877,97 +3102,295 @@
         <v>5</v>
       </c>
       <c r="C28" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D28" s="48"/>
       <c r="E28" s="4">
         <v>45866</v>
       </c>
+      <c r="H28" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="29" spans="1:8">
       <c r="B29" t="s">
         <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D29" s="48"/>
+      <c r="H29" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="30" spans="1:8">
       <c r="B30" t="s">
         <v>16</v>
       </c>
       <c r="C30" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D30" s="48"/>
       <c r="E30" s="4">
         <v>45861</v>
       </c>
+      <c r="H30" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="31" spans="1:8">
       <c r="B31" t="s">
         <v>16</v>
       </c>
       <c r="C31" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D31" s="48"/>
       <c r="E31" s="4">
         <v>45861</v>
       </c>
+      <c r="H31" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="32" spans="1:8">
       <c r="B32" t="s">
         <v>16</v>
       </c>
       <c r="C32" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D32" s="48"/>
       <c r="E32" s="4">
         <v>45861</v>
       </c>
-    </row>
-    <row r="33" spans="2:5">
+      <c r="H32" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
       <c r="B33" t="s">
         <v>16</v>
       </c>
       <c r="C33" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D33" s="48"/>
       <c r="E33" s="4">
         <v>45861</v>
       </c>
-    </row>
-    <row r="34" spans="2:5">
+      <c r="H33" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
       <c r="B34" t="s">
         <v>16</v>
       </c>
       <c r="C34" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D34" s="48"/>
       <c r="E34" s="4">
         <v>45861</v>
       </c>
-    </row>
-    <row r="35" spans="2:5">
+      <c r="H34" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
       <c r="B35" t="s">
         <v>16</v>
       </c>
       <c r="C35" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D35" s="48"/>
       <c r="E35" s="4">
         <v>45861</v>
       </c>
+      <c r="H35" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="49"/>
+      <c r="B36" s="49" t="s">
+        <v>16</v>
+      </c>
+      <c r="C36" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="D36" s="48"/>
+      <c r="E36" s="4">
+        <v>45867</v>
+      </c>
+      <c r="F36" s="49"/>
+      <c r="G36" s="49"/>
+      <c r="H36" s="49" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="49"/>
+      <c r="B37" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" s="49" t="s">
+        <v>62</v>
+      </c>
+      <c r="D37" s="48"/>
+      <c r="E37" s="4">
+        <v>45870</v>
+      </c>
+      <c r="F37" s="49"/>
+      <c r="G37" s="49"/>
+      <c r="H37" s="49" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="15">
+      <c r="A38" s="49"/>
+      <c r="B38" s="49" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D38" s="48"/>
+      <c r="E38" s="4">
+        <v>45870</v>
+      </c>
+      <c r="F38" s="49"/>
+      <c r="G38" s="49"/>
+      <c r="H38" s="49" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="15">
+      <c r="A39" s="49"/>
+      <c r="B39" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D39" s="48"/>
+      <c r="E39" s="4">
+        <v>45870</v>
+      </c>
+      <c r="F39" s="49"/>
+      <c r="G39" s="49"/>
+      <c r="H39" s="49" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="15">
+      <c r="A40" s="49"/>
+      <c r="B40" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D40" s="48"/>
+      <c r="E40" s="4">
+        <v>45870</v>
+      </c>
+      <c r="F40" s="49"/>
+      <c r="G40" s="49"/>
+      <c r="H40" s="49" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="15">
+      <c r="A41" s="49"/>
+      <c r="B41" s="49" t="s">
+        <v>3</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D41" s="48"/>
+      <c r="E41" s="4">
+        <v>45870</v>
+      </c>
+      <c r="F41" s="49"/>
+      <c r="G41" s="49"/>
+      <c r="H41" s="49" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" s="49"/>
+      <c r="B42" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="C42" s="49" t="s">
+        <v>63</v>
+      </c>
+      <c r="D42" s="48"/>
+      <c r="E42" s="4">
+        <v>45869</v>
+      </c>
+      <c r="F42" s="49"/>
+      <c r="G42" s="49"/>
+      <c r="H42" s="49" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" s="49"/>
+      <c r="B43" s="49" t="s">
+        <v>18</v>
+      </c>
+      <c r="C43" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="D43" s="48"/>
+      <c r="E43" s="49"/>
+      <c r="F43" s="49"/>
+      <c r="G43" s="49"/>
+      <c r="H43" s="49" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" s="49"/>
+      <c r="B44" s="49" t="s">
+        <v>18</v>
+      </c>
+      <c r="C44" s="49" t="s">
+        <v>58</v>
+      </c>
+      <c r="D44" s="48"/>
+      <c r="E44" s="49"/>
+      <c r="F44" s="49"/>
+      <c r="G44" s="49"/>
+      <c r="H44" s="49" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" s="49"/>
+      <c r="B45" s="49" t="s">
+        <v>18</v>
+      </c>
+      <c r="C45" s="49" t="s">
+        <v>60</v>
+      </c>
+      <c r="D45" s="48"/>
+      <c r="E45" s="49"/>
+      <c r="F45" s="49"/>
+      <c r="G45" s="49"/>
+      <c r="H45" s="49" t="s">
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A11 C1:C1048576" xr:uid="{8C537B12-83B7-48DB-9398-33493EB60A9D}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A11 C1:C37 C42:C1048576" xr:uid="{8C537B12-83B7-48DB-9398-33493EB60A9D}"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K8:K16" xr:uid="{C3958E6F-28D2-429E-9DF5-7DAD65BBE2ED}">
       <formula1>$K:$K</formula1>
     </dataValidation>
@@ -3028,25 +3451,25 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="C1" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="E1" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="G1" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="I1" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="K1" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="N1" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -3063,10 +3486,10 @@
         <v>32</v>
       </c>
       <c r="K2" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="N2" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -3080,13 +3503,13 @@
         <v>31</v>
       </c>
       <c r="I3" t="s">
-        <v>69</v>
+        <v>38</v>
       </c>
       <c r="K3" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="N3" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -3097,10 +3520,10 @@
         <v>5</v>
       </c>
       <c r="G4" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="I4" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -3124,7 +3547,7 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
@@ -3132,7 +3555,7 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
@@ -3140,7 +3563,7 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
         <v>12</v>
@@ -3194,7 +3617,7 @@
   <dimension ref="A1:K519"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3211,19 +3634,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>24</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E1" s="16"/>
       <c r="F1" s="16"/>
       <c r="G1" s="16"/>
       <c r="H1" s="17" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="I1" s="18"/>
       <c r="J1" s="18"/>
@@ -3234,61 +3657,61 @@
       <c r="B2" s="20"/>
       <c r="C2" s="20"/>
       <c r="D2" s="21" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="F2" s="22" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="G2" s="22" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="H2" s="23" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="I2" s="24" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="J2" s="24" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="K2" s="25" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:11" hidden="1">
       <c r="A3" s="46"/>
       <c r="B3" s="26" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="F3" s="26" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="G3" s="26" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="H3" s="26" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="I3" s="26" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="J3" s="26" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="K3" s="26" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -3296,7 +3719,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="C4" t="s">
         <v>35</v>
@@ -3331,7 +3754,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C5" t="s">
         <v>35</v>
@@ -3362,10 +3785,23 @@
       </c>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="46"/>
+      <c r="A6" s="46" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="46"/>
+      <c r="A7" s="46" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="46"/>
@@ -4906,7 +5342,7 @@
   </sheetData>
   <dataValidations count="3">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 C4:C5" xr:uid="{5C73BBC5-C68D-4586-BDB5-A3BE48854FB6}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B1048576" xr:uid="{18FD80CD-FFDC-48A1-BA45-91576461B09B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B1048576 C7:K7" xr:uid="{18FD80CD-FFDC-48A1-BA45-91576461B09B}">
       <formula1>"FRONT EPE, BACK EVA"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4:A1048576" xr:uid="{CDEE756C-C284-45D8-BDCE-F4798D4B3C50}">
@@ -4934,10 +5370,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E993B7F-E878-4ABA-95AD-A4138848D6EF}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4959,14 +5395,14 @@
       <c r="A1" s="28"/>
       <c r="B1" s="29"/>
       <c r="C1" s="30" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="D1" s="31"/>
       <c r="E1" s="30"/>
       <c r="F1" s="31"/>
       <c r="G1" s="32"/>
       <c r="H1" s="44" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="I1" s="32"/>
       <c r="J1" s="29"/>
@@ -4979,19 +5415,19 @@
         <v>24</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="D2" s="36"/>
       <c r="E2" s="37" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="F2" s="38"/>
       <c r="G2" s="35" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="37" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="J2" s="38"/>
     </row>
@@ -5029,34 +5465,62 @@
     </row>
     <row r="4" spans="1:10" customFormat="1" hidden="1">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="B4" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C4" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D4" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E4" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="F4" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="G4" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="H4" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="I4" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="J4" t="s">
-        <v>89</v>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="45" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="45">
+        <v>75</v>
+      </c>
+      <c r="D5" s="45">
+        <v>55</v>
+      </c>
+      <c r="E5" s="45">
+        <v>145</v>
+      </c>
+      <c r="F5" s="45">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="45" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -5074,7 +5538,7 @@
           <x14:formula1>
             <xm:f>Ref!$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>A3:A4</xm:sqref>
+          <xm:sqref>A3:A6</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5084,10 +5548,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C8152F1-3340-4C7F-9B6C-3F6BB96763BA}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5106,10 +5570,10 @@
         <v>24</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="6" customFormat="1">
@@ -5133,13 +5597,21 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B3 D2:D3 D5:D1048576" xr:uid="{FCBF55FC-869D-43C4-B484-27D4BFDDD5A4}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A1048576 A2:A3" xr:uid="{04F856B6-1846-4FF1-B3BB-4FE58494E678}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576" xr:uid="{04F856B6-1846-4FF1-B3BB-4FE58494E678}">
       <formula1>"ENCAPSULANT, RIBBON"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5152,10 +5624,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C0F3BDD-3989-4880-8737-F370069E1383}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5178,32 +5650,52 @@
         <v>24</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="B2" s="12"/>
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>108</v>
+      </c>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="50"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -5233,10 +5725,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD5452B6-66C2-4964-BBFB-466116F6D217}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5249,16 +5741,44 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="B1" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="C1" t="s">
         <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>104</v>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D3" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -5301,10 +5821,10 @@
         <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="D1" t="s">
-        <v>106</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -5326,7 +5846,7 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C4" s="10">
         <v>0.59791666666666665</v>

</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-08-04 13:25:04
</commit_message>
<xml_diff>
--- a/data/Solar_Lab_Tests.xlsx
+++ b/data/Solar_Lab_Tests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="996" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F442FB0A-140F-4304-8513-5D17AB75BF5A}"/>
+  <xr:revisionPtr revIDLastSave="1019" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{777F9C62-EA83-4CF6-9EB0-BB90F9106BD6}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="5" activeTab="1" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="1" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Tests Map" sheetId="4" state="hidden" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <definedName name="ENCAPTYPE">Ref!$K$2:$K$1048576</definedName>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">'Material Tests Map'!$A$1:$B$20</definedName>
     <definedName name="ExternalData_1" localSheetId="11" hidden="1">'Standard test times'!$A$1:$B$15</definedName>
-    <definedName name="ExternalData_1" localSheetId="1" hidden="1">'Test Data'!$A$1:$H$45</definedName>
+    <definedName name="ExternalData_1" localSheetId="1" hidden="1">'Test Data'!$A$1:$H$52</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="154">
   <si>
     <t>BOM</t>
   </si>
@@ -267,6 +267,27 @@
     <t>BARCODE X 50*15</t>
   </si>
   <si>
+    <t>VishakhaEPE /EVA</t>
+  </si>
+  <si>
+    <t>Wetown INTC</t>
+  </si>
+  <si>
+    <t>Cybrid Raybo EPE/EVA</t>
+  </si>
+  <si>
+    <t>QC Vietnam</t>
+  </si>
+  <si>
+    <t>. QC 30A LINE T</t>
+  </si>
+  <si>
+    <t>ZERUN</t>
+  </si>
+  <si>
+    <t>LINE  EPE/EVA</t>
+  </si>
+  <si>
     <t>RM Type</t>
   </si>
   <si>
@@ -478,9 +499,6 @@
   </si>
   <si>
     <t>301MV</t>
-  </si>
-  <si>
-    <t>QC Vietnam</t>
   </si>
   <si>
     <t>270MV</t>
@@ -823,7 +841,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -902,7 +920,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1418,7 +1435,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{06A3AD80-C098-4015-85FF-3495CE4443EA}" name="Test_Data" displayName="Test_Data" ref="A1:H45" tableType="queryTable" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{06A3AD80-C098-4015-85FF-3495CE4443EA}" name="Test_Data" displayName="Test_Data" ref="A1:H52" tableType="queryTable" totalsRowShown="0">
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{87F75B08-44C4-4718-834D-87FEE9F87970}" uniqueName="1" name="BOM" queryTableFieldId="1" dataDxfId="42"/>
     <tableColumn id="2" xr3:uid="{1E5F4521-5E5C-4948-AEB2-FC5F712DB353}" uniqueName="2" name="TEST NAME" queryTableFieldId="2" dataDxfId="41"/>
@@ -2037,10 +2054,10 @@
         <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="D1" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -2087,19 +2104,19 @@
         <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="D1" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="E1" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="F1" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="G1" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -2107,10 +2124,10 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="D2" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="E2">
         <v>331</v>
@@ -2121,7 +2138,7 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2129,10 +2146,10 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="D4" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="E4">
         <v>176</v>
@@ -2146,7 +2163,7 @@
         <v>46</v>
       </c>
       <c r="D5" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="E5">
         <v>249</v>
@@ -2157,10 +2174,10 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="D6" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="E6">
         <v>197</v>
@@ -2174,7 +2191,7 @@
         <v>48</v>
       </c>
       <c r="D7" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="E7">
         <v>277</v>
@@ -2185,10 +2202,10 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>136</v>
+        <v>68</v>
       </c>
       <c r="D8" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="E8">
         <v>237</v>
@@ -2202,7 +2219,7 @@
         <v>60</v>
       </c>
       <c r="D9" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="E9">
         <v>325</v>
@@ -2216,7 +2233,7 @@
         <v>59</v>
       </c>
       <c r="D10" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="E10">
         <v>155</v>
@@ -2230,7 +2247,7 @@
         <v>57</v>
       </c>
       <c r="D11" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="E11">
         <v>178</v>
@@ -2244,7 +2261,7 @@
         <v>46</v>
       </c>
       <c r="D12" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="E12">
         <v>227</v>
@@ -2255,7 +2272,7 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -2266,7 +2283,7 @@
         <v>56</v>
       </c>
       <c r="D14" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="E14">
         <v>357</v>
@@ -2277,10 +2294,10 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="D15" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="E15">
         <v>158</v>
@@ -2294,7 +2311,7 @@
         <v>52</v>
       </c>
       <c r="D16" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="E16">
         <v>314</v>
@@ -2308,7 +2325,7 @@
         <v>51</v>
       </c>
       <c r="D17" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="E17">
         <v>162</v>
@@ -2322,7 +2339,7 @@
         <v>49</v>
       </c>
       <c r="D18" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="E18">
         <v>275</v>
@@ -2360,7 +2377,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2486,10 +2503,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9401EE47-EA52-49C7-BBC0-21F5B88254FB}">
-  <dimension ref="A1:K45"/>
+  <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B32" workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
+    <sheetView tabSelected="1" topLeftCell="B11" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -3215,44 +3232,37 @@
       </c>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="49"/>
-      <c r="B36" s="49" t="s">
+      <c r="B36" t="s">
         <v>16</v>
       </c>
-      <c r="C36" s="49" t="s">
+      <c r="C36" t="s">
         <v>61</v>
       </c>
       <c r="D36" s="48"/>
       <c r="E36" s="4">
         <v>45867</v>
       </c>
-      <c r="F36" s="49"/>
-      <c r="G36" s="49"/>
-      <c r="H36" s="49" t="s">
+      <c r="H36" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="49"/>
-      <c r="B37" s="49" t="s">
+      <c r="B37" t="s">
         <v>4</v>
       </c>
-      <c r="C37" s="49" t="s">
+      <c r="C37" t="s">
         <v>62</v>
       </c>
       <c r="D37" s="48"/>
       <c r="E37" s="4">
         <v>45870</v>
       </c>
-      <c r="F37" s="49"/>
-      <c r="G37" s="49"/>
-      <c r="H37" s="49" t="s">
+      <c r="H37" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="15">
-      <c r="A38" s="49"/>
-      <c r="B38" s="49" t="s">
+      <c r="B38" t="s">
         <v>5</v>
       </c>
       <c r="C38" s="7" t="s">
@@ -3262,15 +3272,12 @@
       <c r="E38" s="4">
         <v>45870</v>
       </c>
-      <c r="F38" s="49"/>
-      <c r="G38" s="49"/>
-      <c r="H38" s="49" t="s">
+      <c r="H38" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="15">
-      <c r="A39" s="49"/>
-      <c r="B39" s="49" t="s">
+      <c r="B39" t="s">
         <v>6</v>
       </c>
       <c r="C39" s="7" t="s">
@@ -3280,15 +3287,12 @@
       <c r="E39" s="4">
         <v>45870</v>
       </c>
-      <c r="F39" s="49"/>
-      <c r="G39" s="49"/>
-      <c r="H39" s="49" t="s">
+      <c r="H39" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="15">
-      <c r="A40" s="49"/>
-      <c r="B40" s="49" t="s">
+      <c r="B40" t="s">
         <v>7</v>
       </c>
       <c r="C40" s="7" t="s">
@@ -3298,15 +3302,12 @@
       <c r="E40" s="4">
         <v>45870</v>
       </c>
-      <c r="F40" s="49"/>
-      <c r="G40" s="49"/>
-      <c r="H40" s="49" t="s">
+      <c r="H40" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="15">
-      <c r="A41" s="49"/>
-      <c r="B41" s="49" t="s">
+      <c r="B41" t="s">
         <v>3</v>
       </c>
       <c r="C41" s="7" t="s">
@@ -3316,81 +3317,176 @@
       <c r="E41" s="4">
         <v>45870</v>
       </c>
-      <c r="F41" s="49"/>
-      <c r="G41" s="49"/>
-      <c r="H41" s="49" t="s">
+      <c r="H41" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="49"/>
-      <c r="B42" s="49" t="s">
+      <c r="B42" t="s">
         <v>4</v>
       </c>
-      <c r="C42" s="49" t="s">
+      <c r="C42" t="s">
         <v>63</v>
       </c>
       <c r="D42" s="48"/>
       <c r="E42" s="4">
         <v>45869</v>
       </c>
-      <c r="F42" s="49"/>
-      <c r="G42" s="49"/>
-      <c r="H42" s="49" t="s">
+      <c r="H42" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="49"/>
-      <c r="B43" s="49" t="s">
+      <c r="B43" t="s">
         <v>18</v>
       </c>
-      <c r="C43" s="49" t="s">
+      <c r="C43" t="s">
         <v>64</v>
       </c>
       <c r="D43" s="48"/>
-      <c r="E43" s="49"/>
-      <c r="F43" s="49"/>
-      <c r="G43" s="49"/>
-      <c r="H43" s="49" t="s">
+      <c r="H43" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="49"/>
-      <c r="B44" s="49" t="s">
+      <c r="B44" t="s">
         <v>18</v>
       </c>
-      <c r="C44" s="49" t="s">
+      <c r="C44" t="s">
         <v>58</v>
       </c>
       <c r="D44" s="48"/>
-      <c r="E44" s="49"/>
-      <c r="F44" s="49"/>
-      <c r="G44" s="49"/>
-      <c r="H44" s="49" t="s">
+      <c r="H44" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="49"/>
-      <c r="B45" s="49" t="s">
+      <c r="B45" t="s">
         <v>18</v>
       </c>
-      <c r="C45" s="49" t="s">
+      <c r="C45" t="s">
         <v>60</v>
       </c>
       <c r="D45" s="48"/>
-      <c r="E45" s="49"/>
-      <c r="F45" s="49"/>
-      <c r="G45" s="49"/>
-      <c r="H45" s="49" t="s">
+      <c r="H45" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="15">
+      <c r="A46" s="49"/>
+      <c r="B46" s="49" t="s">
+        <v>18</v>
+      </c>
+      <c r="C46" t="s">
+        <v>65</v>
+      </c>
+      <c r="D46" s="48"/>
+      <c r="E46" s="49"/>
+      <c r="F46" s="49"/>
+      <c r="G46" s="49"/>
+      <c r="H46" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="15">
+      <c r="A47" s="49"/>
+      <c r="B47" s="49" t="s">
+        <v>18</v>
+      </c>
+      <c r="C47" t="s">
+        <v>66</v>
+      </c>
+      <c r="D47" s="48"/>
+      <c r="E47" s="49"/>
+      <c r="F47" s="49"/>
+      <c r="G47" s="49"/>
+      <c r="H47" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="15">
+      <c r="A48" s="49"/>
+      <c r="B48" s="49" t="s">
+        <v>18</v>
+      </c>
+      <c r="C48" t="s">
+        <v>67</v>
+      </c>
+      <c r="D48" s="48"/>
+      <c r="E48" s="49"/>
+      <c r="F48" s="49"/>
+      <c r="G48" s="49"/>
+      <c r="H48" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="15">
+      <c r="A49" s="49"/>
+      <c r="B49" s="49" t="s">
+        <v>18</v>
+      </c>
+      <c r="C49" t="s">
+        <v>68</v>
+      </c>
+      <c r="D49" s="48"/>
+      <c r="E49" s="49"/>
+      <c r="F49" s="49"/>
+      <c r="G49" s="49"/>
+      <c r="H49" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="15">
+      <c r="A50" s="49"/>
+      <c r="B50" s="49" t="s">
+        <v>18</v>
+      </c>
+      <c r="C50" t="s">
+        <v>69</v>
+      </c>
+      <c r="D50" s="48"/>
+      <c r="E50" s="49"/>
+      <c r="F50" s="49"/>
+      <c r="G50" s="49"/>
+      <c r="H50" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" s="49"/>
+      <c r="B51" s="49" t="s">
+        <v>18</v>
+      </c>
+      <c r="C51" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="D51" s="48"/>
+      <c r="E51" s="49"/>
+      <c r="F51" s="49"/>
+      <c r="G51" s="49"/>
+      <c r="H51" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" s="49"/>
+      <c r="B52" s="49" t="s">
+        <v>18</v>
+      </c>
+      <c r="C52" s="49" t="s">
+        <v>71</v>
+      </c>
+      <c r="D52" s="48"/>
+      <c r="E52" s="49"/>
+      <c r="F52" s="49"/>
+      <c r="G52" s="49"/>
+      <c r="H52" t="s">
         <v>31</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A11 C1:C37 C42:C1048576" xr:uid="{8C537B12-83B7-48DB-9398-33493EB60A9D}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A11 C1:C37 C42:C45 C51:C1048576" xr:uid="{8C537B12-83B7-48DB-9398-33493EB60A9D}"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K8:K16" xr:uid="{C3958E6F-28D2-429E-9DF5-7DAD65BBE2ED}">
       <formula1>$K:$K</formula1>
     </dataValidation>
@@ -3451,25 +3547,25 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="C1" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="E1" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="G1" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="I1" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="K1" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="N1" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -3486,10 +3582,10 @@
         <v>32</v>
       </c>
       <c r="K2" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="N2" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -3506,10 +3602,10 @@
         <v>38</v>
       </c>
       <c r="K3" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="N3" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -3520,10 +3616,10 @@
         <v>5</v>
       </c>
       <c r="G4" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="I4" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -3634,19 +3730,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>24</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="E1" s="16"/>
       <c r="F1" s="16"/>
       <c r="G1" s="16"/>
       <c r="H1" s="17" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="I1" s="18"/>
       <c r="J1" s="18"/>
@@ -3657,61 +3753,61 @@
       <c r="B2" s="20"/>
       <c r="C2" s="20"/>
       <c r="D2" s="21" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="F2" s="22" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="G2" s="22" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="H2" s="23" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="I2" s="24" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="J2" s="24" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="K2" s="25" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:11" hidden="1">
       <c r="A3" s="46"/>
       <c r="B3" s="26" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="F3" s="26" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="G3" s="26" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="H3" s="26" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="I3" s="26" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="J3" s="26" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="K3" s="26" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -3719,7 +3815,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="C4" t="s">
         <v>35</v>
@@ -3754,7 +3850,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="C5" t="s">
         <v>35</v>
@@ -3789,10 +3885,10 @@
         <v>2</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -3800,7 +3896,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="27" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -5395,14 +5491,14 @@
       <c r="A1" s="28"/>
       <c r="B1" s="29"/>
       <c r="C1" s="30" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="D1" s="31"/>
       <c r="E1" s="30"/>
       <c r="F1" s="31"/>
       <c r="G1" s="32"/>
       <c r="H1" s="44" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="I1" s="32"/>
       <c r="J1" s="29"/>
@@ -5415,19 +5511,19 @@
         <v>24</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="D2" s="36"/>
       <c r="E2" s="37" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="F2" s="38"/>
       <c r="G2" s="35" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="37" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="J2" s="38"/>
     </row>
@@ -5465,34 +5561,34 @@
     </row>
     <row r="4" spans="1:10" customFormat="1" hidden="1">
       <c r="A4" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="B4" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="C4" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="D4" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="E4" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="F4" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="G4" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="H4" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="I4" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="J4" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -5520,7 +5616,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="45" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -5570,10 +5666,10 @@
         <v>24</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="6" customFormat="1">
@@ -5605,7 +5701,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -5650,25 +5746,25 @@
         <v>24</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -5676,26 +5772,22 @@
         <v>2</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="50" t="s">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
+        <v>116</v>
+      </c>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
-      <c r="I3" s="50"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -5741,16 +5833,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="B1" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="C1" t="s">
         <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -5758,13 +5850,13 @@
         <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="C2" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="D2" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -5772,13 +5864,13 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="C3" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="D3" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -5821,10 +5913,10 @@
         <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="D1" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:4">

</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-08-05 09:51:37
</commit_message>
<xml_diff>
--- a/data/Solar_Lab_Tests.xlsx
+++ b/data/Solar_Lab_Tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1019" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{777F9C62-EA83-4CF6-9EB0-BB90F9106BD6}"/>
+  <xr:revisionPtr revIDLastSave="1040" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4EC021B-2ADA-4CF0-95A1-96575AC24655}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="1" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="7" activeTab="1" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Tests Map" sheetId="4" state="hidden" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="155">
   <si>
     <t>BOM</t>
   </si>
@@ -279,7 +279,7 @@
     <t>QC Vietnam</t>
   </si>
   <si>
-    <t>. QC 30A LINE T</t>
+    <t>QC 30A LINE TRIAL</t>
   </si>
   <si>
     <t>ZERUN</t>
@@ -529,6 +529,9 @@
   </si>
   <si>
     <t>255MV</t>
+  </si>
+  <si>
+    <t>QC SOLAR LINE</t>
   </si>
   <si>
     <t>STANDARD DURATION (DAYS)</t>
@@ -841,7 +844,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -919,7 +922,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1408,8 +1410,8 @@
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{5C370BE7-C0F8-462F-9F89-5FC458087319}" name="Table16" displayName="Table16" ref="A1:G18" totalsRowShown="0">
-  <autoFilter ref="A1:G18" xr:uid="{5C370BE7-C0F8-462F-9F89-5FC458087319}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{5C370BE7-C0F8-462F-9F89-5FC458087319}" name="Table16" displayName="Table16" ref="A1:G19" totalsRowShown="0">
+  <autoFilter ref="A1:G19" xr:uid="{5C370BE7-C0F8-462F-9F89-5FC458087319}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{59EA2429-768A-457D-88E6-B34A083DE755}" name="BOM"/>
     <tableColumn id="2" xr3:uid="{C09F236B-325A-4EF9-B484-B1D592C83B7F}" name="VENDOR NAME"/>
@@ -2079,10 +2081,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{333C0630-51CF-46CA-8CAD-98FEF9AC181F}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2343,6 +2345,14 @@
       </c>
       <c r="E18">
         <v>275</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -2377,7 +2387,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2505,8 +2515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9401EE47-EA52-49C7-BBC0-21F5B88254FB}">
   <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B11" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -3137,6 +3147,9 @@
         <v>55</v>
       </c>
       <c r="D29" s="48"/>
+      <c r="E29" s="4">
+        <v>45873</v>
+      </c>
       <c r="H29" t="s">
         <v>31</v>
       </c>
@@ -3186,7 +3199,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="2:8">
       <c r="B33" t="s">
         <v>16</v>
       </c>
@@ -3201,7 +3214,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="2:8">
       <c r="B34" t="s">
         <v>16</v>
       </c>
@@ -3216,7 +3229,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="2:8">
       <c r="B35" t="s">
         <v>16</v>
       </c>
@@ -3231,7 +3244,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="2:8">
       <c r="B36" t="s">
         <v>16</v>
       </c>
@@ -3246,7 +3259,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="2:8">
       <c r="B37" t="s">
         <v>4</v>
       </c>
@@ -3261,7 +3274,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="15">
+    <row r="38" spans="2:8" ht="15">
       <c r="B38" t="s">
         <v>5</v>
       </c>
@@ -3276,7 +3289,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="15">
+    <row r="39" spans="2:8" ht="15">
       <c r="B39" t="s">
         <v>6</v>
       </c>
@@ -3291,7 +3304,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="15">
+    <row r="40" spans="2:8" ht="15">
       <c r="B40" t="s">
         <v>7</v>
       </c>
@@ -3306,7 +3319,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="15">
+    <row r="41" spans="2:8" ht="15">
       <c r="B41" t="s">
         <v>3</v>
       </c>
@@ -3321,7 +3334,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="2:8">
       <c r="B42" t="s">
         <v>4</v>
       </c>
@@ -3336,7 +3349,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="2:8">
       <c r="B43" t="s">
         <v>18</v>
       </c>
@@ -3344,11 +3357,14 @@
         <v>64</v>
       </c>
       <c r="D43" s="48"/>
+      <c r="E43" s="4">
+        <v>45873</v>
+      </c>
       <c r="H43" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8">
       <c r="B44" t="s">
         <v>18</v>
       </c>
@@ -3356,11 +3372,14 @@
         <v>58</v>
       </c>
       <c r="D44" s="48"/>
+      <c r="E44" s="4">
+        <v>45873</v>
+      </c>
       <c r="H44" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8">
       <c r="B45" t="s">
         <v>18</v>
       </c>
@@ -3372,116 +3391,100 @@
         <v>31</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="15">
-      <c r="A46" s="49"/>
-      <c r="B46" s="49" t="s">
+    <row r="46" spans="2:8" ht="15">
+      <c r="B46" t="s">
         <v>18</v>
       </c>
       <c r="C46" t="s">
         <v>65</v>
       </c>
       <c r="D46" s="48"/>
-      <c r="E46" s="49"/>
-      <c r="F46" s="49"/>
-      <c r="G46" s="49"/>
       <c r="H46" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="15">
-      <c r="A47" s="49"/>
-      <c r="B47" s="49" t="s">
+    <row r="47" spans="2:8" ht="15">
+      <c r="B47" t="s">
         <v>18</v>
       </c>
       <c r="C47" t="s">
         <v>66</v>
       </c>
       <c r="D47" s="48"/>
-      <c r="E47" s="49"/>
-      <c r="F47" s="49"/>
-      <c r="G47" s="49"/>
+      <c r="E47" s="4">
+        <v>45873</v>
+      </c>
       <c r="H47" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" ht="15">
-      <c r="A48" s="49"/>
-      <c r="B48" s="49" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" ht="15">
+      <c r="B48" t="s">
         <v>18</v>
       </c>
       <c r="C48" t="s">
         <v>67</v>
       </c>
       <c r="D48" s="48"/>
-      <c r="E48" s="49"/>
-      <c r="F48" s="49"/>
-      <c r="G48" s="49"/>
       <c r="H48" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="15">
-      <c r="A49" s="49"/>
-      <c r="B49" s="49" t="s">
+    <row r="49" spans="2:8" ht="15">
+      <c r="B49" t="s">
         <v>18</v>
       </c>
       <c r="C49" t="s">
         <v>68</v>
       </c>
       <c r="D49" s="48"/>
-      <c r="E49" s="49"/>
-      <c r="F49" s="49"/>
-      <c r="G49" s="49"/>
+      <c r="E49" s="4">
+        <v>45873</v>
+      </c>
       <c r="H49" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" ht="15">
-      <c r="A50" s="49"/>
-      <c r="B50" s="49" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" ht="15">
+      <c r="B50" t="s">
         <v>18</v>
       </c>
       <c r="C50" t="s">
         <v>69</v>
       </c>
       <c r="D50" s="48"/>
-      <c r="E50" s="49"/>
-      <c r="F50" s="49"/>
-      <c r="G50" s="49"/>
+      <c r="E50" s="4">
+        <v>45873</v>
+      </c>
       <c r="H50" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8">
-      <c r="A51" s="49"/>
-      <c r="B51" s="49" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8">
+      <c r="B51" t="s">
         <v>18</v>
       </c>
-      <c r="C51" s="49" t="s">
+      <c r="C51" t="s">
         <v>70</v>
       </c>
       <c r="D51" s="48"/>
-      <c r="E51" s="49"/>
-      <c r="F51" s="49"/>
-      <c r="G51" s="49"/>
+      <c r="E51" s="4">
+        <v>45873</v>
+      </c>
       <c r="H51" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8">
-      <c r="A52" s="49"/>
-      <c r="B52" s="49" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8">
+      <c r="B52" t="s">
         <v>18</v>
       </c>
-      <c r="C52" s="49" t="s">
+      <c r="C52" t="s">
         <v>71</v>
       </c>
       <c r="D52" s="48"/>
-      <c r="E52" s="49"/>
-      <c r="F52" s="49"/>
-      <c r="G52" s="49"/>
       <c r="H52" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -5647,7 +5650,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5820,7 +5823,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-08-06 16:55:51
</commit_message>
<xml_diff>
--- a/data/Solar_Lab_Tests.xlsx
+++ b/data/Solar_Lab_Tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1040" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4EC021B-2ADA-4CF0-95A1-96575AC24655}"/>
+  <xr:revisionPtr revIDLastSave="1043" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{66CA844C-6C2B-4C82-AB04-8BC68CAEFB25}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="7" activeTab="1" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="5" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Tests Map" sheetId="4" state="hidden" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="155">
   <si>
     <t>BOM</t>
   </si>
@@ -1340,8 +1340,8 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{9AF05D4E-990A-4C94-8850-9D7BC3D120A4}" name="Table14" displayName="Table14" ref="A1:D4" totalsRowShown="0">
-  <autoFilter ref="A1:D4" xr:uid="{9AF05D4E-990A-4C94-8850-9D7BC3D120A4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{9AF05D4E-990A-4C94-8850-9D7BC3D120A4}" name="Table14" displayName="Table14" ref="A1:D7" totalsRowShown="0">
+  <autoFilter ref="A1:D7" xr:uid="{9AF05D4E-990A-4C94-8850-9D7BC3D120A4}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{695E2580-F157-4DF3-A6A1-0C66057F77F2}" name="BOM"/>
     <tableColumn id="2" xr3:uid="{93E753E6-35FE-4C78-817F-5319A79D1951}" name="VENDOR NAME"/>
@@ -2515,7 +2515,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9401EE47-EA52-49C7-BBC0-21F5B88254FB}">
   <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+    <sheetView topLeftCell="A38" workbookViewId="0">
       <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
@@ -5647,10 +5647,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C8152F1-3340-4C7F-9B6C-3F6BB96763BA}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5705,6 +5705,21 @@
       </c>
       <c r="B4" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-08-07 09:50:44
</commit_message>
<xml_diff>
--- a/data/Solar_Lab_Tests.xlsx
+++ b/data/Solar_Lab_Tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1043" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{66CA844C-6C2B-4C82-AB04-8BC68CAEFB25}"/>
+  <xr:revisionPtr revIDLastSave="1141" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2EC211B5-18F2-4220-B869-8F2698DFB4E9}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="5" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="5" activeTab="1" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Tests Map" sheetId="4" state="hidden" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <definedName name="ENCAPTYPE">Ref!$K$2:$K$1048576</definedName>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">'Material Tests Map'!$A$1:$B$20</definedName>
     <definedName name="ExternalData_1" localSheetId="11" hidden="1">'Standard test times'!$A$1:$B$15</definedName>
-    <definedName name="ExternalData_1" localSheetId="1" hidden="1">'Test Data'!$A$1:$H$52</definedName>
+    <definedName name="ExternalData_1" localSheetId="1" hidden="1">'Test Data'!$A$1:$H$58</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="169">
   <si>
     <t>BOM</t>
   </si>
@@ -288,6 +288,15 @@
     <t>LINE  EPE/EVA</t>
   </si>
   <si>
+    <t>CYBRIGHT /CYMAX</t>
+  </si>
+  <si>
+    <t>CYBRID/ RAYBO</t>
+  </si>
+  <si>
+    <t>PRODUCTION FIRST</t>
+  </si>
+  <si>
     <t>RM Type</t>
   </si>
   <si>
@@ -390,10 +399,43 @@
     <t xml:space="preserve">                                                         BACKSHEET to ENCAPSULANT</t>
   </si>
   <si>
+    <t>RAYBO</t>
+  </si>
+  <si>
+    <t>FIRST PRODUCTION</t>
+  </si>
+  <si>
     <t>BREAK</t>
   </si>
   <si>
     <t>CHANGE IN ELONGATION %</t>
+  </si>
+  <si>
+    <t>BBETTER EPE</t>
+  </si>
+  <si>
+    <t>VISHAKHA EPE</t>
+  </si>
+  <si>
+    <t>CYBRIGHT EPE</t>
+  </si>
+  <si>
+    <t>FIRST PRO EPE</t>
+  </si>
+  <si>
+    <t>BBETTER EVA</t>
+  </si>
+  <si>
+    <t>VISHAKHA EVA</t>
+  </si>
+  <si>
+    <t>CYBRIGHT EVA</t>
+  </si>
+  <si>
+    <t>RAYBO EVA</t>
+  </si>
+  <si>
+    <t>FIRST PRO EVA</t>
   </si>
   <si>
     <t>Type</t>
@@ -844,7 +886,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -922,6 +964,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1340,8 +1383,8 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{9AF05D4E-990A-4C94-8850-9D7BC3D120A4}" name="Table14" displayName="Table14" ref="A1:D7" totalsRowShown="0">
-  <autoFilter ref="A1:D7" xr:uid="{9AF05D4E-990A-4C94-8850-9D7BC3D120A4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{9AF05D4E-990A-4C94-8850-9D7BC3D120A4}" name="Table14" displayName="Table14" ref="A1:D12" totalsRowShown="0">
+  <autoFilter ref="A1:D12" xr:uid="{9AF05D4E-990A-4C94-8850-9D7BC3D120A4}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{695E2580-F157-4DF3-A6A1-0C66057F77F2}" name="BOM"/>
     <tableColumn id="2" xr3:uid="{93E753E6-35FE-4C78-817F-5319A79D1951}" name="VENDOR NAME"/>
@@ -1437,7 +1480,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{06A3AD80-C098-4015-85FF-3495CE4443EA}" name="Test_Data" displayName="Test_Data" ref="A1:H52" tableType="queryTable" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{06A3AD80-C098-4015-85FF-3495CE4443EA}" name="Test_Data" displayName="Test_Data" ref="A1:H58" tableType="queryTable" totalsRowShown="0">
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{87F75B08-44C4-4718-834D-87FEE9F87970}" uniqueName="1" name="BOM" queryTableFieldId="1" dataDxfId="42"/>
     <tableColumn id="2" xr3:uid="{1E5F4521-5E5C-4948-AEB2-FC5F712DB353}" uniqueName="2" name="TEST NAME" queryTableFieldId="2" dataDxfId="41"/>
@@ -2056,10 +2099,10 @@
         <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>127</v>
+        <v>141</v>
       </c>
       <c r="D1" t="s">
-        <v>128</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -2106,19 +2149,19 @@
         <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
       <c r="D1" t="s">
-        <v>130</v>
+        <v>144</v>
       </c>
       <c r="E1" t="s">
-        <v>131</v>
+        <v>145</v>
       </c>
       <c r="F1" t="s">
-        <v>132</v>
+        <v>146</v>
       </c>
       <c r="G1" t="s">
-        <v>133</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -2126,10 +2169,10 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>134</v>
+        <v>148</v>
       </c>
       <c r="D2" t="s">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="E2">
         <v>331</v>
@@ -2140,7 +2183,7 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>136</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2148,10 +2191,10 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>137</v>
+        <v>151</v>
       </c>
       <c r="D4" t="s">
-        <v>138</v>
+        <v>152</v>
       </c>
       <c r="E4">
         <v>176</v>
@@ -2165,7 +2208,7 @@
         <v>46</v>
       </c>
       <c r="D5" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="E5">
         <v>249</v>
@@ -2176,10 +2219,10 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>140</v>
+        <v>154</v>
       </c>
       <c r="D6" t="s">
-        <v>141</v>
+        <v>155</v>
       </c>
       <c r="E6">
         <v>197</v>
@@ -2193,7 +2236,7 @@
         <v>48</v>
       </c>
       <c r="D7" t="s">
-        <v>142</v>
+        <v>156</v>
       </c>
       <c r="E7">
         <v>277</v>
@@ -2207,7 +2250,7 @@
         <v>68</v>
       </c>
       <c r="D8" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
       <c r="E8">
         <v>237</v>
@@ -2221,7 +2264,7 @@
         <v>60</v>
       </c>
       <c r="D9" t="s">
-        <v>144</v>
+        <v>158</v>
       </c>
       <c r="E9">
         <v>325</v>
@@ -2235,7 +2278,7 @@
         <v>59</v>
       </c>
       <c r="D10" t="s">
-        <v>141</v>
+        <v>155</v>
       </c>
       <c r="E10">
         <v>155</v>
@@ -2249,7 +2292,7 @@
         <v>57</v>
       </c>
       <c r="D11" t="s">
-        <v>138</v>
+        <v>152</v>
       </c>
       <c r="E11">
         <v>178</v>
@@ -2263,7 +2306,7 @@
         <v>46</v>
       </c>
       <c r="D12" t="s">
-        <v>145</v>
+        <v>159</v>
       </c>
       <c r="E12">
         <v>227</v>
@@ -2274,7 +2317,7 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>146</v>
+        <v>160</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -2285,7 +2328,7 @@
         <v>56</v>
       </c>
       <c r="D14" t="s">
-        <v>147</v>
+        <v>161</v>
       </c>
       <c r="E14">
         <v>357</v>
@@ -2296,10 +2339,10 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>148</v>
+        <v>162</v>
       </c>
       <c r="D15" t="s">
-        <v>149</v>
+        <v>163</v>
       </c>
       <c r="E15">
         <v>158</v>
@@ -2313,7 +2356,7 @@
         <v>52</v>
       </c>
       <c r="D16" t="s">
-        <v>150</v>
+        <v>164</v>
       </c>
       <c r="E16">
         <v>314</v>
@@ -2327,7 +2370,7 @@
         <v>51</v>
       </c>
       <c r="D17" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="E17">
         <v>162</v>
@@ -2341,7 +2384,7 @@
         <v>49</v>
       </c>
       <c r="D18" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="E18">
         <v>275</v>
@@ -2352,7 +2395,7 @@
         <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>153</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -2387,7 +2430,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>154</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2513,10 +2556,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9401EE47-EA52-49C7-BBC0-21F5B88254FB}">
-  <dimension ref="A1:K52"/>
+  <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -2924,7 +2967,9 @@
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="1"/>
+      <c r="A17" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="B17" t="s">
         <v>18</v>
       </c>
@@ -2941,7 +2986,9 @@
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="1"/>
+      <c r="A18" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B18" t="s">
         <v>18</v>
       </c>
@@ -2958,7 +3005,9 @@
       </c>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="1"/>
+      <c r="A19" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B19" t="s">
         <v>18</v>
       </c>
@@ -2975,7 +3024,9 @@
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="1"/>
+      <c r="A20" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B20" t="s">
         <v>16</v>
       </c>
@@ -2994,7 +3045,9 @@
       </c>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="1"/>
+      <c r="A21" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B21" t="s">
         <v>16</v>
       </c>
@@ -3013,7 +3066,9 @@
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="1"/>
+      <c r="A22" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B22" t="s">
         <v>16</v>
       </c>
@@ -3032,7 +3087,9 @@
       </c>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="1"/>
+      <c r="A23" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B23" t="s">
         <v>16</v>
       </c>
@@ -3051,7 +3108,9 @@
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="1"/>
+      <c r="A24" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B24" t="s">
         <v>16</v>
       </c>
@@ -3070,7 +3129,9 @@
       </c>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="1"/>
+      <c r="A25" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B25" t="s">
         <v>16</v>
       </c>
@@ -3089,6 +3150,9 @@
       </c>
     </row>
     <row r="26" spans="1:8">
+      <c r="A26" t="s">
+        <v>15</v>
+      </c>
       <c r="B26" t="s">
         <v>16</v>
       </c>
@@ -3107,6 +3171,9 @@
       </c>
     </row>
     <row r="27" spans="1:8">
+      <c r="A27" t="s">
+        <v>15</v>
+      </c>
       <c r="B27" t="s">
         <v>16</v>
       </c>
@@ -3125,6 +3192,9 @@
       </c>
     </row>
     <row r="28" spans="1:8">
+      <c r="A28" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="B28" t="s">
         <v>5</v>
       </c>
@@ -3140,6 +3210,9 @@
       </c>
     </row>
     <row r="29" spans="1:8">
+      <c r="A29" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="B29" t="s">
         <v>3</v>
       </c>
@@ -3155,6 +3228,9 @@
       </c>
     </row>
     <row r="30" spans="1:8">
+      <c r="A30" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B30" t="s">
         <v>16</v>
       </c>
@@ -3170,6 +3246,9 @@
       </c>
     </row>
     <row r="31" spans="1:8">
+      <c r="A31" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B31" t="s">
         <v>16</v>
       </c>
@@ -3185,6 +3264,9 @@
       </c>
     </row>
     <row r="32" spans="1:8">
+      <c r="A32" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B32" t="s">
         <v>16</v>
       </c>
@@ -3199,7 +3281,10 @@
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="2:8">
+    <row r="33" spans="1:8">
+      <c r="A33" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B33" t="s">
         <v>16</v>
       </c>
@@ -3214,7 +3299,10 @@
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="2:8">
+    <row r="34" spans="1:8">
+      <c r="A34" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B34" t="s">
         <v>16</v>
       </c>
@@ -3229,7 +3317,10 @@
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="2:8">
+    <row r="35" spans="1:8">
+      <c r="A35" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B35" t="s">
         <v>16</v>
       </c>
@@ -3244,7 +3335,10 @@
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="2:8">
+    <row r="36" spans="1:8">
+      <c r="A36" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B36" t="s">
         <v>16</v>
       </c>
@@ -3259,7 +3353,10 @@
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="2:8">
+    <row r="37" spans="1:8">
+      <c r="A37" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="B37" t="s">
         <v>4</v>
       </c>
@@ -3274,7 +3371,10 @@
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="2:8" ht="15">
+    <row r="38" spans="1:8" ht="15">
+      <c r="A38" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="B38" t="s">
         <v>5</v>
       </c>
@@ -3289,7 +3389,10 @@
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="2:8" ht="15">
+    <row r="39" spans="1:8" ht="15">
+      <c r="A39" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="B39" t="s">
         <v>6</v>
       </c>
@@ -3304,7 +3407,10 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="2:8" ht="15">
+    <row r="40" spans="1:8" ht="15">
+      <c r="A40" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="B40" t="s">
         <v>7</v>
       </c>
@@ -3319,7 +3425,10 @@
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="2:8" ht="15">
+    <row r="41" spans="1:8" ht="15">
+      <c r="A41" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="B41" t="s">
         <v>3</v>
       </c>
@@ -3334,7 +3443,10 @@
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="2:8">
+    <row r="42" spans="1:8">
+      <c r="A42" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="B42" t="s">
         <v>4</v>
       </c>
@@ -3349,7 +3461,10 @@
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="2:8">
+    <row r="43" spans="1:8">
+      <c r="A43" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="B43" t="s">
         <v>18</v>
       </c>
@@ -3364,7 +3479,10 @@
         <v>38</v>
       </c>
     </row>
-    <row r="44" spans="2:8">
+    <row r="44" spans="1:8">
+      <c r="A44" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B44" t="s">
         <v>18</v>
       </c>
@@ -3379,7 +3497,10 @@
         <v>38</v>
       </c>
     </row>
-    <row r="45" spans="2:8">
+    <row r="45" spans="1:8">
+      <c r="A45" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B45" t="s">
         <v>18</v>
       </c>
@@ -3391,7 +3512,10 @@
         <v>31</v>
       </c>
     </row>
-    <row r="46" spans="2:8" ht="15">
+    <row r="46" spans="1:8" ht="15">
+      <c r="A46" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="B46" t="s">
         <v>18</v>
       </c>
@@ -3403,7 +3527,10 @@
         <v>31</v>
       </c>
     </row>
-    <row r="47" spans="2:8" ht="15">
+    <row r="47" spans="1:8" ht="15">
+      <c r="A47" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="B47" t="s">
         <v>18</v>
       </c>
@@ -3418,7 +3545,10 @@
         <v>38</v>
       </c>
     </row>
-    <row r="48" spans="2:8" ht="15">
+    <row r="48" spans="1:8" ht="15">
+      <c r="A48" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="B48" t="s">
         <v>18</v>
       </c>
@@ -3430,7 +3560,10 @@
         <v>31</v>
       </c>
     </row>
-    <row r="49" spans="2:8" ht="15">
+    <row r="49" spans="1:8" ht="15">
+      <c r="A49" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B49" t="s">
         <v>18</v>
       </c>
@@ -3445,7 +3578,10 @@
         <v>38</v>
       </c>
     </row>
-    <row r="50" spans="2:8" ht="15">
+    <row r="50" spans="1:8" ht="15">
+      <c r="A50" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B50" t="s">
         <v>18</v>
       </c>
@@ -3460,7 +3596,10 @@
         <v>38</v>
       </c>
     </row>
-    <row r="51" spans="2:8">
+    <row r="51" spans="1:8">
+      <c r="A51" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B51" t="s">
         <v>18</v>
       </c>
@@ -3475,7 +3614,10 @@
         <v>38</v>
       </c>
     </row>
-    <row r="52" spans="2:8">
+    <row r="52" spans="1:8">
+      <c r="A52" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="B52" t="s">
         <v>18</v>
       </c>
@@ -3483,9 +3625,114 @@
         <v>71</v>
       </c>
       <c r="D52" s="48"/>
+      <c r="E52" s="4">
+        <v>45875</v>
+      </c>
       <c r="H52" t="s">
         <v>38</v>
       </c>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B53" s="49" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" s="49" t="s">
+        <v>72</v>
+      </c>
+      <c r="D53" s="48"/>
+      <c r="E53" s="4">
+        <v>45875</v>
+      </c>
+      <c r="F53" s="49"/>
+      <c r="G53" s="49"/>
+      <c r="H53" s="49"/>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B54" s="49" t="s">
+        <v>5</v>
+      </c>
+      <c r="C54" s="49" t="s">
+        <v>73</v>
+      </c>
+      <c r="D54" s="48"/>
+      <c r="E54" s="4">
+        <v>45875</v>
+      </c>
+      <c r="F54" s="49"/>
+      <c r="G54" s="49"/>
+      <c r="H54" s="49"/>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B55" s="49" t="s">
+        <v>5</v>
+      </c>
+      <c r="C55" s="49" t="s">
+        <v>74</v>
+      </c>
+      <c r="D55" s="48"/>
+      <c r="E55" s="4">
+        <v>45875</v>
+      </c>
+      <c r="F55" s="49"/>
+      <c r="G55" s="49"/>
+      <c r="H55" s="49"/>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="A56" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="B56" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="C56" s="49" t="s">
+        <v>72</v>
+      </c>
+      <c r="D56" s="48"/>
+      <c r="E56" s="49"/>
+      <c r="F56" s="49"/>
+      <c r="G56" s="49"/>
+      <c r="H56" s="49"/>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="B57" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="C57" s="49" t="s">
+        <v>73</v>
+      </c>
+      <c r="D57" s="48"/>
+      <c r="E57" s="49"/>
+      <c r="F57" s="49"/>
+      <c r="G57" s="49"/>
+      <c r="H57" s="49"/>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="A58" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="B58" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="C58" s="49" t="s">
+        <v>74</v>
+      </c>
+      <c r="D58" s="48"/>
+      <c r="E58" s="49"/>
+      <c r="F58" s="49"/>
+      <c r="G58" s="49"/>
+      <c r="H58" s="49"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -3550,25 +3797,25 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="E1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="G1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="K1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="N1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -3585,10 +3832,10 @@
         <v>32</v>
       </c>
       <c r="K2" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="N2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -3605,10 +3852,10 @@
         <v>38</v>
       </c>
       <c r="K3" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="N3" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -3619,10 +3866,10 @@
         <v>5</v>
       </c>
       <c r="G4" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="I4" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -3733,19 +3980,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>24</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="E1" s="16"/>
       <c r="F1" s="16"/>
       <c r="G1" s="16"/>
       <c r="H1" s="17" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="I1" s="18"/>
       <c r="J1" s="18"/>
@@ -3756,61 +4003,61 @@
       <c r="B2" s="20"/>
       <c r="C2" s="20"/>
       <c r="D2" s="21" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="F2" s="22" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="G2" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="H2" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="H2" s="23" t="s">
-        <v>87</v>
-      </c>
       <c r="I2" s="24" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="J2" s="24" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="K2" s="25" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:11" hidden="1">
       <c r="A3" s="46"/>
       <c r="B3" s="26" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="F3" s="26" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="G3" s="26" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="H3" s="26" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="I3" s="26" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="J3" s="26" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="K3" s="26" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -3818,7 +4065,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C4" t="s">
         <v>35</v>
@@ -3853,7 +4100,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C5" t="s">
         <v>35</v>
@@ -3888,10 +4135,10 @@
         <v>2</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -3899,7 +4146,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="27" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -5469,10 +5716,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E993B7F-E878-4ABA-95AD-A4138848D6EF}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5494,14 +5741,14 @@
       <c r="A1" s="28"/>
       <c r="B1" s="29"/>
       <c r="C1" s="30" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D1" s="31"/>
       <c r="E1" s="30"/>
       <c r="F1" s="31"/>
       <c r="G1" s="32"/>
       <c r="H1" s="44" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="I1" s="32"/>
       <c r="J1" s="29"/>
@@ -5514,19 +5761,19 @@
         <v>24</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="D2" s="36"/>
       <c r="E2" s="37" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F2" s="38"/>
       <c r="G2" s="35" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="37" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="J2" s="38"/>
     </row>
@@ -5564,34 +5811,34 @@
     </row>
     <row r="4" spans="1:10" customFormat="1" hidden="1">
       <c r="A4" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B4" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C4" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="E4" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="F4" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="G4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="H4" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="I4" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="J4" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -5619,7 +5866,59 @@
         <v>2</v>
       </c>
       <c r="B6" s="45" t="s">
-        <v>101</v>
+        <v>104</v>
+      </c>
+      <c r="C6" s="45">
+        <v>125</v>
+      </c>
+      <c r="D6" s="45">
+        <v>110</v>
+      </c>
+      <c r="E6" s="45">
+        <v>126</v>
+      </c>
+      <c r="F6" s="45">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="45" t="s">
+        <v>109</v>
+      </c>
+      <c r="C7" s="45">
+        <v>125</v>
+      </c>
+      <c r="D7" s="45">
+        <v>115</v>
+      </c>
+      <c r="E7" s="45">
+        <v>60</v>
+      </c>
+      <c r="F7" s="45">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="45" t="s">
+        <v>110</v>
+      </c>
+      <c r="C8" s="45">
+        <v>166</v>
+      </c>
+      <c r="D8" s="45">
+        <v>152</v>
+      </c>
+      <c r="E8" s="45">
+        <v>65</v>
+      </c>
+      <c r="F8" s="45">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -5637,7 +5936,7 @@
           <x14:formula1>
             <xm:f>Ref!$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>A3:A6</xm:sqref>
+          <xm:sqref>A3:A8</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5647,10 +5946,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C8152F1-3340-4C7F-9B6C-3F6BB96763BA}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5669,10 +5968,10 @@
         <v>24</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="6" customFormat="1">
@@ -5696,7 +5995,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -5704,27 +6003,76 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>2</v>
       </c>
+      <c r="B5" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>2</v>
       </c>
+      <c r="B6" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>2</v>
       </c>
+      <c r="B7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>121</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B3 D2:D3 D5:D1048576" xr:uid="{FCBF55FC-869D-43C4-B484-27D4BFDDD5A4}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B3 D2:D3 D5:D1048576 B8" xr:uid="{FCBF55FC-869D-43C4-B484-27D4BFDDD5A4}"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576" xr:uid="{04F856B6-1846-4FF1-B3BB-4FE58494E678}">
       <formula1>"ENCAPSULANT, RIBBON"</formula1>
     </dataValidation>
@@ -5764,25 +6112,25 @@
         <v>24</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>109</v>
+        <v>123</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>110</v>
+        <v>124</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>112</v>
+        <v>126</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>113</v>
+        <v>127</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -5790,7 +6138,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
@@ -5801,7 +6149,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>116</v>
+        <v>130</v>
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
@@ -5851,16 +6199,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>117</v>
+        <v>131</v>
       </c>
       <c r="B1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C1" t="s">
         <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>118</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -5868,13 +6216,13 @@
         <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="C2" t="s">
-        <v>120</v>
+        <v>134</v>
       </c>
       <c r="D2" t="s">
-        <v>121</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -5882,13 +6230,13 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
       <c r="C3" t="s">
-        <v>123</v>
+        <v>137</v>
       </c>
       <c r="D3" t="s">
-        <v>124</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -5931,10 +6279,10 @@
         <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>125</v>
+        <v>139</v>
       </c>
       <c r="D1" t="s">
-        <v>126</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:4">

</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-08-08 09:50:37
</commit_message>
<xml_diff>
--- a/data/Solar_Lab_Tests.xlsx
+++ b/data/Solar_Lab_Tests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29203"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1141" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2EC211B5-18F2-4220-B869-8F2698DFB4E9}"/>
+  <xr:revisionPtr revIDLastSave="1163" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A257CC2C-9DFD-4F7F-A42C-BB238FE5993D}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="5" activeTab="1" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="5" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Tests Map" sheetId="4" state="hidden" r:id="rId1"/>
@@ -886,7 +886,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -964,7 +964,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2558,8 +2557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9401EE47-EA52-49C7-BBC0-21F5B88254FB}">
   <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58"/>
+    <sheetView topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -2834,7 +2833,9 @@
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
+      <c r="F11" s="4">
+        <v>45875</v>
+      </c>
       <c r="H11" t="s">
         <v>38</v>
       </c>
@@ -2980,7 +2981,9 @@
       <c r="E17" s="4">
         <v>45869</v>
       </c>
-      <c r="F17" s="4"/>
+      <c r="F17" s="4">
+        <v>45875</v>
+      </c>
       <c r="H17" t="s">
         <v>38</v>
       </c>
@@ -2999,7 +3002,9 @@
       <c r="E18" s="4">
         <v>45869</v>
       </c>
-      <c r="F18" s="4"/>
+      <c r="F18" s="4">
+        <v>45875</v>
+      </c>
       <c r="H18" t="s">
         <v>38</v>
       </c>
@@ -3018,7 +3023,9 @@
       <c r="E19" s="4">
         <v>45869</v>
       </c>
-      <c r="F19" s="4"/>
+      <c r="F19" s="4">
+        <v>45875</v>
+      </c>
       <c r="H19" t="s">
         <v>38</v>
       </c>
@@ -3224,7 +3231,7 @@
         <v>45873</v>
       </c>
       <c r="H29" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -3239,6 +3246,9 @@
       </c>
       <c r="D30" s="48"/>
       <c r="E30" s="4">
+        <v>45855</v>
+      </c>
+      <c r="F30" s="4">
         <v>45861</v>
       </c>
       <c r="H30" t="s">
@@ -3259,6 +3269,9 @@
       <c r="E31" s="4">
         <v>45861</v>
       </c>
+      <c r="F31" s="4">
+        <v>45866</v>
+      </c>
       <c r="H31" t="s">
         <v>38</v>
       </c>
@@ -3277,6 +3290,9 @@
       <c r="E32" s="4">
         <v>45861</v>
       </c>
+      <c r="F32" s="4">
+        <v>45866</v>
+      </c>
       <c r="H32" t="s">
         <v>38</v>
       </c>
@@ -3295,6 +3311,9 @@
       <c r="E33" s="4">
         <v>45861</v>
       </c>
+      <c r="F33" s="4">
+        <v>45866</v>
+      </c>
       <c r="H33" t="s">
         <v>38</v>
       </c>
@@ -3313,6 +3332,9 @@
       <c r="E34" s="4">
         <v>45861</v>
       </c>
+      <c r="F34" s="4">
+        <v>45866</v>
+      </c>
       <c r="H34" t="s">
         <v>38</v>
       </c>
@@ -3331,6 +3353,9 @@
       <c r="E35" s="4">
         <v>45861</v>
       </c>
+      <c r="F35" s="4">
+        <v>45866</v>
+      </c>
       <c r="H35" t="s">
         <v>38</v>
       </c>
@@ -3493,6 +3518,9 @@
       <c r="E44" s="4">
         <v>45873</v>
       </c>
+      <c r="F44" s="4">
+        <v>45875</v>
+      </c>
       <c r="H44" t="s">
         <v>38</v>
       </c>
@@ -3523,8 +3551,11 @@
         <v>65</v>
       </c>
       <c r="D46" s="48"/>
+      <c r="E46" s="4">
+        <v>45876</v>
+      </c>
       <c r="H46" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="15">
@@ -3541,6 +3572,9 @@
       <c r="E47" s="4">
         <v>45873</v>
       </c>
+      <c r="F47" s="4">
+        <v>45876</v>
+      </c>
       <c r="H47" t="s">
         <v>38</v>
       </c>
@@ -3556,8 +3590,11 @@
         <v>67</v>
       </c>
       <c r="D48" s="48"/>
+      <c r="E48" s="4">
+        <v>45876</v>
+      </c>
       <c r="H48" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="15">
@@ -3574,6 +3611,9 @@
       <c r="E49" s="4">
         <v>45873</v>
       </c>
+      <c r="F49" s="4">
+        <v>45876</v>
+      </c>
       <c r="H49" t="s">
         <v>38</v>
       </c>
@@ -3592,6 +3632,9 @@
       <c r="E50" s="4">
         <v>45873</v>
       </c>
+      <c r="F50" s="4">
+        <v>45876</v>
+      </c>
       <c r="H50" t="s">
         <v>38</v>
       </c>
@@ -3610,6 +3653,9 @@
       <c r="E51" s="4">
         <v>45873</v>
       </c>
+      <c r="F51" s="4">
+        <v>45875</v>
+      </c>
       <c r="H51" t="s">
         <v>38</v>
       </c>
@@ -3628,6 +3674,9 @@
       <c r="E52" s="4">
         <v>45875</v>
       </c>
+      <c r="F52" s="4">
+        <v>45876</v>
+      </c>
       <c r="H52" t="s">
         <v>38</v>
       </c>
@@ -3636,103 +3685,82 @@
       <c r="A53" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B53" s="49" t="s">
+      <c r="B53" t="s">
         <v>5</v>
       </c>
-      <c r="C53" s="49" t="s">
+      <c r="C53" t="s">
         <v>72</v>
       </c>
       <c r="D53" s="48"/>
       <c r="E53" s="4">
         <v>45875</v>
       </c>
-      <c r="F53" s="49"/>
-      <c r="G53" s="49"/>
-      <c r="H53" s="49"/>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B54" s="49" t="s">
+      <c r="B54" t="s">
         <v>5</v>
       </c>
-      <c r="C54" s="49" t="s">
+      <c r="C54" t="s">
         <v>73</v>
       </c>
       <c r="D54" s="48"/>
       <c r="E54" s="4">
         <v>45875</v>
       </c>
-      <c r="F54" s="49"/>
-      <c r="G54" s="49"/>
-      <c r="H54" s="49"/>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B55" s="49" t="s">
+      <c r="B55" t="s">
         <v>5</v>
       </c>
-      <c r="C55" s="49" t="s">
+      <c r="C55" t="s">
         <v>74</v>
       </c>
       <c r="D55" s="48"/>
       <c r="E55" s="4">
         <v>45875</v>
       </c>
-      <c r="F55" s="49"/>
-      <c r="G55" s="49"/>
-      <c r="H55" s="49"/>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="49" t="s">
-        <v>2</v>
-      </c>
-      <c r="B56" s="49" t="s">
+      <c r="A56" t="s">
+        <v>2</v>
+      </c>
+      <c r="B56" t="s">
         <v>6</v>
       </c>
-      <c r="C56" s="49" t="s">
+      <c r="C56" t="s">
         <v>72</v>
       </c>
       <c r="D56" s="48"/>
-      <c r="E56" s="49"/>
-      <c r="F56" s="49"/>
-      <c r="G56" s="49"/>
-      <c r="H56" s="49"/>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="49" t="s">
-        <v>2</v>
-      </c>
-      <c r="B57" s="49" t="s">
+      <c r="A57" t="s">
+        <v>2</v>
+      </c>
+      <c r="B57" t="s">
         <v>6</v>
       </c>
-      <c r="C57" s="49" t="s">
+      <c r="C57" t="s">
         <v>73</v>
       </c>
       <c r="D57" s="48"/>
-      <c r="E57" s="49"/>
-      <c r="F57" s="49"/>
-      <c r="G57" s="49"/>
-      <c r="H57" s="49"/>
     </row>
     <row r="58" spans="1:8">
-      <c r="A58" s="49" t="s">
-        <v>2</v>
-      </c>
-      <c r="B58" s="49" t="s">
+      <c r="A58" t="s">
+        <v>2</v>
+      </c>
+      <c r="B58" t="s">
         <v>6</v>
       </c>
-      <c r="C58" s="49" t="s">
+      <c r="C58" t="s">
         <v>74</v>
       </c>
       <c r="D58" s="48"/>
-      <c r="E58" s="49"/>
-      <c r="F58" s="49"/>
-      <c r="G58" s="49"/>
-      <c r="H58" s="49"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -5948,7 +5976,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C8152F1-3340-4C7F-9B6C-3F6BB96763BA}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-08-12 09:45:48
</commit_message>
<xml_diff>
--- a/data/Solar_Lab_Tests.xlsx
+++ b/data/Solar_Lab_Tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1163" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A257CC2C-9DFD-4F7F-A42C-BB238FE5993D}"/>
+  <xr:revisionPtr revIDLastSave="1169" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D3194080-63A6-4876-A60A-3AC786200D90}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="5" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="5" activeTab="5" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Tests Map" sheetId="4" state="hidden" r:id="rId1"/>
@@ -2558,7 +2558,7 @@
   <dimension ref="A1:K58"/>
   <sheetViews>
     <sheetView topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="F59" sqref="F59"/>
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -3230,6 +3230,9 @@
       <c r="E29" s="4">
         <v>45873</v>
       </c>
+      <c r="F29" s="4">
+        <v>45875</v>
+      </c>
       <c r="H29" t="s">
         <v>38</v>
       </c>
@@ -3545,7 +3548,7 @@
         <v>2</v>
       </c>
       <c r="B46" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="C46" t="s">
         <v>65</v>
@@ -3554,6 +3557,9 @@
       <c r="E46" s="4">
         <v>45876</v>
       </c>
+      <c r="F46" s="4">
+        <v>45878</v>
+      </c>
       <c r="H46" t="s">
         <v>38</v>
       </c>
@@ -3584,7 +3590,7 @@
         <v>2</v>
       </c>
       <c r="B48" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="C48" t="s">
         <v>67</v>
@@ -3593,6 +3599,9 @@
       <c r="E48" s="4">
         <v>45876</v>
       </c>
+      <c r="F48" s="4">
+        <v>45878</v>
+      </c>
       <c r="H48" t="s">
         <v>38</v>
       </c>
@@ -3665,7 +3674,7 @@
         <v>2</v>
       </c>
       <c r="B52" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="C52" t="s">
         <v>71</v>

</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-08-12 14:48:13
</commit_message>
<xml_diff>
--- a/data/Solar_Lab_Tests.xlsx
+++ b/data/Solar_Lab_Tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1169" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D3194080-63A6-4876-A60A-3AC786200D90}"/>
+  <xr:revisionPtr revIDLastSave="1217" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F5DB1D1-2C66-4E8A-B7B4-96BE1255A5DA}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="5" activeTab="5" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="10" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Tests Map" sheetId="4" state="hidden" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="173">
   <si>
     <t>BOM</t>
   </si>
@@ -261,165 +261,168 @@
     <t>VISHAKHA</t>
   </si>
   <si>
+    <t>RAYBO EPE/EVA</t>
+  </si>
+  <si>
+    <t>BARCODE X 50*15</t>
+  </si>
+  <si>
+    <t>VishakhaEPE /EVA</t>
+  </si>
+  <si>
+    <t>Wetown INTC</t>
+  </si>
+  <si>
+    <t>Cybrid Raybo EPE/EVA</t>
+  </si>
+  <si>
+    <t>QC Vietnam</t>
+  </si>
+  <si>
+    <t>QC 30A LINE TRIAL</t>
+  </si>
+  <si>
+    <t>ZERUN</t>
+  </si>
+  <si>
+    <t>LINE  EPE/EVA</t>
+  </si>
+  <si>
+    <t>CYBRIGHT /CYMAX</t>
+  </si>
+  <si>
+    <t>CYBRID/ RAYBO</t>
+  </si>
+  <si>
+    <t>PRODUCTION FIRST</t>
+  </si>
+  <si>
+    <t>RM Type</t>
+  </si>
+  <si>
+    <t>Test Type</t>
+  </si>
+  <si>
+    <t>Vendor Names</t>
+  </si>
+  <si>
+    <t>Test Results</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>ENCAPSULANT TYPE</t>
+  </si>
+  <si>
+    <t>TYPE</t>
+  </si>
+  <si>
+    <t>FRONT EPE</t>
+  </si>
+  <si>
+    <t>OLD : 420 to 480</t>
+  </si>
+  <si>
+    <t>BACK EVA</t>
+  </si>
+  <si>
+    <t>NEW: 380 to 440</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                                                              WITHOUT HEAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                                                     WITH HEAT </t>
+  </si>
+  <si>
+    <t>TD1</t>
+  </si>
+  <si>
+    <t>TD2</t>
+  </si>
+  <si>
+    <t>MD1</t>
+  </si>
+  <si>
+    <t>MD2</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Column2</t>
+  </si>
+  <si>
+    <t>Column3</t>
+  </si>
+  <si>
+    <t>Column4</t>
+  </si>
+  <si>
+    <t>Column5</t>
+  </si>
+  <si>
+    <t>Column6</t>
+  </si>
+  <si>
+    <t>Column7</t>
+  </si>
+  <si>
+    <t>Column8</t>
+  </si>
+  <si>
+    <t>Column9</t>
+  </si>
+  <si>
+    <t>Column10</t>
+  </si>
+  <si>
+    <t>VISHKHA</t>
+  </si>
+  <si>
+    <t>RAYBO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                                                                                           PRE PCT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                            POST PCT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                          GLASS to ENCAPSULANT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                         BACKSHEET to ENCAPSULANT</t>
+  </si>
+  <si>
+    <t>FIRST PRODUCTION</t>
+  </si>
+  <si>
+    <t>BREAK</t>
+  </si>
+  <si>
+    <t>CHANGE IN ELONGATION %</t>
+  </si>
+  <si>
+    <t>BBETTER EPE</t>
+  </si>
+  <si>
+    <t>VISHAKHA EPE</t>
+  </si>
+  <si>
+    <t>CYBRIGHT EPE</t>
+  </si>
+  <si>
     <t>RAYBO EPE</t>
   </si>
   <si>
-    <t>BARCODE X 50*15</t>
-  </si>
-  <si>
-    <t>VishakhaEPE /EVA</t>
-  </si>
-  <si>
-    <t>Wetown INTC</t>
-  </si>
-  <si>
-    <t>Cybrid Raybo EPE/EVA</t>
-  </si>
-  <si>
-    <t>QC Vietnam</t>
-  </si>
-  <si>
-    <t>QC 30A LINE TRIAL</t>
-  </si>
-  <si>
-    <t>ZERUN</t>
-  </si>
-  <si>
-    <t>LINE  EPE/EVA</t>
-  </si>
-  <si>
-    <t>CYBRIGHT /CYMAX</t>
-  </si>
-  <si>
-    <t>CYBRID/ RAYBO</t>
-  </si>
-  <si>
-    <t>PRODUCTION FIRST</t>
-  </si>
-  <si>
-    <t>RM Type</t>
-  </si>
-  <si>
-    <t>Test Type</t>
-  </si>
-  <si>
-    <t>Vendor Names</t>
-  </si>
-  <si>
-    <t>Test Results</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>ENCAPSULANT TYPE</t>
-  </si>
-  <si>
-    <t>TYPE</t>
-  </si>
-  <si>
-    <t>FRONT EPE</t>
-  </si>
-  <si>
-    <t>OLD : 420 to 480</t>
-  </si>
-  <si>
-    <t>BACK EVA</t>
-  </si>
-  <si>
-    <t>NEW: 380 to 440</t>
-  </si>
-  <si>
-    <t>Fail</t>
-  </si>
-  <si>
-    <t>Failed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                                                                                              WITHOUT HEAT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                                                                                     WITH HEAT </t>
-  </si>
-  <si>
-    <t>TD1</t>
-  </si>
-  <si>
-    <t>TD2</t>
-  </si>
-  <si>
-    <t>MD1</t>
-  </si>
-  <si>
-    <t>MD2</t>
-  </si>
-  <si>
-    <t>Column1</t>
-  </si>
-  <si>
-    <t>Column2</t>
-  </si>
-  <si>
-    <t>Column3</t>
-  </si>
-  <si>
-    <t>Column4</t>
-  </si>
-  <si>
-    <t>Column5</t>
-  </si>
-  <si>
-    <t>Column6</t>
-  </si>
-  <si>
-    <t>Column7</t>
-  </si>
-  <si>
-    <t>Column8</t>
-  </si>
-  <si>
-    <t>Column9</t>
-  </si>
-  <si>
-    <t>Column10</t>
-  </si>
-  <si>
-    <t>VISHKHA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                                                                                                                           PRE PCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                            POST PCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                                                          GLASS to ENCAPSULANT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                                                         BACKSHEET to ENCAPSULANT</t>
-  </si>
-  <si>
-    <t>RAYBO</t>
-  </si>
-  <si>
-    <t>FIRST PRODUCTION</t>
-  </si>
-  <si>
-    <t>BREAK</t>
-  </si>
-  <si>
-    <t>CHANGE IN ELONGATION %</t>
-  </si>
-  <si>
-    <t>BBETTER EPE</t>
-  </si>
-  <si>
-    <t>VISHAKHA EPE</t>
-  </si>
-  <si>
-    <t>CYBRIGHT EPE</t>
-  </si>
-  <si>
     <t>FIRST PRO EPE</t>
   </si>
   <si>
@@ -463,6 +466,15 @@
   </si>
   <si>
     <t>VISHKHA EVA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RAYBO EVA </t>
+  </si>
+  <si>
+    <t>P FIRST EPE</t>
+  </si>
+  <si>
+    <t>P FIRST EVA</t>
   </si>
   <si>
     <t xml:space="preserve">BOM </t>
@@ -1395,8 +1407,8 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{97A8C2A7-46C0-4446-B562-6550EA520638}" name="Table10" displayName="Table10" ref="A1:I3" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:I3" xr:uid="{97A8C2A7-46C0-4446-B562-6550EA520638}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{97A8C2A7-46C0-4446-B562-6550EA520638}" name="Table10" displayName="Table10" ref="A1:I7" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:I7" xr:uid="{97A8C2A7-46C0-4446-B562-6550EA520638}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{FE721515-FBBB-4487-ABCE-AAB6A5B1513A}" name="BOM" dataDxfId="9"/>
     <tableColumn id="9" xr3:uid="{304FA6D2-898E-427A-8AC1-958C15295938}" name="VENDOR NAME" dataDxfId="8"/>
@@ -2098,10 +2110,10 @@
         <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="D1" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -2125,8 +2137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{333C0630-51CF-46CA-8CAD-98FEF9AC181F}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2148,19 +2160,19 @@
         <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="D1" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="E1" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="F1" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="G1" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -2168,10 +2180,10 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="D2" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="E2">
         <v>331</v>
@@ -2182,7 +2194,7 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2190,10 +2202,10 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="D4" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="E4">
         <v>176</v>
@@ -2207,7 +2219,7 @@
         <v>46</v>
       </c>
       <c r="D5" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="E5">
         <v>249</v>
@@ -2218,10 +2230,10 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="D6" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="E6">
         <v>197</v>
@@ -2235,7 +2247,7 @@
         <v>48</v>
       </c>
       <c r="D7" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="E7">
         <v>277</v>
@@ -2249,7 +2261,7 @@
         <v>68</v>
       </c>
       <c r="D8" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="E8">
         <v>237</v>
@@ -2263,7 +2275,7 @@
         <v>60</v>
       </c>
       <c r="D9" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="E9">
         <v>325</v>
@@ -2277,7 +2289,7 @@
         <v>59</v>
       </c>
       <c r="D10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="E10">
         <v>155</v>
@@ -2291,7 +2303,7 @@
         <v>57</v>
       </c>
       <c r="D11" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="E11">
         <v>178</v>
@@ -2305,7 +2317,7 @@
         <v>46</v>
       </c>
       <c r="D12" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="E12">
         <v>227</v>
@@ -2316,7 +2328,7 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -2327,7 +2339,7 @@
         <v>56</v>
       </c>
       <c r="D14" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="E14">
         <v>357</v>
@@ -2338,10 +2350,10 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="D15" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="E15">
         <v>158</v>
@@ -2355,7 +2367,7 @@
         <v>52</v>
       </c>
       <c r="D16" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="E16">
         <v>314</v>
@@ -2369,7 +2381,7 @@
         <v>51</v>
       </c>
       <c r="D17" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="E17">
         <v>162</v>
@@ -2383,7 +2395,7 @@
         <v>49</v>
       </c>
       <c r="D18" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="E18">
         <v>275</v>
@@ -2394,7 +2406,7 @@
         <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -2429,7 +2441,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2557,8 +2569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9401EE47-EA52-49C7-BBC0-21F5B88254FB}">
   <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -2825,9 +2837,6 @@
       </c>
     </row>
     <row r="11" spans="1:11">
-      <c r="B11" t="s">
-        <v>18</v>
-      </c>
       <c r="C11" t="s">
         <v>37</v>
       </c>
@@ -3212,6 +3221,9 @@
       <c r="E28" s="4">
         <v>45866</v>
       </c>
+      <c r="F28" s="4">
+        <v>45875</v>
+      </c>
       <c r="H28" t="s">
         <v>38</v>
       </c>
@@ -3377,6 +3389,9 @@
       <c r="E36" s="4">
         <v>45867</v>
       </c>
+      <c r="F36" s="4">
+        <v>45880</v>
+      </c>
       <c r="H36" t="s">
         <v>38</v>
       </c>
@@ -3413,6 +3428,9 @@
       <c r="E38" s="4">
         <v>45870</v>
       </c>
+      <c r="F38" s="4">
+        <v>45875</v>
+      </c>
       <c r="H38" t="s">
         <v>38</v>
       </c>
@@ -3449,6 +3467,9 @@
       <c r="E40" s="4">
         <v>45870</v>
       </c>
+      <c r="F40" s="4">
+        <v>45876</v>
+      </c>
       <c r="H40" t="s">
         <v>38</v>
       </c>
@@ -3467,6 +3488,9 @@
       <c r="E41" s="4">
         <v>45870</v>
       </c>
+      <c r="F41" s="4">
+        <v>45878</v>
+      </c>
       <c r="H41" t="s">
         <v>38</v>
       </c>
@@ -3503,6 +3527,9 @@
       <c r="E43" s="4">
         <v>45873</v>
       </c>
+      <c r="F43" s="4">
+        <v>45878</v>
+      </c>
       <c r="H43" t="s">
         <v>38</v>
       </c>
@@ -3704,6 +3731,12 @@
       <c r="E53" s="4">
         <v>45875</v>
       </c>
+      <c r="F53" s="4">
+        <v>45875</v>
+      </c>
+      <c r="H53" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="1" t="s">
@@ -3719,6 +3752,12 @@
       <c r="E54" s="4">
         <v>45875</v>
       </c>
+      <c r="F54" s="4">
+        <v>45875</v>
+      </c>
+      <c r="H54" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" s="1" t="s">
@@ -3734,6 +3773,12 @@
       <c r="E55" s="4">
         <v>45875</v>
       </c>
+      <c r="F55" s="4">
+        <v>45875</v>
+      </c>
+      <c r="H55" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="56" spans="1:8">
       <c r="A56" t="s">
@@ -3746,6 +3791,9 @@
         <v>72</v>
       </c>
       <c r="D56" s="48"/>
+      <c r="H56" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="57" spans="1:8">
       <c r="A57" t="s">
@@ -3758,6 +3806,9 @@
         <v>73</v>
       </c>
       <c r="D57" s="48"/>
+      <c r="H57" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="58" spans="1:8">
       <c r="A58" t="s">
@@ -3770,6 +3821,9 @@
         <v>74</v>
       </c>
       <c r="D58" s="48"/>
+      <c r="H58" t="s">
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -4000,7 +4054,7 @@
   <dimension ref="A1:K519"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4185,12 +4239,31 @@
       <c r="B7" s="27" t="s">
         <v>84</v>
       </c>
+      <c r="C7" s="27" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="46"/>
+      <c r="A8" s="46" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="46"/>
+      <c r="A9" s="46" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="46"/>
@@ -5725,7 +5798,7 @@
   </sheetData>
   <dataValidations count="3">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 C4:C5" xr:uid="{5C73BBC5-C68D-4586-BDB5-A3BE48854FB6}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B1048576 C7:K7" xr:uid="{18FD80CD-FFDC-48A1-BA45-91576461B09B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:K7 B4:B1048576" xr:uid="{18FD80CD-FFDC-48A1-BA45-91576461B09B}">
       <formula1>"FRONT EPE, BACK EVA"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4:A1048576" xr:uid="{CDEE756C-C284-45D8-BDCE-F4798D4B3C50}">
@@ -5756,7 +5829,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5778,14 +5851,14 @@
       <c r="A1" s="28"/>
       <c r="B1" s="29"/>
       <c r="C1" s="30" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D1" s="31"/>
       <c r="E1" s="30"/>
       <c r="F1" s="31"/>
       <c r="G1" s="32"/>
       <c r="H1" s="44" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="I1" s="32"/>
       <c r="J1" s="29"/>
@@ -5798,19 +5871,19 @@
         <v>24</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D2" s="36"/>
       <c r="E2" s="37" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F2" s="38"/>
       <c r="G2" s="35" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="37" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J2" s="38"/>
     </row>
@@ -5897,6 +5970,18 @@
       <c r="F5" s="45">
         <v>101</v>
       </c>
+      <c r="G5" s="45">
+        <v>11</v>
+      </c>
+      <c r="H5" s="45">
+        <v>10</v>
+      </c>
+      <c r="I5" s="45">
+        <v>45</v>
+      </c>
+      <c r="J5" s="45">
+        <v>30</v>
+      </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="39" t="s">
@@ -5917,13 +6002,25 @@
       <c r="F6" s="45">
         <v>120</v>
       </c>
+      <c r="G6" s="45">
+        <v>26</v>
+      </c>
+      <c r="H6" s="45">
+        <v>20</v>
+      </c>
+      <c r="I6" s="45">
+        <v>38</v>
+      </c>
+      <c r="J6" s="45">
+        <v>30</v>
+      </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="39" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="45" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C7" s="45">
         <v>125</v>
@@ -5937,6 +6034,18 @@
       <c r="F7" s="45">
         <v>40</v>
       </c>
+      <c r="G7" s="45">
+        <v>31</v>
+      </c>
+      <c r="H7" s="45">
+        <v>21</v>
+      </c>
+      <c r="I7" s="45">
+        <v>38</v>
+      </c>
+      <c r="J7" s="45">
+        <v>32</v>
+      </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="39" t="s">
@@ -5956,6 +6065,18 @@
       </c>
       <c r="F8" s="45">
         <v>50</v>
+      </c>
+      <c r="G8" s="45">
+        <v>55</v>
+      </c>
+      <c r="H8" s="45">
+        <v>59</v>
+      </c>
+      <c r="I8" s="45">
+        <v>30</v>
+      </c>
+      <c r="J8" s="45">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -5985,7 +6106,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C8152F1-3340-4C7F-9B6C-3F6BB96763BA}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -6056,7 +6177,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -6064,7 +6185,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -6072,7 +6193,7 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -6080,7 +6201,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -6088,7 +6209,7 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -6096,7 +6217,7 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -6104,7 +6225,7 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -6123,10 +6244,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C0F3BDD-3989-4880-8737-F370069E1383}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6149,25 +6270,25 @@
         <v>24</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -6175,7 +6296,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
@@ -6186,11 +6307,55 @@
         <v>2</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -6236,7 +6401,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="B1" t="s">
         <v>81</v>
@@ -6245,7 +6410,7 @@
         <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -6253,13 +6418,13 @@
         <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="C2" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="D2" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -6267,13 +6432,13 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="C3" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="D3" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -6316,10 +6481,10 @@
         <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="D1" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:4">

</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-08-21 13:07:07
</commit_message>
<xml_diff>
--- a/data/Solar_Lab_Tests.xlsx
+++ b/data/Solar_Lab_Tests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29203"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29212"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1217" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F5DB1D1-2C66-4E8A-B7B4-96BE1255A5DA}"/>
+  <xr:revisionPtr revIDLastSave="1270" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DDE49F6B-B2DE-4ADE-A6BD-29D64C7AEBA8}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="10" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="10" activeTab="7" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Tests Map" sheetId="4" state="hidden" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <definedName name="ENCAPTYPE">Ref!$K$2:$K$1048576</definedName>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">'Material Tests Map'!$A$1:$B$20</definedName>
     <definedName name="ExternalData_1" localSheetId="11" hidden="1">'Standard test times'!$A$1:$B$15</definedName>
-    <definedName name="ExternalData_1" localSheetId="1" hidden="1">'Test Data'!$A$1:$H$58</definedName>
+    <definedName name="ExternalData_1" localSheetId="1" hidden="1">'Test Data'!$A$1:$H$66</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="175">
   <si>
     <t>BOM</t>
   </si>
@@ -297,6 +297,15 @@
     <t>PRODUCTION FIRST</t>
   </si>
   <si>
+    <t>CAHORS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P UKTR </t>
+  </si>
+  <si>
+    <t>QC SOLAR CHINA</t>
+  </si>
+  <si>
     <t>RM Type</t>
   </si>
   <si>
@@ -583,9 +592,6 @@
   </si>
   <si>
     <t>255MV</t>
-  </si>
-  <si>
-    <t>QC SOLAR LINE</t>
   </si>
   <si>
     <t>STANDARD DURATION (DAYS)</t>
@@ -898,7 +904,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -976,6 +982,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1464,8 +1471,8 @@
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{5C370BE7-C0F8-462F-9F89-5FC458087319}" name="Table16" displayName="Table16" ref="A1:G19" totalsRowShown="0">
-  <autoFilter ref="A1:G19" xr:uid="{5C370BE7-C0F8-462F-9F89-5FC458087319}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{5C370BE7-C0F8-462F-9F89-5FC458087319}" name="Table16" displayName="Table16" ref="A1:G22" totalsRowShown="0">
+  <autoFilter ref="A1:G22" xr:uid="{5C370BE7-C0F8-462F-9F89-5FC458087319}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{59EA2429-768A-457D-88E6-B34A083DE755}" name="BOM"/>
     <tableColumn id="2" xr3:uid="{C09F236B-325A-4EF9-B484-B1D592C83B7F}" name="VENDOR NAME"/>
@@ -1491,7 +1498,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{06A3AD80-C098-4015-85FF-3495CE4443EA}" name="Test_Data" displayName="Test_Data" ref="A1:H58" tableType="queryTable" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{06A3AD80-C098-4015-85FF-3495CE4443EA}" name="Test_Data" displayName="Test_Data" ref="A1:H66" tableType="queryTable" totalsRowShown="0">
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{87F75B08-44C4-4718-834D-87FEE9F87970}" uniqueName="1" name="BOM" queryTableFieldId="1" dataDxfId="42"/>
     <tableColumn id="2" xr3:uid="{1E5F4521-5E5C-4948-AEB2-FC5F712DB353}" uniqueName="2" name="TEST NAME" queryTableFieldId="2" dataDxfId="41"/>
@@ -2110,10 +2117,10 @@
         <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="D1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -2137,8 +2144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{333C0630-51CF-46CA-8CAD-98FEF9AC181F}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView topLeftCell="B11" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2160,19 +2167,19 @@
         <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="D1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="E1" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="F1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="G1" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -2180,10 +2187,10 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="D2" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="E2">
         <v>331</v>
@@ -2194,7 +2201,7 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2202,10 +2209,10 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="D4" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="E4">
         <v>176</v>
@@ -2219,7 +2226,7 @@
         <v>46</v>
       </c>
       <c r="D5" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="E5">
         <v>249</v>
@@ -2230,10 +2237,10 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="D6" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="E6">
         <v>197</v>
@@ -2247,7 +2254,7 @@
         <v>48</v>
       </c>
       <c r="D7" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="E7">
         <v>277</v>
@@ -2261,7 +2268,7 @@
         <v>68</v>
       </c>
       <c r="D8" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="E8">
         <v>237</v>
@@ -2275,7 +2282,7 @@
         <v>60</v>
       </c>
       <c r="D9" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="E9">
         <v>325</v>
@@ -2289,7 +2296,7 @@
         <v>59</v>
       </c>
       <c r="D10" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="E10">
         <v>155</v>
@@ -2303,7 +2310,7 @@
         <v>57</v>
       </c>
       <c r="D11" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="E11">
         <v>178</v>
@@ -2317,7 +2324,7 @@
         <v>46</v>
       </c>
       <c r="D12" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="E12">
         <v>227</v>
@@ -2328,7 +2335,7 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -2339,7 +2346,7 @@
         <v>56</v>
       </c>
       <c r="D14" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="E14">
         <v>357</v>
@@ -2350,10 +2357,10 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="D15" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="E15">
         <v>158</v>
@@ -2367,7 +2374,7 @@
         <v>52</v>
       </c>
       <c r="D16" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="E16">
         <v>314</v>
@@ -2381,7 +2388,7 @@
         <v>51</v>
       </c>
       <c r="D17" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="E17">
         <v>162</v>
@@ -2395,7 +2402,7 @@
         <v>49</v>
       </c>
       <c r="D18" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="E18">
         <v>275</v>
@@ -2404,9 +2411,6 @@
     <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>15</v>
-      </c>
-      <c r="B19" t="s">
-        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -2441,7 +2445,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2567,10 +2571,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9401EE47-EA52-49C7-BBC0-21F5B88254FB}">
-  <dimension ref="A1:K58"/>
+  <dimension ref="A1:K66"/>
   <sheetViews>
     <sheetView topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+      <selection activeCell="H66" sqref="H66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -3030,11 +3034,9 @@
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="4">
-        <v>45869</v>
-      </c>
-      <c r="F19" s="4">
-        <v>45875</v>
-      </c>
+        <v>45890</v>
+      </c>
+      <c r="F19" s="4"/>
       <c r="H19" t="s">
         <v>38</v>
       </c>
@@ -3566,8 +3568,11 @@
         <v>60</v>
       </c>
       <c r="D45" s="48"/>
+      <c r="E45" s="4">
+        <v>45890</v>
+      </c>
       <c r="H45" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="15">
@@ -3788,9 +3793,15 @@
         <v>6</v>
       </c>
       <c r="C56" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="D56" s="48"/>
+      <c r="E56" s="4">
+        <v>45883</v>
+      </c>
+      <c r="F56" s="4">
+        <v>45885</v>
+      </c>
       <c r="H56" t="s">
         <v>38</v>
       </c>
@@ -3806,6 +3817,12 @@
         <v>73</v>
       </c>
       <c r="D57" s="48"/>
+      <c r="E57" s="4">
+        <v>45883</v>
+      </c>
+      <c r="F57" s="4">
+        <v>45885</v>
+      </c>
       <c r="H57" t="s">
         <v>38</v>
       </c>
@@ -3821,8 +3838,162 @@
         <v>74</v>
       </c>
       <c r="D58" s="48"/>
+      <c r="E58" s="4">
+        <v>45883</v>
+      </c>
+      <c r="F58" s="4">
+        <v>45885</v>
+      </c>
       <c r="H58" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="A59" s="49" t="s">
+        <v>15</v>
+      </c>
+      <c r="B59" s="49" t="s">
+        <v>18</v>
+      </c>
+      <c r="C59" s="49" t="s">
+        <v>75</v>
+      </c>
+      <c r="D59" s="48"/>
+      <c r="E59" s="4">
+        <v>45890</v>
+      </c>
+      <c r="F59" s="49"/>
+      <c r="G59" s="49"/>
+      <c r="H59" s="49" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="A60" s="49" t="s">
+        <v>15</v>
+      </c>
+      <c r="B60" s="49" t="s">
+        <v>18</v>
+      </c>
+      <c r="C60" s="49" t="s">
+        <v>76</v>
+      </c>
+      <c r="D60" s="48"/>
+      <c r="E60" s="4">
+        <v>45890</v>
+      </c>
+      <c r="F60" s="49"/>
+      <c r="G60" s="49"/>
+      <c r="H60" s="49" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="A61" s="49" t="s">
+        <v>15</v>
+      </c>
+      <c r="B61" s="49" t="s">
+        <v>16</v>
+      </c>
+      <c r="C61" s="49" t="s">
+        <v>77</v>
+      </c>
+      <c r="D61" s="48"/>
+      <c r="E61" s="49"/>
+      <c r="F61" s="49"/>
+      <c r="G61" s="49"/>
+      <c r="H61" s="49" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8">
+      <c r="A62" s="49" t="s">
+        <v>15</v>
+      </c>
+      <c r="B62" s="49" t="s">
+        <v>16</v>
+      </c>
+      <c r="C62" s="49" t="s">
+        <v>58</v>
+      </c>
+      <c r="D62" s="48"/>
+      <c r="E62" s="49"/>
+      <c r="F62" s="49"/>
+      <c r="G62" s="49"/>
+      <c r="H62" s="49" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8">
+      <c r="A63" s="49" t="s">
+        <v>15</v>
+      </c>
+      <c r="B63" s="49" t="s">
+        <v>16</v>
+      </c>
+      <c r="C63" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="D63" s="48"/>
+      <c r="E63" s="49"/>
+      <c r="F63" s="49"/>
+      <c r="G63" s="49"/>
+      <c r="H63" s="49" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8">
+      <c r="A64" s="49" t="s">
+        <v>15</v>
+      </c>
+      <c r="B64" s="49" t="s">
+        <v>16</v>
+      </c>
+      <c r="C64" s="49" t="s">
+        <v>51</v>
+      </c>
+      <c r="D64" s="48"/>
+      <c r="E64" s="49"/>
+      <c r="F64" s="49"/>
+      <c r="G64" s="49"/>
+      <c r="H64" s="49" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8">
+      <c r="A65" s="49" t="s">
+        <v>15</v>
+      </c>
+      <c r="B65" s="49" t="s">
+        <v>16</v>
+      </c>
+      <c r="C65" s="49" t="s">
+        <v>50</v>
+      </c>
+      <c r="D65" s="48"/>
+      <c r="E65" s="49"/>
+      <c r="F65" s="49"/>
+      <c r="G65" s="49"/>
+      <c r="H65" s="49" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8">
+      <c r="A66" s="49" t="s">
+        <v>15</v>
+      </c>
+      <c r="B66" s="49" t="s">
+        <v>16</v>
+      </c>
+      <c r="C66" s="49" t="s">
+        <v>49</v>
+      </c>
+      <c r="D66" s="48"/>
+      <c r="E66" s="49"/>
+      <c r="F66" s="49"/>
+      <c r="G66" s="49"/>
+      <c r="H66" s="49" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -3888,25 +4059,25 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="G1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="I1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="K1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="N1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -3923,10 +4094,10 @@
         <v>32</v>
       </c>
       <c r="K2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="N2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -3943,10 +4114,10 @@
         <v>38</v>
       </c>
       <c r="K3" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="N3" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -3957,10 +4128,10 @@
         <v>5</v>
       </c>
       <c r="G4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="I4" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -4071,19 +4242,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>24</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E1" s="16"/>
       <c r="F1" s="16"/>
       <c r="G1" s="16"/>
       <c r="H1" s="17" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="I1" s="18"/>
       <c r="J1" s="18"/>
@@ -4094,61 +4265,61 @@
       <c r="B2" s="20"/>
       <c r="C2" s="20"/>
       <c r="D2" s="21" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="F2" s="22" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="G2" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="H2" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="H2" s="23" t="s">
-        <v>90</v>
-      </c>
       <c r="I2" s="24" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="J2" s="24" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="K2" s="25" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:11" hidden="1">
       <c r="A3" s="46"/>
       <c r="B3" s="26" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="F3" s="26" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="G3" s="26" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="H3" s="26" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="I3" s="26" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="J3" s="26" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="K3" s="26" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -4156,7 +4327,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C4" t="s">
         <v>35</v>
@@ -4191,7 +4362,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C5" t="s">
         <v>35</v>
@@ -4226,10 +4397,10 @@
         <v>2</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -4237,10 +4408,10 @@
         <v>2</v>
       </c>
       <c r="B7" s="27" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C7" s="27" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -4248,10 +4419,10 @@
         <v>2</v>
       </c>
       <c r="B8" s="27" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C8" s="27" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -4259,10 +4430,10 @@
         <v>2</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -5851,14 +6022,14 @@
       <c r="A1" s="28"/>
       <c r="B1" s="29"/>
       <c r="C1" s="30" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="D1" s="31"/>
       <c r="E1" s="30"/>
       <c r="F1" s="31"/>
       <c r="G1" s="32"/>
       <c r="H1" s="44" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="I1" s="32"/>
       <c r="J1" s="29"/>
@@ -5871,19 +6042,19 @@
         <v>24</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="D2" s="36"/>
       <c r="E2" s="37" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="F2" s="38"/>
       <c r="G2" s="35" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="37" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="J2" s="38"/>
     </row>
@@ -5921,34 +6092,34 @@
     </row>
     <row r="4" spans="1:10" customFormat="1" hidden="1">
       <c r="A4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B4" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C4" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="E4" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="F4" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="G4" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="H4" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="I4" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="J4" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -5988,7 +6159,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="45" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C6" s="45">
         <v>125</v>
@@ -6020,7 +6191,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="45" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C7" s="45">
         <v>125</v>
@@ -6052,7 +6223,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="45" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C8" s="45">
         <v>166</v>
@@ -6126,10 +6297,10 @@
         <v>24</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="6" customFormat="1">
@@ -6153,7 +6324,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -6161,7 +6332,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -6169,7 +6340,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -6177,7 +6348,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -6185,7 +6356,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -6193,7 +6364,7 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -6201,7 +6372,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -6209,7 +6380,7 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -6217,7 +6388,7 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -6225,7 +6396,7 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -6270,25 +6441,25 @@
         <v>24</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -6296,7 +6467,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
@@ -6307,7 +6478,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
@@ -6318,7 +6489,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
@@ -6329,7 +6500,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
@@ -6340,7 +6511,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
@@ -6351,7 +6522,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
@@ -6387,7 +6558,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD5452B6-66C2-4964-BBFB-466116F6D217}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -6401,16 +6572,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C1" t="s">
         <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -6418,13 +6589,13 @@
         <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D2" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -6432,13 +6603,13 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="C3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="D3" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -6481,10 +6652,10 @@
         <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="D1" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:4">

</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-08-29 09:42:10
</commit_message>
<xml_diff>
--- a/data/Solar_Lab_Tests.xlsx
+++ b/data/Solar_Lab_Tests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1270" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DDE49F6B-B2DE-4ADE-A6BD-29D64C7AEBA8}"/>
+  <xr:revisionPtr revIDLastSave="1301" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{82881B37-EDA9-4AA6-A47F-00905B6179B6}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="10" activeTab="7" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="7" activeTab="3" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Tests Map" sheetId="4" state="hidden" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <definedName name="ENCAPTYPE">Ref!$K$2:$K$1048576</definedName>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">'Material Tests Map'!$A$1:$B$20</definedName>
     <definedName name="ExternalData_1" localSheetId="11" hidden="1">'Standard test times'!$A$1:$B$15</definedName>
-    <definedName name="ExternalData_1" localSheetId="1" hidden="1">'Test Data'!$A$1:$H$66</definedName>
+    <definedName name="ExternalData_1" localSheetId="1" hidden="1">'Test Data'!$A$1:$H$69</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="177">
   <si>
     <t>BOM</t>
   </si>
@@ -304,6 +304,12 @@
   </si>
   <si>
     <t>QC SOLAR CHINA</t>
+  </si>
+  <si>
+    <t>UKTR B D</t>
+  </si>
+  <si>
+    <t>LINE UKTR</t>
   </si>
   <si>
     <t>RM Type</t>
@@ -1498,7 +1504,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{06A3AD80-C098-4015-85FF-3495CE4443EA}" name="Test_Data" displayName="Test_Data" ref="A1:H66" tableType="queryTable" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{06A3AD80-C098-4015-85FF-3495CE4443EA}" name="Test_Data" displayName="Test_Data" ref="A1:H69" tableType="queryTable" totalsRowShown="0">
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{87F75B08-44C4-4718-834D-87FEE9F87970}" uniqueName="1" name="BOM" queryTableFieldId="1" dataDxfId="42"/>
     <tableColumn id="2" xr3:uid="{1E5F4521-5E5C-4948-AEB2-FC5F712DB353}" uniqueName="2" name="TEST NAME" queryTableFieldId="2" dataDxfId="41"/>
@@ -2117,10 +2123,10 @@
         <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D1" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -2144,7 +2150,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{333C0630-51CF-46CA-8CAD-98FEF9AC181F}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView topLeftCell="B11" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -2167,19 +2173,19 @@
         <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D1" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E1" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="F1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="G1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -2187,10 +2193,10 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D2" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="E2">
         <v>331</v>
@@ -2201,7 +2207,7 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2209,10 +2215,10 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D4" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E4">
         <v>176</v>
@@ -2226,7 +2232,7 @@
         <v>46</v>
       </c>
       <c r="D5" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="E5">
         <v>249</v>
@@ -2237,10 +2243,10 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D6" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="E6">
         <v>197</v>
@@ -2254,7 +2260,7 @@
         <v>48</v>
       </c>
       <c r="D7" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="E7">
         <v>277</v>
@@ -2268,7 +2274,7 @@
         <v>68</v>
       </c>
       <c r="D8" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E8">
         <v>237</v>
@@ -2282,7 +2288,7 @@
         <v>60</v>
       </c>
       <c r="D9" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="E9">
         <v>325</v>
@@ -2296,7 +2302,7 @@
         <v>59</v>
       </c>
       <c r="D10" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="E10">
         <v>155</v>
@@ -2310,7 +2316,7 @@
         <v>57</v>
       </c>
       <c r="D11" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E11">
         <v>178</v>
@@ -2324,7 +2330,7 @@
         <v>46</v>
       </c>
       <c r="D12" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="E12">
         <v>227</v>
@@ -2335,7 +2341,7 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -2346,7 +2352,7 @@
         <v>56</v>
       </c>
       <c r="D14" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="E14">
         <v>357</v>
@@ -2357,10 +2363,10 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="D15" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="E15">
         <v>158</v>
@@ -2374,7 +2380,7 @@
         <v>52</v>
       </c>
       <c r="D16" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E16">
         <v>314</v>
@@ -2388,7 +2394,7 @@
         <v>51</v>
       </c>
       <c r="D17" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="E17">
         <v>162</v>
@@ -2402,7 +2408,7 @@
         <v>49</v>
       </c>
       <c r="D18" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="E18">
         <v>275</v>
@@ -2445,7 +2451,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2571,10 +2577,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9401EE47-EA52-49C7-BBC0-21F5B88254FB}">
-  <dimension ref="A1:K66"/>
+  <dimension ref="A1:K69"/>
   <sheetViews>
     <sheetView topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="H66" sqref="H66"/>
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -3036,7 +3042,9 @@
       <c r="E19" s="4">
         <v>45890</v>
       </c>
-      <c r="F19" s="4"/>
+      <c r="F19" s="4">
+        <v>45892</v>
+      </c>
       <c r="H19" t="s">
         <v>38</v>
       </c>
@@ -3571,6 +3579,9 @@
       <c r="E45" s="4">
         <v>45890</v>
       </c>
+      <c r="F45" s="4">
+        <v>45892</v>
+      </c>
       <c r="H45" t="s">
         <v>38</v>
       </c>
@@ -3849,151 +3860,213 @@
       </c>
     </row>
     <row r="59" spans="1:8">
-      <c r="A59" s="49" t="s">
+      <c r="A59" t="s">
         <v>15</v>
       </c>
-      <c r="B59" s="49" t="s">
+      <c r="B59" t="s">
         <v>18</v>
       </c>
-      <c r="C59" s="49" t="s">
+      <c r="C59" t="s">
         <v>75</v>
       </c>
       <c r="D59" s="48"/>
       <c r="E59" s="4">
         <v>45890</v>
       </c>
-      <c r="F59" s="49"/>
-      <c r="G59" s="49"/>
-      <c r="H59" s="49" t="s">
+      <c r="F59" s="4">
+        <v>45892</v>
+      </c>
+      <c r="H59" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="60" spans="1:8">
-      <c r="A60" s="49" t="s">
+      <c r="A60" t="s">
         <v>15</v>
       </c>
-      <c r="B60" s="49" t="s">
+      <c r="B60" t="s">
         <v>18</v>
       </c>
-      <c r="C60" s="49" t="s">
+      <c r="C60" t="s">
         <v>76</v>
       </c>
       <c r="D60" s="48"/>
       <c r="E60" s="4">
         <v>45890</v>
       </c>
-      <c r="F60" s="49"/>
-      <c r="G60" s="49"/>
-      <c r="H60" s="49" t="s">
+      <c r="F60" s="4">
+        <v>45892</v>
+      </c>
+      <c r="H60" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="61" spans="1:8">
-      <c r="A61" s="49" t="s">
+      <c r="A61" t="s">
         <v>15</v>
       </c>
-      <c r="B61" s="49" t="s">
+      <c r="B61" t="s">
         <v>16</v>
       </c>
-      <c r="C61" s="49" t="s">
+      <c r="C61" t="s">
         <v>77</v>
       </c>
       <c r="D61" s="48"/>
-      <c r="E61" s="49"/>
-      <c r="F61" s="49"/>
-      <c r="G61" s="49"/>
-      <c r="H61" s="49" t="s">
-        <v>31</v>
+      <c r="E61" s="4">
+        <v>45891</v>
+      </c>
+      <c r="H61" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="62" spans="1:8">
-      <c r="A62" s="49" t="s">
+      <c r="A62" t="s">
         <v>15</v>
       </c>
-      <c r="B62" s="49" t="s">
+      <c r="B62" t="s">
         <v>16</v>
       </c>
-      <c r="C62" s="49" t="s">
+      <c r="C62" t="s">
         <v>58</v>
       </c>
       <c r="D62" s="48"/>
-      <c r="E62" s="49"/>
-      <c r="F62" s="49"/>
-      <c r="G62" s="49"/>
-      <c r="H62" s="49" t="s">
-        <v>31</v>
+      <c r="E62" s="4">
+        <v>45891</v>
+      </c>
+      <c r="H62" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="63" spans="1:8">
-      <c r="A63" s="49" t="s">
+      <c r="A63" t="s">
         <v>15</v>
       </c>
-      <c r="B63" s="49" t="s">
+      <c r="B63" t="s">
         <v>16</v>
       </c>
-      <c r="C63" s="49" t="s">
+      <c r="C63" t="s">
         <v>70</v>
       </c>
       <c r="D63" s="48"/>
-      <c r="E63" s="49"/>
-      <c r="F63" s="49"/>
-      <c r="G63" s="49"/>
-      <c r="H63" s="49" t="s">
-        <v>31</v>
+      <c r="E63" s="4">
+        <v>45891</v>
+      </c>
+      <c r="H63" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="64" spans="1:8">
-      <c r="A64" s="49" t="s">
+      <c r="A64" t="s">
         <v>15</v>
       </c>
-      <c r="B64" s="49" t="s">
+      <c r="B64" t="s">
         <v>16</v>
       </c>
-      <c r="C64" s="49" t="s">
+      <c r="C64" t="s">
         <v>51</v>
       </c>
       <c r="D64" s="48"/>
-      <c r="E64" s="49"/>
-      <c r="F64" s="49"/>
-      <c r="G64" s="49"/>
-      <c r="H64" s="49" t="s">
-        <v>31</v>
+      <c r="E64" s="4">
+        <v>45891</v>
+      </c>
+      <c r="H64" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="65" spans="1:8">
-      <c r="A65" s="49" t="s">
+      <c r="A65" t="s">
         <v>15</v>
       </c>
-      <c r="B65" s="49" t="s">
+      <c r="B65" t="s">
         <v>16</v>
       </c>
-      <c r="C65" s="49" t="s">
+      <c r="C65" t="s">
         <v>50</v>
       </c>
       <c r="D65" s="48"/>
-      <c r="E65" s="49"/>
-      <c r="F65" s="49"/>
-      <c r="G65" s="49"/>
-      <c r="H65" s="49" t="s">
-        <v>31</v>
+      <c r="E65" s="4">
+        <v>45891</v>
+      </c>
+      <c r="H65" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="66" spans="1:8">
-      <c r="A66" s="49" t="s">
+      <c r="A66" t="s">
         <v>15</v>
       </c>
-      <c r="B66" s="49" t="s">
+      <c r="B66" t="s">
         <v>16</v>
       </c>
-      <c r="C66" s="49" t="s">
+      <c r="C66" t="s">
         <v>49</v>
       </c>
       <c r="D66" s="48"/>
-      <c r="E66" s="49"/>
-      <c r="F66" s="49"/>
-      <c r="G66" s="49"/>
-      <c r="H66" s="49" t="s">
-        <v>31</v>
+      <c r="E66" s="4">
+        <v>45891</v>
+      </c>
+      <c r="H66" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8">
+      <c r="A67" s="49" t="s">
+        <v>15</v>
+      </c>
+      <c r="B67" s="49" t="s">
+        <v>16</v>
+      </c>
+      <c r="C67" s="49" t="s">
+        <v>78</v>
+      </c>
+      <c r="D67" s="48"/>
+      <c r="E67" s="4">
+        <v>45891</v>
+      </c>
+      <c r="F67" s="49"/>
+      <c r="G67" s="49"/>
+      <c r="H67" s="49" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8">
+      <c r="A68" s="49" t="s">
+        <v>15</v>
+      </c>
+      <c r="B68" s="49" t="s">
+        <v>18</v>
+      </c>
+      <c r="C68" s="49" t="s">
+        <v>78</v>
+      </c>
+      <c r="D68" s="48"/>
+      <c r="E68" s="4">
+        <v>45897</v>
+      </c>
+      <c r="F68" s="49"/>
+      <c r="G68" s="49"/>
+      <c r="H68" s="49" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8">
+      <c r="A69" s="49" t="s">
+        <v>15</v>
+      </c>
+      <c r="B69" s="49" t="s">
+        <v>18</v>
+      </c>
+      <c r="C69" s="49" t="s">
+        <v>79</v>
+      </c>
+      <c r="D69" s="48"/>
+      <c r="E69" s="4">
+        <v>45897</v>
+      </c>
+      <c r="F69" s="49"/>
+      <c r="G69" s="49"/>
+      <c r="H69" s="49" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -4059,25 +4132,25 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="I1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="K1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="N1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -4094,10 +4167,10 @@
         <v>32</v>
       </c>
       <c r="K2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="N2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -4114,10 +4187,10 @@
         <v>38</v>
       </c>
       <c r="K3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="N3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -4128,10 +4201,10 @@
         <v>5</v>
       </c>
       <c r="G4" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="I4" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -4224,7 +4297,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61A5C69B-8639-4E8F-9A05-E59E5511083E}">
   <dimension ref="A1:K519"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -4242,19 +4315,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>24</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E1" s="16"/>
       <c r="F1" s="16"/>
       <c r="G1" s="16"/>
       <c r="H1" s="17" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="I1" s="18"/>
       <c r="J1" s="18"/>
@@ -4265,61 +4338,61 @@
       <c r="B2" s="20"/>
       <c r="C2" s="20"/>
       <c r="D2" s="21" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F2" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="H2" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="I2" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="H2" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="I2" s="24" t="s">
-        <v>94</v>
-      </c>
       <c r="J2" s="24" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="K2" s="25" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:11" hidden="1">
       <c r="A3" s="46"/>
       <c r="B3" s="26" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="F3" s="26" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="G3" s="26" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="H3" s="26" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="I3" s="26" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="J3" s="26" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="K3" s="26" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -4327,7 +4400,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C4" t="s">
         <v>35</v>
@@ -4362,7 +4435,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C5" t="s">
         <v>35</v>
@@ -4397,10 +4470,10 @@
         <v>2</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -4408,10 +4481,10 @@
         <v>2</v>
       </c>
       <c r="B7" s="27" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C7" s="27" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -4419,10 +4492,10 @@
         <v>2</v>
       </c>
       <c r="B8" s="27" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C8" s="27" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -4430,10 +4503,10 @@
         <v>2</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -6022,14 +6095,14 @@
       <c r="A1" s="28"/>
       <c r="B1" s="29"/>
       <c r="C1" s="30" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D1" s="31"/>
       <c r="E1" s="30"/>
       <c r="F1" s="31"/>
       <c r="G1" s="32"/>
       <c r="H1" s="44" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="I1" s="32"/>
       <c r="J1" s="29"/>
@@ -6042,19 +6115,19 @@
         <v>24</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D2" s="36"/>
       <c r="E2" s="37" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="F2" s="38"/>
       <c r="G2" s="35" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="37" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="J2" s="38"/>
     </row>
@@ -6092,34 +6165,34 @@
     </row>
     <row r="4" spans="1:10" customFormat="1" hidden="1">
       <c r="A4" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C4" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D4" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E4" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F4" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="G4" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H4" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I4" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="J4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -6159,7 +6232,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="45" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C6" s="45">
         <v>125</v>
@@ -6191,7 +6264,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="45" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C7" s="45">
         <v>125</v>
@@ -6223,7 +6296,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="45" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C8" s="45">
         <v>166</v>
@@ -6297,10 +6370,10 @@
         <v>24</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="6" customFormat="1">
@@ -6324,7 +6397,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -6332,7 +6405,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -6340,7 +6413,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -6348,7 +6421,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -6356,7 +6429,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -6364,7 +6437,7 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -6372,7 +6445,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -6380,7 +6453,7 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -6388,7 +6461,7 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -6396,7 +6469,7 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -6441,25 +6514,25 @@
         <v>24</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -6467,7 +6540,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
@@ -6478,7 +6551,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
@@ -6489,7 +6562,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
@@ -6500,7 +6573,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
@@ -6511,7 +6584,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
@@ -6522,7 +6595,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
@@ -6558,7 +6631,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD5452B6-66C2-4964-BBFB-466116F6D217}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -6572,16 +6645,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C1" t="s">
         <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -6589,13 +6662,13 @@
         <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -6603,13 +6676,13 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C3" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D3" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -6652,10 +6725,10 @@
         <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:4">

</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-09-08 13:07:40
</commit_message>
<xml_diff>
--- a/data/Solar_Lab_Tests.xlsx
+++ b/data/Solar_Lab_Tests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1301" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{82881B37-EDA9-4AA6-A47F-00905B6179B6}"/>
+  <xr:revisionPtr revIDLastSave="1351" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{45DDA04C-15FC-4B8D-B776-08FF5341D5B5}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="7" activeTab="3" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="3" activeTab="6" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Tests Map" sheetId="4" state="hidden" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <definedName name="ENCAPTYPE">Ref!$K$2:$K$1048576</definedName>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">'Material Tests Map'!$A$1:$B$20</definedName>
     <definedName name="ExternalData_1" localSheetId="11" hidden="1">'Standard test times'!$A$1:$B$15</definedName>
-    <definedName name="ExternalData_1" localSheetId="1" hidden="1">'Test Data'!$A$1:$H$69</definedName>
+    <definedName name="ExternalData_1" localSheetId="1" hidden="1">'Test Data'!$A$1:$H$74</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="180">
   <si>
     <t>BOM</t>
   </si>
@@ -312,6 +312,9 @@
     <t>LINE UKTR</t>
   </si>
   <si>
+    <t>SHEETSOL</t>
+  </si>
+  <si>
     <t>RM Type</t>
   </si>
   <si>
@@ -490,6 +493,12 @@
   </si>
   <si>
     <t>P FIRST EVA</t>
+  </si>
+  <si>
+    <t>SHEETSOL EPE</t>
+  </si>
+  <si>
+    <t>SHEETSOL EVA</t>
   </si>
   <si>
     <t xml:space="preserve">BOM </t>
@@ -910,7 +919,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -989,6 +998,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1420,8 +1430,8 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{97A8C2A7-46C0-4446-B562-6550EA520638}" name="Table10" displayName="Table10" ref="A1:I7" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:I7" xr:uid="{97A8C2A7-46C0-4446-B562-6550EA520638}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{97A8C2A7-46C0-4446-B562-6550EA520638}" name="Table10" displayName="Table10" ref="A1:I11" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:I11" xr:uid="{97A8C2A7-46C0-4446-B562-6550EA520638}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{FE721515-FBBB-4487-ABCE-AAB6A5B1513A}" name="BOM" dataDxfId="9"/>
     <tableColumn id="9" xr3:uid="{304FA6D2-898E-427A-8AC1-958C15295938}" name="VENDOR NAME" dataDxfId="8"/>
@@ -1504,7 +1514,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{06A3AD80-C098-4015-85FF-3495CE4443EA}" name="Test_Data" displayName="Test_Data" ref="A1:H69" tableType="queryTable" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{06A3AD80-C098-4015-85FF-3495CE4443EA}" name="Test_Data" displayName="Test_Data" ref="A1:H74" tableType="queryTable" totalsRowShown="0">
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{87F75B08-44C4-4718-834D-87FEE9F87970}" uniqueName="1" name="BOM" queryTableFieldId="1" dataDxfId="42"/>
     <tableColumn id="2" xr3:uid="{1E5F4521-5E5C-4948-AEB2-FC5F712DB353}" uniqueName="2" name="TEST NAME" queryTableFieldId="2" dataDxfId="41"/>
@@ -2123,10 +2133,10 @@
         <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="D1" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -2173,19 +2183,19 @@
         <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="D1" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="E1" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="F1" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="G1" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -2193,10 +2203,10 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="D2" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="E2">
         <v>331</v>
@@ -2207,7 +2217,7 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2215,10 +2225,10 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="D4" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="E4">
         <v>176</v>
@@ -2232,7 +2242,7 @@
         <v>46</v>
       </c>
       <c r="D5" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="E5">
         <v>249</v>
@@ -2243,10 +2253,10 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="D6" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="E6">
         <v>197</v>
@@ -2260,7 +2270,7 @@
         <v>48</v>
       </c>
       <c r="D7" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="E7">
         <v>277</v>
@@ -2274,7 +2284,7 @@
         <v>68</v>
       </c>
       <c r="D8" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="E8">
         <v>237</v>
@@ -2288,7 +2298,7 @@
         <v>60</v>
       </c>
       <c r="D9" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="E9">
         <v>325</v>
@@ -2302,7 +2312,7 @@
         <v>59</v>
       </c>
       <c r="D10" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="E10">
         <v>155</v>
@@ -2316,7 +2326,7 @@
         <v>57</v>
       </c>
       <c r="D11" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="E11">
         <v>178</v>
@@ -2330,7 +2340,7 @@
         <v>46</v>
       </c>
       <c r="D12" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="E12">
         <v>227</v>
@@ -2341,7 +2351,7 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -2352,7 +2362,7 @@
         <v>56</v>
       </c>
       <c r="D14" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="E14">
         <v>357</v>
@@ -2363,10 +2373,10 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="D15" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="E15">
         <v>158</v>
@@ -2380,7 +2390,7 @@
         <v>52</v>
       </c>
       <c r="D16" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="E16">
         <v>314</v>
@@ -2394,7 +2404,7 @@
         <v>51</v>
       </c>
       <c r="D17" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="E17">
         <v>162</v>
@@ -2408,7 +2418,7 @@
         <v>49</v>
       </c>
       <c r="D18" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="E18">
         <v>275</v>
@@ -2451,7 +2461,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2577,10 +2587,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9401EE47-EA52-49C7-BBC0-21F5B88254FB}">
-  <dimension ref="A1:K69"/>
+  <dimension ref="A1:K74"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="H74" sqref="H74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -4010,62 +4020,156 @@
       </c>
     </row>
     <row r="67" spans="1:8">
-      <c r="A67" s="49" t="s">
+      <c r="A67" t="s">
         <v>15</v>
       </c>
-      <c r="B67" s="49" t="s">
+      <c r="B67" t="s">
         <v>16</v>
       </c>
-      <c r="C67" s="49" t="s">
+      <c r="C67" t="s">
         <v>78</v>
       </c>
       <c r="D67" s="48"/>
       <c r="E67" s="4">
         <v>45891</v>
       </c>
-      <c r="F67" s="49"/>
-      <c r="G67" s="49"/>
-      <c r="H67" s="49" t="s">
+      <c r="H67" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="68" spans="1:8">
-      <c r="A68" s="49" t="s">
+      <c r="A68" t="s">
         <v>15</v>
       </c>
-      <c r="B68" s="49" t="s">
+      <c r="B68" t="s">
         <v>18</v>
       </c>
-      <c r="C68" s="49" t="s">
+      <c r="C68" t="s">
         <v>78</v>
       </c>
       <c r="D68" s="48"/>
       <c r="E68" s="4">
         <v>45897</v>
       </c>
-      <c r="F68" s="49"/>
-      <c r="G68" s="49"/>
-      <c r="H68" s="49" t="s">
+      <c r="H68" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="69" spans="1:8">
-      <c r="A69" s="49" t="s">
+      <c r="A69" t="s">
         <v>15</v>
       </c>
-      <c r="B69" s="49" t="s">
+      <c r="B69" t="s">
         <v>18</v>
       </c>
-      <c r="C69" s="49" t="s">
+      <c r="C69" t="s">
         <v>79</v>
       </c>
       <c r="D69" s="48"/>
       <c r="E69" s="4">
         <v>45897</v>
       </c>
-      <c r="F69" s="49"/>
-      <c r="G69" s="49"/>
-      <c r="H69" s="49" t="s">
+      <c r="H69" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8">
+      <c r="A70" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="B70" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="C70" s="49" t="s">
+        <v>80</v>
+      </c>
+      <c r="D70" s="48"/>
+      <c r="E70" s="4">
+        <v>45906</v>
+      </c>
+      <c r="F70" s="49"/>
+      <c r="G70" s="49"/>
+      <c r="H70" s="49" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8">
+      <c r="A71" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="B71" s="49" t="s">
+        <v>3</v>
+      </c>
+      <c r="C71" s="49" t="s">
+        <v>80</v>
+      </c>
+      <c r="D71" s="48"/>
+      <c r="E71" s="4">
+        <v>45906</v>
+      </c>
+      <c r="F71" s="49"/>
+      <c r="G71" s="49"/>
+      <c r="H71" s="49" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8">
+      <c r="A72" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="B72" s="49" t="s">
+        <v>5</v>
+      </c>
+      <c r="C72" s="49" t="s">
+        <v>80</v>
+      </c>
+      <c r="D72" s="48"/>
+      <c r="E72" s="4">
+        <v>45906</v>
+      </c>
+      <c r="F72" s="49"/>
+      <c r="G72" s="49"/>
+      <c r="H72" s="49" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8">
+      <c r="A73" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="B73" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="C73" s="49" t="s">
+        <v>80</v>
+      </c>
+      <c r="D73" s="48"/>
+      <c r="E73" s="4">
+        <v>45906</v>
+      </c>
+      <c r="F73" s="49"/>
+      <c r="G73" s="49"/>
+      <c r="H73" s="49" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8">
+      <c r="A74" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="B74" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="C74" s="49" t="s">
+        <v>80</v>
+      </c>
+      <c r="D74" s="48"/>
+      <c r="E74" s="4">
+        <v>45906</v>
+      </c>
+      <c r="F74" s="49"/>
+      <c r="G74" s="49"/>
+      <c r="H74" s="49" t="s">
         <v>38</v>
       </c>
     </row>
@@ -4132,25 +4236,25 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="K1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="N1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -4167,10 +4271,10 @@
         <v>32</v>
       </c>
       <c r="K2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="N2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -4187,10 +4291,10 @@
         <v>38</v>
       </c>
       <c r="K3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="N3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -4201,10 +4305,10 @@
         <v>5</v>
       </c>
       <c r="G4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -4297,7 +4401,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61A5C69B-8639-4E8F-9A05-E59E5511083E}">
   <dimension ref="A1:K519"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -4315,19 +4419,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>24</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E1" s="16"/>
       <c r="F1" s="16"/>
       <c r="G1" s="16"/>
       <c r="H1" s="17" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I1" s="18"/>
       <c r="J1" s="18"/>
@@ -4338,61 +4442,61 @@
       <c r="B2" s="20"/>
       <c r="C2" s="20"/>
       <c r="D2" s="21" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E2" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="H2" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="I2" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="J2" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="H2" s="23" t="s">
-        <v>95</v>
-      </c>
-      <c r="I2" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="J2" s="24" t="s">
-        <v>97</v>
-      </c>
       <c r="K2" s="25" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:11" hidden="1">
       <c r="A3" s="46"/>
       <c r="B3" s="26" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F3" s="26" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G3" s="26" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H3" s="26" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="I3" s="26" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="J3" s="26" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="K3" s="26" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -4400,7 +4504,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C4" t="s">
         <v>35</v>
@@ -4435,7 +4539,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C5" t="s">
         <v>35</v>
@@ -4470,10 +4574,10 @@
         <v>2</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -4481,10 +4585,10 @@
         <v>2</v>
       </c>
       <c r="B7" s="27" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C7" s="27" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -4492,10 +4596,10 @@
         <v>2</v>
       </c>
       <c r="B8" s="27" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C8" s="27" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -4503,10 +4607,10 @@
         <v>2</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -6095,14 +6199,14 @@
       <c r="A1" s="28"/>
       <c r="B1" s="29"/>
       <c r="C1" s="30" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D1" s="31"/>
       <c r="E1" s="30"/>
       <c r="F1" s="31"/>
       <c r="G1" s="32"/>
       <c r="H1" s="44" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I1" s="32"/>
       <c r="J1" s="29"/>
@@ -6115,19 +6219,19 @@
         <v>24</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D2" s="36"/>
       <c r="E2" s="37" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F2" s="38"/>
       <c r="G2" s="35" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="37" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="J2" s="38"/>
     </row>
@@ -6165,34 +6269,34 @@
     </row>
     <row r="4" spans="1:10" customFormat="1" hidden="1">
       <c r="A4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H4" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="I4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="J4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -6232,7 +6336,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="45" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C6" s="45">
         <v>125</v>
@@ -6264,7 +6368,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="45" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C7" s="45">
         <v>125</v>
@@ -6296,7 +6400,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="45" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C8" s="45">
         <v>166</v>
@@ -6370,10 +6474,10 @@
         <v>24</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="6" customFormat="1">
@@ -6397,7 +6501,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -6405,7 +6509,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -6413,7 +6517,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -6421,7 +6525,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -6429,7 +6533,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -6437,7 +6541,7 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -6445,7 +6549,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -6453,7 +6557,7 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -6461,7 +6565,7 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -6469,7 +6573,7 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -6488,10 +6592,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C0F3BDD-3989-4880-8737-F370069E1383}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6514,25 +6618,25 @@
         <v>24</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -6540,7 +6644,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
@@ -6551,7 +6655,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
@@ -6562,7 +6666,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
@@ -6573,7 +6677,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
@@ -6584,7 +6688,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
@@ -6595,11 +6699,103 @@
         <v>2</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="C8" s="50"/>
+      <c r="D8" s="50">
+        <v>10.84</v>
+      </c>
+      <c r="E8" s="50">
+        <v>10.73</v>
+      </c>
+      <c r="F8" s="7">
+        <v>10.72</v>
+      </c>
+      <c r="G8" s="7">
+        <v>10.5</v>
+      </c>
+      <c r="H8" s="7"/>
+      <c r="I8" s="50"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C9" s="50"/>
+      <c r="D9" s="50">
+        <v>10.15</v>
+      </c>
+      <c r="E9" s="50">
+        <v>10.220000000000001</v>
+      </c>
+      <c r="F9" s="7">
+        <v>10.119999999999999</v>
+      </c>
+      <c r="G9" s="7">
+        <v>10.11</v>
+      </c>
+      <c r="H9" s="7"/>
+      <c r="I9" s="50"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="C10" s="50"/>
+      <c r="D10" s="50">
+        <v>10.32</v>
+      </c>
+      <c r="E10" s="50">
+        <v>10.27</v>
+      </c>
+      <c r="F10" s="7">
+        <v>10.210000000000001</v>
+      </c>
+      <c r="G10" s="7">
+        <v>10.3</v>
+      </c>
+      <c r="H10" s="7"/>
+      <c r="I10" s="50"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="C11" s="50"/>
+      <c r="D11" s="50">
+        <v>9.91</v>
+      </c>
+      <c r="E11" s="50">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="F11" s="7">
+        <v>9.93</v>
+      </c>
+      <c r="G11" s="7">
+        <v>9.9</v>
+      </c>
+      <c r="H11" s="7"/>
+      <c r="I11" s="50"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -6645,16 +6841,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C1" t="s">
         <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -6662,13 +6858,13 @@
         <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="C2" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="D2" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -6676,13 +6872,13 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="C3" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D3" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -6725,10 +6921,10 @@
         <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D1" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:4">

</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-09-11 09:41:42
</commit_message>
<xml_diff>
--- a/data/Solar_Lab_Tests.xlsx
+++ b/data/Solar_Lab_Tests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29303"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1351" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{45DDA04C-15FC-4B8D-B776-08FF5341D5B5}"/>
+  <xr:revisionPtr revIDLastSave="1514" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0707AE21-33E5-4514-8644-04005D3B4C7B}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="3" activeTab="6" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="3" activeTab="8" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Tests Map" sheetId="4" state="hidden" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="189">
   <si>
     <t>BOM</t>
   </si>
@@ -408,6 +408,12 @@
     <t>RAYBO</t>
   </si>
   <si>
+    <t>sheetsol</t>
+  </si>
+  <si>
+    <t>p first</t>
+  </si>
+  <si>
     <t xml:space="preserve">                                                                                                                           PRE PCT</t>
   </si>
   <si>
@@ -423,69 +429,87 @@
     <t>FIRST PRODUCTION</t>
   </si>
   <si>
+    <t>NORMAL GLASS220.220</t>
+  </si>
+  <si>
     <t>BREAK</t>
   </si>
   <si>
     <t>CHANGE IN ELONGATION %</t>
   </si>
   <si>
-    <t>BBETTER EPE</t>
-  </si>
-  <si>
-    <t>VISHAKHA EPE</t>
-  </si>
-  <si>
-    <t>CYBRIGHT EPE</t>
+    <t>BBETTER EPE MD</t>
+  </si>
+  <si>
+    <t>VISHAKHA EPE MD</t>
+  </si>
+  <si>
+    <t>CYBRIGHT EPE MD</t>
+  </si>
+  <si>
+    <t>RAYBO EPE MD</t>
+  </si>
+  <si>
+    <t>FIRST PRO EPE MD</t>
+  </si>
+  <si>
+    <t>BBETTER EVA MD</t>
+  </si>
+  <si>
+    <t>VISHAKHA EVA MD</t>
+  </si>
+  <si>
+    <t>CYBRIGHT EVA MD</t>
+  </si>
+  <si>
+    <t>RAYBO EVA MD</t>
+  </si>
+  <si>
+    <t>FIRST PRO EVA MD</t>
+  </si>
+  <si>
+    <t>SHEETSOL EPE MD</t>
+  </si>
+  <si>
+    <t>SHEETSOL  EPE TD</t>
+  </si>
+  <si>
+    <t>SHEETSOL EVA MD</t>
+  </si>
+  <si>
+    <t>SHEETSOL  EVA TD</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">min value 1 </t>
+  </si>
+  <si>
+    <t>min value 2</t>
+  </si>
+  <si>
+    <t>min value 3</t>
+  </si>
+  <si>
+    <t>min value 4</t>
+  </si>
+  <si>
+    <t>min value 5</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>VISHKHA EPE</t>
+  </si>
+  <si>
+    <t>VISHKHA EVA</t>
   </si>
   <si>
     <t>RAYBO EPE</t>
   </si>
   <si>
-    <t>FIRST PRO EPE</t>
-  </si>
-  <si>
-    <t>BBETTER EVA</t>
-  </si>
-  <si>
-    <t>VISHAKHA EVA</t>
-  </si>
-  <si>
-    <t>CYBRIGHT EVA</t>
-  </si>
-  <si>
-    <t>RAYBO EVA</t>
-  </si>
-  <si>
-    <t>FIRST PRO EVA</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">min value 1 </t>
-  </si>
-  <si>
-    <t>min value 2</t>
-  </si>
-  <si>
-    <t>min value 3</t>
-  </si>
-  <si>
-    <t>min value 4</t>
-  </si>
-  <si>
-    <t>min value 5</t>
-  </si>
-  <si>
-    <t>Mean</t>
-  </si>
-  <si>
-    <t>VISHKHA EPE</t>
-  </si>
-  <si>
-    <t>VISHKHA EVA</t>
-  </si>
-  <si>
     <t xml:space="preserve">RAYBO EVA </t>
   </si>
   <si>
@@ -529,6 +553,9 @@
   </si>
   <si>
     <t>END TIME</t>
+  </si>
+  <si>
+    <t>FASTO</t>
   </si>
   <si>
     <t>TIME</t>
@@ -619,7 +646,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -675,6 +702,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="14">
@@ -757,7 +790,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -915,6 +948,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -997,8 +1041,8 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1417,8 +1461,8 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{9AF05D4E-990A-4C94-8850-9D7BC3D120A4}" name="Table14" displayName="Table14" ref="A1:D12" totalsRowShown="0">
-  <autoFilter ref="A1:D12" xr:uid="{9AF05D4E-990A-4C94-8850-9D7BC3D120A4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{9AF05D4E-990A-4C94-8850-9D7BC3D120A4}" name="Table14" displayName="Table14" ref="A1:D16" totalsRowShown="0">
+  <autoFilter ref="A1:D16" xr:uid="{9AF05D4E-990A-4C94-8850-9D7BC3D120A4}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{695E2580-F157-4DF3-A6A1-0C66057F77F2}" name="BOM"/>
     <tableColumn id="2" xr3:uid="{93E753E6-35FE-4C78-817F-5319A79D1951}" name="VENDOR NAME"/>
@@ -1448,8 +1492,8 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{20A38E0C-9EF6-4C45-A435-A35C875E6079}" name="Table4" displayName="Table4" ref="A1:D3" totalsRowShown="0">
-  <autoFilter ref="A1:D3" xr:uid="{20A38E0C-9EF6-4C45-A435-A35C875E6079}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{20A38E0C-9EF6-4C45-A435-A35C875E6079}" name="Table4" displayName="Table4" ref="A1:D5" totalsRowShown="0">
+  <autoFilter ref="A1:D5" xr:uid="{20A38E0C-9EF6-4C45-A435-A35C875E6079}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{81484900-FCE7-4687-AE80-25067EEBF4DF}" name="BOM "/>
     <tableColumn id="2" xr3:uid="{98C35052-5143-4722-B228-CDF4595728A7}" name="TYPE"/>
@@ -1461,8 +1505,8 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{8C209182-09AA-48EA-902C-6AAC66F47A76}" name="Table12" displayName="Table12" ref="A1:D4" totalsRowShown="0">
-  <autoFilter ref="A1:D4" xr:uid="{8C209182-09AA-48EA-902C-6AAC66F47A76}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{8C209182-09AA-48EA-902C-6AAC66F47A76}" name="Table12" displayName="Table12" ref="A1:D5" totalsRowShown="0">
+  <autoFilter ref="A1:D5" xr:uid="{8C209182-09AA-48EA-902C-6AAC66F47A76}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{27C63457-5CD9-4E66-9147-3F02C3CC7E21}" name="BOM"/>
     <tableColumn id="2" xr3:uid="{F36AEF9E-FAC6-46B7-9647-9D784C7A5C69}" name="VENDOR NAME"/>
@@ -2133,10 +2177,10 @@
         <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="D1" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -2183,19 +2227,19 @@
         <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="D1" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="E1" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="F1" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="G1" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -2203,10 +2247,10 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
       <c r="D2" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="E2">
         <v>331</v>
@@ -2217,7 +2261,7 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>162</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2225,10 +2269,10 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>163</v>
+        <v>172</v>
       </c>
       <c r="D4" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="E4">
         <v>176</v>
@@ -2242,7 +2286,7 @@
         <v>46</v>
       </c>
       <c r="D5" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="E5">
         <v>249</v>
@@ -2253,10 +2297,10 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>166</v>
+        <v>175</v>
       </c>
       <c r="D6" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="E6">
         <v>197</v>
@@ -2270,7 +2314,7 @@
         <v>48</v>
       </c>
       <c r="D7" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="E7">
         <v>277</v>
@@ -2284,7 +2328,7 @@
         <v>68</v>
       </c>
       <c r="D8" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
       <c r="E8">
         <v>237</v>
@@ -2298,7 +2342,7 @@
         <v>60</v>
       </c>
       <c r="D9" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="E9">
         <v>325</v>
@@ -2312,7 +2356,7 @@
         <v>59</v>
       </c>
       <c r="D10" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="E10">
         <v>155</v>
@@ -2326,7 +2370,7 @@
         <v>57</v>
       </c>
       <c r="D11" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="E11">
         <v>178</v>
@@ -2340,7 +2384,7 @@
         <v>46</v>
       </c>
       <c r="D12" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="E12">
         <v>227</v>
@@ -2351,7 +2395,7 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -2362,7 +2406,7 @@
         <v>56</v>
       </c>
       <c r="D14" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="E14">
         <v>357</v>
@@ -2373,10 +2417,10 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
       <c r="D15" t="s">
-        <v>175</v>
+        <v>184</v>
       </c>
       <c r="E15">
         <v>158</v>
@@ -2390,7 +2434,7 @@
         <v>52</v>
       </c>
       <c r="D16" t="s">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="E16">
         <v>314</v>
@@ -2404,7 +2448,7 @@
         <v>51</v>
       </c>
       <c r="D17" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="E17">
         <v>162</v>
@@ -2418,7 +2462,7 @@
         <v>49</v>
       </c>
       <c r="D18" t="s">
-        <v>178</v>
+        <v>187</v>
       </c>
       <c r="E18">
         <v>275</v>
@@ -2461,7 +2505,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>179</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -4074,102 +4118,95 @@
       </c>
     </row>
     <row r="70" spans="1:8">
-      <c r="A70" s="49" t="s">
-        <v>2</v>
-      </c>
-      <c r="B70" s="49" t="s">
+      <c r="A70" t="s">
+        <v>2</v>
+      </c>
+      <c r="B70" t="s">
         <v>4</v>
       </c>
-      <c r="C70" s="49" t="s">
+      <c r="C70" t="s">
         <v>80</v>
       </c>
       <c r="D70" s="48"/>
       <c r="E70" s="4">
         <v>45906</v>
       </c>
-      <c r="F70" s="49"/>
-      <c r="G70" s="49"/>
-      <c r="H70" s="49" t="s">
+      <c r="F70" s="4">
+        <v>45908</v>
+      </c>
+      <c r="H70" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="71" spans="1:8">
-      <c r="A71" s="49" t="s">
-        <v>2</v>
-      </c>
-      <c r="B71" s="49" t="s">
+      <c r="A71" t="s">
+        <v>2</v>
+      </c>
+      <c r="B71" t="s">
         <v>3</v>
       </c>
-      <c r="C71" s="49" t="s">
+      <c r="C71" t="s">
         <v>80</v>
       </c>
       <c r="D71" s="48"/>
       <c r="E71" s="4">
         <v>45906</v>
       </c>
-      <c r="F71" s="49"/>
-      <c r="G71" s="49"/>
-      <c r="H71" s="49" t="s">
+      <c r="H71" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="72" spans="1:8">
-      <c r="A72" s="49" t="s">
-        <v>2</v>
-      </c>
-      <c r="B72" s="49" t="s">
+      <c r="A72" t="s">
+        <v>2</v>
+      </c>
+      <c r="B72" t="s">
         <v>5</v>
       </c>
-      <c r="C72" s="49" t="s">
+      <c r="C72" t="s">
         <v>80</v>
       </c>
       <c r="D72" s="48"/>
       <c r="E72" s="4">
         <v>45906</v>
       </c>
-      <c r="F72" s="49"/>
-      <c r="G72" s="49"/>
-      <c r="H72" s="49" t="s">
+      <c r="H72" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="73" spans="1:8">
-      <c r="A73" s="49" t="s">
-        <v>2</v>
-      </c>
-      <c r="B73" s="49" t="s">
+      <c r="A73" t="s">
+        <v>2</v>
+      </c>
+      <c r="B73" t="s">
         <v>6</v>
       </c>
-      <c r="C73" s="49" t="s">
+      <c r="C73" t="s">
         <v>80</v>
       </c>
       <c r="D73" s="48"/>
       <c r="E73" s="4">
         <v>45906</v>
       </c>
-      <c r="F73" s="49"/>
-      <c r="G73" s="49"/>
-      <c r="H73" s="49" t="s">
+      <c r="H73" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="74" spans="1:8">
-      <c r="A74" s="49" t="s">
-        <v>2</v>
-      </c>
-      <c r="B74" s="49" t="s">
+      <c r="A74" t="s">
+        <v>2</v>
+      </c>
+      <c r="B74" t="s">
         <v>7</v>
       </c>
-      <c r="C74" s="49" t="s">
+      <c r="C74" t="s">
         <v>80</v>
       </c>
       <c r="D74" s="48"/>
       <c r="E74" s="4">
         <v>45906</v>
       </c>
-      <c r="F74" s="49"/>
-      <c r="G74" s="49"/>
-      <c r="H74" s="49" t="s">
+      <c r="H74" t="s">
         <v>38</v>
       </c>
     </row>
@@ -4402,7 +4439,7 @@
   <dimension ref="A1:K519"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4579,6 +4616,30 @@
       <c r="C6" s="27" t="s">
         <v>110</v>
       </c>
+      <c r="D6" s="27">
+        <v>199.13</v>
+      </c>
+      <c r="E6" s="27">
+        <v>200.13</v>
+      </c>
+      <c r="F6" s="27">
+        <v>200.34</v>
+      </c>
+      <c r="G6" s="27">
+        <v>200.18</v>
+      </c>
+      <c r="H6" s="27">
+        <v>201.76</v>
+      </c>
+      <c r="I6" s="27">
+        <v>200.79</v>
+      </c>
+      <c r="J6" s="27">
+        <v>191.41</v>
+      </c>
+      <c r="K6" s="27">
+        <v>192.51</v>
+      </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="46" t="s">
@@ -4590,6 +4651,7 @@
       <c r="C7" s="27" t="s">
         <v>110</v>
       </c>
+      <c r="D7" s="49"/>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="46" t="s">
@@ -4601,6 +4663,30 @@
       <c r="C8" s="27" t="s">
         <v>111</v>
       </c>
+      <c r="D8" s="27">
+        <v>199.77</v>
+      </c>
+      <c r="E8" s="27">
+        <v>198.87</v>
+      </c>
+      <c r="F8" s="27">
+        <v>199.88</v>
+      </c>
+      <c r="G8" s="27">
+        <v>200.3</v>
+      </c>
+      <c r="H8" s="27">
+        <v>201.46</v>
+      </c>
+      <c r="I8" s="27">
+        <v>198.79</v>
+      </c>
+      <c r="J8" s="27">
+        <v>298.87</v>
+      </c>
+      <c r="K8" s="27">
+        <v>197.29</v>
+      </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="46" t="s">
@@ -4612,18 +4698,170 @@
       <c r="C9" s="27" t="s">
         <v>111</v>
       </c>
+      <c r="D9" s="27">
+        <v>200.81</v>
+      </c>
+      <c r="E9" s="27">
+        <v>199.65</v>
+      </c>
+      <c r="F9" s="27">
+        <v>199.09</v>
+      </c>
+      <c r="G9" s="27">
+        <v>199.92</v>
+      </c>
+      <c r="H9" s="27">
+        <v>201.89</v>
+      </c>
+      <c r="I9" s="27">
+        <v>199.95</v>
+      </c>
+      <c r="J9" s="27">
+        <v>186.5</v>
+      </c>
+      <c r="K9" s="27">
+        <v>197.9</v>
+      </c>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="46"/>
+      <c r="A10" s="46" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="D10" s="27">
+        <v>200.86</v>
+      </c>
+      <c r="E10" s="27">
+        <v>199.89</v>
+      </c>
+      <c r="F10" s="27">
+        <v>199.73</v>
+      </c>
+      <c r="G10" s="27">
+        <v>200.63</v>
+      </c>
+      <c r="H10" s="27">
+        <v>200.94</v>
+      </c>
+      <c r="I10" s="27">
+        <v>199.11</v>
+      </c>
+      <c r="J10" s="27">
+        <v>196.33</v>
+      </c>
+      <c r="K10" s="27">
+        <v>197.23</v>
+      </c>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="46"/>
+      <c r="A11" s="46" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="D11" s="27">
+        <v>199.52</v>
+      </c>
+      <c r="E11" s="27">
+        <v>200.7</v>
+      </c>
+      <c r="F11" s="27">
+        <v>199.82</v>
+      </c>
+      <c r="G11" s="27">
+        <v>199.73</v>
+      </c>
+      <c r="H11" s="27">
+        <v>200.82</v>
+      </c>
+      <c r="I11" s="27">
+        <v>201.2</v>
+      </c>
+      <c r="J11" s="27">
+        <v>197.36</v>
+      </c>
+      <c r="K11" s="27">
+        <v>199.48</v>
+      </c>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="46"/>
+      <c r="A12" s="46" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="C12" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="D12" s="27">
+        <v>198.93</v>
+      </c>
+      <c r="E12" s="27">
+        <v>200.13</v>
+      </c>
+      <c r="F12" s="27">
+        <v>200.15</v>
+      </c>
+      <c r="G12" s="27">
+        <v>200.01</v>
+      </c>
+      <c r="H12" s="27">
+        <v>199</v>
+      </c>
+      <c r="I12" s="27">
+        <v>200.56</v>
+      </c>
+      <c r="J12" s="27">
+        <v>198.6</v>
+      </c>
+      <c r="K12" s="27">
+        <v>199.7</v>
+      </c>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="46"/>
+      <c r="A13" s="46" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="D13" s="27">
+        <v>200.1</v>
+      </c>
+      <c r="E13" s="27">
+        <v>200.2</v>
+      </c>
+      <c r="F13" s="27">
+        <v>199.35</v>
+      </c>
+      <c r="G13" s="27">
+        <v>200.34</v>
+      </c>
+      <c r="H13" s="27">
+        <v>200.15</v>
+      </c>
+      <c r="I13" s="27">
+        <v>199.33</v>
+      </c>
+      <c r="J13" s="27">
+        <v>197.75</v>
+      </c>
+      <c r="K13" s="27">
+        <v>200.15</v>
+      </c>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="46"/>
@@ -6174,10 +6412,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E993B7F-E878-4ABA-95AD-A4138848D6EF}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6199,14 +6437,14 @@
       <c r="A1" s="28"/>
       <c r="B1" s="29"/>
       <c r="C1" s="30" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D1" s="31"/>
       <c r="E1" s="30"/>
       <c r="F1" s="31"/>
       <c r="G1" s="32"/>
       <c r="H1" s="44" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="I1" s="32"/>
       <c r="J1" s="29"/>
@@ -6219,19 +6457,19 @@
         <v>24</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D2" s="36"/>
       <c r="E2" s="37" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="F2" s="38"/>
       <c r="G2" s="35" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="37" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="J2" s="38"/>
     </row>
@@ -6400,7 +6638,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="45" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C8" s="45">
         <v>166</v>
@@ -6425,6 +6663,34 @@
       </c>
       <c r="J8" s="45">
         <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="45" t="s">
+        <v>119</v>
+      </c>
+      <c r="C9" s="45">
+        <v>80</v>
+      </c>
+      <c r="D9" s="45">
+        <v>92</v>
+      </c>
+      <c r="E9" s="45">
+        <v>79</v>
+      </c>
+      <c r="F9" s="45">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="45" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -6442,7 +6708,7 @@
           <x14:formula1>
             <xm:f>Ref!$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>A3:A8</xm:sqref>
+          <xm:sqref>A3:A10</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -6452,10 +6718,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C8152F1-3340-4C7F-9B6C-3F6BB96763BA}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6474,10 +6740,10 @@
         <v>24</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="6" customFormat="1">
@@ -6501,7 +6767,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>119</v>
+        <v>122</v>
+      </c>
+      <c r="C3" s="50">
+        <v>14.6</v>
+      </c>
+      <c r="D3" s="50">
+        <v>1799.5</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -6509,7 +6781,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -6517,7 +6789,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -6525,7 +6797,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -6533,7 +6805,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -6541,7 +6813,13 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>124</v>
+        <v>127</v>
+      </c>
+      <c r="C8" s="50">
+        <v>16.5</v>
+      </c>
+      <c r="D8" s="50">
+        <v>1839.9</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -6549,7 +6827,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -6557,7 +6835,7 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -6565,7 +6843,7 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -6573,12 +6851,68 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>128</v>
+        <v>131</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>132</v>
+      </c>
+      <c r="C13" s="50">
+        <v>42.8</v>
+      </c>
+      <c r="D13" s="50">
+        <v>783.33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>133</v>
+      </c>
+      <c r="C14" s="50">
+        <v>69.3</v>
+      </c>
+      <c r="D14" s="50">
+        <v>1132.77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>134</v>
+      </c>
+      <c r="C15" s="50">
+        <v>68.599999999999994</v>
+      </c>
+      <c r="D15" s="50">
+        <v>1179.1300000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>135</v>
+      </c>
+      <c r="C16" s="50">
+        <v>88.7</v>
+      </c>
+      <c r="D16" s="50">
+        <v>1494.17</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B3 D2:D3 D5:D1048576 B8" xr:uid="{FCBF55FC-869D-43C4-B484-27D4BFDDD5A4}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B3 D9:D12 B8 D5:D7 D17:D1048576 D2" xr:uid="{FCBF55FC-869D-43C4-B484-27D4BFDDD5A4}"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576" xr:uid="{04F856B6-1846-4FF1-B3BB-4FE58494E678}">
       <formula1>"ENCAPSULANT, RIBBON"</formula1>
     </dataValidation>
@@ -6594,8 +6928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C0F3BDD-3989-4880-8737-F370069E1383}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6618,25 +6952,25 @@
         <v>24</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -6644,10 +6978,20 @@
         <v>2</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
+        <v>143</v>
+      </c>
+      <c r="D2">
+        <v>10.31</v>
+      </c>
+      <c r="E2">
+        <v>10.3</v>
+      </c>
+      <c r="F2" s="7">
+        <v>10.28</v>
+      </c>
+      <c r="G2" s="7">
+        <v>10.220000000000001</v>
+      </c>
       <c r="H2" s="7"/>
     </row>
     <row r="3" spans="1:9">
@@ -6655,10 +6999,20 @@
         <v>2</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
+        <v>144</v>
+      </c>
+      <c r="D3">
+        <v>9.92</v>
+      </c>
+      <c r="E3">
+        <v>9.94</v>
+      </c>
+      <c r="F3" s="7">
+        <v>9.93</v>
+      </c>
+      <c r="G3" s="7">
+        <v>9.83</v>
+      </c>
       <c r="H3" s="7"/>
     </row>
     <row r="4" spans="1:9">
@@ -6666,10 +7020,20 @@
         <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
+        <v>145</v>
+      </c>
+      <c r="D4">
+        <v>10.16</v>
+      </c>
+      <c r="E4">
+        <v>10.1</v>
+      </c>
+      <c r="F4" s="7">
+        <v>10.1</v>
+      </c>
+      <c r="G4" s="7">
+        <v>10.11</v>
+      </c>
       <c r="H4" s="7"/>
     </row>
     <row r="5" spans="1:9">
@@ -6677,10 +7041,20 @@
         <v>2</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
+        <v>146</v>
+      </c>
+      <c r="D5">
+        <v>9.66</v>
+      </c>
+      <c r="E5">
+        <v>9.61</v>
+      </c>
+      <c r="F5" s="7">
+        <v>9.7100000000000009</v>
+      </c>
+      <c r="G5" s="7">
+        <v>9.7200000000000006</v>
+      </c>
       <c r="H5" s="7"/>
     </row>
     <row r="6" spans="1:9">
@@ -6688,10 +7062,20 @@
         <v>2</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
+        <v>147</v>
+      </c>
+      <c r="D6">
+        <v>10.53</v>
+      </c>
+      <c r="E6">
+        <v>10.53</v>
+      </c>
+      <c r="F6" s="7">
+        <v>10.42</v>
+      </c>
+      <c r="G6" s="7">
+        <v>10.28</v>
+      </c>
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:9">
@@ -6699,24 +7083,33 @@
         <v>2</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
+        <v>148</v>
+      </c>
+      <c r="D7">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="E7">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="F7" s="7">
+        <v>9.9700000000000006</v>
+      </c>
+      <c r="G7" s="7">
+        <v>10</v>
+      </c>
       <c r="H7" s="7"/>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="50" t="s">
+      <c r="A8" t="s">
         <v>2</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="C8" s="50"/>
-      <c r="D8" s="50">
+        <v>149</v>
+      </c>
+      <c r="D8">
         <v>10.84</v>
       </c>
-      <c r="E8" s="50">
+      <c r="E8">
         <v>10.73</v>
       </c>
       <c r="F8" s="7">
@@ -6726,20 +7119,18 @@
         <v>10.5</v>
       </c>
       <c r="H8" s="7"/>
-      <c r="I8" s="50"/>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="50" t="s">
+      <c r="A9" t="s">
         <v>2</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="C9" s="50"/>
-      <c r="D9" s="50">
+        <v>150</v>
+      </c>
+      <c r="D9">
         <v>10.15</v>
       </c>
-      <c r="E9" s="50">
+      <c r="E9">
         <v>10.220000000000001</v>
       </c>
       <c r="F9" s="7">
@@ -6749,20 +7140,18 @@
         <v>10.11</v>
       </c>
       <c r="H9" s="7"/>
-      <c r="I9" s="50"/>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="50" t="s">
+      <c r="A10" t="s">
         <v>2</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="C10" s="50"/>
-      <c r="D10" s="50">
+        <v>147</v>
+      </c>
+      <c r="D10">
         <v>10.32</v>
       </c>
-      <c r="E10" s="50">
+      <c r="E10">
         <v>10.27</v>
       </c>
       <c r="F10" s="7">
@@ -6772,20 +7161,18 @@
         <v>10.3</v>
       </c>
       <c r="H10" s="7"/>
-      <c r="I10" s="50"/>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="50" t="s">
+      <c r="A11" t="s">
         <v>2</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="C11" s="50"/>
-      <c r="D11" s="50">
+        <v>148</v>
+      </c>
+      <c r="D11">
         <v>9.91</v>
       </c>
-      <c r="E11" s="50">
+      <c r="E11">
         <v>9.9499999999999993</v>
       </c>
       <c r="F11" s="7">
@@ -6795,7 +7182,6 @@
         <v>9.9</v>
       </c>
       <c r="H11" s="7"/>
-      <c r="I11" s="50"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -6825,7 +7211,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD5452B6-66C2-4964-BBFB-466116F6D217}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
@@ -6841,7 +7227,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="B1" t="s">
         <v>87</v>
@@ -6850,7 +7236,7 @@
         <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -6858,13 +7244,13 @@
         <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="C2" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D2" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -6872,13 +7258,29 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="C3" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="D3" t="s">
-        <v>150</v>
+        <v>158</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -6901,8 +7303,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19611726-A899-4D7E-9AA1-680BBD5826DA}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6921,10 +7323,10 @@
         <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="D1" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -6953,6 +7355,20 @@
       </c>
       <c r="D4" s="10">
         <v>0.60763888888888884</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C5" s="10">
+        <v>0.84722222222222221</v>
+      </c>
+      <c r="D5" s="10">
+        <v>0.91319444444444442</v>
       </c>
     </row>
     <row r="30" spans="3:3">

</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-09-11 10:42:29
</commit_message>
<xml_diff>
--- a/data/Solar_Lab_Tests.xlsx
+++ b/data/Solar_Lab_Tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1514" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0707AE21-33E5-4514-8644-04005D3B4C7B}"/>
+  <xr:revisionPtr revIDLastSave="1540" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1BA9E991-90EE-4FEA-9721-22425D22EA88}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="3" activeTab="8" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="10" activeTab="7" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Tests Map" sheetId="4" state="hidden" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="196">
   <si>
     <t>BOM</t>
   </si>
@@ -609,9 +609,21 @@
     <t>270MV</t>
   </si>
   <si>
+    <t>271MV</t>
+  </si>
+  <si>
     <t>252MV</t>
   </si>
   <si>
+    <t>268MV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QC SOLAR CHINA </t>
+  </si>
+  <si>
+    <t>272MV</t>
+  </si>
+  <si>
     <t>257MV</t>
   </si>
   <si>
@@ -633,7 +645,16 @@
     <t>288MV</t>
   </si>
   <si>
+    <t>315MV</t>
+  </si>
+  <si>
     <t>255MV</t>
+  </si>
+  <si>
+    <t>261MV</t>
+  </si>
+  <si>
+    <t>UKTR BD 2000L</t>
   </si>
   <si>
     <t>STANDARD DURATION (DAYS)</t>
@@ -1041,8 +1062,8 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1055,6 +1076,7 @@
       <font>
         <b val="0"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -1474,8 +1496,8 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{97A8C2A7-46C0-4446-B562-6550EA520638}" name="Table10" displayName="Table10" ref="A1:I11" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:I11" xr:uid="{97A8C2A7-46C0-4446-B562-6550EA520638}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{97A8C2A7-46C0-4446-B562-6550EA520638}" name="Table10" displayName="Table10" ref="A1:I15" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:I15" xr:uid="{97A8C2A7-46C0-4446-B562-6550EA520638}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{FE721515-FBBB-4487-ABCE-AAB6A5B1513A}" name="BOM" dataDxfId="9"/>
     <tableColumn id="9" xr3:uid="{304FA6D2-898E-427A-8AC1-958C15295938}" name="VENDOR NAME" dataDxfId="8"/>
@@ -1485,7 +1507,9 @@
     <tableColumn id="5" xr3:uid="{BB8F60AF-F7B1-4306-8198-B69EE3E6D97A}" name="min value 3" dataDxfId="4"/>
     <tableColumn id="6" xr3:uid="{03425EE3-EC03-4913-B402-224F846A29D7}" name="min value 4" dataDxfId="3"/>
     <tableColumn id="7" xr3:uid="{E68E3244-13A5-47AA-8AB7-F602EE938E20}" name="min value 5" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{D5BE9073-1EC1-4D18-A75C-7F63CCD62CB2}" name="Mean" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{D5BE9073-1EC1-4D18-A75C-7F63CCD62CB2}" name="Mean" dataDxfId="1">
+      <calculatedColumnFormula>AVERAGE(Table10[[#This Row],[min value 1 ]:[min value 5]])</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2202,10 +2226,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{333C0630-51CF-46CA-8CAD-98FEF9AC181F}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView topLeftCell="B6" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2333,6 +2357,12 @@
       <c r="E8">
         <v>237</v>
       </c>
+      <c r="F8" t="s">
+        <v>179</v>
+      </c>
+      <c r="G8">
+        <v>217</v>
+      </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
@@ -2342,7 +2372,7 @@
         <v>60</v>
       </c>
       <c r="D9" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E9">
         <v>325</v>
@@ -2361,19 +2391,31 @@
       <c r="E10">
         <v>155</v>
       </c>
+      <c r="F10" t="s">
+        <v>181</v>
+      </c>
+      <c r="G10">
+        <v>202</v>
+      </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>57</v>
+        <v>182</v>
       </c>
       <c r="D11" t="s">
         <v>173</v>
       </c>
       <c r="E11">
         <v>178</v>
+      </c>
+      <c r="F11" t="s">
+        <v>183</v>
+      </c>
+      <c r="G11">
+        <v>185</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -2384,7 +2426,7 @@
         <v>46</v>
       </c>
       <c r="D12" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="E12">
         <v>227</v>
@@ -2395,7 +2437,7 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -2406,7 +2448,7 @@
         <v>56</v>
       </c>
       <c r="D14" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="E14">
         <v>357</v>
@@ -2417,10 +2459,10 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="D15" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="E15">
         <v>158</v>
@@ -2434,13 +2476,13 @@
         <v>52</v>
       </c>
       <c r="D16" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="E16">
         <v>314</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -2448,13 +2490,19 @@
         <v>51</v>
       </c>
       <c r="D17" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="E17">
         <v>162</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="F17" t="s">
+        <v>191</v>
+      </c>
+      <c r="G17">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -2462,15 +2510,29 @@
         <v>49</v>
       </c>
       <c r="D18" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="E18">
         <v>275</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="F18" t="s">
+        <v>193</v>
+      </c>
+      <c r="G18">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>15</v>
+      </c>
+      <c r="B19" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="B20" t="s">
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -2505,7 +2567,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2634,7 +2696,7 @@
   <dimension ref="A1:K74"/>
   <sheetViews>
     <sheetView topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="H74" sqref="H74"/>
+      <selection activeCell="F75" sqref="F75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -4170,6 +4232,9 @@
       <c r="E72" s="4">
         <v>45906</v>
       </c>
+      <c r="F72" s="4">
+        <v>45910</v>
+      </c>
       <c r="H72" t="s">
         <v>38</v>
       </c>
@@ -4188,6 +4253,9 @@
       <c r="E73" s="4">
         <v>45906</v>
       </c>
+      <c r="F73" s="4">
+        <v>45910</v>
+      </c>
       <c r="H73" t="s">
         <v>38</v>
       </c>
@@ -4205,6 +4273,9 @@
       <c r="D74" s="48"/>
       <c r="E74" s="4">
         <v>45906</v>
+      </c>
+      <c r="F74" s="4">
+        <v>45910</v>
       </c>
       <c r="H74" t="s">
         <v>38</v>
@@ -4651,7 +4722,6 @@
       <c r="C7" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="D7" s="49"/>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="46" t="s">
@@ -6384,7 +6454,7 @@
   </sheetData>
   <dataValidations count="3">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 C4:C5" xr:uid="{5C73BBC5-C68D-4586-BDB5-A3BE48854FB6}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:K7 B4:B1048576" xr:uid="{18FD80CD-FFDC-48A1-BA45-91576461B09B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B1048576" xr:uid="{18FD80CD-FFDC-48A1-BA45-91576461B09B}">
       <formula1>"FRONT EPE, BACK EVA"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4:A1048576" xr:uid="{CDEE756C-C284-45D8-BDCE-F4798D4B3C50}">
@@ -6415,7 +6485,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6721,7 +6791,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6769,10 +6839,10 @@
       <c r="B3" t="s">
         <v>122</v>
       </c>
-      <c r="C3" s="50">
+      <c r="C3" s="49">
         <v>14.6</v>
       </c>
-      <c r="D3" s="50">
+      <c r="D3" s="49">
         <v>1799.5</v>
       </c>
     </row>
@@ -6815,10 +6885,10 @@
       <c r="B8" t="s">
         <v>127</v>
       </c>
-      <c r="C8" s="50">
+      <c r="C8" s="49">
         <v>16.5</v>
       </c>
-      <c r="D8" s="50">
+      <c r="D8" s="49">
         <v>1839.9</v>
       </c>
     </row>
@@ -6861,10 +6931,10 @@
       <c r="B13" t="s">
         <v>132</v>
       </c>
-      <c r="C13" s="50">
+      <c r="C13" s="49">
         <v>42.8</v>
       </c>
-      <c r="D13" s="50">
+      <c r="D13" s="49">
         <v>783.33</v>
       </c>
     </row>
@@ -6875,10 +6945,10 @@
       <c r="B14" t="s">
         <v>133</v>
       </c>
-      <c r="C14" s="50">
+      <c r="C14" s="49">
         <v>69.3</v>
       </c>
-      <c r="D14" s="50">
+      <c r="D14" s="49">
         <v>1132.77</v>
       </c>
     </row>
@@ -6889,10 +6959,10 @@
       <c r="B15" t="s">
         <v>134</v>
       </c>
-      <c r="C15" s="50">
+      <c r="C15" s="49">
         <v>68.599999999999994</v>
       </c>
-      <c r="D15" s="50">
+      <c r="D15" s="49">
         <v>1179.1300000000001</v>
       </c>
     </row>
@@ -6903,10 +6973,10 @@
       <c r="B16" t="s">
         <v>135</v>
       </c>
-      <c r="C16" s="50">
+      <c r="C16" s="49">
         <v>88.7</v>
       </c>
-      <c r="D16" s="50">
+      <c r="D16" s="49">
         <v>1494.17</v>
       </c>
     </row>
@@ -6926,10 +6996,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C0F3BDD-3989-4880-8737-F370069E1383}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6993,6 +7063,10 @@
         <v>10.220000000000001</v>
       </c>
       <c r="H2" s="7"/>
+      <c r="I2">
+        <f>AVERAGE(Table10[[#This Row],[min value 1 ]:[min value 5]])</f>
+        <v>10.2775</v>
+      </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
@@ -7014,6 +7088,10 @@
         <v>9.83</v>
       </c>
       <c r="H3" s="7"/>
+      <c r="I3">
+        <f>AVERAGE(Table10[[#This Row],[min value 1 ]:[min value 5]])</f>
+        <v>9.9049999999999994</v>
+      </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
@@ -7035,6 +7113,10 @@
         <v>10.11</v>
       </c>
       <c r="H4" s="7"/>
+      <c r="I4">
+        <f>AVERAGE(Table10[[#This Row],[min value 1 ]:[min value 5]])</f>
+        <v>10.1175</v>
+      </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
@@ -7056,6 +7138,10 @@
         <v>9.7200000000000006</v>
       </c>
       <c r="H5" s="7"/>
+      <c r="I5">
+        <f>AVERAGE(Table10[[#This Row],[min value 1 ]:[min value 5]])</f>
+        <v>9.6750000000000007</v>
+      </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
@@ -7077,6 +7163,10 @@
         <v>10.28</v>
       </c>
       <c r="H6" s="7"/>
+      <c r="I6">
+        <f>AVERAGE(Table10[[#This Row],[min value 1 ]:[min value 5]])</f>
+        <v>10.44</v>
+      </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
@@ -7098,6 +7188,10 @@
         <v>10</v>
       </c>
       <c r="H7" s="7"/>
+      <c r="I7">
+        <f>AVERAGE(Table10[[#This Row],[min value 1 ]:[min value 5]])</f>
+        <v>9.9674999999999994</v>
+      </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
@@ -7119,6 +7213,10 @@
         <v>10.5</v>
       </c>
       <c r="H8" s="7"/>
+      <c r="I8">
+        <f>AVERAGE(Table10[[#This Row],[min value 1 ]:[min value 5]])</f>
+        <v>10.6975</v>
+      </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
@@ -7140,6 +7238,10 @@
         <v>10.11</v>
       </c>
       <c r="H9" s="7"/>
+      <c r="I9">
+        <f>AVERAGE(Table10[[#This Row],[min value 1 ]:[min value 5]])</f>
+        <v>10.15</v>
+      </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
@@ -7161,6 +7263,10 @@
         <v>10.3</v>
       </c>
       <c r="H10" s="7"/>
+      <c r="I10">
+        <f>AVERAGE(Table10[[#This Row],[min value 1 ]:[min value 5]])</f>
+        <v>10.275</v>
+      </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
@@ -7182,6 +7288,50 @@
         <v>9.9</v>
       </c>
       <c r="H11" s="7"/>
+      <c r="I11">
+        <f>AVERAGE(Table10[[#This Row],[min value 1 ]:[min value 5]])</f>
+        <v>9.9224999999999994</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="50"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="50"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="50"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="50"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="50"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="50"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -7213,8 +7363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD5452B6-66C2-4964-BBFB-466116F6D217}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7303,8 +7453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19611726-A899-4D7E-9AA1-680BBD5826DA}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-09-15 13:05:37
</commit_message>
<xml_diff>
--- a/data/Solar_Lab_Tests.xlsx
+++ b/data/Solar_Lab_Tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1540" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1BA9E991-90EE-4FEA-9721-22425D22EA88}"/>
+  <xr:revisionPtr revIDLastSave="1560" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{12A933FC-8908-4573-A661-3915908E0538}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="10" activeTab="7" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="7" activeTab="8" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Tests Map" sheetId="4" state="hidden" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="211">
   <si>
     <t>BOM</t>
   </si>
@@ -582,7 +582,10 @@
     <t>CAHORS 30A</t>
   </si>
   <si>
-    <t>262MV</t>
+    <t>262mV</t>
+  </si>
+  <si>
+    <t>331 µA</t>
   </si>
   <si>
     <t>UKTR BD IEL</t>
@@ -591,28 +594,43 @@
     <t>UKTR 20A MJB</t>
   </si>
   <si>
-    <t>302MV</t>
-  </si>
-  <si>
-    <t>260MV</t>
+    <t>176 µA</t>
+  </si>
+  <si>
+    <t>249 µA</t>
   </si>
   <si>
     <t>UKTR30A</t>
   </si>
   <si>
-    <t>267MV</t>
-  </si>
-  <si>
-    <t>301MV</t>
-  </si>
-  <si>
-    <t>270MV</t>
+    <t>267mV</t>
+  </si>
+  <si>
+    <t>197  µA</t>
+  </si>
+  <si>
+    <t>301mV</t>
+  </si>
+  <si>
+    <t>277µA</t>
+  </si>
+  <si>
+    <t>270mV</t>
+  </si>
+  <si>
+    <t>237µA</t>
   </si>
   <si>
     <t>271MV</t>
   </si>
   <si>
-    <t>252MV</t>
+    <t>252mV</t>
+  </si>
+  <si>
+    <t>325µA</t>
+  </si>
+  <si>
+    <t>155µA</t>
   </si>
   <si>
     <t>268MV</t>
@@ -621,40 +639,67 @@
     <t xml:space="preserve">QC SOLAR CHINA </t>
   </si>
   <si>
+    <t>302mV</t>
+  </si>
+  <si>
+    <t>178µA</t>
+  </si>
+  <si>
     <t>272MV</t>
   </si>
   <si>
-    <t>257MV</t>
+    <t>257mV</t>
+  </si>
+  <si>
+    <t>227µA</t>
   </si>
   <si>
     <t xml:space="preserve">QC SOLAR SMART </t>
   </si>
   <si>
-    <t>243MV</t>
+    <t>243mV</t>
+  </si>
+  <si>
+    <t>357µA</t>
   </si>
   <si>
     <t>VEMOULD20A</t>
   </si>
   <si>
-    <t>285MV</t>
-  </si>
-  <si>
-    <t>247MV</t>
-  </si>
-  <si>
-    <t>288MV</t>
+    <t>285mV</t>
+  </si>
+  <si>
+    <t>158µA</t>
+  </si>
+  <si>
+    <t>247mV</t>
+  </si>
+  <si>
+    <t>314µA</t>
+  </si>
+  <si>
+    <t>288mV</t>
+  </si>
+  <si>
+    <t>162µA</t>
   </si>
   <si>
     <t>315MV</t>
   </si>
   <si>
-    <t>255MV</t>
+    <t>255mV</t>
+  </si>
+  <si>
+    <t>275µA</t>
   </si>
   <si>
     <t>261MV</t>
   </si>
   <si>
     <t>UKTR BD 2000L</t>
+  </si>
+  <si>
+    <t>UKTR BD 7500L</t>
   </si>
   <si>
     <t>STANDARD DURATION (DAYS)</t>
@@ -984,7 +1029,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1063,7 +1108,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2228,7 +2272,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{333C0630-51CF-46CA-8CAD-98FEF9AC181F}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView topLeftCell="B6" workbookViewId="0">
+    <sheetView topLeftCell="B16" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -2276,8 +2320,8 @@
       <c r="D2" t="s">
         <v>170</v>
       </c>
-      <c r="E2">
-        <v>331</v>
+      <c r="E2" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2285,7 +2329,7 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2293,13 +2337,13 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>172</v>
-      </c>
-      <c r="D4" t="s">
         <v>173</v>
       </c>
-      <c r="E4">
-        <v>176</v>
+      <c r="D4">
+        <v>302</v>
+      </c>
+      <c r="E4" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -2309,11 +2353,11 @@
       <c r="B5" t="s">
         <v>46</v>
       </c>
-      <c r="D5" t="s">
-        <v>174</v>
-      </c>
-      <c r="E5">
-        <v>249</v>
+      <c r="D5">
+        <v>260</v>
+      </c>
+      <c r="E5" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -2321,13 +2365,13 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D6" t="s">
-        <v>176</v>
-      </c>
-      <c r="E6">
-        <v>197</v>
+        <v>177</v>
+      </c>
+      <c r="E6" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -2338,10 +2382,10 @@
         <v>48</v>
       </c>
       <c r="D7" t="s">
-        <v>177</v>
-      </c>
-      <c r="E7">
-        <v>277</v>
+        <v>179</v>
+      </c>
+      <c r="E7" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -2352,13 +2396,13 @@
         <v>68</v>
       </c>
       <c r="D8" t="s">
-        <v>178</v>
-      </c>
-      <c r="E8">
-        <v>237</v>
+        <v>181</v>
+      </c>
+      <c r="E8" t="s">
+        <v>182</v>
       </c>
       <c r="F8" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="G8">
         <v>217</v>
@@ -2372,10 +2416,10 @@
         <v>60</v>
       </c>
       <c r="D9" t="s">
-        <v>180</v>
-      </c>
-      <c r="E9">
-        <v>325</v>
+        <v>184</v>
+      </c>
+      <c r="E9" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -2386,13 +2430,13 @@
         <v>59</v>
       </c>
       <c r="D10" t="s">
-        <v>176</v>
-      </c>
-      <c r="E10">
-        <v>155</v>
+        <v>177</v>
+      </c>
+      <c r="E10" t="s">
+        <v>186</v>
       </c>
       <c r="F10" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="G10">
         <v>202</v>
@@ -2403,16 +2447,16 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="D11" t="s">
-        <v>173</v>
-      </c>
-      <c r="E11">
-        <v>178</v>
+        <v>189</v>
+      </c>
+      <c r="E11" t="s">
+        <v>190</v>
       </c>
       <c r="F11" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="G11">
         <v>185</v>
@@ -2426,10 +2470,10 @@
         <v>46</v>
       </c>
       <c r="D12" t="s">
-        <v>184</v>
-      </c>
-      <c r="E12">
-        <v>227</v>
+        <v>192</v>
+      </c>
+      <c r="E12" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -2437,7 +2481,7 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>185</v>
+        <v>194</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -2448,10 +2492,10 @@
         <v>56</v>
       </c>
       <c r="D14" t="s">
-        <v>186</v>
-      </c>
-      <c r="E14">
-        <v>357</v>
+        <v>195</v>
+      </c>
+      <c r="E14" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -2459,13 +2503,13 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
       <c r="D15" t="s">
-        <v>188</v>
-      </c>
-      <c r="E15">
-        <v>158</v>
+        <v>198</v>
+      </c>
+      <c r="E15" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -2476,10 +2520,10 @@
         <v>52</v>
       </c>
       <c r="D16" t="s">
-        <v>189</v>
-      </c>
-      <c r="E16">
-        <v>314</v>
+        <v>200</v>
+      </c>
+      <c r="E16" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -2490,13 +2534,13 @@
         <v>51</v>
       </c>
       <c r="D17" t="s">
-        <v>190</v>
-      </c>
-      <c r="E17">
-        <v>162</v>
+        <v>202</v>
+      </c>
+      <c r="E17" t="s">
+        <v>203</v>
       </c>
       <c r="F17" t="s">
-        <v>191</v>
+        <v>204</v>
       </c>
       <c r="G17">
         <v>134</v>
@@ -2510,13 +2554,13 @@
         <v>49</v>
       </c>
       <c r="D18" t="s">
-        <v>192</v>
-      </c>
-      <c r="E18">
-        <v>275</v>
+        <v>205</v>
+      </c>
+      <c r="E18" t="s">
+        <v>206</v>
       </c>
       <c r="F18" t="s">
-        <v>193</v>
+        <v>207</v>
       </c>
       <c r="G18">
         <v>297</v>
@@ -2527,12 +2571,12 @@
         <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>194</v>
+        <v>208</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="B20" t="s">
-        <v>194</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -2567,7 +2611,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>195</v>
+        <v>210</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2695,7 +2739,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9401EE47-EA52-49C7-BBC0-21F5B88254FB}">
   <dimension ref="A1:K74"/>
   <sheetViews>
-    <sheetView topLeftCell="A59" workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="F75" sqref="F75"/>
     </sheetView>
   </sheetViews>
@@ -7294,41 +7338,25 @@
       </c>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="50"/>
       <c r="B12" s="8"/>
-      <c r="C12" s="50"/>
-      <c r="D12" s="50"/>
-      <c r="E12" s="50"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="50"/>
       <c r="B13" s="8"/>
-      <c r="C13" s="50"/>
-      <c r="D13" s="50"/>
-      <c r="E13" s="50"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="50"/>
       <c r="B14" s="8"/>
-      <c r="C14" s="50"/>
-      <c r="D14" s="50"/>
-      <c r="E14" s="50"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="50"/>
       <c r="B15" s="8"/>
-      <c r="C15" s="50"/>
-      <c r="D15" s="50"/>
-      <c r="E15" s="50"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
@@ -7363,7 +7391,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD5452B6-66C2-4964-BBFB-466116F6D217}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -7453,7 +7481,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19611726-A899-4D7E-9AA1-680BBD5826DA}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-09-18 09:42:33
</commit_message>
<xml_diff>
--- a/data/Solar_Lab_Tests.xlsx
+++ b/data/Solar_Lab_Tests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29303"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1560" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{12A933FC-8908-4573-A661-3915908E0538}"/>
+  <xr:revisionPtr revIDLastSave="1606" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{128B1E71-991A-4C08-B8DE-507265C723C7}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="7" activeTab="8" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="8" activeTab="8" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Tests Map" sheetId="4" state="hidden" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <definedName name="ENCAPTYPE">Ref!$K$2:$K$1048576</definedName>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">'Material Tests Map'!$A$1:$B$20</definedName>
     <definedName name="ExternalData_1" localSheetId="11" hidden="1">'Standard test times'!$A$1:$B$15</definedName>
-    <definedName name="ExternalData_1" localSheetId="1" hidden="1">'Test Data'!$A$1:$H$74</definedName>
+    <definedName name="ExternalData_1" localSheetId="1" hidden="1">'Test Data'!$A$1:$H$80</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="212">
   <si>
     <t>BOM</t>
   </si>
@@ -315,6 +315,9 @@
     <t>SHEETSOL</t>
   </si>
   <si>
+    <t>ENERLITE</t>
+  </si>
+  <si>
     <t>RM Type</t>
   </si>
   <si>
@@ -555,7 +558,7 @@
     <t>END TIME</t>
   </si>
   <si>
-    <t>FASTO</t>
+    <t>FASTO POTTING</t>
   </si>
   <si>
     <t>TIME</t>
@@ -1029,7 +1032,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1108,6 +1111,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1626,7 +1630,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{06A3AD80-C098-4015-85FF-3495CE4443EA}" name="Test_Data" displayName="Test_Data" ref="A1:H74" tableType="queryTable" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{06A3AD80-C098-4015-85FF-3495CE4443EA}" name="Test_Data" displayName="Test_Data" ref="A1:H80" tableType="queryTable" totalsRowShown="0">
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{87F75B08-44C4-4718-834D-87FEE9F87970}" uniqueName="1" name="BOM" queryTableFieldId="1" dataDxfId="42"/>
     <tableColumn id="2" xr3:uid="{1E5F4521-5E5C-4948-AEB2-FC5F712DB353}" uniqueName="2" name="TEST NAME" queryTableFieldId="2" dataDxfId="41"/>
@@ -2245,10 +2249,10 @@
         <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -2295,19 +2299,19 @@
         <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="F1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="G1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -2315,13 +2319,13 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2329,7 +2333,7 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2337,13 +2341,13 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D4">
         <v>302</v>
       </c>
       <c r="E4" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -2357,7 +2361,7 @@
         <v>260</v>
       </c>
       <c r="E5" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -2365,13 +2369,13 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D6" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E6" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -2382,10 +2386,10 @@
         <v>48</v>
       </c>
       <c r="D7" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E7" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -2396,13 +2400,13 @@
         <v>68</v>
       </c>
       <c r="D8" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E8" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="F8" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="G8">
         <v>217</v>
@@ -2416,10 +2420,10 @@
         <v>60</v>
       </c>
       <c r="D9" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E9" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -2430,13 +2434,13 @@
         <v>59</v>
       </c>
       <c r="D10" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E10" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F10" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G10">
         <v>202</v>
@@ -2447,16 +2451,16 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D11" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E11" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="F11" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="G11">
         <v>185</v>
@@ -2470,10 +2474,10 @@
         <v>46</v>
       </c>
       <c r="D12" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E12" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -2481,7 +2485,7 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -2492,10 +2496,10 @@
         <v>56</v>
       </c>
       <c r="D14" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E14" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -2503,13 +2507,13 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D15" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E15" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -2520,10 +2524,10 @@
         <v>52</v>
       </c>
       <c r="D16" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E16" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -2534,13 +2538,13 @@
         <v>51</v>
       </c>
       <c r="D17" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E17" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F17" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="G17">
         <v>134</v>
@@ -2554,13 +2558,13 @@
         <v>49</v>
       </c>
       <c r="D18" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E18" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F18" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="G18">
         <v>297</v>
@@ -2571,12 +2575,12 @@
         <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="B20" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -2611,7 +2615,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2737,10 +2741,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9401EE47-EA52-49C7-BBC0-21F5B88254FB}">
-  <dimension ref="A1:K74"/>
+  <dimension ref="A1:K80"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="F75" sqref="F75"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -4324,6 +4328,115 @@
       <c r="H74" t="s">
         <v>38</v>
       </c>
+    </row>
+    <row r="75" spans="1:8">
+      <c r="A75" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="B75" t="s">
+        <v>4</v>
+      </c>
+      <c r="C75" s="50" t="s">
+        <v>81</v>
+      </c>
+      <c r="D75" s="48"/>
+      <c r="E75" s="4">
+        <v>45916</v>
+      </c>
+      <c r="F75" s="50"/>
+      <c r="G75" s="50"/>
+      <c r="H75" s="50" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8">
+      <c r="A76" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="B76" t="s">
+        <v>3</v>
+      </c>
+      <c r="C76" s="50" t="s">
+        <v>81</v>
+      </c>
+      <c r="D76" s="48"/>
+      <c r="E76" s="4">
+        <v>45916</v>
+      </c>
+      <c r="F76" s="50"/>
+      <c r="G76" s="50"/>
+      <c r="H76" s="50" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8">
+      <c r="A77" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="B77" t="s">
+        <v>5</v>
+      </c>
+      <c r="C77" s="50" t="s">
+        <v>81</v>
+      </c>
+      <c r="D77" s="48"/>
+      <c r="E77" s="4">
+        <v>45916</v>
+      </c>
+      <c r="F77" s="50"/>
+      <c r="G77" s="50"/>
+      <c r="H77" s="50" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8">
+      <c r="A78" t="s">
+        <v>2</v>
+      </c>
+      <c r="B78" t="s">
+        <v>6</v>
+      </c>
+      <c r="C78" s="50" t="s">
+        <v>81</v>
+      </c>
+      <c r="D78" s="48"/>
+      <c r="E78" s="4">
+        <v>45916</v>
+      </c>
+      <c r="F78" s="50"/>
+      <c r="G78" s="50"/>
+      <c r="H78" s="50" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8">
+      <c r="A79" t="s">
+        <v>2</v>
+      </c>
+      <c r="B79" t="s">
+        <v>7</v>
+      </c>
+      <c r="C79" s="50" t="s">
+        <v>81</v>
+      </c>
+      <c r="D79" s="48"/>
+      <c r="E79" s="4">
+        <v>45916</v>
+      </c>
+      <c r="F79" s="50"/>
+      <c r="G79" s="50"/>
+      <c r="H79" s="50" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8">
+      <c r="B80" s="50"/>
+      <c r="C80" s="50"/>
+      <c r="D80" s="48"/>
+      <c r="E80" s="50"/>
+      <c r="F80" s="50"/>
+      <c r="G80" s="50"/>
+      <c r="H80" s="50"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -4388,25 +4501,25 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="I1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="N1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -4423,10 +4536,10 @@
         <v>32</v>
       </c>
       <c r="K2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="N2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -4443,10 +4556,10 @@
         <v>38</v>
       </c>
       <c r="K3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="N3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -4457,10 +4570,10 @@
         <v>5</v>
       </c>
       <c r="G4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -4571,19 +4684,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>24</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E1" s="16"/>
       <c r="F1" s="16"/>
       <c r="G1" s="16"/>
       <c r="H1" s="17" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I1" s="18"/>
       <c r="J1" s="18"/>
@@ -4594,61 +4707,61 @@
       <c r="B2" s="20"/>
       <c r="C2" s="20"/>
       <c r="D2" s="21" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E2" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="H2" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="I2" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="J2" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="H2" s="23" t="s">
-        <v>96</v>
-      </c>
-      <c r="I2" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="J2" s="24" t="s">
-        <v>98</v>
-      </c>
       <c r="K2" s="25" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:11" hidden="1">
       <c r="A3" s="46"/>
       <c r="B3" s="26" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F3" s="26" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G3" s="26" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H3" s="26" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="I3" s="26" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="J3" s="26" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="K3" s="26" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -4656,7 +4769,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C4" t="s">
         <v>35</v>
@@ -4691,7 +4804,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C5" t="s">
         <v>35</v>
@@ -4726,10 +4839,10 @@
         <v>2</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D6" s="27">
         <v>199.13</v>
@@ -4761,10 +4874,10 @@
         <v>2</v>
       </c>
       <c r="B7" s="27" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C7" s="27" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -4772,10 +4885,10 @@
         <v>2</v>
       </c>
       <c r="B8" s="27" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C8" s="27" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D8" s="27">
         <v>199.77</v>
@@ -4807,10 +4920,10 @@
         <v>2</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D9" s="27">
         <v>200.81</v>
@@ -4842,10 +4955,10 @@
         <v>2</v>
       </c>
       <c r="B10" s="27" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D10" s="27">
         <v>200.86</v>
@@ -4877,10 +4990,10 @@
         <v>2</v>
       </c>
       <c r="B11" s="27" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D11" s="27">
         <v>199.52</v>
@@ -4912,10 +5025,10 @@
         <v>2</v>
       </c>
       <c r="B12" s="27" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D12" s="27">
         <v>198.93</v>
@@ -4947,10 +5060,10 @@
         <v>2</v>
       </c>
       <c r="B13" s="27" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C13" s="27" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D13" s="27">
         <v>200.1</v>
@@ -6526,10 +6639,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E993B7F-E878-4ABA-95AD-A4138848D6EF}">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6551,14 +6664,14 @@
       <c r="A1" s="28"/>
       <c r="B1" s="29"/>
       <c r="C1" s="30" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D1" s="31"/>
       <c r="E1" s="30"/>
       <c r="F1" s="31"/>
       <c r="G1" s="32"/>
       <c r="H1" s="44" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I1" s="32"/>
       <c r="J1" s="29"/>
@@ -6571,19 +6684,19 @@
         <v>24</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D2" s="36"/>
       <c r="E2" s="37" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F2" s="38"/>
       <c r="G2" s="35" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="37" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J2" s="38"/>
     </row>
@@ -6621,34 +6734,34 @@
     </row>
     <row r="4" spans="1:10" customFormat="1" hidden="1">
       <c r="A4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G4" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="I4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -6688,7 +6801,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="45" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C6" s="45">
         <v>125</v>
@@ -6720,7 +6833,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="45" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C7" s="45">
         <v>125</v>
@@ -6752,7 +6865,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="45" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C8" s="45">
         <v>166</v>
@@ -6784,7 +6897,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="45" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C9" s="45">
         <v>80</v>
@@ -6805,6 +6918,58 @@
       </c>
       <c r="B10" s="45" t="s">
         <v>80</v>
+      </c>
+      <c r="C10" s="45">
+        <v>58</v>
+      </c>
+      <c r="D10" s="45">
+        <v>50</v>
+      </c>
+      <c r="E10" s="45">
+        <v>95</v>
+      </c>
+      <c r="F10" s="45">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="45" t="s">
+        <v>81</v>
+      </c>
+      <c r="C11" s="45">
+        <v>11</v>
+      </c>
+      <c r="D11" s="45">
+        <v>3</v>
+      </c>
+      <c r="E11" s="45">
+        <v>70</v>
+      </c>
+      <c r="F11" s="45">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="45" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" s="45">
+        <v>2</v>
+      </c>
+      <c r="D12" s="45">
+        <v>8</v>
+      </c>
+      <c r="E12" s="45">
+        <v>101</v>
+      </c>
+      <c r="F12" s="45">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -6822,7 +6987,7 @@
           <x14:formula1>
             <xm:f>Ref!$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>A3:A10</xm:sqref>
+          <xm:sqref>A3:A12</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -6854,10 +7019,10 @@
         <v>24</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="6" customFormat="1">
@@ -6881,7 +7046,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C3" s="49">
         <v>14.6</v>
@@ -6895,7 +7060,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -6903,7 +7068,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -6911,7 +7076,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -6919,7 +7084,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -6927,7 +7092,7 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C8" s="49">
         <v>16.5</v>
@@ -6941,7 +7106,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -6949,7 +7114,7 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -6957,7 +7122,7 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -6965,7 +7130,7 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -6973,7 +7138,7 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C13" s="49">
         <v>42.8</v>
@@ -6987,7 +7152,7 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C14" s="49">
         <v>69.3</v>
@@ -7001,7 +7166,7 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C15" s="49">
         <v>68.599999999999994</v>
@@ -7015,7 +7180,7 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C16" s="49">
         <v>88.7</v>
@@ -7066,25 +7231,25 @@
         <v>24</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -7092,7 +7257,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D2">
         <v>10.31</v>
@@ -7117,7 +7282,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D3">
         <v>9.92</v>
@@ -7142,7 +7307,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D4">
         <v>10.16</v>
@@ -7167,7 +7332,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D5">
         <v>9.66</v>
@@ -7192,7 +7357,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D6">
         <v>10.53</v>
@@ -7217,7 +7382,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D7">
         <v>9.9499999999999993</v>
@@ -7242,7 +7407,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D8">
         <v>10.84</v>
@@ -7267,7 +7432,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D9">
         <v>10.15</v>
@@ -7292,7 +7457,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D10">
         <v>10.32</v>
@@ -7317,7 +7482,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D11">
         <v>9.91</v>
@@ -7405,16 +7570,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C1" t="s">
         <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -7422,13 +7587,13 @@
         <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -7436,13 +7601,13 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -7450,7 +7615,7 @@
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -7458,7 +7623,7 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -7482,7 +7647,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7501,10 +7666,10 @@
         <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -7540,7 +7705,7 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C5" s="10">
         <v>0.84722222222222221</v>

</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-09-18 10:43:08
</commit_message>
<xml_diff>
--- a/data/Solar_Lab_Tests.xlsx
+++ b/data/Solar_Lab_Tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1606" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{128B1E71-991A-4C08-B8DE-507265C723C7}"/>
+  <xr:revisionPtr revIDLastSave="1641" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C545FB25-487B-45EC-A13A-F5371AA74558}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="8" activeTab="8" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="8" activeTab="6" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Tests Map" sheetId="4" state="hidden" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="214">
   <si>
     <t>BOM</t>
   </si>
@@ -526,6 +526,12 @@
   </si>
   <si>
     <t>SHEETSOL EVA</t>
+  </si>
+  <si>
+    <t>ENERLITE EPE</t>
+  </si>
+  <si>
+    <t>ENERLITE EVA</t>
   </si>
   <si>
     <t xml:space="preserve">BOM </t>
@@ -1032,7 +1038,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1111,7 +1117,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2249,10 +2254,10 @@
         <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D1" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -2299,19 +2304,19 @@
         <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="E1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="F1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="G1" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -2319,13 +2324,13 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D2" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2333,7 +2338,7 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2341,13 +2346,13 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D4">
         <v>302</v>
       </c>
       <c r="E4" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -2361,7 +2366,7 @@
         <v>260</v>
       </c>
       <c r="E5" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -2369,13 +2374,13 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D6" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="E6" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -2386,10 +2391,10 @@
         <v>48</v>
       </c>
       <c r="D7" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="E7" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -2400,13 +2405,13 @@
         <v>68</v>
       </c>
       <c r="D8" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="E8" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="F8" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="G8">
         <v>217</v>
@@ -2420,10 +2425,10 @@
         <v>60</v>
       </c>
       <c r="D9" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="E9" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -2434,13 +2439,13 @@
         <v>59</v>
       </c>
       <c r="D10" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="E10" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="F10" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="G10">
         <v>202</v>
@@ -2451,16 +2456,16 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="D11" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="E11" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="F11" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="G11">
         <v>185</v>
@@ -2474,10 +2479,10 @@
         <v>46</v>
       </c>
       <c r="D12" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="E12" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -2485,7 +2490,7 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -2496,10 +2501,10 @@
         <v>56</v>
       </c>
       <c r="D14" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="E14" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -2507,13 +2512,13 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="D15" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="E15" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -2524,10 +2529,10 @@
         <v>52</v>
       </c>
       <c r="D16" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="E16" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -2538,13 +2543,13 @@
         <v>51</v>
       </c>
       <c r="D17" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="E17" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="F17" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="G17">
         <v>134</v>
@@ -2558,13 +2563,13 @@
         <v>49</v>
       </c>
       <c r="D18" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="E18" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="F18" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="G18">
         <v>297</v>
@@ -2575,12 +2580,12 @@
         <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="B20" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -2615,7 +2620,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -4330,62 +4335,56 @@
       </c>
     </row>
     <row r="75" spans="1:8">
-      <c r="A75" s="50" t="s">
+      <c r="A75" t="s">
         <v>2</v>
       </c>
       <c r="B75" t="s">
         <v>4</v>
       </c>
-      <c r="C75" s="50" t="s">
+      <c r="C75" t="s">
         <v>81</v>
       </c>
       <c r="D75" s="48"/>
       <c r="E75" s="4">
         <v>45916</v>
       </c>
-      <c r="F75" s="50"/>
-      <c r="G75" s="50"/>
-      <c r="H75" s="50" t="s">
+      <c r="H75" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="76" spans="1:8">
-      <c r="A76" s="50" t="s">
+      <c r="A76" t="s">
         <v>2</v>
       </c>
       <c r="B76" t="s">
         <v>3</v>
       </c>
-      <c r="C76" s="50" t="s">
+      <c r="C76" t="s">
         <v>81</v>
       </c>
       <c r="D76" s="48"/>
       <c r="E76" s="4">
         <v>45916</v>
       </c>
-      <c r="F76" s="50"/>
-      <c r="G76" s="50"/>
-      <c r="H76" s="50" t="s">
+      <c r="H76" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="77" spans="1:8">
-      <c r="A77" s="50" t="s">
+      <c r="A77" t="s">
         <v>2</v>
       </c>
       <c r="B77" t="s">
         <v>5</v>
       </c>
-      <c r="C77" s="50" t="s">
+      <c r="C77" t="s">
         <v>81</v>
       </c>
       <c r="D77" s="48"/>
       <c r="E77" s="4">
         <v>45916</v>
       </c>
-      <c r="F77" s="50"/>
-      <c r="G77" s="50"/>
-      <c r="H77" s="50" t="s">
+      <c r="H77" t="s">
         <v>38</v>
       </c>
     </row>
@@ -4396,16 +4395,14 @@
       <c r="B78" t="s">
         <v>6</v>
       </c>
-      <c r="C78" s="50" t="s">
+      <c r="C78" t="s">
         <v>81</v>
       </c>
       <c r="D78" s="48"/>
       <c r="E78" s="4">
         <v>45916</v>
       </c>
-      <c r="F78" s="50"/>
-      <c r="G78" s="50"/>
-      <c r="H78" s="50" t="s">
+      <c r="H78" t="s">
         <v>38</v>
       </c>
     </row>
@@ -4416,27 +4413,19 @@
       <c r="B79" t="s">
         <v>7</v>
       </c>
-      <c r="C79" s="50" t="s">
+      <c r="C79" t="s">
         <v>81</v>
       </c>
       <c r="D79" s="48"/>
       <c r="E79" s="4">
         <v>45916</v>
       </c>
-      <c r="F79" s="50"/>
-      <c r="G79" s="50"/>
-      <c r="H79" s="50" t="s">
+      <c r="H79" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="80" spans="1:8">
-      <c r="B80" s="50"/>
-      <c r="C80" s="50"/>
       <c r="D80" s="48"/>
-      <c r="E80" s="50"/>
-      <c r="F80" s="50"/>
-      <c r="G80" s="50"/>
-      <c r="H80" s="50"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -7207,8 +7196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C0F3BDD-3989-4880-8737-F370069E1383}">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7259,6 +7248,9 @@
       <c r="B2" s="12" t="s">
         <v>144</v>
       </c>
+      <c r="C2" t="s">
+        <v>90</v>
+      </c>
       <c r="D2">
         <v>10.31</v>
       </c>
@@ -7271,10 +7263,12 @@
       <c r="G2" s="7">
         <v>10.220000000000001</v>
       </c>
-      <c r="H2" s="7"/>
+      <c r="H2" s="7">
+        <v>10.19</v>
+      </c>
       <c r="I2">
         <f>AVERAGE(Table10[[#This Row],[min value 1 ]:[min value 5]])</f>
-        <v>10.2775</v>
+        <v>10.26</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -7284,6 +7278,9 @@
       <c r="B3" s="12" t="s">
         <v>145</v>
       </c>
+      <c r="C3" t="s">
+        <v>90</v>
+      </c>
       <c r="D3">
         <v>9.92</v>
       </c>
@@ -7296,10 +7293,12 @@
       <c r="G3" s="7">
         <v>9.83</v>
       </c>
-      <c r="H3" s="7"/>
+      <c r="H3" s="7">
+        <v>9.84</v>
+      </c>
       <c r="I3">
         <f>AVERAGE(Table10[[#This Row],[min value 1 ]:[min value 5]])</f>
-        <v>9.9049999999999994</v>
+        <v>9.8919999999999995</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -7321,10 +7320,12 @@
       <c r="G4" s="7">
         <v>10.11</v>
       </c>
-      <c r="H4" s="7"/>
+      <c r="H4" s="7">
+        <v>10.029999999999999</v>
+      </c>
       <c r="I4">
         <f>AVERAGE(Table10[[#This Row],[min value 1 ]:[min value 5]])</f>
-        <v>10.1175</v>
+        <v>10.1</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -7346,10 +7347,12 @@
       <c r="G5" s="7">
         <v>9.7200000000000006</v>
       </c>
-      <c r="H5" s="7"/>
+      <c r="H5" s="7">
+        <v>9.7100000000000009</v>
+      </c>
       <c r="I5">
         <f>AVERAGE(Table10[[#This Row],[min value 1 ]:[min value 5]])</f>
-        <v>9.6750000000000007</v>
+        <v>9.6820000000000004</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -7359,6 +7362,9 @@
       <c r="B6" s="8" t="s">
         <v>148</v>
       </c>
+      <c r="C6" t="s">
+        <v>90</v>
+      </c>
       <c r="D6">
         <v>10.53</v>
       </c>
@@ -7371,10 +7377,12 @@
       <c r="G6" s="7">
         <v>10.28</v>
       </c>
-      <c r="H6" s="7"/>
+      <c r="H6" s="7">
+        <v>10.35</v>
+      </c>
       <c r="I6">
         <f>AVERAGE(Table10[[#This Row],[min value 1 ]:[min value 5]])</f>
-        <v>10.44</v>
+        <v>10.422000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -7384,6 +7392,9 @@
       <c r="B7" s="8" t="s">
         <v>149</v>
       </c>
+      <c r="C7" t="s">
+        <v>90</v>
+      </c>
       <c r="D7">
         <v>9.9499999999999993</v>
       </c>
@@ -7396,10 +7407,12 @@
       <c r="G7" s="7">
         <v>10</v>
       </c>
-      <c r="H7" s="7"/>
+      <c r="H7" s="7">
+        <v>9.99</v>
+      </c>
       <c r="I7">
         <f>AVERAGE(Table10[[#This Row],[min value 1 ]:[min value 5]])</f>
-        <v>9.9674999999999994</v>
+        <v>9.9719999999999995</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -7421,10 +7434,12 @@
       <c r="G8" s="7">
         <v>10.5</v>
       </c>
-      <c r="H8" s="7"/>
+      <c r="H8" s="7">
+        <v>10.53</v>
+      </c>
       <c r="I8">
         <f>AVERAGE(Table10[[#This Row],[min value 1 ]:[min value 5]])</f>
-        <v>10.6975</v>
+        <v>10.664</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -7446,10 +7461,12 @@
       <c r="G9" s="7">
         <v>10.11</v>
       </c>
-      <c r="H9" s="7"/>
+      <c r="H9" s="7">
+        <v>10.16</v>
+      </c>
       <c r="I9">
         <f>AVERAGE(Table10[[#This Row],[min value 1 ]:[min value 5]])</f>
-        <v>10.15</v>
+        <v>10.152000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -7459,6 +7476,9 @@
       <c r="B10" s="8" t="s">
         <v>148</v>
       </c>
+      <c r="C10" t="s">
+        <v>90</v>
+      </c>
       <c r="D10">
         <v>10.32</v>
       </c>
@@ -7471,10 +7491,12 @@
       <c r="G10" s="7">
         <v>10.3</v>
       </c>
-      <c r="H10" s="7"/>
+      <c r="H10" s="7">
+        <v>10.28</v>
+      </c>
       <c r="I10">
         <f>AVERAGE(Table10[[#This Row],[min value 1 ]:[min value 5]])</f>
-        <v>10.275</v>
+        <v>10.276</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -7484,6 +7506,9 @@
       <c r="B11" s="8" t="s">
         <v>149</v>
       </c>
+      <c r="C11" t="s">
+        <v>90</v>
+      </c>
       <c r="D11">
         <v>9.91</v>
       </c>
@@ -7496,23 +7521,73 @@
       <c r="G11" s="7">
         <v>9.9</v>
       </c>
-      <c r="H11" s="7"/>
+      <c r="H11" s="7">
+        <v>9.9499999999999993</v>
+      </c>
       <c r="I11">
         <f>AVERAGE(Table10[[#This Row],[min value 1 ]:[min value 5]])</f>
-        <v>9.9224999999999994</v>
+        <v>9.9280000000000008</v>
       </c>
     </row>
     <row r="12" spans="1:9">
-      <c r="B12" s="8"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="C12" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12">
+        <v>11.13</v>
+      </c>
+      <c r="E12">
+        <v>10.99</v>
+      </c>
+      <c r="F12" s="7">
+        <v>11</v>
+      </c>
+      <c r="G12" s="7">
+        <v>11.1</v>
+      </c>
+      <c r="H12" s="7">
+        <v>11.03</v>
+      </c>
+      <c r="I12">
+        <f>AVERAGE(Table10[[#This Row],[min value 1 ]:[min value 5]])</f>
+        <v>11.05</v>
+      </c>
     </row>
     <row r="13" spans="1:9">
-      <c r="B13" s="8"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="C13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D13">
+        <v>10.14</v>
+      </c>
+      <c r="E13">
+        <v>10.130000000000001</v>
+      </c>
+      <c r="F13" s="7">
+        <v>10.16</v>
+      </c>
+      <c r="G13" s="7">
+        <v>10.26</v>
+      </c>
+      <c r="H13" s="7">
+        <v>10.25</v>
+      </c>
+      <c r="I13">
+        <f>AVERAGE(Table10[[#This Row],[min value 1 ]:[min value 5]])</f>
+        <v>10.188000000000001</v>
+      </c>
     </row>
     <row r="14" spans="1:9">
       <c r="B14" s="8"/>
@@ -7570,7 +7645,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B1" t="s">
         <v>88</v>
@@ -7579,7 +7654,7 @@
         <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -7587,13 +7662,13 @@
         <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C2" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D2" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -7601,13 +7676,13 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C3" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D3" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -7615,7 +7690,7 @@
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -7623,7 +7698,7 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -7646,7 +7721,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19611726-A899-4D7E-9AA1-680BBD5826DA}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -7666,10 +7741,10 @@
         <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -7705,7 +7780,7 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C5" s="10">
         <v>0.84722222222222221</v>

</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-09-18 13:05:12
</commit_message>
<xml_diff>
--- a/data/Solar_Lab_Tests.xlsx
+++ b/data/Solar_Lab_Tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1641" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C545FB25-487B-45EC-A13A-F5371AA74558}"/>
+  <xr:revisionPtr revIDLastSave="1658" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36112293-7C9A-4D05-9225-08373F2F0C4A}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="8" activeTab="6" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="6" activeTab="10" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Tests Map" sheetId="4" state="hidden" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="219">
   <si>
     <t>BOM</t>
   </si>
@@ -708,7 +708,22 @@
     <t>UKTR BD 2000L</t>
   </si>
   <si>
+    <t>349VBD/265VBY</t>
+  </si>
+  <si>
+    <t>256IBY/322IBD</t>
+  </si>
+  <si>
+    <t>341VBD/269VBY</t>
+  </si>
+  <si>
     <t>UKTR BD 7500L</t>
+  </si>
+  <si>
+    <t>345VBD/264VBY</t>
+  </si>
+  <si>
+    <t>205IBY/318IBD</t>
   </si>
   <si>
     <t>STANDARD DURATION (DAYS)</t>
@@ -2281,8 +2296,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{333C0630-51CF-46CA-8CAD-98FEF9AC181F}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView topLeftCell="B16" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="B11" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2582,10 +2597,28 @@
       <c r="B19" t="s">
         <v>211</v>
       </c>
+      <c r="D19" t="s">
+        <v>212</v>
+      </c>
+      <c r="E19" t="s">
+        <v>213</v>
+      </c>
+      <c r="F19" t="s">
+        <v>214</v>
+      </c>
+      <c r="G19" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="20" spans="1:7">
       <c r="B20" t="s">
-        <v>212</v>
+        <v>215</v>
+      </c>
+      <c r="F20" t="s">
+        <v>216</v>
+      </c>
+      <c r="G20" t="s">
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -2620,7 +2653,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2748,7 +2781,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9401EE47-EA52-49C7-BBC0-21F5B88254FB}">
   <dimension ref="A1:K80"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
+    <sheetView topLeftCell="A63" workbookViewId="0">
       <selection activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
@@ -4656,7 +4689,7 @@
   <dimension ref="A1:K519"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4867,6 +4900,30 @@
       </c>
       <c r="C7" s="27" t="s">
         <v>111</v>
+      </c>
+      <c r="D7" s="27">
+        <v>200.14</v>
+      </c>
+      <c r="E7" s="27">
+        <v>199.71</v>
+      </c>
+      <c r="F7" s="27">
+        <v>198.75</v>
+      </c>
+      <c r="G7" s="27">
+        <v>200.24</v>
+      </c>
+      <c r="H7" s="27">
+        <v>201.84</v>
+      </c>
+      <c r="I7" s="27">
+        <v>200.95</v>
+      </c>
+      <c r="J7" s="27">
+        <v>188.5</v>
+      </c>
+      <c r="K7" s="27">
+        <v>194.81</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -7196,7 +7253,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C0F3BDD-3989-4880-8737-F370069E1383}">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-09-29 09:43:37
</commit_message>
<xml_diff>
--- a/data/Solar_Lab_Tests.xlsx
+++ b/data/Solar_Lab_Tests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29322"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vikramsolar0-my.sharepoint.com/personal/naveen_chamaria_vikramsolar_com/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1747" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0A959D75-5C7C-4E3A-96B6-302F58CDD832}"/>
+  <xr:revisionPtr revIDLastSave="1756" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C1190AD4-6E69-4A4F-8B8B-2F1A5510E8B9}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="11" activeTab="7" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="7" activeTab="1" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Tests Map" sheetId="4" state="hidden" r:id="rId1"/>
@@ -1112,7 +1112,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1189,7 +1189,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -2777,7 +2776,7 @@
       <c r="A21" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="50" t="s">
+      <c r="B21" t="s">
         <v>83</v>
       </c>
       <c r="D21" t="s">
@@ -2962,8 +2961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9401EE47-EA52-49C7-BBC0-21F5B88254FB}">
   <dimension ref="A1:K88"/>
   <sheetViews>
-    <sheetView topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="C81" sqref="C81"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="F68" sqref="F68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -4652,167 +4651,178 @@
       <c r="E80" s="4">
         <v>45924</v>
       </c>
+      <c r="F80" s="4">
+        <v>45926</v>
+      </c>
       <c r="H80" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="81" spans="1:8">
-      <c r="A81" s="50" t="s">
+      <c r="A81" t="s">
         <v>15</v>
       </c>
-      <c r="B81" s="50" t="s">
+      <c r="B81" t="s">
         <v>18</v>
       </c>
-      <c r="C81" s="50" t="s">
+      <c r="C81" t="s">
         <v>83</v>
       </c>
-      <c r="D81" s="51"/>
+      <c r="D81" s="50"/>
       <c r="E81" s="4">
         <v>45924</v>
       </c>
-      <c r="F81" s="50"/>
-      <c r="G81" s="50"/>
-      <c r="H81" s="50" t="s">
+      <c r="F81" s="4">
+        <v>45926</v>
+      </c>
+      <c r="H81" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="82" spans="1:8">
-      <c r="A82" s="50" t="s">
+      <c r="A82" t="s">
         <v>15</v>
       </c>
-      <c r="B82" s="50" t="s">
+      <c r="B82" t="s">
         <v>18</v>
       </c>
-      <c r="C82" s="50" t="s">
+      <c r="C82" t="s">
         <v>84</v>
       </c>
-      <c r="D82" s="51"/>
+      <c r="D82" s="50"/>
       <c r="E82" s="4">
         <v>45924</v>
       </c>
-      <c r="F82" s="50"/>
-      <c r="G82" s="50"/>
-      <c r="H82" s="50" t="s">
+      <c r="F82" s="4">
+        <v>45926</v>
+      </c>
+      <c r="H82" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="83" spans="1:8">
-      <c r="A83" s="50" t="s">
+      <c r="A83" t="s">
         <v>15</v>
       </c>
-      <c r="B83" s="50" t="s">
+      <c r="B83" t="s">
         <v>18</v>
       </c>
-      <c r="C83" s="50" t="s">
+      <c r="C83" t="s">
         <v>85</v>
       </c>
-      <c r="D83" s="51"/>
+      <c r="D83" s="50"/>
       <c r="E83" s="4">
         <v>45924</v>
       </c>
-      <c r="F83" s="50"/>
-      <c r="G83" s="50"/>
-      <c r="H83" s="50" t="s">
+      <c r="F83" s="4">
+        <v>45926</v>
+      </c>
+      <c r="H83" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="84" spans="1:8">
-      <c r="A84" s="50" t="s">
+      <c r="A84" t="s">
         <v>15</v>
       </c>
-      <c r="B84" s="50" t="s">
+      <c r="B84" t="s">
         <v>18</v>
       </c>
-      <c r="C84" s="50" t="s">
+      <c r="C84" t="s">
         <v>86</v>
       </c>
-      <c r="D84" s="51"/>
+      <c r="D84" s="50"/>
       <c r="E84" s="4">
         <v>45924</v>
       </c>
-      <c r="F84" s="50"/>
-      <c r="G84" s="50"/>
-      <c r="H84" s="50" t="s">
+      <c r="F84" s="4">
+        <v>45926</v>
+      </c>
+      <c r="H84" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="85" spans="1:8">
-      <c r="A85" s="50" t="s">
+      <c r="A85" t="s">
         <v>15</v>
       </c>
-      <c r="B85" s="50" t="s">
+      <c r="B85" t="s">
         <v>18</v>
       </c>
-      <c r="C85" s="50" t="s">
+      <c r="C85" t="s">
         <v>87</v>
       </c>
-      <c r="D85" s="51"/>
+      <c r="D85" s="50"/>
       <c r="E85" s="4">
         <v>45924</v>
       </c>
-      <c r="F85" s="50"/>
-      <c r="G85" s="50"/>
-      <c r="H85" s="50" t="s">
+      <c r="F85" s="4">
+        <v>45926</v>
+      </c>
+      <c r="H85" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="86" spans="1:8">
-      <c r="A86" s="50" t="s">
+      <c r="A86" t="s">
         <v>15</v>
       </c>
-      <c r="B86" s="50" t="s">
+      <c r="B86" t="s">
         <v>18</v>
       </c>
-      <c r="C86" s="50" t="s">
+      <c r="C86" t="s">
         <v>88</v>
       </c>
-      <c r="D86" s="51"/>
+      <c r="D86" s="50"/>
       <c r="E86" s="4">
         <v>45924</v>
       </c>
-      <c r="F86" s="50"/>
-      <c r="G86" s="50"/>
-      <c r="H86" s="50" t="s">
+      <c r="F86" s="4">
+        <v>45926</v>
+      </c>
+      <c r="H86" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="87" spans="1:8">
-      <c r="A87" s="50" t="s">
+      <c r="A87" t="s">
         <v>15</v>
       </c>
-      <c r="B87" s="50" t="s">
+      <c r="B87" t="s">
         <v>18</v>
       </c>
-      <c r="C87" s="50" t="s">
+      <c r="C87" t="s">
         <v>89</v>
       </c>
-      <c r="D87" s="51"/>
+      <c r="D87" s="50"/>
       <c r="E87" s="4">
         <v>45924</v>
       </c>
-      <c r="F87" s="50"/>
-      <c r="G87" s="50"/>
-      <c r="H87" s="50" t="s">
+      <c r="F87" s="4">
+        <v>45926</v>
+      </c>
+      <c r="H87" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="88" spans="1:8">
-      <c r="A88" s="50" t="s">
+      <c r="A88" t="s">
         <v>15</v>
       </c>
-      <c r="B88" s="50" t="s">
+      <c r="B88" t="s">
         <v>18</v>
       </c>
-      <c r="C88" s="50" t="s">
+      <c r="C88" t="s">
         <v>88</v>
       </c>
-      <c r="D88" s="51"/>
+      <c r="D88" s="50"/>
       <c r="E88" s="4">
         <v>45924</v>
       </c>
-      <c r="F88" s="50"/>
-      <c r="G88" s="50"/>
-      <c r="H88" s="50" t="s">
+      <c r="F88" s="4">
+        <v>45926</v>
+      </c>
+      <c r="H88" t="s">
         <v>38</v>
       </c>
     </row>
@@ -8044,8 +8054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD5452B6-66C2-4964-BBFB-466116F6D217}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>

</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-10-09 09:42:25
</commit_message>
<xml_diff>
--- a/data/Solar_Lab_Tests.xlsx
+++ b/data/Solar_Lab_Tests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29401"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29404"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vikramsolar0-my.sharepoint.com/personal/naveen_chamaria_vikramsolar_com/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1770" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C5C6C9D-CFD3-4315-B4F5-C841557AFD0D}"/>
+  <xr:revisionPtr revIDLastSave="1807" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C1A4661-2445-4DFF-B548-72C139B80930}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="3" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="11" activeTab="7" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Tests Map" sheetId="4" state="hidden" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <definedName name="ENCAPTYPE">Ref!$K$2:$K$1048576</definedName>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">'Material Tests Map'!$A$1:$B$20</definedName>
     <definedName name="ExternalData_1" localSheetId="12" hidden="1">'Standard test times'!$A$1:$B$15</definedName>
-    <definedName name="ExternalData_1" localSheetId="3" hidden="1">'Test Data'!$A$1:$H$89</definedName>
+    <definedName name="ExternalData_1" localSheetId="3" hidden="1">'Test Data'!$A$1:$H$91</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="249">
   <si>
     <t>BOM</t>
   </si>
@@ -445,6 +445,12 @@
     <t>VIDYA0.24/6MM/4MM</t>
   </si>
   <si>
+    <t>VALEO0.24/6mm/4mm</t>
+  </si>
+  <si>
+    <t>LINE JUREN0.24/6/4m</t>
+  </si>
+  <si>
     <t xml:space="preserve">                                                                                                                           PRE PCT</t>
   </si>
   <si>
@@ -574,7 +580,7 @@
     <t>WETOWN 0.24MM</t>
   </si>
   <si>
-    <t>.421M</t>
+    <t>0.421Ω</t>
   </si>
   <si>
     <t>BUS RIBBON</t>
@@ -583,25 +589,43 @@
     <t>WETOWN 5MM</t>
   </si>
   <si>
-    <t>.009M</t>
+    <t>.009Ω</t>
   </si>
   <si>
     <t>vidya 0.24mm</t>
   </si>
   <si>
-    <t>0.457M</t>
+    <t>0.457Ω</t>
   </si>
   <si>
     <t>vidya4mm</t>
   </si>
   <si>
-    <t>13.79M</t>
+    <t>13.79Ω</t>
   </si>
   <si>
     <t>vidya6mm</t>
   </si>
   <si>
-    <t>9.24M</t>
+    <t>9.24Ω</t>
+  </si>
+  <si>
+    <t>valeo 0.24mm</t>
+  </si>
+  <si>
+    <t>0.472Ω</t>
+  </si>
+  <si>
+    <t>valeo4mm</t>
+  </si>
+  <si>
+    <t>15.7Ω</t>
+  </si>
+  <si>
+    <t>valeo6mm</t>
+  </si>
+  <si>
+    <t>10.1Ω</t>
   </si>
   <si>
     <t>START TIME</t>
@@ -1213,12 +1237,14 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="48">
+  <dxfs count="49">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -1263,6 +1289,9 @@
         <top/>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
     </dxf>
     <dxf>
       <font>
@@ -1667,8 +1696,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2651D75B-871E-4C48-A5BC-EA62B7E4365B}" name="materialmap" displayName="materialmap" ref="A1:B20" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:B20" xr:uid="{2651D75B-871E-4C48-A5BC-EA62B7E4365B}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{FB02FE47-E9DA-4BCF-85A4-754E419FEDE3}" uniqueName="1" name="BOM" queryTableFieldId="1" dataDxfId="47"/>
-    <tableColumn id="2" xr3:uid="{887E7320-FACA-4349-93A6-9DD0A9102ACA}" uniqueName="2" name="TEST NAME" queryTableFieldId="2" dataDxfId="46"/>
+    <tableColumn id="1" xr3:uid="{FB02FE47-E9DA-4BCF-85A4-754E419FEDE3}" uniqueName="1" name="BOM" queryTableFieldId="1" dataDxfId="48"/>
+    <tableColumn id="2" xr3:uid="{887E7320-FACA-4349-93A6-9DD0A9102ACA}" uniqueName="2" name="TEST NAME" queryTableFieldId="2" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1688,18 +1717,18 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{97A8C2A7-46C0-4446-B562-6550EA520638}" name="Table10" displayName="Table10" ref="A1:I15" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{97A8C2A7-46C0-4446-B562-6550EA520638}" name="Table10" displayName="Table10" ref="A1:I15" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
   <autoFilter ref="A1:I15" xr:uid="{97A8C2A7-46C0-4446-B562-6550EA520638}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{FE721515-FBBB-4487-ABCE-AAB6A5B1513A}" name="BOM" dataDxfId="12"/>
-    <tableColumn id="9" xr3:uid="{304FA6D2-898E-427A-8AC1-958C15295938}" name="VENDOR NAME" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{CB22B1B1-F2DB-4A16-825A-FE463620DEF9}" name="Type" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{37372ACB-68A6-4423-8A58-7EF31F49D3C5}" name="min value 1 " dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{87A17A4F-6A43-4AB0-9B0F-B213AAD6E601}" name="min value 2" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{BB8F60AF-F7B1-4306-8198-B69EE3E6D97A}" name="min value 3" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{03425EE3-EC03-4913-B402-224F846A29D7}" name="min value 4" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{E68E3244-13A5-47AA-8AB7-F602EE938E20}" name="min value 5" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{D5BE9073-1EC1-4D18-A75C-7F63CCD62CB2}" name="Mean" dataDxfId="4">
+    <tableColumn id="1" xr3:uid="{FE721515-FBBB-4487-ABCE-AAB6A5B1513A}" name="BOM" dataDxfId="13"/>
+    <tableColumn id="9" xr3:uid="{304FA6D2-898E-427A-8AC1-958C15295938}" name="VENDOR NAME" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{CB22B1B1-F2DB-4A16-825A-FE463620DEF9}" name="Type" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{37372ACB-68A6-4423-8A58-7EF31F49D3C5}" name="min value 1 " dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{87A17A4F-6A43-4AB0-9B0F-B213AAD6E601}" name="min value 2" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{BB8F60AF-F7B1-4306-8198-B69EE3E6D97A}" name="min value 3" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{03425EE3-EC03-4913-B402-224F846A29D7}" name="min value 4" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{E68E3244-13A5-47AA-8AB7-F602EE938E20}" name="min value 5" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{D5BE9073-1EC1-4D18-A75C-7F63CCD62CB2}" name="Mean" dataDxfId="5">
       <calculatedColumnFormula>AVERAGE(Table10[[#This Row],[min value 1 ]:[min value 5]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1708,13 +1737,13 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{20A38E0C-9EF6-4C45-A435-A35C875E6079}" name="Table4" displayName="Table4" ref="A1:D6" totalsRowShown="0">
-  <autoFilter ref="A1:D6" xr:uid="{20A38E0C-9EF6-4C45-A435-A35C875E6079}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{20A38E0C-9EF6-4C45-A435-A35C875E6079}" name="Table4" displayName="Table4" ref="A1:D9" totalsRowShown="0">
+  <autoFilter ref="A1:D9" xr:uid="{20A38E0C-9EF6-4C45-A435-A35C875E6079}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{81484900-FCE7-4687-AE80-25067EEBF4DF}" name="BOM "/>
     <tableColumn id="2" xr3:uid="{98C35052-5143-4722-B228-CDF4595728A7}" name="TYPE"/>
     <tableColumn id="3" xr3:uid="{DC0A72BF-A20E-4169-808D-31BFAFA45357}" name="VENDOR NAME"/>
-    <tableColumn id="4" xr3:uid="{C58F8BC5-05CB-47D9-818A-1926632D9181}" name="MEASURED VALUE"/>
+    <tableColumn id="4" xr3:uid="{C58F8BC5-05CB-47D9-818A-1926632D9181}" name="MEASURED VALUE" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1832,54 +1861,54 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{7FFEF855-2CB7-4EF4-BE50-FB81C544017B}" name="Table18" displayName="Table18" ref="B3:K1048576" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{7FFEF855-2CB7-4EF4-BE50-FB81C544017B}" name="Table18" displayName="Table18" ref="B3:K1048576" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45">
   <autoFilter ref="B3:K1048576" xr:uid="{7FFEF855-2CB7-4EF4-BE50-FB81C544017B}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{96E09178-FF72-435C-90A9-F2F7FEC7E80C}" name="Column1" dataDxfId="43"/>
-    <tableColumn id="2" xr3:uid="{B7D3E49F-4F89-454D-B9FA-E1364CBF3239}" name="Column2" dataDxfId="42"/>
-    <tableColumn id="3" xr3:uid="{CCA06B22-44E5-4255-8F26-0C1B1279B22C}" name="Column3" dataDxfId="41"/>
-    <tableColumn id="4" xr3:uid="{6F565555-BB1C-4294-A1BA-3B6ADB9C2D2F}" name="Column4" dataDxfId="40"/>
-    <tableColumn id="5" xr3:uid="{33CA8E10-7021-4A52-853E-A6227866156B}" name="Column5" dataDxfId="39"/>
-    <tableColumn id="6" xr3:uid="{870E308E-FC7E-4A0A-A66A-ED0B8741D8AF}" name="Column6" dataDxfId="38"/>
-    <tableColumn id="7" xr3:uid="{FEEFF96D-1CCA-48C1-982D-EAFDB6BC3200}" name="Column7" dataDxfId="37"/>
-    <tableColumn id="8" xr3:uid="{4FEE2433-7AE2-4CF7-A1FC-541524E1FAAF}" name="Column8" dataDxfId="36"/>
-    <tableColumn id="9" xr3:uid="{A6BC8484-A791-4583-A77F-7F6A667CE8C5}" name="Column9" dataDxfId="35"/>
-    <tableColumn id="10" xr3:uid="{192E7774-55A7-4BD2-9715-330A7F12089B}" name="Column10" dataDxfId="34"/>
+    <tableColumn id="1" xr3:uid="{96E09178-FF72-435C-90A9-F2F7FEC7E80C}" name="Column1" dataDxfId="44"/>
+    <tableColumn id="2" xr3:uid="{B7D3E49F-4F89-454D-B9FA-E1364CBF3239}" name="Column2" dataDxfId="43"/>
+    <tableColumn id="3" xr3:uid="{CCA06B22-44E5-4255-8F26-0C1B1279B22C}" name="Column3" dataDxfId="42"/>
+    <tableColumn id="4" xr3:uid="{6F565555-BB1C-4294-A1BA-3B6ADB9C2D2F}" name="Column4" dataDxfId="41"/>
+    <tableColumn id="5" xr3:uid="{33CA8E10-7021-4A52-853E-A6227866156B}" name="Column5" dataDxfId="40"/>
+    <tableColumn id="6" xr3:uid="{870E308E-FC7E-4A0A-A66A-ED0B8741D8AF}" name="Column6" dataDxfId="39"/>
+    <tableColumn id="7" xr3:uid="{FEEFF96D-1CCA-48C1-982D-EAFDB6BC3200}" name="Column7" dataDxfId="38"/>
+    <tableColumn id="8" xr3:uid="{4FEE2433-7AE2-4CF7-A1FC-541524E1FAAF}" name="Column8" dataDxfId="37"/>
+    <tableColumn id="9" xr3:uid="{A6BC8484-A791-4583-A77F-7F6A667CE8C5}" name="Column9" dataDxfId="36"/>
+    <tableColumn id="10" xr3:uid="{192E7774-55A7-4BD2-9715-330A7F12089B}" name="Column10" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{06A3AD80-C098-4015-85FF-3495CE4443EA}" name="Test_Data" displayName="Test_Data" ref="A1:H89" tableType="queryTable" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{06A3AD80-C098-4015-85FF-3495CE4443EA}" name="Test_Data" displayName="Test_Data" ref="A1:H91" tableType="queryTable" totalsRowShown="0">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{87F75B08-44C4-4718-834D-87FEE9F87970}" uniqueName="1" name="BOM" queryTableFieldId="1" dataDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{1E5F4521-5E5C-4948-AEB2-FC5F712DB353}" uniqueName="2" name="TEST NAME" queryTableFieldId="2" dataDxfId="32"/>
-    <tableColumn id="3" xr3:uid="{22629B97-1F38-4A88-B08E-7589CFF4C28D}" uniqueName="3" name="VENDOR NAME" queryTableFieldId="3" dataDxfId="31"/>
-    <tableColumn id="4" xr3:uid="{D6678E87-972B-4807-86C4-4086EF552262}" uniqueName="4" name="GRN GENERATION TIME" queryTableFieldId="4" dataDxfId="30"/>
-    <tableColumn id="5" xr3:uid="{62C80EA2-76AB-4742-87FF-05248307AF93}" uniqueName="5" name="TEST START DATE AND TIME" queryTableFieldId="5" dataDxfId="29"/>
-    <tableColumn id="6" xr3:uid="{DDA3B4DC-3A06-4223-8D24-00B8C4C20678}" uniqueName="6" name="TEST END DATE AND TIME" queryTableFieldId="6" dataDxfId="28"/>
-    <tableColumn id="7" xr3:uid="{F2102600-A33C-449C-8C79-361FEA6C4BCE}" uniqueName="7" name="TEST RESULT" queryTableFieldId="7" dataDxfId="27"/>
-    <tableColumn id="8" xr3:uid="{E5E91A8D-E194-48B6-8D9A-FFD1939E8ACF}" uniqueName="8" name="STATUS" queryTableFieldId="8" dataDxfId="26"/>
+    <tableColumn id="1" xr3:uid="{87F75B08-44C4-4718-834D-87FEE9F87970}" uniqueName="1" name="BOM" queryTableFieldId="1" dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{1E5F4521-5E5C-4948-AEB2-FC5F712DB353}" uniqueName="2" name="TEST NAME" queryTableFieldId="2" dataDxfId="33"/>
+    <tableColumn id="3" xr3:uid="{22629B97-1F38-4A88-B08E-7589CFF4C28D}" uniqueName="3" name="VENDOR NAME" queryTableFieldId="3" dataDxfId="32"/>
+    <tableColumn id="4" xr3:uid="{D6678E87-972B-4807-86C4-4086EF552262}" uniqueName="4" name="GRN GENERATION TIME" queryTableFieldId="4" dataDxfId="31"/>
+    <tableColumn id="5" xr3:uid="{62C80EA2-76AB-4742-87FF-05248307AF93}" uniqueName="5" name="TEST START DATE AND TIME" queryTableFieldId="5" dataDxfId="30"/>
+    <tableColumn id="6" xr3:uid="{DDA3B4DC-3A06-4223-8D24-00B8C4C20678}" uniqueName="6" name="TEST END DATE AND TIME" queryTableFieldId="6" dataDxfId="29"/>
+    <tableColumn id="7" xr3:uid="{F2102600-A33C-449C-8C79-361FEA6C4BCE}" uniqueName="7" name="TEST RESULT" queryTableFieldId="7" dataDxfId="28"/>
+    <tableColumn id="8" xr3:uid="{E5E91A8D-E194-48B6-8D9A-FFD1939E8ACF}" uniqueName="8" name="STATUS" queryTableFieldId="8" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{67926097-CCFB-425B-9820-DDDFB77C87C9}" name="Table11" displayName="Table11" ref="A4:J1048576" totalsRowShown="0" dataDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{67926097-CCFB-425B-9820-DDDFB77C87C9}" name="Table11" displayName="Table11" ref="A4:J1048576" totalsRowShown="0" dataDxfId="26">
   <autoFilter ref="A4:J1048576" xr:uid="{67926097-CCFB-425B-9820-DDDFB77C87C9}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{EA92BD46-85A5-4BF3-9843-966A2E5861D9}" name="Column1" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{C24A9AB3-E538-4185-9C80-E9DDC6A05A90}" name="Column2" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{0CA46B2C-315A-49B7-A313-787EA669AF33}" name="Column3" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{AA05AB49-E5DC-4F39-BF84-5C21AE004473}" name="Column4" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{8D9CD07A-CD8E-459F-AD52-C1C64282E998}" name="Column5" dataDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{953BA2E8-443D-4DD4-ACF1-1ECEDB5DE6DD}" name="Column6" dataDxfId="19"/>
-    <tableColumn id="7" xr3:uid="{8ED40F5F-1EB7-4C33-83D6-002E5FC5C1EC}" name="Column7" dataDxfId="18"/>
-    <tableColumn id="8" xr3:uid="{3EC62242-31F0-4282-815A-7D5C6B4310FD}" name="Column8" dataDxfId="17"/>
-    <tableColumn id="9" xr3:uid="{514AC0BC-C14D-43E8-9076-A902208889C3}" name="Column9" dataDxfId="16"/>
-    <tableColumn id="10" xr3:uid="{94E39AAC-5F2B-4668-8EAE-7D440F802CF1}" name="Column10" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{EA92BD46-85A5-4BF3-9843-966A2E5861D9}" name="Column1" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{C24A9AB3-E538-4185-9C80-E9DDC6A05A90}" name="Column2" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{0CA46B2C-315A-49B7-A313-787EA669AF33}" name="Column3" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{AA05AB49-E5DC-4F39-BF84-5C21AE004473}" name="Column4" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{8D9CD07A-CD8E-459F-AD52-C1C64282E998}" name="Column5" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{953BA2E8-443D-4DD4-ACF1-1ECEDB5DE6DD}" name="Column6" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{8ED40F5F-1EB7-4C33-83D6-002E5FC5C1EC}" name="Column7" dataDxfId="19"/>
+    <tableColumn id="8" xr3:uid="{3EC62242-31F0-4282-815A-7D5C6B4310FD}" name="Column8" dataDxfId="18"/>
+    <tableColumn id="9" xr3:uid="{514AC0BC-C14D-43E8-9076-A902208889C3}" name="Column9" dataDxfId="17"/>
+    <tableColumn id="10" xr3:uid="{94E39AAC-5F2B-4668-8EAE-7D440F802CF1}" name="Column10" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2405,10 +2434,10 @@
         <v>44</v>
       </c>
       <c r="C1" s="49" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="D1" s="49" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -2442,10 +2471,10 @@
         <v>44</v>
       </c>
       <c r="C1" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="D1" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -2470,7 +2499,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -2492,19 +2521,19 @@
         <v>44</v>
       </c>
       <c r="C1" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="D1" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="E1" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="F1" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="G1" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -2512,13 +2541,13 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="D2" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="E2" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2526,7 +2555,7 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2534,13 +2563,13 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="D4">
         <v>302</v>
       </c>
       <c r="E4" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -2554,7 +2583,7 @@
         <v>260</v>
       </c>
       <c r="E5" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -2562,13 +2591,13 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="D6" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="E6" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -2579,10 +2608,10 @@
         <v>81</v>
       </c>
       <c r="D7" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="E7" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -2593,13 +2622,13 @@
         <v>101</v>
       </c>
       <c r="D8" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="E8" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="F8" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="G8">
         <v>217</v>
@@ -2613,10 +2642,10 @@
         <v>93</v>
       </c>
       <c r="D9" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="E9" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -2627,13 +2656,13 @@
         <v>92</v>
       </c>
       <c r="D10" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="E10" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="F10" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="G10">
         <v>202</v>
@@ -2644,16 +2673,16 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="D11" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="E11" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="F11" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="G11">
         <v>185</v>
@@ -2667,10 +2696,10 @@
         <v>79</v>
       </c>
       <c r="D12" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="E12" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -2678,7 +2707,7 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -2689,10 +2718,10 @@
         <v>89</v>
       </c>
       <c r="D14" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="E14" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -2700,13 +2729,13 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="D15" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="E15" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -2717,10 +2746,10 @@
         <v>85</v>
       </c>
       <c r="D16" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="E16" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -2731,13 +2760,13 @@
         <v>84</v>
       </c>
       <c r="D17" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="E17" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="F17" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="G17">
         <v>134</v>
@@ -2751,13 +2780,13 @@
         <v>82</v>
       </c>
       <c r="D18" t="s">
-        <v>225</v>
+        <v>233</v>
       </c>
       <c r="E18" t="s">
-        <v>226</v>
+        <v>234</v>
       </c>
       <c r="F18" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="G18">
         <v>297</v>
@@ -2768,30 +2797,30 @@
         <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>228</v>
+        <v>236</v>
       </c>
       <c r="D19" t="s">
-        <v>229</v>
+        <v>237</v>
       </c>
       <c r="E19" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="F19" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="G19" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="B20" t="s">
-        <v>232</v>
+        <v>240</v>
       </c>
       <c r="F20" t="s">
-        <v>233</v>
+        <v>241</v>
       </c>
       <c r="G20" t="s">
-        <v>234</v>
+        <v>242</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15">
@@ -2802,10 +2831,10 @@
         <v>116</v>
       </c>
       <c r="D21" t="s">
-        <v>235</v>
+        <v>243</v>
       </c>
       <c r="E21" t="s">
-        <v>236</v>
+        <v>244</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -2813,13 +2842,13 @@
         <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>237</v>
+        <v>245</v>
       </c>
       <c r="F22" t="s">
-        <v>238</v>
+        <v>246</v>
       </c>
       <c r="G22" t="s">
-        <v>239</v>
+        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -2855,7 +2884,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>240</v>
+        <v>248</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -5160,10 +5189,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9401EE47-EA52-49C7-BBC0-21F5B88254FB}">
-  <dimension ref="A1:K89"/>
+  <dimension ref="A1:K91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="H89" sqref="H89"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E91" sqref="E91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -7028,21 +7057,57 @@
       </c>
     </row>
     <row r="89" spans="1:8">
-      <c r="A89" s="51" t="s">
+      <c r="A89" t="s">
         <v>20</v>
       </c>
       <c r="B89" t="s">
         <v>18</v>
       </c>
-      <c r="C89" s="51" t="s">
+      <c r="C89" t="s">
         <v>123</v>
       </c>
       <c r="D89" s="50"/>
-      <c r="E89" s="51"/>
-      <c r="F89" s="51"/>
-      <c r="G89" s="51"/>
-      <c r="H89" s="51" t="s">
-        <v>35</v>
+      <c r="E89" s="4">
+        <v>45939</v>
+      </c>
+      <c r="H89" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8">
+      <c r="A90" t="s">
+        <v>20</v>
+      </c>
+      <c r="B90" t="s">
+        <v>18</v>
+      </c>
+      <c r="C90" t="s">
+        <v>124</v>
+      </c>
+      <c r="D90" s="50"/>
+      <c r="E90" s="4">
+        <v>45939</v>
+      </c>
+      <c r="H90" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8">
+      <c r="A91" t="s">
+        <v>20</v>
+      </c>
+      <c r="B91" t="s">
+        <v>18</v>
+      </c>
+      <c r="C91" t="s">
+        <v>125</v>
+      </c>
+      <c r="D91" s="50"/>
+      <c r="E91" s="4">
+        <v>45939</v>
+      </c>
+      <c r="H91" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -7116,14 +7181,14 @@
       <c r="A1" s="28"/>
       <c r="B1" s="29"/>
       <c r="C1" s="30" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D1" s="31"/>
       <c r="E1" s="30"/>
       <c r="F1" s="31"/>
       <c r="G1" s="32"/>
       <c r="H1" s="44" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="I1" s="32"/>
       <c r="J1" s="29"/>
@@ -7136,19 +7201,19 @@
         <v>44</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D2" s="36"/>
       <c r="E2" s="37" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F2" s="38"/>
       <c r="G2" s="35" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="37" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="J2" s="38"/>
     </row>
@@ -7317,7 +7382,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="45" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C8" s="45">
         <v>166</v>
@@ -7349,7 +7414,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="45" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C9" s="45">
         <v>80</v>
@@ -7471,10 +7536,10 @@
         <v>44</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="6" customFormat="1">
@@ -7498,7 +7563,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C3" s="48">
         <v>14.6</v>
@@ -7512,7 +7577,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -7520,7 +7585,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -7528,7 +7593,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -7536,7 +7601,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -7544,7 +7609,7 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C8" s="48">
         <v>16.5</v>
@@ -7558,7 +7623,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -7566,7 +7631,7 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -7574,7 +7639,7 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -7582,7 +7647,7 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -7590,7 +7655,7 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C13" s="48">
         <v>42.8</v>
@@ -7604,7 +7669,7 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C14" s="48">
         <v>69.3</v>
@@ -7618,7 +7683,7 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C15" s="48">
         <v>68.599999999999994</v>
@@ -7632,7 +7697,7 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C16" s="48">
         <v>88.7</v>
@@ -7683,25 +7748,25 @@
         <v>44</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -7709,7 +7774,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C2" t="s">
         <v>34</v>
@@ -7739,7 +7804,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C3" t="s">
         <v>34</v>
@@ -7769,7 +7834,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D4">
         <v>10.16</v>
@@ -7796,7 +7861,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D5">
         <v>9.66</v>
@@ -7823,7 +7888,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C6" t="s">
         <v>34</v>
@@ -7853,7 +7918,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C7" t="s">
         <v>34</v>
@@ -7883,7 +7948,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D8">
         <v>10.84</v>
@@ -7910,7 +7975,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D9">
         <v>10.15</v>
@@ -7937,7 +8002,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C10" t="s">
         <v>34</v>
@@ -7967,7 +8032,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C11" t="s">
         <v>34</v>
@@ -7997,7 +8062,7 @@
         <v>2</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C12" t="s">
         <v>34</v>
@@ -8027,7 +8092,7 @@
         <v>2</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C13" t="s">
         <v>34</v>
@@ -8092,10 +8157,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD5452B6-66C2-4964-BBFB-466116F6D217}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -8108,7 +8173,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B1" t="s">
         <v>30</v>
@@ -8117,7 +8182,7 @@
         <v>44</v>
       </c>
       <c r="D1" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -8125,13 +8190,13 @@
         <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C2" t="s">
-        <v>166</v>
-      </c>
-      <c r="D2" t="s">
-        <v>167</v>
+        <v>168</v>
+      </c>
+      <c r="D2" s="51" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -8139,13 +8204,13 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C3" t="s">
-        <v>169</v>
-      </c>
-      <c r="D3" t="s">
-        <v>170</v>
+        <v>171</v>
+      </c>
+      <c r="D3" s="51" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -8153,13 +8218,13 @@
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C4" t="s">
-        <v>171</v>
-      </c>
-      <c r="D4" t="s">
-        <v>172</v>
+        <v>173</v>
+      </c>
+      <c r="D4" s="51" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -8167,13 +8232,13 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C5" t="s">
-        <v>173</v>
-      </c>
-      <c r="D5" t="s">
-        <v>174</v>
+        <v>175</v>
+      </c>
+      <c r="D5" s="51" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -8181,13 +8246,55 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C6" t="s">
-        <v>175</v>
-      </c>
-      <c r="D6" t="s">
-        <v>176</v>
+        <v>177</v>
+      </c>
+      <c r="D6" s="51" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>167</v>
+      </c>
+      <c r="C7" t="s">
+        <v>179</v>
+      </c>
+      <c r="D7" s="51" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>170</v>
+      </c>
+      <c r="C8" t="s">
+        <v>181</v>
+      </c>
+      <c r="D8" s="51" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>170</v>
+      </c>
+      <c r="C9" t="s">
+        <v>183</v>
+      </c>
+      <c r="D9" s="51" t="s">
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -8230,10 +8337,10 @@
         <v>44</v>
       </c>
       <c r="C1" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="D1" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -8269,7 +8376,7 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="C5" s="10">
         <v>0.84722222222222221</v>

</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-10-10 13:05:15
</commit_message>
<xml_diff>
--- a/data/Solar_Lab_Tests.xlsx
+++ b/data/Solar_Lab_Tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vikramsolar0-my.sharepoint.com/personal/naveen_chamaria_vikramsolar_com/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1807" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C1A4661-2445-4DFF-B548-72C139B80930}"/>
+  <xr:revisionPtr revIDLastSave="1813" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{690731DC-B418-49B7-9ADF-424E2414A3D3}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="11" activeTab="7" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="7" activeTab="11" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Tests Map" sheetId="4" state="hidden" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="251">
   <si>
     <t>BOM</t>
   </si>
@@ -662,6 +662,12 @@
   </si>
   <si>
     <t>Avg. Id (Post PCT)</t>
+  </si>
+  <si>
+    <t>RESISTANCE(Pre PCT)</t>
+  </si>
+  <si>
+    <t>RESISTANCE(Post PCT)</t>
   </si>
   <si>
     <t>CAHORS 30A</t>
@@ -824,10 +830,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
-  </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -889,6 +892,13 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="14">
@@ -1234,12 +1244,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1526,7 +1534,7 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1789,9 +1797,9 @@
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{5C370BE7-C0F8-462F-9F89-5FC458087319}" name="Table16" displayName="Table16" ref="A1:G22" totalsRowShown="0">
-  <autoFilter ref="A1:G22" xr:uid="{5C370BE7-C0F8-462F-9F89-5FC458087319}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{5C370BE7-C0F8-462F-9F89-5FC458087319}" name="Table16" displayName="Table16" ref="A1:I22" totalsRowShown="0">
+  <autoFilter ref="A1:I22" xr:uid="{5C370BE7-C0F8-462F-9F89-5FC458087319}"/>
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{59EA2429-768A-457D-88E6-B34A083DE755}" name="BOM"/>
     <tableColumn id="2" xr3:uid="{C09F236B-325A-4EF9-B484-B1D592C83B7F}" name="VENDOR NAME"/>
     <tableColumn id="3" xr3:uid="{038FF345-6349-48D1-AECF-86999B680B6F}" name="AVG. MAX TEMPERATURE OF DIODE(Tj) IN ON state"/>
@@ -1799,6 +1807,8 @@
     <tableColumn id="5" xr3:uid="{06876625-B87D-43D1-94E5-A1298F168708}" name="Avg. Id (Pre PCT)"/>
     <tableColumn id="6" xr3:uid="{D302E131-903E-47D9-87BC-2E463FD51E89}" name="Avg. Vd (Post PCT)"/>
     <tableColumn id="7" xr3:uid="{2A14738D-0ADB-4B84-BA1B-287E8603F866}" name="Avg. Id (Post PCT)"/>
+    <tableColumn id="8" xr3:uid="{2062BFD7-AF12-40A1-82A6-F8210996D827}" name="RESISTANCE(Pre PCT)"/>
+    <tableColumn id="9" xr3:uid="{368F865D-670A-4F25-A0B8-8D912EDAAAB6}" name="RESISTANCE(Post PCT)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2496,10 +2506,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{333C0630-51CF-46CA-8CAD-98FEF9AC181F}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -2511,9 +2521,11 @@
     <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.140625" customWidth="1"/>
+    <col min="9" max="9" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:9" ht="15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2535,44 +2547,50 @@
       <c r="G1" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" t="s">
+        <v>197</v>
+      </c>
+      <c r="I1" s="51" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="D2" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="E2" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="D4">
         <v>302</v>
       </c>
       <c r="E4" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -2583,24 +2601,24 @@
         <v>260</v>
       </c>
       <c r="E5" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="D6" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="E6" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -2608,13 +2626,13 @@
         <v>81</v>
       </c>
       <c r="D7" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="E7" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -2622,19 +2640,19 @@
         <v>101</v>
       </c>
       <c r="D8" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="E8" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="F8" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="G8">
         <v>217</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -2642,13 +2660,13 @@
         <v>93</v>
       </c>
       <c r="D9" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="E9" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -2656,39 +2674,39 @@
         <v>92</v>
       </c>
       <c r="D10" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="E10" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="F10" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="G10">
         <v>202</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="D11" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="E11" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="F11" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="G11">
         <v>185</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -2696,21 +2714,21 @@
         <v>79</v>
       </c>
       <c r="D12" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="E12" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -2718,27 +2736,27 @@
         <v>89</v>
       </c>
       <c r="D14" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="E14" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="D15" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="E15" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -2746,10 +2764,10 @@
         <v>85</v>
       </c>
       <c r="D16" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="E16" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -2760,13 +2778,13 @@
         <v>84</v>
       </c>
       <c r="D17" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="E17" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="F17" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="G17">
         <v>134</v>
@@ -2780,13 +2798,13 @@
         <v>82</v>
       </c>
       <c r="D18" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="E18" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="F18" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="G18">
         <v>297</v>
@@ -2797,30 +2815,30 @@
         <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D19" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="E19" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="F19" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="G19" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="B20" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="F20" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="G20" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15">
@@ -2831,10 +2849,10 @@
         <v>116</v>
       </c>
       <c r="D21" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="E21" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -2842,13 +2860,13 @@
         <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="F22" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="G22" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
   </sheetData>
@@ -2884,7 +2902,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -6898,7 +6916,7 @@
       <c r="C81" t="s">
         <v>116</v>
       </c>
-      <c r="D81" s="50"/>
+      <c r="D81" s="5"/>
       <c r="E81" s="4">
         <v>45924</v>
       </c>
@@ -6919,7 +6937,7 @@
       <c r="C82" t="s">
         <v>117</v>
       </c>
-      <c r="D82" s="50"/>
+      <c r="D82" s="5"/>
       <c r="E82" s="4">
         <v>45924</v>
       </c>
@@ -6940,7 +6958,7 @@
       <c r="C83" t="s">
         <v>118</v>
       </c>
-      <c r="D83" s="50"/>
+      <c r="D83" s="5"/>
       <c r="E83" s="4">
         <v>45924</v>
       </c>
@@ -6961,7 +6979,7 @@
       <c r="C84" t="s">
         <v>119</v>
       </c>
-      <c r="D84" s="50"/>
+      <c r="D84" s="5"/>
       <c r="E84" s="4">
         <v>45924</v>
       </c>
@@ -6982,7 +7000,7 @@
       <c r="C85" t="s">
         <v>120</v>
       </c>
-      <c r="D85" s="50"/>
+      <c r="D85" s="5"/>
       <c r="E85" s="4">
         <v>45924</v>
       </c>
@@ -7003,7 +7021,7 @@
       <c r="C86" t="s">
         <v>121</v>
       </c>
-      <c r="D86" s="50"/>
+      <c r="D86" s="5"/>
       <c r="E86" s="4">
         <v>45924</v>
       </c>
@@ -7024,7 +7042,7 @@
       <c r="C87" t="s">
         <v>122</v>
       </c>
-      <c r="D87" s="50"/>
+      <c r="D87" s="5"/>
       <c r="E87" s="4">
         <v>45924</v>
       </c>
@@ -7045,7 +7063,7 @@
       <c r="C88" t="s">
         <v>121</v>
       </c>
-      <c r="D88" s="50"/>
+      <c r="D88" s="5"/>
       <c r="E88" s="4">
         <v>45924</v>
       </c>
@@ -7066,7 +7084,7 @@
       <c r="C89" t="s">
         <v>123</v>
       </c>
-      <c r="D89" s="50"/>
+      <c r="D89" s="5"/>
       <c r="E89" s="4">
         <v>45939</v>
       </c>
@@ -7084,7 +7102,7 @@
       <c r="C90" t="s">
         <v>124</v>
       </c>
-      <c r="D90" s="50"/>
+      <c r="D90" s="5"/>
       <c r="E90" s="4">
         <v>45939</v>
       </c>
@@ -7102,7 +7120,7 @@
       <c r="C91" t="s">
         <v>125</v>
       </c>
-      <c r="D91" s="50"/>
+      <c r="D91" s="5"/>
       <c r="E91" s="4">
         <v>45939</v>
       </c>
@@ -8159,7 +8177,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD5452B6-66C2-4964-BBFB-466116F6D217}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -8195,7 +8213,7 @@
       <c r="C2" t="s">
         <v>168</v>
       </c>
-      <c r="D2" s="51" t="s">
+      <c r="D2" s="50" t="s">
         <v>169</v>
       </c>
     </row>
@@ -8209,7 +8227,7 @@
       <c r="C3" t="s">
         <v>171</v>
       </c>
-      <c r="D3" s="51" t="s">
+      <c r="D3" s="50" t="s">
         <v>172</v>
       </c>
     </row>
@@ -8223,7 +8241,7 @@
       <c r="C4" t="s">
         <v>173</v>
       </c>
-      <c r="D4" s="51" t="s">
+      <c r="D4" s="50" t="s">
         <v>174</v>
       </c>
     </row>
@@ -8237,7 +8255,7 @@
       <c r="C5" t="s">
         <v>175</v>
       </c>
-      <c r="D5" s="51" t="s">
+      <c r="D5" s="50" t="s">
         <v>176</v>
       </c>
     </row>
@@ -8251,7 +8269,7 @@
       <c r="C6" t="s">
         <v>177</v>
       </c>
-      <c r="D6" s="51" t="s">
+      <c r="D6" s="50" t="s">
         <v>178</v>
       </c>
     </row>
@@ -8265,7 +8283,7 @@
       <c r="C7" t="s">
         <v>179</v>
       </c>
-      <c r="D7" s="51" t="s">
+      <c r="D7" s="50" t="s">
         <v>180</v>
       </c>
     </row>
@@ -8279,7 +8297,7 @@
       <c r="C8" t="s">
         <v>181</v>
       </c>
-      <c r="D8" s="51" t="s">
+      <c r="D8" s="50" t="s">
         <v>182</v>
       </c>
     </row>
@@ -8293,7 +8311,7 @@
       <c r="C9" t="s">
         <v>183</v>
       </c>
-      <c r="D9" s="51" t="s">
+      <c r="D9" s="50" t="s">
         <v>184</v>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-10-13 09:45:06
</commit_message>
<xml_diff>
--- a/data/Solar_Lab_Tests.xlsx
+++ b/data/Solar_Lab_Tests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29404"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29406"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vikramsolar0-my.sharepoint.com/personal/naveen_chamaria_vikramsolar_com/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1813" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{690731DC-B418-49B7-9ADF-424E2414A3D3}"/>
+  <xr:revisionPtr revIDLastSave="1819" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B6AEBA20-30D9-4B71-A056-7A58731E17EE}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="7" activeTab="11" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="11" activeTab="3" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Tests Map" sheetId="4" state="hidden" r:id="rId1"/>
@@ -1534,7 +1534,7 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2508,7 +2508,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{333C0630-51CF-46CA-8CAD-98FEF9AC181F}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
@@ -5209,8 +5209,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9401EE47-EA52-49C7-BBC0-21F5B88254FB}">
   <dimension ref="A1:K91"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E91" sqref="E91"/>
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="H91" sqref="H91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -7088,8 +7088,11 @@
       <c r="E89" s="4">
         <v>45939</v>
       </c>
+      <c r="F89" s="4">
+        <v>45941</v>
+      </c>
       <c r="H89" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="90" spans="1:8">
@@ -7106,8 +7109,11 @@
       <c r="E90" s="4">
         <v>45939</v>
       </c>
+      <c r="F90" s="4">
+        <v>45941</v>
+      </c>
       <c r="H90" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="91" spans="1:8">
@@ -7124,8 +7130,11 @@
       <c r="E91" s="4">
         <v>45939</v>
       </c>
+      <c r="F91" s="4">
+        <v>45941</v>
+      </c>
       <c r="H91" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-10-13 10:46:26
</commit_message>
<xml_diff>
--- a/data/Solar_Lab_Tests.xlsx
+++ b/data/Solar_Lab_Tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vikramsolar0-my.sharepoint.com/personal/naveen_chamaria_vikramsolar_com/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1819" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B6AEBA20-30D9-4B71-A056-7A58731E17EE}"/>
+  <xr:revisionPtr revIDLastSave="1850" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{770CD4BC-F157-46ED-8160-F9D904FD9FB9}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="11" activeTab="3" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="3" activeTab="8" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Tests Map" sheetId="4" state="hidden" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <definedName name="ENCAPTYPE">Ref!$K$2:$K$1048576</definedName>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">'Material Tests Map'!$A$1:$B$20</definedName>
     <definedName name="ExternalData_1" localSheetId="12" hidden="1">'Standard test times'!$A$1:$B$15</definedName>
-    <definedName name="ExternalData_1" localSheetId="3" hidden="1">'Test Data'!$A$1:$H$91</definedName>
+    <definedName name="ExternalData_1" localSheetId="3" hidden="1">'Test Data'!$A$1:$H$93</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="257">
   <si>
     <t>BOM</t>
   </si>
@@ -451,6 +451,12 @@
     <t>LINE JUREN0.24/6/4m</t>
   </si>
   <si>
+    <t>FASTO4:1</t>
+  </si>
+  <si>
+    <t>FASTO6:1</t>
+  </si>
+  <si>
     <t xml:space="preserve">                                                                                                                           PRE PCT</t>
   </si>
   <si>
@@ -635,6 +641,18 @@
   </si>
   <si>
     <t>FASTO POTTING</t>
+  </si>
+  <si>
+    <t>FASTO 4:1</t>
+  </si>
+  <si>
+    <t>FASTO 6:1</t>
+  </si>
+  <si>
+    <t>TONSON 4:1</t>
+  </si>
+  <si>
+    <t>TONSON 6:1</t>
   </si>
   <si>
     <t>SPEED (RPM)</t>
@@ -830,6 +848,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+  </numFmts>
   <fonts count="10">
     <font>
       <sz val="11"/>
@@ -1167,7 +1188,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1248,6 +1269,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1758,8 +1783,8 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{8C209182-09AA-48EA-902C-6AAC66F47A76}" name="Table12" displayName="Table12" ref="A1:D5" totalsRowShown="0">
-  <autoFilter ref="A1:D5" xr:uid="{8C209182-09AA-48EA-902C-6AAC66F47A76}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{8C209182-09AA-48EA-902C-6AAC66F47A76}" name="Table12" displayName="Table12" ref="A1:D9" totalsRowShown="0">
+  <autoFilter ref="A1:D9" xr:uid="{8C209182-09AA-48EA-902C-6AAC66F47A76}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{27C63457-5CD9-4E66-9147-3F02C3CC7E21}" name="BOM"/>
     <tableColumn id="2" xr3:uid="{F36AEF9E-FAC6-46B7-9647-9D784C7A5C69}" name="VENDOR NAME"/>
@@ -1890,7 +1915,7 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{06A3AD80-C098-4015-85FF-3495CE4443EA}" name="Test_Data" displayName="Test_Data" ref="A1:H91" tableType="queryTable" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{06A3AD80-C098-4015-85FF-3495CE4443EA}" name="Test_Data" displayName="Test_Data" ref="A1:H93" tableType="queryTable" totalsRowShown="0">
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{87F75B08-44C4-4718-834D-87FEE9F87970}" uniqueName="1" name="BOM" queryTableFieldId="1" dataDxfId="34"/>
     <tableColumn id="2" xr3:uid="{1E5F4521-5E5C-4948-AEB2-FC5F712DB353}" uniqueName="2" name="TEST NAME" queryTableFieldId="2" dataDxfId="33"/>
@@ -2444,10 +2469,10 @@
         <v>44</v>
       </c>
       <c r="C1" s="49" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="D1" s="49" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -2481,10 +2506,10 @@
         <v>44</v>
       </c>
       <c r="C1" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="D1" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>
@@ -2533,25 +2558,25 @@
         <v>44</v>
       </c>
       <c r="C1" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="D1" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="E1" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="F1" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="G1" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="H1" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="I1" s="51" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -2559,13 +2584,13 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="D2" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="E2" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -2573,7 +2598,7 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -2581,13 +2606,13 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="D4">
         <v>302</v>
       </c>
       <c r="E4" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -2601,7 +2626,7 @@
         <v>260</v>
       </c>
       <c r="E5" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -2609,13 +2634,13 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="D6" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="E6" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -2626,10 +2651,10 @@
         <v>81</v>
       </c>
       <c r="D7" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="E7" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -2640,13 +2665,13 @@
         <v>101</v>
       </c>
       <c r="D8" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="E8" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="F8" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="G8">
         <v>217</v>
@@ -2660,10 +2685,10 @@
         <v>93</v>
       </c>
       <c r="D9" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="E9" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -2674,13 +2699,13 @@
         <v>92</v>
       </c>
       <c r="D10" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="E10" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="F10" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="G10">
         <v>202</v>
@@ -2691,16 +2716,16 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="D11" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="E11" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="F11" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="G11">
         <v>185</v>
@@ -2714,10 +2739,10 @@
         <v>79</v>
       </c>
       <c r="D12" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="E12" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -2725,7 +2750,7 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -2736,10 +2761,10 @@
         <v>89</v>
       </c>
       <c r="D14" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="E14" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -2747,13 +2772,13 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="D15" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="E15" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -2764,10 +2789,10 @@
         <v>85</v>
       </c>
       <c r="D16" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="E16" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -2778,13 +2803,13 @@
         <v>84</v>
       </c>
       <c r="D17" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="E17" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="F17" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="G17">
         <v>134</v>
@@ -2798,13 +2823,13 @@
         <v>82</v>
       </c>
       <c r="D18" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="E18" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="F18" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="G18">
         <v>297</v>
@@ -2815,30 +2840,30 @@
         <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="D19" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="E19" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="F19" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="G19" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="B20" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="F20" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="G20" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15">
@@ -2849,10 +2874,10 @@
         <v>116</v>
       </c>
       <c r="D21" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="E21" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -2860,13 +2885,13 @@
         <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="F22" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="G22" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -2902,7 +2927,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -5207,10 +5232,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9401EE47-EA52-49C7-BBC0-21F5B88254FB}">
-  <dimension ref="A1:K91"/>
+  <dimension ref="A1:K93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="H91" sqref="H91"/>
+    <sheetView topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="H93" sqref="H93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -7134,6 +7159,50 @@
         <v>45941</v>
       </c>
       <c r="H91" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8">
+      <c r="A92" s="52" t="s">
+        <v>11</v>
+      </c>
+      <c r="B92" s="52" t="s">
+        <v>12</v>
+      </c>
+      <c r="C92" s="52" t="s">
+        <v>126</v>
+      </c>
+      <c r="D92" s="53"/>
+      <c r="E92" s="4">
+        <v>45942</v>
+      </c>
+      <c r="F92" s="4">
+        <v>45943</v>
+      </c>
+      <c r="G92" s="52"/>
+      <c r="H92" s="52" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8">
+      <c r="A93" s="52" t="s">
+        <v>11</v>
+      </c>
+      <c r="B93" s="52" t="s">
+        <v>12</v>
+      </c>
+      <c r="C93" s="52" t="s">
+        <v>127</v>
+      </c>
+      <c r="D93" s="53"/>
+      <c r="E93" s="4">
+        <v>45942</v>
+      </c>
+      <c r="F93" s="4">
+        <v>45943</v>
+      </c>
+      <c r="G93" s="52"/>
+      <c r="H93" s="52" t="s">
         <v>32</v>
       </c>
     </row>
@@ -7208,14 +7277,14 @@
       <c r="A1" s="28"/>
       <c r="B1" s="29"/>
       <c r="C1" s="30" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D1" s="31"/>
       <c r="E1" s="30"/>
       <c r="F1" s="31"/>
       <c r="G1" s="32"/>
       <c r="H1" s="44" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="I1" s="32"/>
       <c r="J1" s="29"/>
@@ -7228,19 +7297,19 @@
         <v>44</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D2" s="36"/>
       <c r="E2" s="37" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="F2" s="38"/>
       <c r="G2" s="35" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="37" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="J2" s="38"/>
     </row>
@@ -7409,7 +7478,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="45" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C8" s="45">
         <v>166</v>
@@ -7441,7 +7510,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="45" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C9" s="45">
         <v>80</v>
@@ -7563,10 +7632,10 @@
         <v>44</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="6" customFormat="1">
@@ -7590,7 +7659,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C3" s="48">
         <v>14.6</v>
@@ -7604,7 +7673,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -7612,7 +7681,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -7620,7 +7689,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -7628,7 +7697,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -7636,7 +7705,7 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C8" s="48">
         <v>16.5</v>
@@ -7650,7 +7719,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -7658,7 +7727,7 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -7666,7 +7735,7 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -7674,7 +7743,7 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -7682,7 +7751,7 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C13" s="48">
         <v>42.8</v>
@@ -7696,7 +7765,7 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C14" s="48">
         <v>69.3</v>
@@ -7710,7 +7779,7 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C15" s="48">
         <v>68.599999999999994</v>
@@ -7724,7 +7793,7 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C16" s="48">
         <v>88.7</v>
@@ -7775,25 +7844,25 @@
         <v>44</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -7801,7 +7870,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C2" t="s">
         <v>34</v>
@@ -7831,7 +7900,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C3" t="s">
         <v>34</v>
@@ -7861,7 +7930,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D4">
         <v>10.16</v>
@@ -7888,7 +7957,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D5">
         <v>9.66</v>
@@ -7915,7 +7984,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C6" t="s">
         <v>34</v>
@@ -7945,7 +8014,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C7" t="s">
         <v>34</v>
@@ -7975,7 +8044,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D8">
         <v>10.84</v>
@@ -8002,7 +8071,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D9">
         <v>10.15</v>
@@ -8029,7 +8098,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C10" t="s">
         <v>34</v>
@@ -8059,7 +8128,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C11" t="s">
         <v>34</v>
@@ -8089,7 +8158,7 @@
         <v>2</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C12" t="s">
         <v>34</v>
@@ -8119,7 +8188,7 @@
         <v>2</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C13" t="s">
         <v>34</v>
@@ -8200,7 +8269,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B1" t="s">
         <v>30</v>
@@ -8209,7 +8278,7 @@
         <v>44</v>
       </c>
       <c r="D1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -8217,13 +8286,13 @@
         <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C2" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D2" s="50" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -8231,13 +8300,13 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C3" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D3" s="50" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -8245,13 +8314,13 @@
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C4" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="D4" s="50" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -8259,13 +8328,13 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C5" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D5" s="50" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -8273,13 +8342,13 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C6" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D6" s="50" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -8287,13 +8356,13 @@
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C7" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="D7" s="50" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -8301,13 +8370,13 @@
         <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C8" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="D8" s="50" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -8315,13 +8384,13 @@
         <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C9" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="D9" s="50" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -8344,8 +8413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19611726-A899-4D7E-9AA1-680BBD5826DA}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -8364,10 +8433,10 @@
         <v>44</v>
       </c>
       <c r="C1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D1" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -8403,13 +8472,69 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C5" s="10">
         <v>0.84722222222222221</v>
       </c>
       <c r="D5" s="10">
         <v>0.91319444444444442</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C6" s="10">
+        <v>0.50972222222222219</v>
+      </c>
+      <c r="D6" s="10">
+        <v>9.7222222222222224E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>191</v>
+      </c>
+      <c r="C7" s="10">
+        <v>0.50347222222222221</v>
+      </c>
+      <c r="D7" s="10">
+        <v>0.12847222222222221</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>192</v>
+      </c>
+      <c r="C8" s="10">
+        <v>9.375E-2</v>
+      </c>
+      <c r="D8" s="10">
+        <v>0.11874999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>193</v>
+      </c>
+      <c r="C9" s="10">
+        <v>9.0277777777777776E-2</v>
+      </c>
+      <c r="D9" s="10">
+        <v>0.12083333333333333</v>
       </c>
     </row>
     <row r="30" spans="3:3">

</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-10-16 09:43:56
</commit_message>
<xml_diff>
--- a/data/Solar_Lab_Tests.xlsx
+++ b/data/Solar_Lab_Tests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29406"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29409"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vikramsolar0-my.sharepoint.com/personal/naveen_chamaria_vikramsolar_com/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1850" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{770CD4BC-F157-46ED-8160-F9D904FD9FB9}"/>
+  <xr:revisionPtr revIDLastSave="2010" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{26AC50EC-73EE-4737-939E-66F3BFF25795}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="3" activeTab="8" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="11" activeTab="7" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Tests Map" sheetId="4" state="hidden" r:id="rId1"/>
@@ -25,12 +25,13 @@
     <sheet name="VISCOCITY" sheetId="19" r:id="rId10"/>
     <sheet name="CURING DEPTH" sheetId="15" r:id="rId11"/>
     <sheet name="BYPASS DIODE TEST" sheetId="16" r:id="rId12"/>
-    <sheet name="Standard test times" sheetId="6" state="hidden" r:id="rId13"/>
+    <sheet name="BLOCKING DIODE TEST" sheetId="20" r:id="rId13"/>
+    <sheet name="Standard test times" sheetId="6" state="hidden" r:id="rId14"/>
   </sheets>
   <definedNames>
     <definedName name="ENCAPTYPE">Ref!$K$2:$K$1048576</definedName>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">'Material Tests Map'!$A$1:$B$20</definedName>
-    <definedName name="ExternalData_1" localSheetId="12" hidden="1">'Standard test times'!$A$1:$B$15</definedName>
+    <definedName name="ExternalData_1" localSheetId="13" hidden="1">'Standard test times'!$A$1:$B$15</definedName>
     <definedName name="ExternalData_1" localSheetId="3" hidden="1">'Test Data'!$A$1:$H$93</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
@@ -70,8 +71,30 @@
 </connections>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="274">
   <si>
     <t>BOM</t>
   </si>
@@ -442,19 +465,19 @@
     <t>UKTR CON 4545 30U</t>
   </si>
   <si>
-    <t>VIDYA0.24/6MM/4MM</t>
-  </si>
-  <si>
-    <t>VALEO0.24/6mm/4mm</t>
-  </si>
-  <si>
-    <t>LINE JUREN0.24/6/4m</t>
-  </si>
-  <si>
-    <t>FASTO4:1</t>
-  </si>
-  <si>
-    <t>FASTO6:1</t>
+    <t>VIDYA 0.24/6MM/4MM</t>
+  </si>
+  <si>
+    <t>VALEO 0.24/6mm/4mm</t>
+  </si>
+  <si>
+    <t>LINE JUREN 0.24/6/4m</t>
+  </si>
+  <si>
+    <t>FASTO 4:1</t>
+  </si>
+  <si>
+    <t>FASTO 6:1</t>
   </si>
   <si>
     <t xml:space="preserve">                                                                                                                           PRE PCT</t>
@@ -577,7 +600,22 @@
     <t xml:space="preserve">BOM </t>
   </si>
   <si>
-    <t>MEASURED VALUE</t>
+    <t>WIDTH/DIAMETER OBSERVED (mm)</t>
+  </si>
+  <si>
+    <t>THICKNESS OBSERVED (mm)</t>
+  </si>
+  <si>
+    <t>AREA CALCULATED (sq.mm)</t>
+  </si>
+  <si>
+    <t>MEASURED  RESISTANCE (OHM)</t>
+  </si>
+  <si>
+    <t>LENGTH OF WIRE (M)</t>
+  </si>
+  <si>
+    <t>MEASURED RESISTIVITY (OHM-M)</t>
   </si>
   <si>
     <t>INTERCONNECT RIBBON</t>
@@ -586,7 +624,7 @@
     <t>WETOWN 0.24MM</t>
   </si>
   <si>
-    <t>0.421Ω</t>
+    <t>=([@[MEASURED  RESISTANCE (OHM)]]*[@[AREA CALCULATED (sq.mm)]*pow(10,-6)])/[@[LENGTH OF WIRE (M)]]</t>
   </si>
   <si>
     <t>BUS RIBBON</t>
@@ -595,43 +633,22 @@
     <t>WETOWN 5MM</t>
   </si>
   <si>
-    <t>.009Ω</t>
-  </si>
-  <si>
     <t>vidya 0.24mm</t>
   </si>
   <si>
-    <t>0.457Ω</t>
-  </si>
-  <si>
-    <t>vidya4mm</t>
-  </si>
-  <si>
-    <t>13.79Ω</t>
-  </si>
-  <si>
-    <t>vidya6mm</t>
-  </si>
-  <si>
-    <t>9.24Ω</t>
+    <t>vidya 4mm</t>
+  </si>
+  <si>
+    <t>vidya 6mm</t>
   </si>
   <si>
     <t>valeo 0.24mm</t>
   </si>
   <si>
-    <t>0.472Ω</t>
-  </si>
-  <si>
-    <t>valeo4mm</t>
-  </si>
-  <si>
-    <t>15.7Ω</t>
-  </si>
-  <si>
-    <t>valeo6mm</t>
-  </si>
-  <si>
-    <t>10.1Ω</t>
+    <t>valeo 4mm</t>
+  </si>
+  <si>
+    <t>valeo 6mm</t>
   </si>
   <si>
     <t>START TIME</t>
@@ -643,12 +660,6 @@
     <t>FASTO POTTING</t>
   </si>
   <si>
-    <t>FASTO 4:1</t>
-  </si>
-  <si>
-    <t>FASTO 6:1</t>
-  </si>
-  <si>
     <t>TONSON 4:1</t>
   </si>
   <si>
@@ -805,40 +816,103 @@
     <t>261MV</t>
   </si>
   <si>
+    <t>349VBD/265VBY</t>
+  </si>
+  <si>
+    <t>256IBY/322IBD</t>
+  </si>
+  <si>
+    <t>341VBD/269VBY</t>
+  </si>
+  <si>
+    <t>UKTR BD 7500L</t>
+  </si>
+  <si>
+    <t>345VBD/264VBY</t>
+  </si>
+  <si>
+    <t>205IBY/318IBD</t>
+  </si>
+  <si>
+    <t>259MV</t>
+  </si>
+  <si>
+    <t>492µA</t>
+  </si>
+  <si>
+    <t>QC  SOLAR</t>
+  </si>
+  <si>
+    <t>VBD52MV/VBY28MV</t>
+  </si>
+  <si>
+    <t>IBY2.0/IBD1.2</t>
+  </si>
+  <si>
+    <t>Avg. VBD (Pre PCT)</t>
+  </si>
+  <si>
+    <t>Avg. VBY (Pre PCT)</t>
+  </si>
+  <si>
+    <t>Avg. IBY (Pre PCT)</t>
+  </si>
+  <si>
+    <t>Avg. IBD (Pre PCT)</t>
+  </si>
+  <si>
+    <t>Avg. VBD (Post PCT)</t>
+  </si>
+  <si>
+    <t>Avg. VBY (Post PCT)</t>
+  </si>
+  <si>
+    <t>Avg. IBY (Post PCT)</t>
+  </si>
+  <si>
+    <t>Avg. IBD (Post PCT)</t>
+  </si>
+  <si>
     <t>UKTR BD 2000L</t>
   </si>
   <si>
-    <t>349VBD/265VBY</t>
-  </si>
-  <si>
-    <t>256IBY/322IBD</t>
-  </si>
-  <si>
-    <t>341VBD/269VBY</t>
-  </si>
-  <si>
-    <t>UKTR BD 7500L</t>
-  </si>
-  <si>
-    <t>345VBD/264VBY</t>
-  </si>
-  <si>
-    <t>205IBY/318IBD</t>
-  </si>
-  <si>
-    <t>259MV</t>
-  </si>
-  <si>
-    <t>492µA</t>
-  </si>
-  <si>
-    <t>QC  SOLAR</t>
-  </si>
-  <si>
-    <t>VBD52MV/VBY28MV</t>
-  </si>
-  <si>
-    <t>IBY2.0/IBD1.2</t>
+    <t>349mV</t>
+  </si>
+  <si>
+    <t>265mV</t>
+  </si>
+  <si>
+    <t>256µA</t>
+  </si>
+  <si>
+    <t>322µA</t>
+  </si>
+  <si>
+    <t>341mV</t>
+  </si>
+  <si>
+    <t>269mV</t>
+  </si>
+  <si>
+    <t>345mV</t>
+  </si>
+  <si>
+    <t>205µA</t>
+  </si>
+  <si>
+    <t>318µA</t>
+  </si>
+  <si>
+    <t>QC Solar</t>
+  </si>
+  <si>
+    <t>52mV</t>
+  </si>
+  <si>
+    <t>2µA</t>
+  </si>
+  <si>
+    <t>1.2µA</t>
   </si>
   <si>
     <t>STANDARD DURATION (DAYS)</t>
@@ -848,10 +922,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
-  </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -919,6 +990,14 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -1002,7 +1081,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -1184,11 +1263,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1269,17 +1376,312 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="49">
+  <dxfs count="71">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color theme="4"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="4"/>
+        </left>
+        <right style="thin">
+          <color theme="4"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <border outline="0">
@@ -1322,6 +1724,23 @@
         <top/>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
     </dxf>
     <dxf>
       <alignment horizontal="center"/>
@@ -1729,8 +2148,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2651D75B-871E-4C48-A5BC-EA62B7E4365B}" name="materialmap" displayName="materialmap" ref="A1:B20" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:B20" xr:uid="{2651D75B-871E-4C48-A5BC-EA62B7E4365B}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{FB02FE47-E9DA-4BCF-85A4-754E419FEDE3}" uniqueName="1" name="BOM" queryTableFieldId="1" dataDxfId="48"/>
-    <tableColumn id="2" xr3:uid="{887E7320-FACA-4349-93A6-9DD0A9102ACA}" uniqueName="2" name="TEST NAME" queryTableFieldId="2" dataDxfId="47"/>
+    <tableColumn id="1" xr3:uid="{FB02FE47-E9DA-4BCF-85A4-754E419FEDE3}" uniqueName="1" name="BOM" queryTableFieldId="1" dataDxfId="70"/>
+    <tableColumn id="2" xr3:uid="{887E7320-FACA-4349-93A6-9DD0A9102ACA}" uniqueName="2" name="TEST NAME" queryTableFieldId="2" dataDxfId="69"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1750,18 +2169,18 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{97A8C2A7-46C0-4446-B562-6550EA520638}" name="Table10" displayName="Table10" ref="A1:I15" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{97A8C2A7-46C0-4446-B562-6550EA520638}" name="Table10" displayName="Table10" ref="A1:I15" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
   <autoFilter ref="A1:I15" xr:uid="{97A8C2A7-46C0-4446-B562-6550EA520638}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{FE721515-FBBB-4487-ABCE-AAB6A5B1513A}" name="BOM" dataDxfId="13"/>
-    <tableColumn id="9" xr3:uid="{304FA6D2-898E-427A-8AC1-958C15295938}" name="VENDOR NAME" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{CB22B1B1-F2DB-4A16-825A-FE463620DEF9}" name="Type" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{37372ACB-68A6-4423-8A58-7EF31F49D3C5}" name="min value 1 " dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{87A17A4F-6A43-4AB0-9B0F-B213AAD6E601}" name="min value 2" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{BB8F60AF-F7B1-4306-8198-B69EE3E6D97A}" name="min value 3" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{03425EE3-EC03-4913-B402-224F846A29D7}" name="min value 4" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{E68E3244-13A5-47AA-8AB7-F602EE938E20}" name="min value 5" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{D5BE9073-1EC1-4D18-A75C-7F63CCD62CB2}" name="Mean" dataDxfId="5">
+    <tableColumn id="1" xr3:uid="{FE721515-FBBB-4487-ABCE-AAB6A5B1513A}" name="BOM" dataDxfId="35"/>
+    <tableColumn id="9" xr3:uid="{304FA6D2-898E-427A-8AC1-958C15295938}" name="VENDOR NAME" dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{CB22B1B1-F2DB-4A16-825A-FE463620DEF9}" name="Type" dataDxfId="33"/>
+    <tableColumn id="3" xr3:uid="{37372ACB-68A6-4423-8A58-7EF31F49D3C5}" name="min value 1 " dataDxfId="32"/>
+    <tableColumn id="4" xr3:uid="{87A17A4F-6A43-4AB0-9B0F-B213AAD6E601}" name="min value 2" dataDxfId="31"/>
+    <tableColumn id="5" xr3:uid="{BB8F60AF-F7B1-4306-8198-B69EE3E6D97A}" name="min value 3" dataDxfId="30"/>
+    <tableColumn id="6" xr3:uid="{03425EE3-EC03-4913-B402-224F846A29D7}" name="min value 4" dataDxfId="29"/>
+    <tableColumn id="7" xr3:uid="{E68E3244-13A5-47AA-8AB7-F602EE938E20}" name="min value 5" dataDxfId="28"/>
+    <tableColumn id="8" xr3:uid="{D5BE9073-1EC1-4D18-A75C-7F63CCD62CB2}" name="Mean" dataDxfId="27">
       <calculatedColumnFormula>AVERAGE(Table10[[#This Row],[min value 1 ]:[min value 5]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1770,13 +2189,24 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{20A38E0C-9EF6-4C45-A435-A35C875E6079}" name="Table4" displayName="Table4" ref="A1:D9" totalsRowShown="0">
-  <autoFilter ref="A1:D9" xr:uid="{20A38E0C-9EF6-4C45-A435-A35C875E6079}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{20A38E0C-9EF6-4C45-A435-A35C875E6079}" name="Table4" displayName="Table4" ref="A1:I9" totalsRowShown="0">
+  <autoFilter ref="A1:I9" xr:uid="{20A38E0C-9EF6-4C45-A435-A35C875E6079}"/>
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{81484900-FCE7-4687-AE80-25067EEBF4DF}" name="BOM "/>
     <tableColumn id="2" xr3:uid="{98C35052-5143-4722-B228-CDF4595728A7}" name="TYPE"/>
     <tableColumn id="3" xr3:uid="{DC0A72BF-A20E-4169-808D-31BFAFA45357}" name="VENDOR NAME"/>
-    <tableColumn id="4" xr3:uid="{C58F8BC5-05CB-47D9-818A-1926632D9181}" name="MEASURED VALUE" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{4735B835-F72D-4A2B-8B81-6E751AAC725F}" name="WIDTH/DIAMETER OBSERVED (mm)" dataDxfId="26">
+      <calculatedColumnFormula>VALUE(MID(LEFT(Table4[[#This Row],[VENDOR NAME]], LEN(Table4[[#This Row],[VENDOR NAME]]) - 2), FIND(" ", Table4[[#This Row],[VENDOR NAME]]) + 1, LEN(Table4[[#This Row],[VENDOR NAME]])))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{1749FD71-BC7F-4688-B5BB-58AB1E957DD0}" name="THICKNESS OBSERVED (mm)" dataDxfId="25"/>
+    <tableColumn id="9" xr3:uid="{C6009A87-4599-4EE2-88B2-ED4AF719D57F}" name="AREA CALCULATED (sq.mm)" dataDxfId="24">
+      <calculatedColumnFormula array="1">(_xleta.PI/4)*pow(Table4[[#This Row],[WIDTH/DIAMETER OBSERVED (mm)]],2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{C58F8BC5-05CB-47D9-818A-1926632D9181}" name="MEASURED  RESISTANCE (OHM)" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{0C266AA4-6084-4AC6-A053-78531731EDD5}" name="LENGTH OF WIRE (M)" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{3237FBF2-FB95-457B-8B4A-4DD03AC08D27}" name="MEASURED RESISTIVITY (OHM-M)" dataDxfId="21">
+      <calculatedColumnFormula>(Table4[[#This Row],[MEASURED  RESISTANCE (OHM)]]*Table4[[#This Row],[AREA CALCULATED (sq.mm)]])/Table4[[#This Row],[LENGTH OF WIRE (M)]]</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1796,7 +2226,7 @@
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{7D52E9E1-FA71-4119-BB85-0C937D311733}" name="Table19" displayName="Table19" ref="A1:D2" insertRow="1" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="1" tableBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{7D52E9E1-FA71-4119-BB85-0C937D311733}" name="Table19" displayName="Table19" ref="A1:D2" insertRow="1" totalsRowShown="0" headerRowDxfId="20" headerRowBorderDxfId="18" tableBorderDxfId="19">
   <autoFilter ref="A1:D2" xr:uid="{7D52E9E1-FA71-4119-BB85-0C937D311733}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{064AD3EC-978F-4DB6-BD86-F369665BDD0B}" name="BOM"/>
@@ -1840,6 +2270,28 @@
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{4B7112A1-93DC-48E7-B447-65BD878441CD}" name="Table17" displayName="Table17" ref="A1:M2" insertRow="1" insertRowShift="1" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16" headerRowBorderDxfId="14" tableBorderDxfId="15">
+  <autoFilter ref="A1:M2" xr:uid="{4B7112A1-93DC-48E7-B447-65BD878441CD}"/>
+  <tableColumns count="13">
+    <tableColumn id="1" xr3:uid="{30A8BEDF-1B2B-4821-A619-C3E0749A32C5}" name="BOM" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{E3F6AD09-C0D8-43FF-B5D1-87CF2C1B7B37}" name="VENDOR NAME" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{98CA40BC-553D-4F4C-B8B5-66259039F448}" name="AVG. MAX TEMPERATURE OF DIODE(Tj) IN ON state" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{66320D00-9F3F-45A8-AA17-1A51AD0F943F}" name="Avg. VBD (Pre PCT)" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{B082FEF3-8B8A-4B71-A497-93B9AA618A53}" name="Avg. VBY (Pre PCT)" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{C690C6D8-CD4B-4634-AC02-8FEEEF33AA37}" name="Avg. IBY (Pre PCT)" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{4B70AE10-E0C3-4223-9E36-F1FAA112F53A}" name="Avg. IBD (Pre PCT)" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{52C881BC-D641-4C18-9033-CD9A8B5083AF}" name="Avg. VBD (Post PCT)" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{F7DC931D-B133-4E78-9F5B-1920F61B624D}" name="Avg. VBY (Post PCT)" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{2D67268D-96C7-4C5A-A9BE-3DEC543787A1}" name="Avg. IBY (Post PCT)" dataDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{7E833A43-8EE9-4398-9B48-AE6686B8701F}" name="Avg. IBD (Post PCT)" dataDxfId="3"/>
+    <tableColumn id="12" xr3:uid="{2A2B5106-9EEC-4BE0-9D7A-FD61527D560F}" name="RESISTANCE(Pre PCT)" dataDxfId="2"/>
+    <tableColumn id="13" xr3:uid="{05C6CA44-C293-4598-9DFA-B86A5190E2D1}" name="RESISTANCE(Post PCT)" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{68171DB0-643B-43C2-B0C7-B755548E6CA4}" name="standard_test_time" displayName="standard_test_time" ref="A1:B15" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:B15" xr:uid="{68171DB0-643B-43C2-B0C7-B755548E6CA4}"/>
   <tableColumns count="2">
@@ -1896,19 +2348,19 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{7FFEF855-2CB7-4EF4-BE50-FB81C544017B}" name="Table18" displayName="Table18" ref="B3:K1048576" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{7FFEF855-2CB7-4EF4-BE50-FB81C544017B}" name="Table18" displayName="Table18" ref="B3:K1048576" totalsRowShown="0" headerRowDxfId="68" dataDxfId="67">
   <autoFilter ref="B3:K1048576" xr:uid="{7FFEF855-2CB7-4EF4-BE50-FB81C544017B}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{96E09178-FF72-435C-90A9-F2F7FEC7E80C}" name="Column1" dataDxfId="44"/>
-    <tableColumn id="2" xr3:uid="{B7D3E49F-4F89-454D-B9FA-E1364CBF3239}" name="Column2" dataDxfId="43"/>
-    <tableColumn id="3" xr3:uid="{CCA06B22-44E5-4255-8F26-0C1B1279B22C}" name="Column3" dataDxfId="42"/>
-    <tableColumn id="4" xr3:uid="{6F565555-BB1C-4294-A1BA-3B6ADB9C2D2F}" name="Column4" dataDxfId="41"/>
-    <tableColumn id="5" xr3:uid="{33CA8E10-7021-4A52-853E-A6227866156B}" name="Column5" dataDxfId="40"/>
-    <tableColumn id="6" xr3:uid="{870E308E-FC7E-4A0A-A66A-ED0B8741D8AF}" name="Column6" dataDxfId="39"/>
-    <tableColumn id="7" xr3:uid="{FEEFF96D-1CCA-48C1-982D-EAFDB6BC3200}" name="Column7" dataDxfId="38"/>
-    <tableColumn id="8" xr3:uid="{4FEE2433-7AE2-4CF7-A1FC-541524E1FAAF}" name="Column8" dataDxfId="37"/>
-    <tableColumn id="9" xr3:uid="{A6BC8484-A791-4583-A77F-7F6A667CE8C5}" name="Column9" dataDxfId="36"/>
-    <tableColumn id="10" xr3:uid="{192E7774-55A7-4BD2-9715-330A7F12089B}" name="Column10" dataDxfId="35"/>
+    <tableColumn id="1" xr3:uid="{96E09178-FF72-435C-90A9-F2F7FEC7E80C}" name="Column1" dataDxfId="66"/>
+    <tableColumn id="2" xr3:uid="{B7D3E49F-4F89-454D-B9FA-E1364CBF3239}" name="Column2" dataDxfId="65"/>
+    <tableColumn id="3" xr3:uid="{CCA06B22-44E5-4255-8F26-0C1B1279B22C}" name="Column3" dataDxfId="64"/>
+    <tableColumn id="4" xr3:uid="{6F565555-BB1C-4294-A1BA-3B6ADB9C2D2F}" name="Column4" dataDxfId="63"/>
+    <tableColumn id="5" xr3:uid="{33CA8E10-7021-4A52-853E-A6227866156B}" name="Column5" dataDxfId="62"/>
+    <tableColumn id="6" xr3:uid="{870E308E-FC7E-4A0A-A66A-ED0B8741D8AF}" name="Column6" dataDxfId="61"/>
+    <tableColumn id="7" xr3:uid="{FEEFF96D-1CCA-48C1-982D-EAFDB6BC3200}" name="Column7" dataDxfId="60"/>
+    <tableColumn id="8" xr3:uid="{4FEE2433-7AE2-4CF7-A1FC-541524E1FAAF}" name="Column8" dataDxfId="59"/>
+    <tableColumn id="9" xr3:uid="{A6BC8484-A791-4583-A77F-7F6A667CE8C5}" name="Column9" dataDxfId="58"/>
+    <tableColumn id="10" xr3:uid="{192E7774-55A7-4BD2-9715-330A7F12089B}" name="Column10" dataDxfId="57"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1917,33 +2369,33 @@
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{06A3AD80-C098-4015-85FF-3495CE4443EA}" name="Test_Data" displayName="Test_Data" ref="A1:H93" tableType="queryTable" totalsRowShown="0">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{87F75B08-44C4-4718-834D-87FEE9F87970}" uniqueName="1" name="BOM" queryTableFieldId="1" dataDxfId="34"/>
-    <tableColumn id="2" xr3:uid="{1E5F4521-5E5C-4948-AEB2-FC5F712DB353}" uniqueName="2" name="TEST NAME" queryTableFieldId="2" dataDxfId="33"/>
-    <tableColumn id="3" xr3:uid="{22629B97-1F38-4A88-B08E-7589CFF4C28D}" uniqueName="3" name="VENDOR NAME" queryTableFieldId="3" dataDxfId="32"/>
-    <tableColumn id="4" xr3:uid="{D6678E87-972B-4807-86C4-4086EF552262}" uniqueName="4" name="GRN GENERATION TIME" queryTableFieldId="4" dataDxfId="31"/>
-    <tableColumn id="5" xr3:uid="{62C80EA2-76AB-4742-87FF-05248307AF93}" uniqueName="5" name="TEST START DATE AND TIME" queryTableFieldId="5" dataDxfId="30"/>
-    <tableColumn id="6" xr3:uid="{DDA3B4DC-3A06-4223-8D24-00B8C4C20678}" uniqueName="6" name="TEST END DATE AND TIME" queryTableFieldId="6" dataDxfId="29"/>
-    <tableColumn id="7" xr3:uid="{F2102600-A33C-449C-8C79-361FEA6C4BCE}" uniqueName="7" name="TEST RESULT" queryTableFieldId="7" dataDxfId="28"/>
-    <tableColumn id="8" xr3:uid="{E5E91A8D-E194-48B6-8D9A-FFD1939E8ACF}" uniqueName="8" name="STATUS" queryTableFieldId="8" dataDxfId="27"/>
+    <tableColumn id="1" xr3:uid="{87F75B08-44C4-4718-834D-87FEE9F87970}" uniqueName="1" name="BOM" queryTableFieldId="1" dataDxfId="56"/>
+    <tableColumn id="2" xr3:uid="{1E5F4521-5E5C-4948-AEB2-FC5F712DB353}" uniqueName="2" name="TEST NAME" queryTableFieldId="2" dataDxfId="55"/>
+    <tableColumn id="3" xr3:uid="{22629B97-1F38-4A88-B08E-7589CFF4C28D}" uniqueName="3" name="VENDOR NAME" queryTableFieldId="3" dataDxfId="54"/>
+    <tableColumn id="4" xr3:uid="{D6678E87-972B-4807-86C4-4086EF552262}" uniqueName="4" name="GRN GENERATION TIME" queryTableFieldId="4" dataDxfId="53"/>
+    <tableColumn id="5" xr3:uid="{62C80EA2-76AB-4742-87FF-05248307AF93}" uniqueName="5" name="TEST START DATE AND TIME" queryTableFieldId="5" dataDxfId="52"/>
+    <tableColumn id="6" xr3:uid="{DDA3B4DC-3A06-4223-8D24-00B8C4C20678}" uniqueName="6" name="TEST END DATE AND TIME" queryTableFieldId="6" dataDxfId="51"/>
+    <tableColumn id="7" xr3:uid="{F2102600-A33C-449C-8C79-361FEA6C4BCE}" uniqueName="7" name="TEST RESULT" queryTableFieldId="7" dataDxfId="50"/>
+    <tableColumn id="8" xr3:uid="{E5E91A8D-E194-48B6-8D9A-FFD1939E8ACF}" uniqueName="8" name="STATUS" queryTableFieldId="8" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{67926097-CCFB-425B-9820-DDDFB77C87C9}" name="Table11" displayName="Table11" ref="A4:J1048576" totalsRowShown="0" dataDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{67926097-CCFB-425B-9820-DDDFB77C87C9}" name="Table11" displayName="Table11" ref="A4:J1048576" totalsRowShown="0" dataDxfId="48">
   <autoFilter ref="A4:J1048576" xr:uid="{67926097-CCFB-425B-9820-DDDFB77C87C9}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{EA92BD46-85A5-4BF3-9843-966A2E5861D9}" name="Column1" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{C24A9AB3-E538-4185-9C80-E9DDC6A05A90}" name="Column2" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{0CA46B2C-315A-49B7-A313-787EA669AF33}" name="Column3" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{AA05AB49-E5DC-4F39-BF84-5C21AE004473}" name="Column4" dataDxfId="22"/>
-    <tableColumn id="5" xr3:uid="{8D9CD07A-CD8E-459F-AD52-C1C64282E998}" name="Column5" dataDxfId="21"/>
-    <tableColumn id="6" xr3:uid="{953BA2E8-443D-4DD4-ACF1-1ECEDB5DE6DD}" name="Column6" dataDxfId="20"/>
-    <tableColumn id="7" xr3:uid="{8ED40F5F-1EB7-4C33-83D6-002E5FC5C1EC}" name="Column7" dataDxfId="19"/>
-    <tableColumn id="8" xr3:uid="{3EC62242-31F0-4282-815A-7D5C6B4310FD}" name="Column8" dataDxfId="18"/>
-    <tableColumn id="9" xr3:uid="{514AC0BC-C14D-43E8-9076-A902208889C3}" name="Column9" dataDxfId="17"/>
-    <tableColumn id="10" xr3:uid="{94E39AAC-5F2B-4668-8EAE-7D440F802CF1}" name="Column10" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{EA92BD46-85A5-4BF3-9843-966A2E5861D9}" name="Column1" dataDxfId="47"/>
+    <tableColumn id="2" xr3:uid="{C24A9AB3-E538-4185-9C80-E9DDC6A05A90}" name="Column2" dataDxfId="46"/>
+    <tableColumn id="3" xr3:uid="{0CA46B2C-315A-49B7-A313-787EA669AF33}" name="Column3" dataDxfId="45"/>
+    <tableColumn id="4" xr3:uid="{AA05AB49-E5DC-4F39-BF84-5C21AE004473}" name="Column4" dataDxfId="44"/>
+    <tableColumn id="5" xr3:uid="{8D9CD07A-CD8E-459F-AD52-C1C64282E998}" name="Column5" dataDxfId="43"/>
+    <tableColumn id="6" xr3:uid="{953BA2E8-443D-4DD4-ACF1-1ECEDB5DE6DD}" name="Column6" dataDxfId="42"/>
+    <tableColumn id="7" xr3:uid="{8ED40F5F-1EB7-4C33-83D6-002E5FC5C1EC}" name="Column7" dataDxfId="41"/>
+    <tableColumn id="8" xr3:uid="{3EC62242-31F0-4282-815A-7D5C6B4310FD}" name="Column8" dataDxfId="40"/>
+    <tableColumn id="9" xr3:uid="{514AC0BC-C14D-43E8-9076-A902208889C3}" name="Column9" dataDxfId="39"/>
+    <tableColumn id="10" xr3:uid="{94E39AAC-5F2B-4668-8EAE-7D440F802CF1}" name="Column10" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2469,10 +2921,10 @@
         <v>44</v>
       </c>
       <c r="C1" s="49" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="D1" s="49" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -2506,10 +2958,10 @@
         <v>44</v>
       </c>
       <c r="C1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D1" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -2533,8 +2985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{333C0630-51CF-46CA-8CAD-98FEF9AC181F}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -2558,25 +3010,25 @@
         <v>44</v>
       </c>
       <c r="C1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E1" t="s">
+        <v>196</v>
+      </c>
+      <c r="F1" t="s">
+        <v>197</v>
+      </c>
+      <c r="G1" t="s">
         <v>198</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
         <v>199</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" s="51" t="s">
         <v>200</v>
-      </c>
-      <c r="F1" t="s">
-        <v>201</v>
-      </c>
-      <c r="G1" t="s">
-        <v>202</v>
-      </c>
-      <c r="H1" t="s">
-        <v>203</v>
-      </c>
-      <c r="I1" s="51" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -2584,13 +3036,13 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D2" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="E2" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -2598,7 +3050,7 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -2606,13 +3058,13 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D4">
         <v>302</v>
       </c>
       <c r="E4" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -2626,7 +3078,7 @@
         <v>260</v>
       </c>
       <c r="E5" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -2634,13 +3086,13 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D6" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="E6" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -2651,10 +3103,10 @@
         <v>81</v>
       </c>
       <c r="D7" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="E7" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -2665,13 +3117,13 @@
         <v>101</v>
       </c>
       <c r="D8" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="E8" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="F8" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="G8">
         <v>217</v>
@@ -2685,10 +3137,10 @@
         <v>93</v>
       </c>
       <c r="D9" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E9" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -2699,13 +3151,13 @@
         <v>92</v>
       </c>
       <c r="D10" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="E10" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="F10" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="G10">
         <v>202</v>
@@ -2716,16 +3168,16 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D11" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="E11" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="F11" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="G11">
         <v>185</v>
@@ -2739,10 +3191,10 @@
         <v>79</v>
       </c>
       <c r="D12" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="E12" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -2750,7 +3202,7 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -2761,10 +3213,10 @@
         <v>89</v>
       </c>
       <c r="D14" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E14" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -2772,13 +3224,13 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="D15" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="E15" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -2789,10 +3241,10 @@
         <v>85</v>
       </c>
       <c r="D16" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="E16" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -2803,13 +3255,13 @@
         <v>84</v>
       </c>
       <c r="D17" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="E17" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="F17" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="G17">
         <v>134</v>
@@ -2823,13 +3275,13 @@
         <v>82</v>
       </c>
       <c r="D18" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E18" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="F18" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="G18">
         <v>297</v>
@@ -2839,34 +3291,31 @@
       <c r="A19" t="s">
         <v>15</v>
       </c>
-      <c r="B19" t="s">
+      <c r="D19" t="s">
+        <v>240</v>
+      </c>
+      <c r="E19" t="s">
+        <v>241</v>
+      </c>
+      <c r="F19" t="s">
+        <v>242</v>
+      </c>
+      <c r="G19" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" hidden="1">
+      <c r="B20" t="s">
+        <v>243</v>
+      </c>
+      <c r="F20" t="s">
         <v>244</v>
       </c>
-      <c r="D19" t="s">
+      <c r="G20" t="s">
         <v>245</v>
       </c>
-      <c r="E19" t="s">
-        <v>246</v>
-      </c>
-      <c r="F19" t="s">
-        <v>247</v>
-      </c>
-      <c r="G19" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="B20" t="s">
-        <v>248</v>
-      </c>
-      <c r="F20" t="s">
-        <v>249</v>
-      </c>
-      <c r="G20" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="15">
+    </row>
+    <row r="21" spans="1:7" ht="15" hidden="1">
       <c r="A21" t="s">
         <v>15</v>
       </c>
@@ -2874,24 +3323,24 @@
         <v>116</v>
       </c>
       <c r="D21" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="E21" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" hidden="1">
       <c r="A22" t="s">
         <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="F22" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="G22" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -2909,6 +3358,172 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6479E4F1-BC59-4550-8B9C-28E93C6F8271}">
+  <dimension ref="A1:M5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" customWidth="1"/>
+    <col min="3" max="3" width="46.5703125" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" customWidth="1"/>
+    <col min="8" max="8" width="21" customWidth="1"/>
+    <col min="9" max="9" width="20.85546875" customWidth="1"/>
+    <col min="10" max="11" width="21.7109375" customWidth="1"/>
+    <col min="12" max="12" width="23.140625" customWidth="1"/>
+    <col min="13" max="13" width="31.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="53" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="53" t="s">
+        <v>194</v>
+      </c>
+      <c r="D1" s="53" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1" s="53" t="s">
+        <v>252</v>
+      </c>
+      <c r="F1" s="53" t="s">
+        <v>253</v>
+      </c>
+      <c r="G1" s="53" t="s">
+        <v>254</v>
+      </c>
+      <c r="H1" s="53" t="s">
+        <v>255</v>
+      </c>
+      <c r="I1" s="53" t="s">
+        <v>256</v>
+      </c>
+      <c r="J1" s="53" t="s">
+        <v>257</v>
+      </c>
+      <c r="K1" s="53" t="s">
+        <v>258</v>
+      </c>
+      <c r="L1" s="53" t="s">
+        <v>199</v>
+      </c>
+      <c r="M1" s="54" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" hidden="1">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="52"/>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="55" t="s">
+        <v>259</v>
+      </c>
+      <c r="D3" t="s">
+        <v>260</v>
+      </c>
+      <c r="E3" t="s">
+        <v>261</v>
+      </c>
+      <c r="F3" t="s">
+        <v>262</v>
+      </c>
+      <c r="G3" t="s">
+        <v>263</v>
+      </c>
+      <c r="H3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I3" t="s">
+        <v>265</v>
+      </c>
+      <c r="J3" t="s">
+        <v>262</v>
+      </c>
+      <c r="K3" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="55" t="s">
+        <v>116</v>
+      </c>
+      <c r="H4" t="s">
+        <v>266</v>
+      </c>
+      <c r="I4">
+        <v>264</v>
+      </c>
+      <c r="J4" t="s">
+        <v>267</v>
+      </c>
+      <c r="K4" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>269</v>
+      </c>
+      <c r="H5" t="s">
+        <v>270</v>
+      </c>
+      <c r="I5">
+        <v>28</v>
+      </c>
+      <c r="J5" t="s">
+        <v>271</v>
+      </c>
+      <c r="K5" t="s">
+        <v>272</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A1048576" xr:uid="{9F65D898-6259-4AB2-AEA4-CA987C017830}">
+      <formula1>"JB"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{7CB51786-457C-4641-8CFA-E389406920A2}"/>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBA2255C-9286-47F7-8F7E-14EDD259611E}">
   <dimension ref="A1:B15"/>
   <sheetViews>
@@ -2927,7 +3542,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>256</v>
+        <v>273</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -5234,8 +5849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9401EE47-EA52-49C7-BBC0-21F5B88254FB}">
   <dimension ref="A1:K93"/>
   <sheetViews>
-    <sheetView topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="H93" sqref="H93"/>
+    <sheetView topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -7163,46 +7778,44 @@
       </c>
     </row>
     <row r="92" spans="1:8">
-      <c r="A92" s="52" t="s">
+      <c r="A92" t="s">
         <v>11</v>
       </c>
-      <c r="B92" s="52" t="s">
+      <c r="B92" t="s">
         <v>12</v>
       </c>
-      <c r="C92" s="52" t="s">
+      <c r="C92" t="s">
         <v>126</v>
       </c>
-      <c r="D92" s="53"/>
+      <c r="D92" s="5"/>
       <c r="E92" s="4">
         <v>45942</v>
       </c>
       <c r="F92" s="4">
         <v>45943</v>
       </c>
-      <c r="G92" s="52"/>
-      <c r="H92" s="52" t="s">
+      <c r="H92" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="93" spans="1:8">
-      <c r="A93" s="52" t="s">
+      <c r="A93" t="s">
         <v>11</v>
       </c>
-      <c r="B93" s="52" t="s">
+      <c r="B93" t="s">
         <v>12</v>
       </c>
-      <c r="C93" s="52" t="s">
+      <c r="C93" t="s">
         <v>127</v>
       </c>
-      <c r="D93" s="53"/>
+      <c r="D93" s="5"/>
       <c r="E93" s="4">
         <v>45942</v>
       </c>
       <c r="F93" s="4">
         <v>45943</v>
       </c>
-      <c r="G93" s="52"/>
-      <c r="H93" s="52" t="s">
+      <c r="H93" t="s">
         <v>32</v>
       </c>
     </row>
@@ -7612,7 +8225,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C8152F1-3340-4C7F-9B6C-3F6BB96763BA}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
@@ -8253,10 +8866,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD5452B6-66C2-4964-BBFB-466116F6D217}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -8264,10 +8877,15 @@
     <col min="1" max="1" width="11.5703125" customWidth="1"/>
     <col min="2" max="2" width="22.85546875" customWidth="1"/>
     <col min="3" max="3" width="20.7109375" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="28.28515625" style="50" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.5703125" style="50" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.5703125" style="50" customWidth="1"/>
+    <col min="7" max="7" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.85546875" style="50" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.42578125" style="50" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>167</v>
       </c>
@@ -8277,120 +8895,231 @@
       <c r="C1" t="s">
         <v>44</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="50" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="50" t="s">
+        <v>169</v>
+      </c>
+      <c r="F1" s="50" t="s">
+        <v>170</v>
+      </c>
+      <c r="G1" t="s">
+        <v>171</v>
+      </c>
+      <c r="H1" s="50" t="s">
+        <v>172</v>
+      </c>
+      <c r="I1" s="50" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="C2" t="s">
-        <v>170</v>
-      </c>
-      <c r="D2" s="50" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>175</v>
+      </c>
+      <c r="D2" s="50">
+        <f>VALUE(MID(LEFT(Table4[[#This Row],[VENDOR NAME]], LEN(Table4[[#This Row],[VENDOR NAME]]) - 2), FIND(" ", Table4[[#This Row],[VENDOR NAME]]) + 1, LEN(Table4[[#This Row],[VENDOR NAME]])))</f>
+        <v>0.24</v>
+      </c>
+      <c r="E2" s="50">
+        <v>0</v>
+      </c>
+      <c r="F2" s="50" t="e">
+        <f>(_xleta.PI/4)*(Table4[[#This Row],[WIDTH/DIAMETER OBSERVED (mm)]])*(Table4[[#This Row],[WIDTH/DIAMETER OBSERVED (mm)]])</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G2" s="50">
+        <v>0.42099999999999999</v>
+      </c>
+      <c r="H2" s="50">
+        <v>1</v>
+      </c>
+      <c r="I2" s="50" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="C3" t="s">
-        <v>173</v>
-      </c>
-      <c r="D3" s="50" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>178</v>
+      </c>
+      <c r="D3" s="50">
+        <f>VALUE(MID(LEFT(Table4[[#This Row],[VENDOR NAME]], LEN(Table4[[#This Row],[VENDOR NAME]]) - 2), FIND(" ", Table4[[#This Row],[VENDOR NAME]]) + 1, LEN(Table4[[#This Row],[VENDOR NAME]])))</f>
+        <v>5</v>
+      </c>
+      <c r="F3" s="50" t="e" cm="1">
+        <f t="array" aca="1" ref="F3" ca="1">(_xleta.PI/4)*pow(Table4[[#This Row],[WIDTH/DIAMETER OBSERVED (mm)]],2)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G3" s="50">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="H3" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="C4" t="s">
-        <v>175</v>
-      </c>
-      <c r="D4" s="50" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>179</v>
+      </c>
+      <c r="D4" s="50">
+        <f>VALUE(MID(LEFT(Table4[[#This Row],[VENDOR NAME]], LEN(Table4[[#This Row],[VENDOR NAME]]) - 2), FIND(" ", Table4[[#This Row],[VENDOR NAME]]) + 1, LEN(Table4[[#This Row],[VENDOR NAME]])))</f>
+        <v>0.24</v>
+      </c>
+      <c r="F4" s="50" t="e" cm="1">
+        <f t="array" aca="1" ref="F4" ca="1">(_xleta.PI/4)*pow(Table4[[#This Row],[WIDTH/DIAMETER OBSERVED (mm)]],2)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G4" s="50">
+        <v>0.45700000000000002</v>
+      </c>
+      <c r="H4" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="C5" t="s">
-        <v>177</v>
-      </c>
-      <c r="D5" s="50" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>180</v>
+      </c>
+      <c r="D5" s="50">
+        <f>VALUE(MID(LEFT(Table4[[#This Row],[VENDOR NAME]], LEN(Table4[[#This Row],[VENDOR NAME]]) - 2), FIND(" ", Table4[[#This Row],[VENDOR NAME]]) + 1, LEN(Table4[[#This Row],[VENDOR NAME]])))</f>
+        <v>4</v>
+      </c>
+      <c r="F5" s="50" t="e" cm="1">
+        <f t="array" aca="1" ref="F5" ca="1">(_xleta.PI/4)*pow(Table4[[#This Row],[WIDTH/DIAMETER OBSERVED (mm)]],2)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G5" s="50">
+        <v>13.79</v>
+      </c>
+      <c r="H5" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="C6" t="s">
-        <v>179</v>
-      </c>
-      <c r="D6" s="50" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>181</v>
+      </c>
+      <c r="D6" s="50">
+        <f>VALUE(MID(LEFT(Table4[[#This Row],[VENDOR NAME]], LEN(Table4[[#This Row],[VENDOR NAME]]) - 2), FIND(" ", Table4[[#This Row],[VENDOR NAME]]) + 1, LEN(Table4[[#This Row],[VENDOR NAME]])))</f>
+        <v>6</v>
+      </c>
+      <c r="F6" s="50" t="e" cm="1">
+        <f t="array" aca="1" ref="F6" ca="1">(_xleta.PI/4)*pow(Table4[[#This Row],[WIDTH/DIAMETER OBSERVED (mm)]],2)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G6" s="50">
+        <v>9.24</v>
+      </c>
+      <c r="H6" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="C7" t="s">
-        <v>181</v>
-      </c>
-      <c r="D7" s="50" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="D7" s="50">
+        <f>VALUE(MID(LEFT(Table4[[#This Row],[VENDOR NAME]], LEN(Table4[[#This Row],[VENDOR NAME]]) - 2), FIND(" ", Table4[[#This Row],[VENDOR NAME]]) + 1, LEN(Table4[[#This Row],[VENDOR NAME]])))</f>
+        <v>0.24</v>
+      </c>
+      <c r="F7" s="50" t="e" cm="1">
+        <f t="array" aca="1" ref="F7" ca="1">(_xleta.PI/4)*pow(Table4[[#This Row],[WIDTH/DIAMETER OBSERVED (mm)]],2)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G7" s="50">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="H7" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="C8" t="s">
         <v>183</v>
       </c>
-      <c r="D8" s="50" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="D8" s="50">
+        <f>VALUE(MID(LEFT(Table4[[#This Row],[VENDOR NAME]], LEN(Table4[[#This Row],[VENDOR NAME]]) - 2), FIND(" ", Table4[[#This Row],[VENDOR NAME]]) + 1, LEN(Table4[[#This Row],[VENDOR NAME]])))</f>
+        <v>4</v>
+      </c>
+      <c r="F8" s="50" t="e" cm="1">
+        <f t="array" aca="1" ref="F8" ca="1">(_xleta.PI/4)*pow(Table4[[#This Row],[WIDTH/DIAMETER OBSERVED (mm)]],2)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G8" s="50">
+        <f>15.7/1000</f>
+        <v>1.5699999999999999E-2</v>
+      </c>
+      <c r="H8" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="C9" t="s">
-        <v>185</v>
-      </c>
-      <c r="D9" s="50" t="s">
-        <v>186</v>
+        <v>184</v>
+      </c>
+      <c r="D9" s="50">
+        <f>VALUE(MID(LEFT(Table4[[#This Row],[VENDOR NAME]], LEN(Table4[[#This Row],[VENDOR NAME]]) - 2), FIND(" ", Table4[[#This Row],[VENDOR NAME]]) + 1, LEN(Table4[[#This Row],[VENDOR NAME]])))</f>
+        <v>6</v>
+      </c>
+      <c r="F9" s="50" t="e" cm="1">
+        <f t="array" aca="1" ref="F9" ca="1">(_xleta.PI/4)*pow(Table4[[#This Row],[WIDTH/DIAMETER OBSERVED (mm)]],2)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G9" s="50">
+        <f>10.1/1000</f>
+        <v>1.01E-2</v>
+      </c>
+      <c r="H9" s="50">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -8413,7 +9142,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19611726-A899-4D7E-9AA1-680BBD5826DA}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -8433,10 +9162,10 @@
         <v>44</v>
       </c>
       <c r="C1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -8472,7 +9201,7 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C5" s="10">
         <v>0.84722222222222221</v>
@@ -8486,7 +9215,7 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>190</v>
+        <v>126</v>
       </c>
       <c r="C6" s="10">
         <v>0.50972222222222219</v>
@@ -8500,7 +9229,7 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>191</v>
+        <v>127</v>
       </c>
       <c r="C7" s="10">
         <v>0.50347222222222221</v>
@@ -8514,7 +9243,7 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C8" s="10">
         <v>9.375E-2</v>
@@ -8528,7 +9257,7 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C9" s="10">
         <v>9.0277777777777776E-2</v>

</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-10-16 10:45:39
</commit_message>
<xml_diff>
--- a/data/Solar_Lab_Tests.xlsx
+++ b/data/Solar_Lab_Tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vikramsolar0-my.sharepoint.com/personal/naveen_chamaria_vikramsolar_com/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2010" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{26AC50EC-73EE-4737-939E-66F3BFF25795}"/>
+  <xr:revisionPtr revIDLastSave="2024" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F46BCE05-8FE3-4715-84E5-C7799AEB9F67}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="11" activeTab="7" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="7" activeTab="11" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Tests Map" sheetId="4" state="hidden" r:id="rId1"/>
@@ -32,7 +32,7 @@
     <definedName name="ENCAPTYPE">Ref!$K$2:$K$1048576</definedName>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">'Material Tests Map'!$A$1:$B$20</definedName>
     <definedName name="ExternalData_1" localSheetId="13" hidden="1">'Standard test times'!$A$1:$B$15</definedName>
-    <definedName name="ExternalData_1" localSheetId="3" hidden="1">'Test Data'!$A$1:$H$93</definedName>
+    <definedName name="ExternalData_1" localSheetId="3" hidden="1">'Test Data'!$A$1:$H$96</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -71,30 +71,8 @@
 </connections>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="277">
   <si>
     <t>BOM</t>
   </si>
@@ -478,6 +456,15 @@
   </si>
   <si>
     <t>FASTO 6:1</t>
+  </si>
+  <si>
+    <t>RFID PRODUCTION</t>
+  </si>
+  <si>
+    <t>RFID SAMPLE 1</t>
+  </si>
+  <si>
+    <t>RFID SAMPLE 2</t>
   </si>
   <si>
     <t xml:space="preserve">                                                                                                                           PRE PCT</t>
@@ -922,6 +909,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+  </numFmts>
   <fonts count="11">
     <font>
       <sz val="11"/>
@@ -1295,7 +1285,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1380,6 +1370,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2367,7 +2361,7 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{06A3AD80-C098-4015-85FF-3495CE4443EA}" name="Test_Data" displayName="Test_Data" ref="A1:H93" tableType="queryTable" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{06A3AD80-C098-4015-85FF-3495CE4443EA}" name="Test_Data" displayName="Test_Data" ref="A1:H96" tableType="queryTable" totalsRowShown="0">
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{87F75B08-44C4-4718-834D-87FEE9F87970}" uniqueName="1" name="BOM" queryTableFieldId="1" dataDxfId="56"/>
     <tableColumn id="2" xr3:uid="{1E5F4521-5E5C-4948-AEB2-FC5F712DB353}" uniqueName="2" name="TEST NAME" queryTableFieldId="2" dataDxfId="55"/>
@@ -2921,10 +2915,10 @@
         <v>44</v>
       </c>
       <c r="C1" s="49" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="D1" s="49" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -2958,10 +2952,10 @@
         <v>44</v>
       </c>
       <c r="C1" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="D1" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -2985,7 +2979,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{333C0630-51CF-46CA-8CAD-98FEF9AC181F}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
@@ -3010,25 +3004,25 @@
         <v>44</v>
       </c>
       <c r="C1" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="D1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="E1" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="F1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="G1" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="H1" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="I1" s="51" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -3036,13 +3030,13 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="D2" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="E2" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -3050,7 +3044,7 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -3058,13 +3052,13 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="D4">
         <v>302</v>
       </c>
       <c r="E4" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -3078,7 +3072,7 @@
         <v>260</v>
       </c>
       <c r="E5" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -3086,13 +3080,13 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="D6" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="E6" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -3103,10 +3097,10 @@
         <v>81</v>
       </c>
       <c r="D7" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="E7" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -3117,13 +3111,13 @@
         <v>101</v>
       </c>
       <c r="D8" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="E8" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="F8" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="G8">
         <v>217</v>
@@ -3137,10 +3131,10 @@
         <v>93</v>
       </c>
       <c r="D9" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="E9" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -3151,13 +3145,13 @@
         <v>92</v>
       </c>
       <c r="D10" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="E10" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="F10" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="G10">
         <v>202</v>
@@ -3168,16 +3162,16 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="D11" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="E11" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="F11" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="G11">
         <v>185</v>
@@ -3191,10 +3185,10 @@
         <v>79</v>
       </c>
       <c r="D12" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="E12" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -3202,7 +3196,7 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -3213,10 +3207,10 @@
         <v>89</v>
       </c>
       <c r="D14" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="E14" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -3224,13 +3218,13 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="D15" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="E15" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -3241,10 +3235,10 @@
         <v>85</v>
       </c>
       <c r="D16" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="E16" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -3255,13 +3249,13 @@
         <v>84</v>
       </c>
       <c r="D17" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="E17" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="F17" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="G17">
         <v>134</v>
@@ -3275,13 +3269,13 @@
         <v>82</v>
       </c>
       <c r="D18" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="E18" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="F18" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="G18">
         <v>297</v>
@@ -3292,27 +3286,27 @@
         <v>15</v>
       </c>
       <c r="D19" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="E19" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="F19" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="G19" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
     </row>
     <row r="20" spans="1:7" hidden="1">
       <c r="B20" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="F20" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="G20" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15" hidden="1">
@@ -3323,10 +3317,10 @@
         <v>116</v>
       </c>
       <c r="D21" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="E21" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
     </row>
     <row r="22" spans="1:7" hidden="1">
@@ -3334,13 +3328,13 @@
         <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="F22" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="G22" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -3389,37 +3383,37 @@
         <v>44</v>
       </c>
       <c r="C1" s="53" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="D1" s="53" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="E1" s="53" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="F1" s="53" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="G1" s="53" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="H1" s="53" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="I1" s="53" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="J1" s="53" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="K1" s="53" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="L1" s="53" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="M1" s="54" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
     </row>
     <row r="2" spans="1:13" hidden="1">
@@ -3442,31 +3436,31 @@
         <v>15</v>
       </c>
       <c r="B3" s="55" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="D3" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="E3" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="F3" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="G3" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="H3" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="I3" t="s">
+        <v>268</v>
+      </c>
+      <c r="J3" t="s">
         <v>265</v>
       </c>
-      <c r="J3" t="s">
-        <v>262</v>
-      </c>
       <c r="K3" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -3477,16 +3471,16 @@
         <v>116</v>
       </c>
       <c r="H4" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="I4">
         <v>264</v>
       </c>
       <c r="J4" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="K4" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -3494,19 +3488,19 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="H5" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="I5">
         <v>28</v>
       </c>
       <c r="J5" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="K5" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
     </row>
   </sheetData>
@@ -3542,7 +3536,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -5847,10 +5841,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9401EE47-EA52-49C7-BBC0-21F5B88254FB}">
-  <dimension ref="A1:K93"/>
+  <dimension ref="A1:K96"/>
   <sheetViews>
-    <sheetView topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="C88" sqref="C88"/>
+    <sheetView topLeftCell="B84" workbookViewId="0">
+      <selection activeCell="H96" sqref="H96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -7817,6 +7811,60 @@
       </c>
       <c r="H93" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8">
+      <c r="A94" s="56"/>
+      <c r="B94" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="C94" s="56" t="s">
+        <v>128</v>
+      </c>
+      <c r="D94" s="57"/>
+      <c r="E94" s="4">
+        <v>45945</v>
+      </c>
+      <c r="F94" s="56"/>
+      <c r="G94" s="56"/>
+      <c r="H94" s="56" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8">
+      <c r="A95" s="56"/>
+      <c r="B95" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="C95" s="56" t="s">
+        <v>129</v>
+      </c>
+      <c r="D95" s="57"/>
+      <c r="E95" s="4">
+        <v>45945</v>
+      </c>
+      <c r="F95" s="56"/>
+      <c r="G95" s="56"/>
+      <c r="H95" s="56" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8">
+      <c r="A96" s="56"/>
+      <c r="B96" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="C96" s="56" t="s">
+        <v>130</v>
+      </c>
+      <c r="D96" s="57"/>
+      <c r="E96" s="4">
+        <v>45945</v>
+      </c>
+      <c r="F96" s="56"/>
+      <c r="G96" s="56"/>
+      <c r="H96" s="56" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -7890,14 +7938,14 @@
       <c r="A1" s="28"/>
       <c r="B1" s="29"/>
       <c r="C1" s="30" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D1" s="31"/>
       <c r="E1" s="30"/>
       <c r="F1" s="31"/>
       <c r="G1" s="32"/>
       <c r="H1" s="44" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="I1" s="32"/>
       <c r="J1" s="29"/>
@@ -7910,19 +7958,19 @@
         <v>44</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D2" s="36"/>
       <c r="E2" s="37" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="F2" s="38"/>
       <c r="G2" s="35" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="37" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="J2" s="38"/>
     </row>
@@ -8091,7 +8139,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="45" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="C8" s="45">
         <v>166</v>
@@ -8123,7 +8171,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="45" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="C9" s="45">
         <v>80</v>
@@ -8245,10 +8293,10 @@
         <v>44</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="6" customFormat="1">
@@ -8272,7 +8320,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="C3" s="48">
         <v>14.6</v>
@@ -8286,7 +8334,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -8294,7 +8342,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -8302,7 +8350,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -8310,7 +8358,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -8318,7 +8366,7 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C8" s="48">
         <v>16.5</v>
@@ -8332,7 +8380,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -8340,7 +8388,7 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -8348,7 +8396,7 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -8356,7 +8404,7 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -8364,7 +8412,7 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C13" s="48">
         <v>42.8</v>
@@ -8378,7 +8426,7 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="C14" s="48">
         <v>69.3</v>
@@ -8392,7 +8440,7 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C15" s="48">
         <v>68.599999999999994</v>
@@ -8406,7 +8454,7 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="C16" s="48">
         <v>88.7</v>
@@ -8457,25 +8505,25 @@
         <v>44</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -8483,7 +8531,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C2" t="s">
         <v>34</v>
@@ -8513,7 +8561,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="C3" t="s">
         <v>34</v>
@@ -8543,7 +8591,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="D4">
         <v>10.16</v>
@@ -8570,7 +8618,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="D5">
         <v>9.66</v>
@@ -8597,7 +8645,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="C6" t="s">
         <v>34</v>
@@ -8627,7 +8675,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C7" t="s">
         <v>34</v>
@@ -8657,7 +8705,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="D8">
         <v>10.84</v>
@@ -8684,7 +8732,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="D9">
         <v>10.15</v>
@@ -8711,7 +8759,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="C10" t="s">
         <v>34</v>
@@ -8741,7 +8789,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C11" t="s">
         <v>34</v>
@@ -8771,7 +8819,7 @@
         <v>2</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="C12" t="s">
         <v>34</v>
@@ -8801,7 +8849,7 @@
         <v>2</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C13" t="s">
         <v>34</v>
@@ -8868,7 +8916,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD5452B6-66C2-4964-BBFB-466116F6D217}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -8887,7 +8935,7 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="B1" t="s">
         <v>30</v>
@@ -8896,22 +8944,22 @@
         <v>44</v>
       </c>
       <c r="D1" s="50" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="E1" s="50" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="F1" s="50" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="G1" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="H1" s="50" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="I1" s="50" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -8919,10 +8967,10 @@
         <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="C2" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="D2" s="50">
         <f>VALUE(MID(LEFT(Table4[[#This Row],[VENDOR NAME]], LEN(Table4[[#This Row],[VENDOR NAME]]) - 2), FIND(" ", Table4[[#This Row],[VENDOR NAME]]) + 1, LEN(Table4[[#This Row],[VENDOR NAME]])))</f>
@@ -8942,7 +8990,7 @@
         <v>1</v>
       </c>
       <c r="I2" s="50" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -8950,17 +8998,17 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="C3" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="D3" s="50">
         <f>VALUE(MID(LEFT(Table4[[#This Row],[VENDOR NAME]], LEN(Table4[[#This Row],[VENDOR NAME]]) - 2), FIND(" ", Table4[[#This Row],[VENDOR NAME]]) + 1, LEN(Table4[[#This Row],[VENDOR NAME]])))</f>
         <v>5</v>
       </c>
-      <c r="F3" s="50" t="e" cm="1">
-        <f t="array" aca="1" ref="F3" ca="1">(_xleta.PI/4)*pow(Table4[[#This Row],[WIDTH/DIAMETER OBSERVED (mm)]],2)</f>
+      <c r="F3" s="50" t="e">
+        <f>(_xleta.PI / 4) * (Table4[[#This Row],[WIDTH/DIAMETER OBSERVED (mm)]] ^ 2)</f>
         <v>#VALUE!</v>
       </c>
       <c r="G3" s="50">
@@ -8975,17 +9023,17 @@
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="C4" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="D4" s="50">
         <f>VALUE(MID(LEFT(Table4[[#This Row],[VENDOR NAME]], LEN(Table4[[#This Row],[VENDOR NAME]]) - 2), FIND(" ", Table4[[#This Row],[VENDOR NAME]]) + 1, LEN(Table4[[#This Row],[VENDOR NAME]])))</f>
         <v>0.24</v>
       </c>
-      <c r="F4" s="50" t="e" cm="1">
-        <f t="array" aca="1" ref="F4" ca="1">(_xleta.PI/4)*pow(Table4[[#This Row],[WIDTH/DIAMETER OBSERVED (mm)]],2)</f>
+      <c r="F4" s="50" t="e">
+        <f>(_xleta.PI / 4) * (Table4[[#This Row],[WIDTH/DIAMETER OBSERVED (mm)]] ^ 2)</f>
         <v>#VALUE!</v>
       </c>
       <c r="G4" s="50">
@@ -9000,17 +9048,17 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="C5" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="D5" s="50">
         <f>VALUE(MID(LEFT(Table4[[#This Row],[VENDOR NAME]], LEN(Table4[[#This Row],[VENDOR NAME]]) - 2), FIND(" ", Table4[[#This Row],[VENDOR NAME]]) + 1, LEN(Table4[[#This Row],[VENDOR NAME]])))</f>
         <v>4</v>
       </c>
-      <c r="F5" s="50" t="e" cm="1">
-        <f t="array" aca="1" ref="F5" ca="1">(_xleta.PI/4)*pow(Table4[[#This Row],[WIDTH/DIAMETER OBSERVED (mm)]],2)</f>
+      <c r="F5" s="50" t="e">
+        <f>(_xleta.PI / 4) * (Table4[[#This Row],[WIDTH/DIAMETER OBSERVED (mm)]] ^ 2)</f>
         <v>#VALUE!</v>
       </c>
       <c r="G5" s="50">
@@ -9025,17 +9073,17 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="C6" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="D6" s="50">
         <f>VALUE(MID(LEFT(Table4[[#This Row],[VENDOR NAME]], LEN(Table4[[#This Row],[VENDOR NAME]]) - 2), FIND(" ", Table4[[#This Row],[VENDOR NAME]]) + 1, LEN(Table4[[#This Row],[VENDOR NAME]])))</f>
         <v>6</v>
       </c>
-      <c r="F6" s="50" t="e" cm="1">
-        <f t="array" aca="1" ref="F6" ca="1">(_xleta.PI/4)*pow(Table4[[#This Row],[WIDTH/DIAMETER OBSERVED (mm)]],2)</f>
+      <c r="F6" s="50" t="e">
+        <f>(_xleta.PI / 4) * (Table4[[#This Row],[WIDTH/DIAMETER OBSERVED (mm)]] ^ 2)</f>
         <v>#VALUE!</v>
       </c>
       <c r="G6" s="50">
@@ -9050,17 +9098,17 @@
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="C7" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="D7" s="50">
         <f>VALUE(MID(LEFT(Table4[[#This Row],[VENDOR NAME]], LEN(Table4[[#This Row],[VENDOR NAME]]) - 2), FIND(" ", Table4[[#This Row],[VENDOR NAME]]) + 1, LEN(Table4[[#This Row],[VENDOR NAME]])))</f>
         <v>0.24</v>
       </c>
-      <c r="F7" s="50" t="e" cm="1">
-        <f t="array" aca="1" ref="F7" ca="1">(_xleta.PI/4)*pow(Table4[[#This Row],[WIDTH/DIAMETER OBSERVED (mm)]],2)</f>
+      <c r="F7" s="50" t="e">
+        <f>(_xleta.PI / 4) * (Table4[[#This Row],[WIDTH/DIAMETER OBSERVED (mm)]] ^ 2)</f>
         <v>#VALUE!</v>
       </c>
       <c r="G7" s="50">
@@ -9075,17 +9123,17 @@
         <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="C8" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="D8" s="50">
         <f>VALUE(MID(LEFT(Table4[[#This Row],[VENDOR NAME]], LEN(Table4[[#This Row],[VENDOR NAME]]) - 2), FIND(" ", Table4[[#This Row],[VENDOR NAME]]) + 1, LEN(Table4[[#This Row],[VENDOR NAME]])))</f>
         <v>4</v>
       </c>
-      <c r="F8" s="50" t="e" cm="1">
-        <f t="array" aca="1" ref="F8" ca="1">(_xleta.PI/4)*pow(Table4[[#This Row],[WIDTH/DIAMETER OBSERVED (mm)]],2)</f>
+      <c r="F8" s="50" t="e">
+        <f>(_xleta.PI / 4) * (Table4[[#This Row],[WIDTH/DIAMETER OBSERVED (mm)]] ^ 2)</f>
         <v>#VALUE!</v>
       </c>
       <c r="G8" s="50">
@@ -9101,17 +9149,17 @@
         <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="C9" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="D9" s="50">
         <f>VALUE(MID(LEFT(Table4[[#This Row],[VENDOR NAME]], LEN(Table4[[#This Row],[VENDOR NAME]]) - 2), FIND(" ", Table4[[#This Row],[VENDOR NAME]]) + 1, LEN(Table4[[#This Row],[VENDOR NAME]])))</f>
         <v>6</v>
       </c>
-      <c r="F9" s="50" t="e" cm="1">
-        <f t="array" aca="1" ref="F9" ca="1">(_xleta.PI/4)*pow(Table4[[#This Row],[WIDTH/DIAMETER OBSERVED (mm)]],2)</f>
+      <c r="F9" s="50" t="e">
+        <f>(_xleta.PI / 4) * (Table4[[#This Row],[WIDTH/DIAMETER OBSERVED (mm)]] ^ 2)</f>
         <v>#VALUE!</v>
       </c>
       <c r="G9" s="50">
@@ -9162,10 +9210,10 @@
         <v>44</v>
       </c>
       <c r="C1" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="D1" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -9201,7 +9249,7 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="C5" s="10">
         <v>0.84722222222222221</v>
@@ -9243,7 +9291,7 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="C8" s="10">
         <v>9.375E-2</v>
@@ -9257,7 +9305,7 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="C9" s="10">
         <v>9.0277777777777776E-2</v>

</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-10-17 09:42:27
</commit_message>
<xml_diff>
--- a/data/Solar_Lab_Tests.xlsx
+++ b/data/Solar_Lab_Tests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29415"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vikramsolar0-my.sharepoint.com/personal/naveen_chamaria_vikramsolar_com/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2024" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F46BCE05-8FE3-4715-84E5-C7799AEB9F67}"/>
+  <xr:revisionPtr revIDLastSave="2026" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F0CCFC2-6628-4E20-9B43-61BDA4FBECB7}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="7" activeTab="11" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="11" activeTab="11" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Tests Map" sheetId="4" state="hidden" r:id="rId1"/>
@@ -1285,7 +1285,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1370,7 +1370,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -7814,56 +7813,47 @@
       </c>
     </row>
     <row r="94" spans="1:8">
-      <c r="A94" s="56"/>
-      <c r="B94" s="56" t="s">
+      <c r="B94" t="s">
         <v>18</v>
       </c>
-      <c r="C94" s="56" t="s">
+      <c r="C94" t="s">
         <v>128</v>
       </c>
-      <c r="D94" s="57"/>
+      <c r="D94" s="56"/>
       <c r="E94" s="4">
         <v>45945</v>
       </c>
-      <c r="F94" s="56"/>
-      <c r="G94" s="56"/>
-      <c r="H94" s="56" t="s">
+      <c r="H94" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="95" spans="1:8">
-      <c r="A95" s="56"/>
-      <c r="B95" s="56" t="s">
+      <c r="B95" t="s">
         <v>18</v>
       </c>
-      <c r="C95" s="56" t="s">
+      <c r="C95" t="s">
         <v>129</v>
       </c>
-      <c r="D95" s="57"/>
+      <c r="D95" s="56"/>
       <c r="E95" s="4">
         <v>45945</v>
       </c>
-      <c r="F95" s="56"/>
-      <c r="G95" s="56"/>
-      <c r="H95" s="56" t="s">
+      <c r="H95" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="96" spans="1:8">
-      <c r="A96" s="56"/>
-      <c r="B96" s="56" t="s">
+      <c r="B96" t="s">
         <v>18</v>
       </c>
-      <c r="C96" s="56" t="s">
+      <c r="C96" t="s">
         <v>130</v>
       </c>
-      <c r="D96" s="57"/>
+      <c r="D96" s="56"/>
       <c r="E96" s="4">
         <v>45945</v>
       </c>
-      <c r="F96" s="56"/>
-      <c r="G96" s="56"/>
-      <c r="H96" s="56" t="s">
+      <c r="H96" t="s">
         <v>36</v>
       </c>
     </row>
@@ -8917,7 +8907,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -9062,7 +9052,8 @@
         <v>#VALUE!</v>
       </c>
       <c r="G5" s="50">
-        <v>13.79</v>
+        <f>13.79/1000</f>
+        <v>1.3789999999999998E-2</v>
       </c>
       <c r="H5" s="50">
         <v>1</v>
@@ -9087,7 +9078,8 @@
         <v>#VALUE!</v>
       </c>
       <c r="G6" s="50">
-        <v>9.24</v>
+        <f>9.24/1000</f>
+        <v>9.2399999999999999E-3</v>
       </c>
       <c r="H6" s="50">
         <v>1</v>

</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-10-21 09:43:54
</commit_message>
<xml_diff>
--- a/data/Solar_Lab_Tests.xlsx
+++ b/data/Solar_Lab_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vikramsolar0-my.sharepoint.com/personal/naveen_chamaria_vikramsolar_com/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2026" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F0CCFC2-6628-4E20-9B43-61BDA4FBECB7}"/>
+  <xr:revisionPtr revIDLastSave="2145" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{09D0C72E-741E-496C-A837-2B3A073A2A5D}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="11" activeTab="11" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
   </bookViews>
@@ -32,7 +32,7 @@
     <definedName name="ENCAPTYPE">Ref!$K$2:$K$1048576</definedName>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">'Material Tests Map'!$A$1:$B$20</definedName>
     <definedName name="ExternalData_1" localSheetId="13" hidden="1">'Standard test times'!$A$1:$B$15</definedName>
-    <definedName name="ExternalData_1" localSheetId="3" hidden="1">'Test Data'!$A$1:$H$96</definedName>
+    <definedName name="ExternalData_1" localSheetId="3" hidden="1">'Test Data'!$A$1:$H$98</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="281">
   <si>
     <t>BOM</t>
   </si>
@@ -467,6 +467,12 @@
     <t>RFID SAMPLE 2</t>
   </si>
   <si>
+    <t>SOLARLOK</t>
+  </si>
+  <si>
+    <t>DZ2000V</t>
+  </si>
+  <si>
     <t xml:space="preserve">                                                                                                                           PRE PCT</t>
   </si>
   <si>
@@ -707,6 +713,9 @@
     <t>249 µA</t>
   </si>
   <si>
+    <t>254MV</t>
+  </si>
+  <si>
     <t>UKTR30A</t>
   </si>
   <si>
@@ -737,6 +746,9 @@
     <t>325µA</t>
   </si>
   <si>
+    <t>248MV</t>
+  </si>
+  <si>
     <t>155µA</t>
   </si>
   <si>
@@ -770,6 +782,9 @@
     <t>357µA</t>
   </si>
   <si>
+    <t>246MV</t>
+  </si>
+  <si>
     <t>VEMOULD20A</t>
   </si>
   <si>
@@ -785,6 +800,9 @@
     <t>314µA</t>
   </si>
   <si>
+    <t>251MV</t>
+  </si>
+  <si>
     <t>288mV</t>
   </si>
   <si>
@@ -803,15 +821,6 @@
     <t>261MV</t>
   </si>
   <si>
-    <t>349VBD/265VBY</t>
-  </si>
-  <si>
-    <t>256IBY/322IBD</t>
-  </si>
-  <si>
-    <t>341VBD/269VBY</t>
-  </si>
-  <si>
     <t>UKTR BD 7500L</t>
   </si>
   <si>
@@ -834,6 +843,9 @@
   </si>
   <si>
     <t>IBY2.0/IBD1.2</t>
+  </si>
+  <si>
+    <t>257MV</t>
   </si>
   <si>
     <t>Avg. VBD (Pre PCT)</t>
@@ -1285,7 +1297,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1373,6 +1385,8 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2245,8 +2259,8 @@
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{5C370BE7-C0F8-462F-9F89-5FC458087319}" name="Table16" displayName="Table16" ref="A1:I22" totalsRowShown="0">
-  <autoFilter ref="A1:I22" xr:uid="{5C370BE7-C0F8-462F-9F89-5FC458087319}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{5C370BE7-C0F8-462F-9F89-5FC458087319}" name="Table16" displayName="Table16" ref="A1:I25" totalsRowShown="0">
+  <autoFilter ref="A1:I25" xr:uid="{5C370BE7-C0F8-462F-9F89-5FC458087319}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{59EA2429-768A-457D-88E6-B34A083DE755}" name="BOM"/>
     <tableColumn id="2" xr3:uid="{C09F236B-325A-4EF9-B484-B1D592C83B7F}" name="VENDOR NAME"/>
@@ -2360,7 +2374,7 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{06A3AD80-C098-4015-85FF-3495CE4443EA}" name="Test_Data" displayName="Test_Data" ref="A1:H96" tableType="queryTable" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{06A3AD80-C098-4015-85FF-3495CE4443EA}" name="Test_Data" displayName="Test_Data" ref="A1:H98" tableType="queryTable" totalsRowShown="0">
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{87F75B08-44C4-4718-834D-87FEE9F87970}" uniqueName="1" name="BOM" queryTableFieldId="1" dataDxfId="56"/>
     <tableColumn id="2" xr3:uid="{1E5F4521-5E5C-4948-AEB2-FC5F712DB353}" uniqueName="2" name="TEST NAME" queryTableFieldId="2" dataDxfId="55"/>
@@ -2914,10 +2928,10 @@
         <v>44</v>
       </c>
       <c r="C1" s="49" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="D1" s="49" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -2951,10 +2965,10 @@
         <v>44</v>
       </c>
       <c r="C1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="D1" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -2976,10 +2990,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{333C0630-51CF-46CA-8CAD-98FEF9AC181F}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -3003,25 +3017,25 @@
         <v>44</v>
       </c>
       <c r="C1" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="D1" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="E1" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="F1" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="G1" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="H1" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="I1" s="51" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -3029,13 +3043,13 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="D2" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="E2" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -3043,7 +3057,7 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -3051,13 +3065,13 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="D4">
         <v>302</v>
       </c>
       <c r="E4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -3071,7 +3085,13 @@
         <v>260</v>
       </c>
       <c r="E5" t="s">
-        <v>210</v>
+        <v>212</v>
+      </c>
+      <c r="F5" t="s">
+        <v>213</v>
+      </c>
+      <c r="G5">
+        <v>470</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -3079,13 +3099,13 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="D6" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="E6" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -3096,10 +3116,10 @@
         <v>81</v>
       </c>
       <c r="D7" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="E7" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -3110,13 +3130,13 @@
         <v>101</v>
       </c>
       <c r="D8" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="E8" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="F8" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="G8">
         <v>217</v>
@@ -3130,10 +3150,16 @@
         <v>93</v>
       </c>
       <c r="D9" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="E9" t="s">
-        <v>220</v>
+        <v>223</v>
+      </c>
+      <c r="F9" t="s">
+        <v>224</v>
+      </c>
+      <c r="G9">
+        <v>446</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -3144,13 +3170,13 @@
         <v>92</v>
       </c>
       <c r="D10" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="E10" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="F10" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="G10">
         <v>202</v>
@@ -3161,16 +3187,16 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="D11" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="E11" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="F11" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="G11">
         <v>185</v>
@@ -3184,10 +3210,16 @@
         <v>79</v>
       </c>
       <c r="D12" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="E12" t="s">
-        <v>228</v>
+        <v>232</v>
+      </c>
+      <c r="F12" t="s">
+        <v>213</v>
+      </c>
+      <c r="G12">
+        <v>457</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -3195,7 +3227,7 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -3206,10 +3238,16 @@
         <v>89</v>
       </c>
       <c r="D14" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="E14" t="s">
-        <v>231</v>
+        <v>235</v>
+      </c>
+      <c r="F14" t="s">
+        <v>236</v>
+      </c>
+      <c r="G14">
+        <v>437</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -3217,13 +3255,13 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="D15" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="E15" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -3234,10 +3272,16 @@
         <v>85</v>
       </c>
       <c r="D16" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="E16" t="s">
-        <v>236</v>
+        <v>241</v>
+      </c>
+      <c r="F16" t="s">
+        <v>242</v>
+      </c>
+      <c r="G16">
+        <v>357</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -3248,13 +3292,13 @@
         <v>84</v>
       </c>
       <c r="D17" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="E17" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="F17" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="G17">
         <v>134</v>
@@ -3268,13 +3312,13 @@
         <v>82</v>
       </c>
       <c r="D18" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="E18" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="F18" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="G18">
         <v>297</v>
@@ -3284,28 +3328,19 @@
       <c r="A19" t="s">
         <v>15</v>
       </c>
-      <c r="D19" t="s">
-        <v>243</v>
-      </c>
-      <c r="E19" t="s">
-        <v>244</v>
-      </c>
-      <c r="F19" t="s">
-        <v>245</v>
-      </c>
-      <c r="G19" t="s">
-        <v>244</v>
+      <c r="B19" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="20" spans="1:7" hidden="1">
       <c r="B20" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="F20" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="G20" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15" hidden="1">
@@ -3316,10 +3351,10 @@
         <v>116</v>
       </c>
       <c r="D21" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="E21" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
     </row>
     <row r="22" spans="1:7" hidden="1">
@@ -3327,13 +3362,40 @@
         <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="F22" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="G22" t="s">
-        <v>253</v>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" t="s">
+        <v>132</v>
+      </c>
+      <c r="F23" t="s">
+        <v>257</v>
+      </c>
+      <c r="G23">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -3382,37 +3444,37 @@
         <v>44</v>
       </c>
       <c r="C1" s="53" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="D1" s="53" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="E1" s="53" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="F1" s="53" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="G1" s="53" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="H1" s="53" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="I1" s="53" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="J1" s="53" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="K1" s="53" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="L1" s="53" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="M1" s="54" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:13" hidden="1">
@@ -3435,31 +3497,31 @@
         <v>15</v>
       </c>
       <c r="B3" s="55" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="D3" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="E3" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="F3" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="G3" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="H3" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="I3" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="J3" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="K3" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -3470,16 +3532,16 @@
         <v>116</v>
       </c>
       <c r="H4" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="I4">
         <v>264</v>
       </c>
       <c r="J4" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="K4" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -3487,19 +3549,19 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="H5" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="I5">
         <v>28</v>
       </c>
       <c r="J5" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="K5" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
     </row>
   </sheetData>
@@ -3535,7 +3597,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -5840,10 +5902,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9401EE47-EA52-49C7-BBC0-21F5B88254FB}">
-  <dimension ref="A1:K96"/>
+  <dimension ref="A1:K98"/>
   <sheetViews>
-    <sheetView topLeftCell="B84" workbookViewId="0">
-      <selection activeCell="H96" sqref="H96"/>
+    <sheetView topLeftCell="B95" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -5960,7 +6022,7 @@
         <v>35</v>
       </c>
       <c r="H4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -6498,7 +6560,7 @@
         <v>45875</v>
       </c>
       <c r="H28" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -6519,7 +6581,7 @@
         <v>45875</v>
       </c>
       <c r="H29" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -6540,7 +6602,7 @@
         <v>45861</v>
       </c>
       <c r="H30" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -6561,7 +6623,7 @@
         <v>45866</v>
       </c>
       <c r="H31" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -6582,7 +6644,7 @@
         <v>45866</v>
       </c>
       <c r="H32" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -6603,7 +6665,7 @@
         <v>45866</v>
       </c>
       <c r="H33" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -6624,7 +6686,7 @@
         <v>45866</v>
       </c>
       <c r="H34" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -6645,7 +6707,7 @@
         <v>45866</v>
       </c>
       <c r="H35" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -6666,7 +6728,7 @@
         <v>45880</v>
       </c>
       <c r="H36" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -6683,8 +6745,11 @@
       <c r="E37" s="4">
         <v>45870</v>
       </c>
+      <c r="F37" s="4">
+        <v>45936</v>
+      </c>
       <c r="H37" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -6705,7 +6770,7 @@
         <v>45875</v>
       </c>
       <c r="H38" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -6744,7 +6809,7 @@
         <v>45876</v>
       </c>
       <c r="H40" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -6765,7 +6830,7 @@
         <v>45878</v>
       </c>
       <c r="H41" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -6804,7 +6869,7 @@
         <v>45878</v>
       </c>
       <c r="H43" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -6825,7 +6890,7 @@
         <v>45875</v>
       </c>
       <c r="H44" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -6846,7 +6911,7 @@
         <v>45892</v>
       </c>
       <c r="H45" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -6867,7 +6932,7 @@
         <v>45878</v>
       </c>
       <c r="H46" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -6888,7 +6953,7 @@
         <v>45876</v>
       </c>
       <c r="H47" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -6909,7 +6974,7 @@
         <v>45878</v>
       </c>
       <c r="H48" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -6930,7 +6995,7 @@
         <v>45876</v>
       </c>
       <c r="H49" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -6951,7 +7016,7 @@
         <v>45876</v>
       </c>
       <c r="H50" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -6972,7 +7037,7 @@
         <v>45875</v>
       </c>
       <c r="H51" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -6993,7 +7058,7 @@
         <v>45876</v>
       </c>
       <c r="H52" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -7014,7 +7079,7 @@
         <v>45875</v>
       </c>
       <c r="H53" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="54" spans="1:8">
@@ -7035,7 +7100,7 @@
         <v>45875</v>
       </c>
       <c r="H54" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -7056,7 +7121,7 @@
         <v>45875</v>
       </c>
       <c r="H55" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -7077,7 +7142,7 @@
         <v>45885</v>
       </c>
       <c r="H56" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -7098,7 +7163,7 @@
         <v>45885</v>
       </c>
       <c r="H57" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -7119,7 +7184,7 @@
         <v>45885</v>
       </c>
       <c r="H58" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -7140,7 +7205,7 @@
         <v>45892</v>
       </c>
       <c r="H59" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -7161,7 +7226,7 @@
         <v>45892</v>
       </c>
       <c r="H60" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -7178,8 +7243,11 @@
       <c r="E61" s="4">
         <v>45891</v>
       </c>
+      <c r="F61" s="4">
+        <v>45897</v>
+      </c>
       <c r="H61" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -7196,11 +7264,14 @@
       <c r="E62" s="4">
         <v>45891</v>
       </c>
+      <c r="F62" s="4">
+        <v>45897</v>
+      </c>
       <c r="H62" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="15">
       <c r="A63" t="s">
         <v>15</v>
       </c>
@@ -7214,8 +7285,11 @@
       <c r="E63" s="4">
         <v>45891</v>
       </c>
+      <c r="F63" s="57">
+        <v>45897</v>
+      </c>
       <c r="H63" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="64" spans="1:8">
@@ -7232,8 +7306,11 @@
       <c r="E64" s="4">
         <v>45891</v>
       </c>
+      <c r="F64" s="4">
+        <v>45897</v>
+      </c>
       <c r="H64" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="65" spans="1:8">
@@ -7250,8 +7327,11 @@
       <c r="E65" s="4">
         <v>45891</v>
       </c>
+      <c r="F65" s="4">
+        <v>45897</v>
+      </c>
       <c r="H65" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="66" spans="1:8">
@@ -7268,8 +7348,11 @@
       <c r="E66" s="4">
         <v>45891</v>
       </c>
+      <c r="F66" s="4">
+        <v>45897</v>
+      </c>
       <c r="H66" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="67" spans="1:8">
@@ -7286,8 +7369,11 @@
       <c r="E67" s="4">
         <v>45891</v>
       </c>
+      <c r="F67" s="4">
+        <v>45897</v>
+      </c>
       <c r="H67" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="68" spans="1:8">
@@ -7304,8 +7390,11 @@
       <c r="E68" s="4">
         <v>45897</v>
       </c>
+      <c r="F68" s="4">
+        <v>45899</v>
+      </c>
       <c r="H68" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="69" spans="1:8">
@@ -7322,8 +7411,11 @@
       <c r="E69" s="4">
         <v>45897</v>
       </c>
+      <c r="F69" s="4">
+        <v>45899</v>
+      </c>
       <c r="H69" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="70" spans="1:8">
@@ -7344,7 +7436,7 @@
         <v>45908</v>
       </c>
       <c r="H70" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="71" spans="1:8">
@@ -7361,8 +7453,11 @@
       <c r="E71" s="4">
         <v>45906</v>
       </c>
+      <c r="F71" s="4">
+        <v>45908</v>
+      </c>
       <c r="H71" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="72" spans="1:8">
@@ -7383,7 +7478,7 @@
         <v>45910</v>
       </c>
       <c r="H72" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="73" spans="1:8">
@@ -7404,7 +7499,7 @@
         <v>45910</v>
       </c>
       <c r="H73" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="74" spans="1:8">
@@ -7425,7 +7520,7 @@
         <v>45910</v>
       </c>
       <c r="H74" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="75" spans="1:8">
@@ -7442,8 +7537,11 @@
       <c r="E75" s="4">
         <v>45916</v>
       </c>
+      <c r="F75" s="4">
+        <v>45926</v>
+      </c>
       <c r="H75" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="76" spans="1:8">
@@ -7460,8 +7558,11 @@
       <c r="E76" s="4">
         <v>45916</v>
       </c>
+      <c r="F76" s="4">
+        <v>45926</v>
+      </c>
       <c r="H76" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="77" spans="1:8">
@@ -7478,8 +7579,11 @@
       <c r="E77" s="4">
         <v>45916</v>
       </c>
+      <c r="F77" s="4">
+        <v>45926</v>
+      </c>
       <c r="H77" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="78" spans="1:8">
@@ -7496,8 +7600,11 @@
       <c r="E78" s="4">
         <v>45916</v>
       </c>
+      <c r="F78" s="4">
+        <v>45926</v>
+      </c>
       <c r="H78" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="79" spans="1:8">
@@ -7514,8 +7621,11 @@
       <c r="E79" s="4">
         <v>45916</v>
       </c>
+      <c r="F79" s="4">
+        <v>45926</v>
+      </c>
       <c r="H79" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="80" spans="1:8">
@@ -7536,7 +7646,7 @@
         <v>45926</v>
       </c>
       <c r="H80" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="81" spans="1:8">
@@ -7557,7 +7667,7 @@
         <v>45926</v>
       </c>
       <c r="H81" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="82" spans="1:8">
@@ -7578,7 +7688,7 @@
         <v>45926</v>
       </c>
       <c r="H82" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="83" spans="1:8">
@@ -7599,7 +7709,7 @@
         <v>45926</v>
       </c>
       <c r="H83" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="84" spans="1:8">
@@ -7620,7 +7730,7 @@
         <v>45926</v>
       </c>
       <c r="H84" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="85" spans="1:8">
@@ -7641,7 +7751,7 @@
         <v>45926</v>
       </c>
       <c r="H85" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="86" spans="1:8">
@@ -7662,7 +7772,7 @@
         <v>45926</v>
       </c>
       <c r="H86" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="87" spans="1:8">
@@ -7683,7 +7793,7 @@
         <v>45926</v>
       </c>
       <c r="H87" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="88" spans="1:8">
@@ -7704,7 +7814,7 @@
         <v>45926</v>
       </c>
       <c r="H88" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="89" spans="1:8">
@@ -7823,8 +7933,11 @@
       <c r="E94" s="4">
         <v>45945</v>
       </c>
+      <c r="F94" s="4">
+        <v>45947</v>
+      </c>
       <c r="H94" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="95" spans="1:8">
@@ -7838,8 +7951,11 @@
       <c r="E95" s="4">
         <v>45945</v>
       </c>
+      <c r="F95" s="4">
+        <v>45947</v>
+      </c>
       <c r="H95" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="96" spans="1:8">
@@ -7853,7 +7969,46 @@
       <c r="E96" s="4">
         <v>45945</v>
       </c>
+      <c r="F96" s="4">
+        <v>45947</v>
+      </c>
       <c r="H96" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8">
+      <c r="A97" s="58"/>
+      <c r="B97" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="C97" s="58" t="s">
+        <v>131</v>
+      </c>
+      <c r="D97" s="56"/>
+      <c r="E97" s="4">
+        <v>45951</v>
+      </c>
+      <c r="F97" s="58"/>
+      <c r="G97" s="58"/>
+      <c r="H97" s="58" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8">
+      <c r="A98" s="58"/>
+      <c r="B98" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="C98" s="58" t="s">
+        <v>132</v>
+      </c>
+      <c r="D98" s="56"/>
+      <c r="E98" s="4">
+        <v>45951</v>
+      </c>
+      <c r="F98" s="58"/>
+      <c r="G98" s="58"/>
+      <c r="H98" s="58" t="s">
         <v>36</v>
       </c>
     </row>
@@ -7928,14 +8083,14 @@
       <c r="A1" s="28"/>
       <c r="B1" s="29"/>
       <c r="C1" s="30" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D1" s="31"/>
       <c r="E1" s="30"/>
       <c r="F1" s="31"/>
       <c r="G1" s="32"/>
       <c r="H1" s="44" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="I1" s="32"/>
       <c r="J1" s="29"/>
@@ -7948,19 +8103,19 @@
         <v>44</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D2" s="36"/>
       <c r="E2" s="37" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F2" s="38"/>
       <c r="G2" s="35" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="37" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="J2" s="38"/>
     </row>
@@ -8129,7 +8284,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="45" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C8" s="45">
         <v>166</v>
@@ -8161,7 +8316,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="45" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C9" s="45">
         <v>80</v>
@@ -8283,10 +8438,10 @@
         <v>44</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="6" customFormat="1">
@@ -8310,7 +8465,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C3" s="48">
         <v>14.6</v>
@@ -8324,7 +8479,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -8332,7 +8487,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -8340,7 +8495,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -8348,7 +8503,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -8356,7 +8511,7 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C8" s="48">
         <v>16.5</v>
@@ -8370,7 +8525,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -8378,7 +8533,7 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -8386,7 +8541,7 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -8394,7 +8549,7 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -8402,7 +8557,7 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C13" s="48">
         <v>42.8</v>
@@ -8416,7 +8571,7 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C14" s="48">
         <v>69.3</v>
@@ -8430,7 +8585,7 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C15" s="48">
         <v>68.599999999999994</v>
@@ -8444,7 +8599,7 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C16" s="48">
         <v>88.7</v>
@@ -8495,25 +8650,25 @@
         <v>44</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -8521,7 +8676,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C2" t="s">
         <v>34</v>
@@ -8551,7 +8706,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C3" t="s">
         <v>34</v>
@@ -8581,7 +8736,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D4">
         <v>10.16</v>
@@ -8608,7 +8763,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D5">
         <v>9.66</v>
@@ -8635,7 +8790,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C6" t="s">
         <v>34</v>
@@ -8665,7 +8820,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C7" t="s">
         <v>34</v>
@@ -8695,7 +8850,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D8">
         <v>10.84</v>
@@ -8722,7 +8877,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D9">
         <v>10.15</v>
@@ -8749,7 +8904,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C10" t="s">
         <v>34</v>
@@ -8779,7 +8934,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C11" t="s">
         <v>34</v>
@@ -8809,7 +8964,7 @@
         <v>2</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C12" t="s">
         <v>34</v>
@@ -8839,7 +8994,7 @@
         <v>2</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C13" t="s">
         <v>34</v>
@@ -8925,7 +9080,7 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B1" t="s">
         <v>30</v>
@@ -8934,22 +9089,22 @@
         <v>44</v>
       </c>
       <c r="D1" s="50" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E1" s="50" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="F1" s="50" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G1" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="H1" s="50" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="I1" s="50" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -8957,10 +9112,10 @@
         <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C2" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D2" s="50">
         <f>VALUE(MID(LEFT(Table4[[#This Row],[VENDOR NAME]], LEN(Table4[[#This Row],[VENDOR NAME]]) - 2), FIND(" ", Table4[[#This Row],[VENDOR NAME]]) + 1, LEN(Table4[[#This Row],[VENDOR NAME]])))</f>
@@ -8980,7 +9135,7 @@
         <v>1</v>
       </c>
       <c r="I2" s="50" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -8988,10 +9143,10 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C3" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="D3" s="50">
         <f>VALUE(MID(LEFT(Table4[[#This Row],[VENDOR NAME]], LEN(Table4[[#This Row],[VENDOR NAME]]) - 2), FIND(" ", Table4[[#This Row],[VENDOR NAME]]) + 1, LEN(Table4[[#This Row],[VENDOR NAME]])))</f>
@@ -9013,10 +9168,10 @@
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C4" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D4" s="50">
         <f>VALUE(MID(LEFT(Table4[[#This Row],[VENDOR NAME]], LEN(Table4[[#This Row],[VENDOR NAME]]) - 2), FIND(" ", Table4[[#This Row],[VENDOR NAME]]) + 1, LEN(Table4[[#This Row],[VENDOR NAME]])))</f>
@@ -9038,10 +9193,10 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C5" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="D5" s="50">
         <f>VALUE(MID(LEFT(Table4[[#This Row],[VENDOR NAME]], LEN(Table4[[#This Row],[VENDOR NAME]]) - 2), FIND(" ", Table4[[#This Row],[VENDOR NAME]]) + 1, LEN(Table4[[#This Row],[VENDOR NAME]])))</f>
@@ -9064,10 +9219,10 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C6" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="D6" s="50">
         <f>VALUE(MID(LEFT(Table4[[#This Row],[VENDOR NAME]], LEN(Table4[[#This Row],[VENDOR NAME]]) - 2), FIND(" ", Table4[[#This Row],[VENDOR NAME]]) + 1, LEN(Table4[[#This Row],[VENDOR NAME]])))</f>
@@ -9090,10 +9245,10 @@
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C7" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D7" s="50">
         <f>VALUE(MID(LEFT(Table4[[#This Row],[VENDOR NAME]], LEN(Table4[[#This Row],[VENDOR NAME]]) - 2), FIND(" ", Table4[[#This Row],[VENDOR NAME]]) + 1, LEN(Table4[[#This Row],[VENDOR NAME]])))</f>
@@ -9115,10 +9270,10 @@
         <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C8" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="D8" s="50">
         <f>VALUE(MID(LEFT(Table4[[#This Row],[VENDOR NAME]], LEN(Table4[[#This Row],[VENDOR NAME]]) - 2), FIND(" ", Table4[[#This Row],[VENDOR NAME]]) + 1, LEN(Table4[[#This Row],[VENDOR NAME]])))</f>
@@ -9141,10 +9296,10 @@
         <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C9" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="D9" s="50">
         <f>VALUE(MID(LEFT(Table4[[#This Row],[VENDOR NAME]], LEN(Table4[[#This Row],[VENDOR NAME]]) - 2), FIND(" ", Table4[[#This Row],[VENDOR NAME]]) + 1, LEN(Table4[[#This Row],[VENDOR NAME]])))</f>
@@ -9202,10 +9357,10 @@
         <v>44</v>
       </c>
       <c r="C1" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="D1" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -9241,7 +9396,7 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C5" s="10">
         <v>0.84722222222222221</v>
@@ -9283,7 +9438,7 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C8" s="10">
         <v>9.375E-2</v>
@@ -9297,7 +9452,7 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C9" s="10">
         <v>9.0277777777777776E-2</v>

</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-10-24 09:42:41
</commit_message>
<xml_diff>
--- a/data/Solar_Lab_Tests.xlsx
+++ b/data/Solar_Lab_Tests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29415"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vikramsolar0-my.sharepoint.com/personal/naveen_chamaria_vikramsolar_com/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2145" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{09D0C72E-741E-496C-A837-2B3A073A2A5D}"/>
+  <xr:revisionPtr revIDLastSave="2207" documentId="13_ncr:1_{FA10C959-8CED-4789-9566-99862FBF39BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{55AE783E-6EBA-4856-9754-12C6A2B19110}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="11" activeTab="11" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="11" activeTab="3" xr2:uid="{B3214F99-ED3C-4E77-AA9D-96AFA19CF590}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Tests Map" sheetId="4" state="hidden" r:id="rId1"/>
@@ -32,7 +32,7 @@
     <definedName name="ENCAPTYPE">Ref!$K$2:$K$1048576</definedName>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">'Material Tests Map'!$A$1:$B$20</definedName>
     <definedName name="ExternalData_1" localSheetId="13" hidden="1">'Standard test times'!$A$1:$B$15</definedName>
-    <definedName name="ExternalData_1" localSheetId="3" hidden="1">'Test Data'!$A$1:$H$98</definedName>
+    <definedName name="ExternalData_1" localSheetId="3" hidden="1">'Test Data'!$A$1:$H$101</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="284">
   <si>
     <t>BOM</t>
   </si>
@@ -272,6 +272,9 @@
     <t>p first</t>
   </si>
   <si>
+    <t>UV CONVERSION</t>
+  </si>
+  <si>
     <t>GRN GENERATION TIME</t>
   </si>
   <si>
@@ -588,6 +591,12 @@
   </si>
   <si>
     <t>ENERLITE EVA</t>
+  </si>
+  <si>
+    <t>UV CONVERSION FRONT EPE 55mm</t>
+  </si>
+  <si>
+    <t>UV CONVERSION BACK EPE 60mm</t>
   </si>
   <si>
     <t xml:space="preserve">BOM </t>
@@ -2374,7 +2383,7 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{06A3AD80-C098-4015-85FF-3495CE4443EA}" name="Test_Data" displayName="Test_Data" ref="A1:H98" tableType="queryTable" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{06A3AD80-C098-4015-85FF-3495CE4443EA}" name="Test_Data" displayName="Test_Data" ref="A1:H101" tableType="queryTable" totalsRowShown="0">
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{87F75B08-44C4-4718-834D-87FEE9F87970}" uniqueName="1" name="BOM" queryTableFieldId="1" dataDxfId="56"/>
     <tableColumn id="2" xr3:uid="{1E5F4521-5E5C-4948-AEB2-FC5F712DB353}" uniqueName="2" name="TEST NAME" queryTableFieldId="2" dataDxfId="55"/>
@@ -2928,10 +2937,10 @@
         <v>44</v>
       </c>
       <c r="C1" s="49" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="D1" s="49" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -2965,10 +2974,10 @@
         <v>44</v>
       </c>
       <c r="C1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="D1" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -2992,7 +3001,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{333C0630-51CF-46CA-8CAD-98FEF9AC181F}">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
@@ -3017,25 +3026,25 @@
         <v>44</v>
       </c>
       <c r="C1" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="D1" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="E1" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="F1" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="G1" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="H1" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="I1" s="51" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -3043,13 +3052,13 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D2" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="E2" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -3057,7 +3066,7 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -3065,13 +3074,13 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="D4">
         <v>302</v>
       </c>
       <c r="E4" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -3079,16 +3088,16 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D5">
         <v>260</v>
       </c>
       <c r="E5" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="F5" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="G5">
         <v>470</v>
@@ -3099,13 +3108,13 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="D6" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="E6" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -3113,13 +3122,13 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D7" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="E7" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -3127,16 +3136,16 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D8" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="E8" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="F8" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="G8">
         <v>217</v>
@@ -3147,16 +3156,16 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D9" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="E9" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="F9" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="G9">
         <v>446</v>
@@ -3167,16 +3176,16 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D10" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="E10" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="F10" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="G10">
         <v>202</v>
@@ -3187,16 +3196,16 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="D11" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="E11" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="F11" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="G11">
         <v>185</v>
@@ -3207,16 +3216,16 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D12" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="E12" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="F12" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="G12">
         <v>457</v>
@@ -3227,7 +3236,7 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -3235,16 +3244,16 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D14" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="E14" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="F14" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="G14">
         <v>437</v>
@@ -3255,13 +3264,13 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="D15" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="E15" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -3269,16 +3278,16 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D16" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="E16" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="F16" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="G16">
         <v>357</v>
@@ -3289,16 +3298,16 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D17" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="E17" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="F17" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="G17">
         <v>134</v>
@@ -3309,16 +3318,16 @@
         <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D18" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="E18" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="F18" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="G18">
         <v>297</v>
@@ -3329,18 +3338,18 @@
         <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="20" spans="1:7" hidden="1">
       <c r="B20" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="F20" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="G20" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15" hidden="1">
@@ -3348,13 +3357,13 @@
         <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D21" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="E21" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
     </row>
     <row r="22" spans="1:7" hidden="1">
@@ -3362,13 +3371,13 @@
         <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="F22" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="G22" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -3376,10 +3385,10 @@
         <v>15</v>
       </c>
       <c r="B23" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F23" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="G23">
         <v>425</v>
@@ -3390,7 +3399,7 @@
         <v>15</v>
       </c>
       <c r="B24" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -3444,37 +3453,37 @@
         <v>44</v>
       </c>
       <c r="C1" s="53" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="D1" s="53" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="E1" s="53" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="F1" s="53" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="G1" s="53" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="H1" s="53" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="I1" s="53" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="J1" s="53" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="K1" s="53" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="L1" s="53" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="M1" s="54" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:13" hidden="1">
@@ -3497,31 +3506,31 @@
         <v>15</v>
       </c>
       <c r="B3" s="55" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="D3" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="E3" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="F3" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="G3" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="H3" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="I3" t="s">
+        <v>275</v>
+      </c>
+      <c r="J3" t="s">
         <v>272</v>
       </c>
-      <c r="J3" t="s">
-        <v>269</v>
-      </c>
       <c r="K3" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -3529,19 +3538,19 @@
         <v>15</v>
       </c>
       <c r="B4" s="55" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H4" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="I4">
         <v>264</v>
       </c>
       <c r="J4" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="K4" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -3549,19 +3558,19 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="H5" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="I5">
         <v>28</v>
       </c>
       <c r="J5" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="K5" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -3597,7 +3606,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -3906,7 +3915,7 @@
   <dimension ref="A1:K519"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -4354,10 +4363,74 @@
       </c>
     </row>
     <row r="14" spans="1:11">
-      <c r="A14" s="46"/>
+      <c r="A14" s="46" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="58" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="27">
+        <v>200.7</v>
+      </c>
+      <c r="E14" s="27">
+        <v>200.7</v>
+      </c>
+      <c r="F14" s="27">
+        <v>199.68</v>
+      </c>
+      <c r="G14" s="27">
+        <v>200.57</v>
+      </c>
+      <c r="H14" s="27">
+        <v>198.24</v>
+      </c>
+      <c r="I14" s="27">
+        <v>198.28</v>
+      </c>
+      <c r="J14" s="27">
+        <v>198.7</v>
+      </c>
+      <c r="K14" s="27">
+        <v>201.2</v>
+      </c>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="46"/>
+      <c r="A15" s="46" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="58" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="27">
+        <v>199.23</v>
+      </c>
+      <c r="E15" s="27">
+        <v>201.15</v>
+      </c>
+      <c r="F15" s="27">
+        <v>199.15</v>
+      </c>
+      <c r="G15" s="27">
+        <v>200</v>
+      </c>
+      <c r="H15" s="27">
+        <v>200.6</v>
+      </c>
+      <c r="I15" s="27">
+        <v>202.3</v>
+      </c>
+      <c r="J15" s="27">
+        <v>197.87</v>
+      </c>
+      <c r="K15" s="27">
+        <v>200.18</v>
+      </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="46"/>
@@ -5873,7 +5946,7 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 C4:C5" xr:uid="{5C73BBC5-C68D-4586-BDB5-A3BE48854FB6}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 C4:C5 C14:C15" xr:uid="{5C73BBC5-C68D-4586-BDB5-A3BE48854FB6}"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B1048576" xr:uid="{18FD80CD-FFDC-48A1-BA45-91576461B09B}">
       <formula1>"FRONT EPE, BACK EVA"</formula1>
     </dataValidation>
@@ -5902,10 +5975,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9401EE47-EA52-49C7-BBC0-21F5B88254FB}">
-  <dimension ref="A1:K98"/>
+  <dimension ref="A1:K101"/>
   <sheetViews>
-    <sheetView topLeftCell="B95" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="E101" sqref="E101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -5932,19 +6005,19 @@
         <v>44</v>
       </c>
       <c r="D1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -5955,7 +6028,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D2" s="5">
         <v>45773</v>
@@ -5981,7 +6054,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D3" s="5">
         <v>45773</v>
@@ -6007,7 +6080,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D4" s="5">
         <v>45777</v>
@@ -6033,7 +6106,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D5" s="5">
         <v>45777</v>
@@ -6155,7 +6228,7 @@
         <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="4">
@@ -6173,7 +6246,7 @@
     </row>
     <row r="11" spans="1:11">
       <c r="C11" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="4"/>
@@ -6195,7 +6268,7 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="4">
@@ -6219,7 +6292,7 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="4">
@@ -6243,7 +6316,7 @@
         <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="4">
@@ -6319,7 +6392,7 @@
         <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="4">
@@ -6340,7 +6413,7 @@
         <v>18</v>
       </c>
       <c r="C18" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="4">
@@ -6361,7 +6434,7 @@
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="4">
@@ -6382,7 +6455,7 @@
         <v>16</v>
       </c>
       <c r="C20" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="4">
@@ -6403,7 +6476,7 @@
         <v>16</v>
       </c>
       <c r="C21" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="4">
@@ -6424,7 +6497,7 @@
         <v>16</v>
       </c>
       <c r="C22" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="4">
@@ -6445,7 +6518,7 @@
         <v>16</v>
       </c>
       <c r="C23" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="4">
@@ -6466,7 +6539,7 @@
         <v>16</v>
       </c>
       <c r="C24" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="4">
@@ -6487,7 +6560,7 @@
         <v>16</v>
       </c>
       <c r="C25" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="4">
@@ -6508,7 +6581,7 @@
         <v>16</v>
       </c>
       <c r="C26" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="4">
@@ -6529,7 +6602,7 @@
         <v>16</v>
       </c>
       <c r="C27" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="4">
@@ -6550,7 +6623,7 @@
         <v>5</v>
       </c>
       <c r="C28" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="4">
@@ -6571,7 +6644,7 @@
         <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D29" s="5"/>
       <c r="E29" s="4">
@@ -6592,7 +6665,7 @@
         <v>16</v>
       </c>
       <c r="C30" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D30" s="5"/>
       <c r="E30" s="4">
@@ -6613,7 +6686,7 @@
         <v>16</v>
       </c>
       <c r="C31" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D31" s="5"/>
       <c r="E31" s="4">
@@ -6634,7 +6707,7 @@
         <v>16</v>
       </c>
       <c r="C32" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D32" s="5"/>
       <c r="E32" s="4">
@@ -6655,7 +6728,7 @@
         <v>16</v>
       </c>
       <c r="C33" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D33" s="5"/>
       <c r="E33" s="4">
@@ -6676,7 +6749,7 @@
         <v>16</v>
       </c>
       <c r="C34" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D34" s="5"/>
       <c r="E34" s="4">
@@ -6697,7 +6770,7 @@
         <v>16</v>
       </c>
       <c r="C35" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D35" s="5"/>
       <c r="E35" s="4">
@@ -6718,7 +6791,7 @@
         <v>16</v>
       </c>
       <c r="C36" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D36" s="5"/>
       <c r="E36" s="4">
@@ -6739,7 +6812,7 @@
         <v>4</v>
       </c>
       <c r="C37" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D37" s="5"/>
       <c r="E37" s="4">
@@ -6760,7 +6833,7 @@
         <v>5</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D38" s="5"/>
       <c r="E38" s="4">
@@ -6781,7 +6854,7 @@
         <v>6</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D39" s="5"/>
       <c r="E39" s="4">
@@ -6799,7 +6872,7 @@
         <v>7</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D40" s="5"/>
       <c r="E40" s="4">
@@ -6820,7 +6893,7 @@
         <v>3</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D41" s="5"/>
       <c r="E41" s="4">
@@ -6841,7 +6914,7 @@
         <v>4</v>
       </c>
       <c r="C42" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="4">
@@ -6859,7 +6932,7 @@
         <v>18</v>
       </c>
       <c r="C43" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="4">
@@ -6880,7 +6953,7 @@
         <v>18</v>
       </c>
       <c r="C44" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D44" s="5"/>
       <c r="E44" s="4">
@@ -6901,7 +6974,7 @@
         <v>18</v>
       </c>
       <c r="C45" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D45" s="5"/>
       <c r="E45" s="4">
@@ -6922,7 +6995,7 @@
         <v>3</v>
       </c>
       <c r="C46" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D46" s="5"/>
       <c r="E46" s="4">
@@ -6943,7 +7016,7 @@
         <v>18</v>
       </c>
       <c r="C47" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D47" s="5"/>
       <c r="E47" s="4">
@@ -6964,7 +7037,7 @@
         <v>3</v>
       </c>
       <c r="C48" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D48" s="5"/>
       <c r="E48" s="4">
@@ -6985,7 +7058,7 @@
         <v>18</v>
       </c>
       <c r="C49" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D49" s="5"/>
       <c r="E49" s="4">
@@ -7006,7 +7079,7 @@
         <v>18</v>
       </c>
       <c r="C50" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D50" s="5"/>
       <c r="E50" s="4">
@@ -7027,7 +7100,7 @@
         <v>18</v>
       </c>
       <c r="C51" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D51" s="5"/>
       <c r="E51" s="4">
@@ -7048,7 +7121,7 @@
         <v>3</v>
       </c>
       <c r="C52" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D52" s="5"/>
       <c r="E52" s="4">
@@ -7069,7 +7142,7 @@
         <v>5</v>
       </c>
       <c r="C53" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D53" s="5"/>
       <c r="E53" s="4">
@@ -7090,7 +7163,7 @@
         <v>5</v>
       </c>
       <c r="C54" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D54" s="5"/>
       <c r="E54" s="4">
@@ -7111,7 +7184,7 @@
         <v>5</v>
       </c>
       <c r="C55" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D55" s="5"/>
       <c r="E55" s="4">
@@ -7132,7 +7205,7 @@
         <v>6</v>
       </c>
       <c r="C56" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D56" s="5"/>
       <c r="E56" s="4">
@@ -7153,7 +7226,7 @@
         <v>6</v>
       </c>
       <c r="C57" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D57" s="5"/>
       <c r="E57" s="4">
@@ -7174,7 +7247,7 @@
         <v>6</v>
       </c>
       <c r="C58" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D58" s="5"/>
       <c r="E58" s="4">
@@ -7195,7 +7268,7 @@
         <v>18</v>
       </c>
       <c r="C59" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D59" s="5"/>
       <c r="E59" s="4">
@@ -7216,7 +7289,7 @@
         <v>18</v>
       </c>
       <c r="C60" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D60" s="5"/>
       <c r="E60" s="4">
@@ -7237,7 +7310,7 @@
         <v>16</v>
       </c>
       <c r="C61" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D61" s="5"/>
       <c r="E61" s="4">
@@ -7258,7 +7331,7 @@
         <v>16</v>
       </c>
       <c r="C62" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D62" s="5"/>
       <c r="E62" s="4">
@@ -7279,7 +7352,7 @@
         <v>16</v>
       </c>
       <c r="C63" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D63" s="5"/>
       <c r="E63" s="4">
@@ -7300,7 +7373,7 @@
         <v>16</v>
       </c>
       <c r="C64" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D64" s="5"/>
       <c r="E64" s="4">
@@ -7321,7 +7394,7 @@
         <v>16</v>
       </c>
       <c r="C65" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D65" s="5"/>
       <c r="E65" s="4">
@@ -7342,7 +7415,7 @@
         <v>16</v>
       </c>
       <c r="C66" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D66" s="5"/>
       <c r="E66" s="4">
@@ -7363,7 +7436,7 @@
         <v>16</v>
       </c>
       <c r="C67" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D67" s="5"/>
       <c r="E67" s="4">
@@ -7384,7 +7457,7 @@
         <v>18</v>
       </c>
       <c r="C68" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D68" s="5"/>
       <c r="E68" s="4">
@@ -7405,7 +7478,7 @@
         <v>18</v>
       </c>
       <c r="C69" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D69" s="5"/>
       <c r="E69" s="4">
@@ -7426,7 +7499,7 @@
         <v>4</v>
       </c>
       <c r="C70" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D70" s="5"/>
       <c r="E70" s="4">
@@ -7447,7 +7520,7 @@
         <v>3</v>
       </c>
       <c r="C71" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D71" s="5"/>
       <c r="E71" s="4">
@@ -7468,7 +7541,7 @@
         <v>5</v>
       </c>
       <c r="C72" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D72" s="5"/>
       <c r="E72" s="4">
@@ -7489,7 +7562,7 @@
         <v>6</v>
       </c>
       <c r="C73" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D73" s="5"/>
       <c r="E73" s="4">
@@ -7510,7 +7583,7 @@
         <v>7</v>
       </c>
       <c r="C74" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D74" s="5"/>
       <c r="E74" s="4">
@@ -7531,7 +7604,7 @@
         <v>4</v>
       </c>
       <c r="C75" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D75" s="5"/>
       <c r="E75" s="4">
@@ -7552,7 +7625,7 @@
         <v>3</v>
       </c>
       <c r="C76" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D76" s="5"/>
       <c r="E76" s="4">
@@ -7573,7 +7646,7 @@
         <v>5</v>
       </c>
       <c r="C77" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D77" s="5"/>
       <c r="E77" s="4">
@@ -7594,7 +7667,7 @@
         <v>6</v>
       </c>
       <c r="C78" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D78" s="5"/>
       <c r="E78" s="4">
@@ -7615,7 +7688,7 @@
         <v>7</v>
       </c>
       <c r="C79" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D79" s="5"/>
       <c r="E79" s="4">
@@ -7636,7 +7709,7 @@
         <v>18</v>
       </c>
       <c r="C80" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D80" s="5"/>
       <c r="E80" s="4">
@@ -7657,7 +7730,7 @@
         <v>18</v>
       </c>
       <c r="C81" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D81" s="5"/>
       <c r="E81" s="4">
@@ -7678,7 +7751,7 @@
         <v>18</v>
       </c>
       <c r="C82" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D82" s="5"/>
       <c r="E82" s="4">
@@ -7699,7 +7772,7 @@
         <v>18</v>
       </c>
       <c r="C83" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D83" s="5"/>
       <c r="E83" s="4">
@@ -7720,7 +7793,7 @@
         <v>18</v>
       </c>
       <c r="C84" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D84" s="5"/>
       <c r="E84" s="4">
@@ -7741,7 +7814,7 @@
         <v>18</v>
       </c>
       <c r="C85" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D85" s="5"/>
       <c r="E85" s="4">
@@ -7762,7 +7835,7 @@
         <v>18</v>
       </c>
       <c r="C86" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D86" s="5"/>
       <c r="E86" s="4">
@@ -7783,7 +7856,7 @@
         <v>18</v>
       </c>
       <c r="C87" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D87" s="5"/>
       <c r="E87" s="4">
@@ -7804,7 +7877,7 @@
         <v>18</v>
       </c>
       <c r="C88" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D88" s="5"/>
       <c r="E88" s="4">
@@ -7825,7 +7898,7 @@
         <v>18</v>
       </c>
       <c r="C89" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D89" s="5"/>
       <c r="E89" s="4">
@@ -7846,7 +7919,7 @@
         <v>18</v>
       </c>
       <c r="C90" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D90" s="5"/>
       <c r="E90" s="4">
@@ -7867,7 +7940,7 @@
         <v>18</v>
       </c>
       <c r="C91" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D91" s="5"/>
       <c r="E91" s="4">
@@ -7888,7 +7961,7 @@
         <v>12</v>
       </c>
       <c r="C92" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D92" s="5"/>
       <c r="E92" s="4">
@@ -7909,7 +7982,7 @@
         <v>12</v>
       </c>
       <c r="C93" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D93" s="5"/>
       <c r="E93" s="4">
@@ -7927,7 +8000,7 @@
         <v>18</v>
       </c>
       <c r="C94" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D94" s="56"/>
       <c r="E94" s="4">
@@ -7945,7 +8018,7 @@
         <v>18</v>
       </c>
       <c r="C95" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D95" s="56"/>
       <c r="E95" s="4">
@@ -7963,7 +8036,7 @@
         <v>18</v>
       </c>
       <c r="C96" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D96" s="56"/>
       <c r="E96" s="4">
@@ -7977,40 +8050,92 @@
       </c>
     </row>
     <row r="97" spans="1:8">
-      <c r="A97" s="58"/>
-      <c r="B97" s="58" t="s">
+      <c r="B97" t="s">
         <v>16</v>
       </c>
-      <c r="C97" s="58" t="s">
-        <v>131</v>
+      <c r="C97" t="s">
+        <v>132</v>
       </c>
       <c r="D97" s="56"/>
       <c r="E97" s="4">
         <v>45951</v>
       </c>
-      <c r="F97" s="58"/>
-      <c r="G97" s="58"/>
-      <c r="H97" s="58" t="s">
+      <c r="H97" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="98" spans="1:8">
-      <c r="A98" s="58"/>
-      <c r="B98" s="58" t="s">
+      <c r="B98" t="s">
         <v>16</v>
       </c>
-      <c r="C98" s="58" t="s">
-        <v>132</v>
+      <c r="C98" t="s">
+        <v>133</v>
       </c>
       <c r="D98" s="56"/>
       <c r="E98" s="4">
         <v>45951</v>
       </c>
-      <c r="F98" s="58"/>
-      <c r="G98" s="58"/>
-      <c r="H98" s="58" t="s">
+      <c r="H98" t="s">
         <v>36</v>
       </c>
+    </row>
+    <row r="99" spans="1:8">
+      <c r="A99" s="58" t="s">
+        <v>2</v>
+      </c>
+      <c r="B99" s="58" t="s">
+        <v>6</v>
+      </c>
+      <c r="C99" s="58" t="s">
+        <v>66</v>
+      </c>
+      <c r="D99" s="56"/>
+      <c r="E99" s="4">
+        <v>45946</v>
+      </c>
+      <c r="F99" s="58"/>
+      <c r="G99" s="58"/>
+      <c r="H99" s="58" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8">
+      <c r="A100" s="58" t="s">
+        <v>2</v>
+      </c>
+      <c r="B100" s="58" t="s">
+        <v>5</v>
+      </c>
+      <c r="C100" s="58" t="s">
+        <v>66</v>
+      </c>
+      <c r="D100" s="56"/>
+      <c r="E100" s="4">
+        <v>45946</v>
+      </c>
+      <c r="F100" s="58"/>
+      <c r="G100" s="58"/>
+      <c r="H100" s="58" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8">
+      <c r="A101" s="58" t="s">
+        <v>2</v>
+      </c>
+      <c r="B101" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="C101" s="58" t="s">
+        <v>66</v>
+      </c>
+      <c r="D101" s="56"/>
+      <c r="E101" s="4">
+        <v>45946</v>
+      </c>
+      <c r="F101" s="58"/>
+      <c r="G101" s="58"/>
+      <c r="H101" s="58"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -8083,14 +8208,14 @@
       <c r="A1" s="28"/>
       <c r="B1" s="29"/>
       <c r="C1" s="30" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D1" s="31"/>
       <c r="E1" s="30"/>
       <c r="F1" s="31"/>
       <c r="G1" s="32"/>
       <c r="H1" s="44" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="I1" s="32"/>
       <c r="J1" s="29"/>
@@ -8103,19 +8228,19 @@
         <v>44</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D2" s="36"/>
       <c r="E2" s="37" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F2" s="38"/>
       <c r="G2" s="35" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="37" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="J2" s="38"/>
     </row>
@@ -8188,7 +8313,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="45" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C5" s="45">
         <v>75</v>
@@ -8284,7 +8409,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="45" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C8" s="45">
         <v>166</v>
@@ -8316,7 +8441,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="45" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C9" s="45">
         <v>80</v>
@@ -8336,7 +8461,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="45" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C10" s="45">
         <v>58</v>
@@ -8356,7 +8481,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="45" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C11" s="45">
         <v>11</v>
@@ -8376,7 +8501,7 @@
         <v>2</v>
       </c>
       <c r="B12" s="45" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C12" s="45">
         <v>2</v>
@@ -8438,10 +8563,10 @@
         <v>44</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="6" customFormat="1">
@@ -8465,7 +8590,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C3" s="48">
         <v>14.6</v>
@@ -8479,7 +8604,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -8487,7 +8612,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -8495,7 +8620,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -8503,7 +8628,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -8511,7 +8636,7 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C8" s="48">
         <v>16.5</v>
@@ -8525,7 +8650,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -8533,7 +8658,7 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -8541,7 +8666,7 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -8549,7 +8674,7 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -8557,7 +8682,7 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C13" s="48">
         <v>42.8</v>
@@ -8571,7 +8696,7 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C14" s="48">
         <v>69.3</v>
@@ -8585,7 +8710,7 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C15" s="48">
         <v>68.599999999999994</v>
@@ -8599,7 +8724,7 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C16" s="48">
         <v>88.7</v>
@@ -8627,14 +8752,14 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
     <col min="1" max="1" width="13.85546875" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="35" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" customWidth="1"/>
     <col min="5" max="6" width="12.5703125" customWidth="1"/>
     <col min="7" max="7" width="12.28515625" customWidth="1"/>
@@ -8650,25 +8775,25 @@
         <v>44</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -8676,7 +8801,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C2" t="s">
         <v>34</v>
@@ -8706,7 +8831,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C3" t="s">
         <v>34</v>
@@ -8736,7 +8861,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D4">
         <v>10.16</v>
@@ -8763,7 +8888,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D5">
         <v>9.66</v>
@@ -8790,7 +8915,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C6" t="s">
         <v>34</v>
@@ -8820,7 +8945,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C7" t="s">
         <v>34</v>
@@ -8850,7 +8975,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D8">
         <v>10.84</v>
@@ -8877,7 +9002,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D9">
         <v>10.15</v>
@@ -8904,7 +9029,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C10" t="s">
         <v>34</v>
@@ -8934,7 +9059,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C11" t="s">
         <v>34</v>
@@ -8964,7 +9089,7 @@
         <v>2</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C12" t="s">
         <v>34</v>
@@ -8994,7 +9119,7 @@
         <v>2</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C13" t="s">
         <v>34</v>
@@ -9019,17 +9144,65 @@
         <v>10.188000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
-      <c r="B14" s="8"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="B15" s="8"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
+    <row r="14" spans="1:9" ht="15">
+      <c r="A14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="58" t="s">
+        <v>173</v>
+      </c>
+      <c r="C14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14">
+        <v>10.44</v>
+      </c>
+      <c r="E14">
+        <v>10.42</v>
+      </c>
+      <c r="F14" s="7">
+        <v>10.48</v>
+      </c>
+      <c r="G14" s="7">
+        <v>10.61</v>
+      </c>
+      <c r="H14" s="7">
+        <v>10.61</v>
+      </c>
+      <c r="I14">
+        <f>AVERAGE(Table10[[#This Row],[min value 1 ]:[min value 5]])</f>
+        <v>10.512</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15">
+      <c r="A15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="58" t="s">
+        <v>174</v>
+      </c>
+      <c r="C15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15">
+        <v>10.55</v>
+      </c>
+      <c r="E15">
+        <v>10.66</v>
+      </c>
+      <c r="F15" s="7">
+        <v>10.67</v>
+      </c>
+      <c r="G15" s="7">
+        <v>10.63</v>
+      </c>
+      <c r="H15" s="7">
+        <v>10.66</v>
+      </c>
+      <c r="I15">
+        <f>AVERAGE(Table10[[#This Row],[min value 1 ]:[min value 5]])</f>
+        <v>10.634</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -9080,7 +9253,7 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="B1" t="s">
         <v>30</v>
@@ -9089,22 +9262,22 @@
         <v>44</v>
       </c>
       <c r="D1" s="50" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="E1" s="50" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="F1" s="50" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="G1" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="H1" s="50" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="I1" s="50" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -9112,10 +9285,10 @@
         <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="C2" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="D2" s="50">
         <f>VALUE(MID(LEFT(Table4[[#This Row],[VENDOR NAME]], LEN(Table4[[#This Row],[VENDOR NAME]]) - 2), FIND(" ", Table4[[#This Row],[VENDOR NAME]]) + 1, LEN(Table4[[#This Row],[VENDOR NAME]])))</f>
@@ -9135,7 +9308,7 @@
         <v>1</v>
       </c>
       <c r="I2" s="50" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -9143,10 +9316,10 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C3" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="D3" s="50">
         <f>VALUE(MID(LEFT(Table4[[#This Row],[VENDOR NAME]], LEN(Table4[[#This Row],[VENDOR NAME]]) - 2), FIND(" ", Table4[[#This Row],[VENDOR NAME]]) + 1, LEN(Table4[[#This Row],[VENDOR NAME]])))</f>
@@ -9168,10 +9341,10 @@
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="C4" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="D4" s="50">
         <f>VALUE(MID(LEFT(Table4[[#This Row],[VENDOR NAME]], LEN(Table4[[#This Row],[VENDOR NAME]]) - 2), FIND(" ", Table4[[#This Row],[VENDOR NAME]]) + 1, LEN(Table4[[#This Row],[VENDOR NAME]])))</f>
@@ -9193,10 +9366,10 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C5" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="D5" s="50">
         <f>VALUE(MID(LEFT(Table4[[#This Row],[VENDOR NAME]], LEN(Table4[[#This Row],[VENDOR NAME]]) - 2), FIND(" ", Table4[[#This Row],[VENDOR NAME]]) + 1, LEN(Table4[[#This Row],[VENDOR NAME]])))</f>
@@ -9219,10 +9392,10 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C6" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="D6" s="50">
         <f>VALUE(MID(LEFT(Table4[[#This Row],[VENDOR NAME]], LEN(Table4[[#This Row],[VENDOR NAME]]) - 2), FIND(" ", Table4[[#This Row],[VENDOR NAME]]) + 1, LEN(Table4[[#This Row],[VENDOR NAME]])))</f>
@@ -9245,10 +9418,10 @@
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="C7" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="D7" s="50">
         <f>VALUE(MID(LEFT(Table4[[#This Row],[VENDOR NAME]], LEN(Table4[[#This Row],[VENDOR NAME]]) - 2), FIND(" ", Table4[[#This Row],[VENDOR NAME]]) + 1, LEN(Table4[[#This Row],[VENDOR NAME]])))</f>
@@ -9270,10 +9443,10 @@
         <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C8" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="D8" s="50">
         <f>VALUE(MID(LEFT(Table4[[#This Row],[VENDOR NAME]], LEN(Table4[[#This Row],[VENDOR NAME]]) - 2), FIND(" ", Table4[[#This Row],[VENDOR NAME]]) + 1, LEN(Table4[[#This Row],[VENDOR NAME]])))</f>
@@ -9296,10 +9469,10 @@
         <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C9" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="D9" s="50">
         <f>VALUE(MID(LEFT(Table4[[#This Row],[VENDOR NAME]], LEN(Table4[[#This Row],[VENDOR NAME]]) - 2), FIND(" ", Table4[[#This Row],[VENDOR NAME]]) + 1, LEN(Table4[[#This Row],[VENDOR NAME]])))</f>
@@ -9357,10 +9530,10 @@
         <v>44</v>
       </c>
       <c r="C1" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="D1" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -9368,7 +9541,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C3" s="10">
         <v>0.63541666666666663</v>
@@ -9382,7 +9555,7 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C4" s="10">
         <v>0.59791666666666665</v>
@@ -9396,7 +9569,7 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="C5" s="10">
         <v>0.84722222222222221</v>
@@ -9410,7 +9583,7 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C6" s="10">
         <v>0.50972222222222219</v>
@@ -9424,7 +9597,7 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C7" s="10">
         <v>0.50347222222222221</v>
@@ -9438,7 +9611,7 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="C8" s="10">
         <v>9.375E-2</v>
@@ -9452,7 +9625,7 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="C9" s="10">
         <v>9.0277777777777776E-2</v>

</xml_diff>